<commit_message>
Updated: št 10. 12. 2020
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_AgTests_District.xlsx
+++ b/OpenData_Slovakia_Covid_AgTests_District.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2953"/>
+  <dimension ref="A1:E3027"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -13647,13 +13647,13 @@
         </is>
       </c>
       <c r="C701">
-        <v>213</v>
+        <v>0</v>
       </c>
       <c r="D701">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E701">
-        <v>234</v>
+        <v>0</v>
       </c>
     </row>
     <row r="702">
@@ -34680,13 +34680,13 @@
         </is>
       </c>
       <c r="C1813">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D1813">
         <v>0</v>
       </c>
       <c r="E1813">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1814">
@@ -35929,13 +35929,13 @@
         </is>
       </c>
       <c r="C1879">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D1879">
         <v>0</v>
       </c>
       <c r="E1879">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1880">
@@ -38821,13 +38821,13 @@
         </is>
       </c>
       <c r="C2032">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D2032">
         <v>0</v>
       </c>
       <c r="E2032">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2033">
@@ -40089,13 +40089,13 @@
         </is>
       </c>
       <c r="C2099">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D2099">
         <v>0</v>
       </c>
       <c r="E2099">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2100">
@@ -41414,13 +41414,13 @@
         </is>
       </c>
       <c r="C2169">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="D2169">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2169">
-        <v>352</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2170">
@@ -42758,13 +42758,13 @@
         </is>
       </c>
       <c r="C2240">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="D2240">
         <v>0</v>
       </c>
       <c r="E2240">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2241">
@@ -44064,13 +44064,13 @@
         </is>
       </c>
       <c r="C2309">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="D2309">
         <v>0</v>
       </c>
       <c r="E2309">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2310">
@@ -46614,13 +46614,13 @@
         </is>
       </c>
       <c r="C2444">
-        <v>670</v>
+        <v>697</v>
       </c>
       <c r="D2444">
         <v>15</v>
       </c>
       <c r="E2444">
-        <v>685</v>
+        <v>712</v>
       </c>
     </row>
     <row r="2445">
@@ -46861,13 +46861,13 @@
         </is>
       </c>
       <c r="C2457">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2457">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2457">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2458">
@@ -48039,13 +48039,13 @@
         </is>
       </c>
       <c r="C2519">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D2519">
         <v>4</v>
       </c>
       <c r="E2519">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2520">
@@ -49293,13 +49293,13 @@
         </is>
       </c>
       <c r="C2585">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="D2585">
         <v>26</v>
       </c>
       <c r="E2585">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2586">
@@ -50338,13 +50338,13 @@
         </is>
       </c>
       <c r="C2640">
-        <v>1641</v>
+        <v>1658</v>
       </c>
       <c r="D2640">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E2640">
-        <v>1653</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="2641">
@@ -51744,13 +51744,13 @@
         </is>
       </c>
       <c r="C2714">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="D2714">
         <v>15</v>
       </c>
       <c r="E2714">
-        <v>265</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2715">
@@ -52713,13 +52713,13 @@
         </is>
       </c>
       <c r="C2765">
-        <v>644</v>
+        <v>671</v>
       </c>
       <c r="D2765">
         <v>38</v>
       </c>
       <c r="E2765">
-        <v>682</v>
+        <v>709</v>
       </c>
     </row>
     <row r="2766">
@@ -54214,13 +54214,13 @@
         </is>
       </c>
       <c r="C2844">
-        <v>393</v>
+        <v>518</v>
       </c>
       <c r="D2844">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E2844">
-        <v>407</v>
+        <v>538</v>
       </c>
     </row>
     <row r="2845">
@@ -54233,13 +54233,13 @@
         </is>
       </c>
       <c r="C2845">
-        <v>719</v>
+        <v>757</v>
       </c>
       <c r="D2845">
         <v>37</v>
       </c>
       <c r="E2845">
-        <v>756</v>
+        <v>794</v>
       </c>
     </row>
     <row r="2846">
@@ -54252,13 +54252,13 @@
         </is>
       </c>
       <c r="C2846">
-        <v>908</v>
+        <v>1132</v>
       </c>
       <c r="D2846">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="E2846">
-        <v>960</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="2847">
@@ -54293,10 +54293,10 @@
         <v>260</v>
       </c>
       <c r="D2848">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2848">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2849">
@@ -54328,13 +54328,13 @@
         </is>
       </c>
       <c r="C2850">
-        <v>500</v>
+        <v>597</v>
       </c>
       <c r="D2850">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E2850">
-        <v>514</v>
+        <v>615</v>
       </c>
     </row>
     <row r="2851">
@@ -54404,13 +54404,13 @@
         </is>
       </c>
       <c r="C2854">
-        <v>316</v>
+        <v>358</v>
       </c>
       <c r="D2854">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E2854">
-        <v>398</v>
+        <v>443</v>
       </c>
     </row>
     <row r="2855">
@@ -54822,13 +54822,13 @@
         </is>
       </c>
       <c r="C2876">
-        <v>105</v>
+        <v>475</v>
       </c>
       <c r="D2876">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E2876">
-        <v>106</v>
+        <v>496</v>
       </c>
     </row>
     <row r="2877">
@@ -54841,13 +54841,13 @@
         </is>
       </c>
       <c r="C2877">
-        <v>395</v>
+        <v>590</v>
       </c>
       <c r="D2877">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E2877">
-        <v>414</v>
+        <v>619</v>
       </c>
     </row>
     <row r="2878">
@@ -55065,17 +55065,17 @@
       </c>
       <c r="B2889" t="inlineStr">
         <is>
-          <t>Okres Skalica</t>
+          <t>Okres Senica</t>
         </is>
       </c>
       <c r="C2889">
-        <v>5</v>
+        <v>275</v>
       </c>
       <c r="D2889">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E2889">
-        <v>5</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2890">
@@ -55084,17 +55084,17 @@
       </c>
       <c r="B2890" t="inlineStr">
         <is>
-          <t>Okres Snina</t>
+          <t>Okres Skalica</t>
         </is>
       </c>
       <c r="C2890">
-        <v>148</v>
+        <v>5</v>
       </c>
       <c r="D2890">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="E2890">
-        <v>177</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2891">
@@ -55103,17 +55103,17 @@
       </c>
       <c r="B2891" t="inlineStr">
         <is>
-          <t>Okres Sobrance</t>
+          <t>Okres Snina</t>
         </is>
       </c>
       <c r="C2891">
-        <v>6</v>
+        <v>148</v>
       </c>
       <c r="D2891">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E2891">
-        <v>6</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2892">
@@ -55122,17 +55122,17 @@
       </c>
       <c r="B2892" t="inlineStr">
         <is>
-          <t>Okres Spišská Nová Ves</t>
+          <t>Okres Sobrance</t>
         </is>
       </c>
       <c r="C2892">
-        <v>324</v>
+        <v>6</v>
       </c>
       <c r="D2892">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E2892">
-        <v>349</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2893">
@@ -55141,17 +55141,17 @@
       </c>
       <c r="B2893" t="inlineStr">
         <is>
-          <t>Okres Stará Ľubovňa</t>
+          <t>Okres Spišská Nová Ves</t>
         </is>
       </c>
       <c r="C2893">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D2893">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E2893">
-        <v>342</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2894">
@@ -55160,17 +55160,17 @@
       </c>
       <c r="B2894" t="inlineStr">
         <is>
-          <t>Okres Svidník</t>
+          <t>Okres Stará Ľubovňa</t>
         </is>
       </c>
       <c r="C2894">
-        <v>62</v>
+        <v>329</v>
       </c>
       <c r="D2894">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2894">
-        <v>73</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2895">
@@ -55179,17 +55179,17 @@
       </c>
       <c r="B2895" t="inlineStr">
         <is>
-          <t>Okres Topoľčany</t>
+          <t>Okres Svidník</t>
         </is>
       </c>
       <c r="C2895">
-        <v>3572</v>
+        <v>62</v>
       </c>
       <c r="D2895">
-        <v>340</v>
+        <v>11</v>
       </c>
       <c r="E2895">
-        <v>3912</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2896">
@@ -55198,17 +55198,17 @@
       </c>
       <c r="B2896" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Topoľčany</t>
         </is>
       </c>
       <c r="C2896">
-        <v>556</v>
+        <v>3572</v>
       </c>
       <c r="D2896">
-        <v>9</v>
+        <v>340</v>
       </c>
       <c r="E2896">
-        <v>565</v>
+        <v>3912</v>
       </c>
     </row>
     <row r="2897">
@@ -55217,17 +55217,17 @@
       </c>
       <c r="B2897" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Trebišov</t>
         </is>
       </c>
       <c r="C2897">
-        <v>2142</v>
+        <v>556</v>
       </c>
       <c r="D2897">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="E2897">
-        <v>2337</v>
+        <v>565</v>
       </c>
     </row>
     <row r="2898">
@@ -55236,17 +55236,17 @@
       </c>
       <c r="B2898" t="inlineStr">
         <is>
-          <t>Okres Trnava</t>
+          <t>Okres Trenčín</t>
         </is>
       </c>
       <c r="C2898">
-        <v>362</v>
+        <v>2142</v>
       </c>
       <c r="D2898">
-        <v>10</v>
+        <v>195</v>
       </c>
       <c r="E2898">
-        <v>372</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="2899">
@@ -55255,17 +55255,17 @@
       </c>
       <c r="B2899" t="inlineStr">
         <is>
-          <t>Okres Tvrdošín</t>
+          <t>Okres Trnava</t>
         </is>
       </c>
       <c r="C2899">
-        <v>167</v>
+        <v>362</v>
       </c>
       <c r="D2899">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E2899">
-        <v>185</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2900">
@@ -55274,17 +55274,17 @@
       </c>
       <c r="B2900" t="inlineStr">
         <is>
-          <t>Okres Veľký Krtíš</t>
+          <t>Okres Tvrdošín</t>
         </is>
       </c>
       <c r="C2900">
-        <v>256</v>
+        <v>167</v>
       </c>
       <c r="D2900">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2900">
-        <v>275</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2901">
@@ -55293,17 +55293,17 @@
       </c>
       <c r="B2901" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Veľký Krtíš</t>
         </is>
       </c>
       <c r="C2901">
-        <v>116</v>
+        <v>256</v>
       </c>
       <c r="D2901">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E2901">
-        <v>126</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2902">
@@ -55312,17 +55312,17 @@
       </c>
       <c r="B2902" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Zvolen</t>
         </is>
       </c>
       <c r="C2902">
-        <v>197</v>
+        <v>116</v>
       </c>
       <c r="D2902">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E2902">
-        <v>203</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2903">
@@ -55331,55 +55331,55 @@
       </c>
       <c r="B2903" t="inlineStr">
         <is>
-          <t>Okres Žilina</t>
+          <t>Okres Žarnovica</t>
         </is>
       </c>
       <c r="C2903">
-        <v>266</v>
+        <v>1547</v>
       </c>
       <c r="D2903">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="E2903">
-        <v>281</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="2904">
       <c r="A2904" s="2">
-        <v>44173</v>
+        <v>44172</v>
       </c>
       <c r="B2904" t="inlineStr">
         <is>
-          <t>Okres Banská Bystrica</t>
+          <t>Okres Žiar nad Hronom</t>
         </is>
       </c>
       <c r="C2904">
-        <v>477</v>
+        <v>197</v>
       </c>
       <c r="D2904">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="E2904">
-        <v>517</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2905">
       <c r="A2905" s="2">
-        <v>44173</v>
+        <v>44172</v>
       </c>
       <c r="B2905" t="inlineStr">
         <is>
-          <t>Okres Bratislava I</t>
+          <t>Okres Žilina</t>
         </is>
       </c>
       <c r="C2905">
-        <v>148</v>
+        <v>266</v>
       </c>
       <c r="D2905">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E2905">
-        <v>153</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2906">
@@ -55388,17 +55388,17 @@
       </c>
       <c r="B2906" t="inlineStr">
         <is>
-          <t>Okres Bratislava II</t>
+          <t>Okres Bánovce nad Bebravou</t>
         </is>
       </c>
       <c r="C2906">
-        <v>346</v>
+        <v>189</v>
       </c>
       <c r="D2906">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E2906">
-        <v>361</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2907">
@@ -55407,17 +55407,17 @@
       </c>
       <c r="B2907" t="inlineStr">
         <is>
-          <t>Okres Bratislava III</t>
+          <t>Okres Banská Bystrica</t>
         </is>
       </c>
       <c r="C2907">
-        <v>690</v>
+        <v>527</v>
       </c>
       <c r="D2907">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="E2907">
-        <v>708</v>
+        <v>592</v>
       </c>
     </row>
     <row r="2908">
@@ -55426,17 +55426,17 @@
       </c>
       <c r="B2908" t="inlineStr">
         <is>
-          <t>Okres Bratislava V</t>
+          <t>Okres Bardejov</t>
         </is>
       </c>
       <c r="C2908">
-        <v>1</v>
+        <v>803</v>
       </c>
       <c r="D2908">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E2908">
-        <v>1</v>
+        <v>827</v>
       </c>
     </row>
     <row r="2909">
@@ -55445,17 +55445,17 @@
       </c>
       <c r="B2909" t="inlineStr">
         <is>
-          <t>Okres Dolný Kubín</t>
+          <t>Okres Bratislava I</t>
         </is>
       </c>
       <c r="C2909">
-        <v>168</v>
+        <v>278</v>
       </c>
       <c r="D2909">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2909">
-        <v>181</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2910">
@@ -55464,17 +55464,17 @@
       </c>
       <c r="B2910" t="inlineStr">
         <is>
-          <t>Okres Dunajská Streda</t>
+          <t>Okres Bratislava II</t>
         </is>
       </c>
       <c r="C2910">
-        <v>540</v>
+        <v>1919</v>
       </c>
       <c r="D2910">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E2910">
-        <v>580</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="2911">
@@ -55483,17 +55483,17 @@
       </c>
       <c r="B2911" t="inlineStr">
         <is>
-          <t>Okres Galanta</t>
+          <t>Okres Bratislava III</t>
         </is>
       </c>
       <c r="C2911">
-        <v>508</v>
+        <v>844</v>
       </c>
       <c r="D2911">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="E2911">
-        <v>548</v>
+        <v>862</v>
       </c>
     </row>
     <row r="2912">
@@ -55502,17 +55502,17 @@
       </c>
       <c r="B2912" t="inlineStr">
         <is>
-          <t>Okres Humenné</t>
+          <t>Okres Bratislava V</t>
         </is>
       </c>
       <c r="C2912">
-        <v>150</v>
+        <v>725</v>
       </c>
       <c r="D2912">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="E2912">
-        <v>161</v>
+        <v>769</v>
       </c>
     </row>
     <row r="2913">
@@ -55521,17 +55521,17 @@
       </c>
       <c r="B2913" t="inlineStr">
         <is>
-          <t>Okres Ilava</t>
+          <t>Okres Brezno</t>
         </is>
       </c>
       <c r="C2913">
-        <v>220</v>
+        <v>351</v>
       </c>
       <c r="D2913">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E2913">
-        <v>277</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2914">
@@ -55540,17 +55540,17 @@
       </c>
       <c r="B2914" t="inlineStr">
         <is>
-          <t>Okres Kežmarok</t>
+          <t>Okres Čadca</t>
         </is>
       </c>
       <c r="C2914">
-        <v>152</v>
+        <v>570</v>
       </c>
       <c r="D2914">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="E2914">
-        <v>184</v>
+        <v>619</v>
       </c>
     </row>
     <row r="2915">
@@ -55559,17 +55559,17 @@
       </c>
       <c r="B2915" t="inlineStr">
         <is>
-          <t>Okres Komárno</t>
+          <t>Okres Detva</t>
         </is>
       </c>
       <c r="C2915">
-        <v>369</v>
+        <v>199</v>
       </c>
       <c r="D2915">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E2915">
-        <v>380</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2916">
@@ -55578,17 +55578,17 @@
       </c>
       <c r="B2916" t="inlineStr">
         <is>
-          <t>Okres Košice I</t>
+          <t>Okres Dolný Kubín</t>
         </is>
       </c>
       <c r="C2916">
-        <v>525</v>
+        <v>171</v>
       </c>
       <c r="D2916">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E2916">
-        <v>570</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2917">
@@ -55597,17 +55597,17 @@
       </c>
       <c r="B2917" t="inlineStr">
         <is>
-          <t>Okres Košice II</t>
+          <t>Okres Dunajská Streda</t>
         </is>
       </c>
       <c r="C2917">
-        <v>184</v>
+        <v>568</v>
       </c>
       <c r="D2917">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="E2917">
-        <v>191</v>
+        <v>608</v>
       </c>
     </row>
     <row r="2918">
@@ -55616,17 +55616,17 @@
       </c>
       <c r="B2918" t="inlineStr">
         <is>
-          <t>Okres Košice IV</t>
+          <t>Okres Galanta</t>
         </is>
       </c>
       <c r="C2918">
-        <v>154</v>
+        <v>607</v>
       </c>
       <c r="D2918">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="E2918">
-        <v>163</v>
+        <v>649</v>
       </c>
     </row>
     <row r="2919">
@@ -55635,17 +55635,17 @@
       </c>
       <c r="B2919" t="inlineStr">
         <is>
-          <t>Okres Krupina</t>
+          <t>Okres Gelnica</t>
         </is>
       </c>
       <c r="C2919">
-        <v>7</v>
+        <v>148</v>
       </c>
       <c r="D2919">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E2919">
-        <v>7</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2920">
@@ -55654,17 +55654,17 @@
       </c>
       <c r="B2920" t="inlineStr">
         <is>
-          <t>Okres Levice</t>
+          <t>Okres Hlohovec</t>
         </is>
       </c>
       <c r="C2920">
-        <v>529</v>
+        <v>47</v>
       </c>
       <c r="D2920">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E2920">
-        <v>558</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2921">
@@ -55673,17 +55673,17 @@
       </c>
       <c r="B2921" t="inlineStr">
         <is>
-          <t>Okres Levoča</t>
+          <t>Okres Humenné</t>
         </is>
       </c>
       <c r="C2921">
-        <v>337</v>
+        <v>379</v>
       </c>
       <c r="D2921">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E2921">
-        <v>370</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2922">
@@ -55692,17 +55692,17 @@
       </c>
       <c r="B2922" t="inlineStr">
         <is>
-          <t>Okres Liptovský Mikuláš</t>
+          <t>Okres Ilava</t>
         </is>
       </c>
       <c r="C2922">
-        <v>984</v>
+        <v>229</v>
       </c>
       <c r="D2922">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E2922">
-        <v>1052</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2923">
@@ -55711,17 +55711,17 @@
       </c>
       <c r="B2923" t="inlineStr">
         <is>
-          <t>Okres Lučenec</t>
+          <t>Okres Kežmarok</t>
         </is>
       </c>
       <c r="C2923">
-        <v>267</v>
+        <v>371</v>
       </c>
       <c r="D2923">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="E2923">
-        <v>280</v>
+        <v>430</v>
       </c>
     </row>
     <row r="2924">
@@ -55730,17 +55730,17 @@
       </c>
       <c r="B2924" t="inlineStr">
         <is>
-          <t>Okres Martin</t>
+          <t>Okres Komárno</t>
         </is>
       </c>
       <c r="C2924">
-        <v>40</v>
+        <v>704</v>
       </c>
       <c r="D2924">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E2924">
-        <v>40</v>
+        <v>729</v>
       </c>
     </row>
     <row r="2925">
@@ -55749,17 +55749,17 @@
       </c>
       <c r="B2925" t="inlineStr">
         <is>
-          <t>Okres Michalovce</t>
+          <t>Okres Košice I</t>
         </is>
       </c>
       <c r="C2925">
-        <v>376</v>
+        <v>725</v>
       </c>
       <c r="D2925">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="E2925">
-        <v>441</v>
+        <v>771</v>
       </c>
     </row>
     <row r="2926">
@@ -55768,17 +55768,17 @@
       </c>
       <c r="B2926" t="inlineStr">
         <is>
-          <t>Okres Myjava</t>
+          <t>Okres Košice II</t>
         </is>
       </c>
       <c r="C2926">
-        <v>186</v>
+        <v>529</v>
       </c>
       <c r="D2926">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="E2926">
-        <v>225</v>
+        <v>538</v>
       </c>
     </row>
     <row r="2927">
@@ -55787,17 +55787,17 @@
       </c>
       <c r="B2927" t="inlineStr">
         <is>
-          <t>Okres Nitra</t>
+          <t>Okres Košice IV</t>
         </is>
       </c>
       <c r="C2927">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="D2927">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2927">
-        <v>226</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2928">
@@ -55806,17 +55806,17 @@
       </c>
       <c r="B2928" t="inlineStr">
         <is>
-          <t>Okres Nové Mesto nad Váhom</t>
+          <t>Okres Krupina</t>
         </is>
       </c>
       <c r="C2928">
-        <v>245</v>
+        <v>7</v>
       </c>
       <c r="D2928">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E2928">
-        <v>265</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2929">
@@ -55825,17 +55825,17 @@
       </c>
       <c r="B2929" t="inlineStr">
         <is>
-          <t>Okres Nové Zámky</t>
+          <t>Okres Levice</t>
         </is>
       </c>
       <c r="C2929">
-        <v>4439</v>
+        <v>2089</v>
       </c>
       <c r="D2929">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="E2929">
-        <v>4653</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="2930">
@@ -55844,17 +55844,17 @@
       </c>
       <c r="B2930" t="inlineStr">
         <is>
-          <t>Okres Partizánske</t>
+          <t>Okres Levoča</t>
         </is>
       </c>
       <c r="C2930">
-        <v>406</v>
+        <v>337</v>
       </c>
       <c r="D2930">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E2930">
-        <v>451</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2931">
@@ -55863,17 +55863,17 @@
       </c>
       <c r="B2931" t="inlineStr">
         <is>
-          <t>Okres Pezinok</t>
+          <t>Okres Liptovský Mikuláš</t>
         </is>
       </c>
       <c r="C2931">
-        <v>240</v>
+        <v>984</v>
       </c>
       <c r="D2931">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="E2931">
-        <v>254</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="2932">
@@ -55882,17 +55882,17 @@
       </c>
       <c r="B2932" t="inlineStr">
         <is>
-          <t>Okres Piešťany</t>
+          <t>Okres Lučenec</t>
         </is>
       </c>
       <c r="C2932">
-        <v>55</v>
+        <v>283</v>
       </c>
       <c r="D2932">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E2932">
-        <v>61</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2933">
@@ -55901,17 +55901,17 @@
       </c>
       <c r="B2933" t="inlineStr">
         <is>
-          <t>Okres Poprad</t>
+          <t>Okres Malacky</t>
         </is>
       </c>
       <c r="C2933">
-        <v>295</v>
+        <v>179</v>
       </c>
       <c r="D2933">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="E2933">
-        <v>326</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2934">
@@ -55920,17 +55920,17 @@
       </c>
       <c r="B2934" t="inlineStr">
         <is>
-          <t>Okres Považská Bystrica</t>
+          <t>Okres Martin</t>
         </is>
       </c>
       <c r="C2934">
-        <v>31</v>
+        <v>193</v>
       </c>
       <c r="D2934">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E2934">
-        <v>40</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2935">
@@ -55939,17 +55939,17 @@
       </c>
       <c r="B2935" t="inlineStr">
         <is>
-          <t>Okres Prievidza</t>
+          <t>Okres Medzilaborce</t>
         </is>
       </c>
       <c r="C2935">
-        <v>522</v>
+        <v>71</v>
       </c>
       <c r="D2935">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="E2935">
-        <v>574</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2936">
@@ -55958,17 +55958,17 @@
       </c>
       <c r="B2936" t="inlineStr">
         <is>
-          <t>Okres Revúca</t>
+          <t>Okres Michalovce</t>
         </is>
       </c>
       <c r="C2936">
-        <v>483</v>
+        <v>953</v>
       </c>
       <c r="D2936">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="E2936">
-        <v>495</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="2937">
@@ -55977,17 +55977,17 @@
       </c>
       <c r="B2937" t="inlineStr">
         <is>
-          <t>Okres Rimavská Sobota</t>
+          <t>Okres Myjava</t>
         </is>
       </c>
       <c r="C2937">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="D2937">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="E2937">
-        <v>210</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2938">
@@ -55996,17 +55996,17 @@
       </c>
       <c r="B2938" t="inlineStr">
         <is>
-          <t>Okres Rožňava</t>
+          <t>Okres Námestovo</t>
         </is>
       </c>
       <c r="C2938">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="D2938">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2938">
-        <v>225</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2939">
@@ -56015,17 +56015,17 @@
       </c>
       <c r="B2939" t="inlineStr">
         <is>
-          <t>Okres Ružomberok</t>
+          <t>Okres Nitra</t>
         </is>
       </c>
       <c r="C2939">
-        <v>1199</v>
+        <v>929</v>
       </c>
       <c r="D2939">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="E2939">
-        <v>1210</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="2940">
@@ -56034,17 +56034,17 @@
       </c>
       <c r="B2940" t="inlineStr">
         <is>
-          <t>Okres Skalica</t>
+          <t>Okres Nové Mesto nad Váhom</t>
         </is>
       </c>
       <c r="C2940">
-        <v>382</v>
+        <v>345</v>
       </c>
       <c r="D2940">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2940">
-        <v>411</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2941">
@@ -56053,17 +56053,17 @@
       </c>
       <c r="B2941" t="inlineStr">
         <is>
-          <t>Okres Snina</t>
+          <t>Okres Nové Zámky</t>
         </is>
       </c>
       <c r="C2941">
-        <v>11</v>
+        <v>5041</v>
       </c>
       <c r="D2941">
-        <v>1</v>
+        <v>240</v>
       </c>
       <c r="E2941">
-        <v>12</v>
+        <v>5281</v>
       </c>
     </row>
     <row r="2942">
@@ -56072,17 +56072,17 @@
       </c>
       <c r="B2942" t="inlineStr">
         <is>
-          <t>Okres Spišská Nová Ves</t>
+          <t>Okres Partizánske</t>
         </is>
       </c>
       <c r="C2942">
-        <v>355</v>
+        <v>406</v>
       </c>
       <c r="D2942">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="E2942">
-        <v>477</v>
+        <v>451</v>
       </c>
     </row>
     <row r="2943">
@@ -56091,17 +56091,17 @@
       </c>
       <c r="B2943" t="inlineStr">
         <is>
-          <t>Okres Stará Ľubovňa</t>
+          <t>Okres Pezinok</t>
         </is>
       </c>
       <c r="C2943">
-        <v>262</v>
+        <v>565</v>
       </c>
       <c r="D2943">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E2943">
-        <v>308</v>
+        <v>591</v>
       </c>
     </row>
     <row r="2944">
@@ -56110,17 +56110,17 @@
       </c>
       <c r="B2944" t="inlineStr">
         <is>
-          <t>Okres Svidník</t>
+          <t>Okres Piešťany</t>
         </is>
       </c>
       <c r="C2944">
-        <v>135</v>
+        <v>536</v>
       </c>
       <c r="D2944">
         <v>20</v>
       </c>
       <c r="E2944">
-        <v>155</v>
+        <v>556</v>
       </c>
     </row>
     <row r="2945">
@@ -56129,17 +56129,17 @@
       </c>
       <c r="B2945" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Poprad</t>
         </is>
       </c>
       <c r="C2945">
-        <v>434</v>
+        <v>2060</v>
       </c>
       <c r="D2945">
-        <v>21</v>
+        <v>227</v>
       </c>
       <c r="E2945">
-        <v>455</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="2946">
@@ -56148,17 +56148,17 @@
       </c>
       <c r="B2946" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Považská Bystrica</t>
         </is>
       </c>
       <c r="C2946">
-        <v>374</v>
+        <v>192</v>
       </c>
       <c r="D2946">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="E2946">
-        <v>410</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2947">
@@ -56167,17 +56167,17 @@
       </c>
       <c r="B2947" t="inlineStr">
         <is>
-          <t>Okres Trnava</t>
+          <t>Okres Prešov</t>
         </is>
       </c>
       <c r="C2947">
-        <v>715</v>
+        <v>971</v>
       </c>
       <c r="D2947">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E2947">
-        <v>781</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="2948">
@@ -56186,17 +56186,17 @@
       </c>
       <c r="B2948" t="inlineStr">
         <is>
-          <t>Okres Tvrdošín</t>
+          <t>Okres Prievidza</t>
         </is>
       </c>
       <c r="C2948">
-        <v>40</v>
+        <v>754</v>
       </c>
       <c r="D2948">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="E2948">
-        <v>42</v>
+        <v>837</v>
       </c>
     </row>
     <row r="2949">
@@ -56205,17 +56205,17 @@
       </c>
       <c r="B2949" t="inlineStr">
         <is>
-          <t>Okres Veľký Krtíš</t>
+          <t>Okres Púchov</t>
         </is>
       </c>
       <c r="C2949">
-        <v>274</v>
+        <v>19</v>
       </c>
       <c r="D2949">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E2949">
-        <v>294</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2950">
@@ -56224,17 +56224,17 @@
       </c>
       <c r="B2950" t="inlineStr">
         <is>
-          <t>Okres Vranov nad Topľou</t>
+          <t>Okres Revúca</t>
         </is>
       </c>
       <c r="C2950">
-        <v>329</v>
+        <v>578</v>
       </c>
       <c r="D2950">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="E2950">
-        <v>412</v>
+        <v>591</v>
       </c>
     </row>
     <row r="2951">
@@ -56243,17 +56243,17 @@
       </c>
       <c r="B2951" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Rimavská Sobota</t>
         </is>
       </c>
       <c r="C2951">
-        <v>303</v>
+        <v>204</v>
       </c>
       <c r="D2951">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E2951">
-        <v>316</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2952">
@@ -56262,17 +56262,17 @@
       </c>
       <c r="B2952" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Rožňava</t>
         </is>
       </c>
       <c r="C2952">
-        <v>241</v>
+        <v>319</v>
       </c>
       <c r="D2952">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E2952">
-        <v>270</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2953">
@@ -56281,17 +56281,1423 @@
       </c>
       <c r="B2953" t="inlineStr">
         <is>
+          <t>Okres Ružomberok</t>
+        </is>
+      </c>
+      <c r="C2953">
+        <v>1295</v>
+      </c>
+      <c r="D2953">
+        <v>25</v>
+      </c>
+      <c r="E2953">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="2954">
+      <c r="A2954" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2954" t="inlineStr">
+        <is>
+          <t>Okres Sabinov</t>
+        </is>
+      </c>
+      <c r="C2954">
+        <v>341</v>
+      </c>
+      <c r="D2954">
+        <v>20</v>
+      </c>
+      <c r="E2954">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2955">
+      <c r="A2955" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2955" t="inlineStr">
+        <is>
+          <t>Okres Senica</t>
+        </is>
+      </c>
+      <c r="C2955">
+        <v>284</v>
+      </c>
+      <c r="D2955">
+        <v>16</v>
+      </c>
+      <c r="E2955">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2956">
+      <c r="A2956" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2956" t="inlineStr">
+        <is>
+          <t>Okres Skalica</t>
+        </is>
+      </c>
+      <c r="C2956">
+        <v>382</v>
+      </c>
+      <c r="D2956">
+        <v>29</v>
+      </c>
+      <c r="E2956">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2957">
+      <c r="A2957" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2957" t="inlineStr">
+        <is>
+          <t>Okres Snina</t>
+        </is>
+      </c>
+      <c r="C2957">
+        <v>114</v>
+      </c>
+      <c r="D2957">
+        <v>6</v>
+      </c>
+      <c r="E2957">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2958">
+      <c r="A2958" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2958" t="inlineStr">
+        <is>
+          <t>Okres Sobrance</t>
+        </is>
+      </c>
+      <c r="C2958">
+        <v>227</v>
+      </c>
+      <c r="D2958">
+        <v>23</v>
+      </c>
+      <c r="E2958">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2959">
+      <c r="A2959" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2959" t="inlineStr">
+        <is>
+          <t>Okres Spišská Nová Ves</t>
+        </is>
+      </c>
+      <c r="C2959">
+        <v>549</v>
+      </c>
+      <c r="D2959">
+        <v>137</v>
+      </c>
+      <c r="E2959">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="2960">
+      <c r="A2960" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2960" t="inlineStr">
+        <is>
+          <t>Okres Stará Ľubovňa</t>
+        </is>
+      </c>
+      <c r="C2960">
+        <v>262</v>
+      </c>
+      <c r="D2960">
+        <v>46</v>
+      </c>
+      <c r="E2960">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2961">
+      <c r="A2961" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2961" t="inlineStr">
+        <is>
+          <t>Okres Svidník</t>
+        </is>
+      </c>
+      <c r="C2961">
+        <v>135</v>
+      </c>
+      <c r="D2961">
+        <v>20</v>
+      </c>
+      <c r="E2961">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2962">
+      <c r="A2962" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2962" t="inlineStr">
+        <is>
+          <t>Okres Topoľčany</t>
+        </is>
+      </c>
+      <c r="C2962">
+        <v>231</v>
+      </c>
+      <c r="D2962">
+        <v>30</v>
+      </c>
+      <c r="E2962">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2963">
+      <c r="A2963" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2963" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C2963">
+        <v>448</v>
+      </c>
+      <c r="D2963">
+        <v>23</v>
+      </c>
+      <c r="E2963">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="2964">
+      <c r="A2964" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2964" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C2964">
+        <v>558</v>
+      </c>
+      <c r="D2964">
+        <v>68</v>
+      </c>
+      <c r="E2964">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="2965">
+      <c r="A2965" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2965" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C2965">
+        <v>715</v>
+      </c>
+      <c r="D2965">
+        <v>66</v>
+      </c>
+      <c r="E2965">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="2966">
+      <c r="A2966" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2966" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C2966">
+        <v>184</v>
+      </c>
+      <c r="D2966">
+        <v>13</v>
+      </c>
+      <c r="E2966">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2967">
+      <c r="A2967" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2967" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C2967">
+        <v>521</v>
+      </c>
+      <c r="D2967">
+        <v>32</v>
+      </c>
+      <c r="E2967">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="2968">
+      <c r="A2968" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2968" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C2968">
+        <v>329</v>
+      </c>
+      <c r="D2968">
+        <v>83</v>
+      </c>
+      <c r="E2968">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="2969">
+      <c r="A2969" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2969" t="inlineStr">
+        <is>
+          <t>Okres Zlaté Moravce</t>
+        </is>
+      </c>
+      <c r="C2969">
+        <v>472</v>
+      </c>
+      <c r="D2969">
+        <v>29</v>
+      </c>
+      <c r="E2969">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2970">
+      <c r="A2970" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2970" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C2970">
+        <v>311</v>
+      </c>
+      <c r="D2970">
+        <v>13</v>
+      </c>
+      <c r="E2970">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2971">
+      <c r="A2971" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2971" t="inlineStr">
+        <is>
+          <t>Okres Žarnovica</t>
+        </is>
+      </c>
+      <c r="C2971">
+        <v>313</v>
+      </c>
+      <c r="D2971">
+        <v>18</v>
+      </c>
+      <c r="E2971">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="2972">
+      <c r="A2972" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2972" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C2972">
+        <v>241</v>
+      </c>
+      <c r="D2972">
+        <v>29</v>
+      </c>
+      <c r="E2972">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2973">
+      <c r="A2973" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B2973" t="inlineStr">
+        <is>
           <t>Okres Žilina</t>
         </is>
       </c>
-      <c r="C2953">
-        <v>226</v>
-      </c>
-      <c r="D2953">
+      <c r="C2973">
+        <v>315</v>
+      </c>
+      <c r="D2973">
+        <v>7</v>
+      </c>
+      <c r="E2973">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2974">
+      <c r="A2974" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2974" t="inlineStr">
+        <is>
+          <t>Okres Banská Bystrica</t>
+        </is>
+      </c>
+      <c r="C2974">
+        <v>575</v>
+      </c>
+      <c r="D2974">
+        <v>52</v>
+      </c>
+      <c r="E2974">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="2975">
+      <c r="A2975" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2975" t="inlineStr">
+        <is>
+          <t>Okres Banská Štiavnica</t>
+        </is>
+      </c>
+      <c r="C2975">
+        <v>15</v>
+      </c>
+      <c r="D2975">
+        <v>3</v>
+      </c>
+      <c r="E2975">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2976">
+      <c r="A2976" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2976" t="inlineStr">
+        <is>
+          <t>Okres Bardejov</t>
+        </is>
+      </c>
+      <c r="C2976">
+        <v>7</v>
+      </c>
+      <c r="D2976">
+        <v>0</v>
+      </c>
+      <c r="E2976">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2977">
+      <c r="A2977" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2977" t="inlineStr">
+        <is>
+          <t>Okres Bratislava I</t>
+        </is>
+      </c>
+      <c r="C2977">
+        <v>65</v>
+      </c>
+      <c r="D2977">
+        <v>1</v>
+      </c>
+      <c r="E2977">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2978">
+      <c r="A2978" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2978" t="inlineStr">
+        <is>
+          <t>Okres Bratislava II</t>
+        </is>
+      </c>
+      <c r="C2978">
+        <v>852</v>
+      </c>
+      <c r="D2978">
+        <v>18</v>
+      </c>
+      <c r="E2978">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="2979">
+      <c r="A2979" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2979" t="inlineStr">
+        <is>
+          <t>Okres Bratislava III</t>
+        </is>
+      </c>
+      <c r="C2979">
+        <v>487</v>
+      </c>
+      <c r="D2979">
+        <v>17</v>
+      </c>
+      <c r="E2979">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2980">
+      <c r="A2980" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2980" t="inlineStr">
+        <is>
+          <t>Okres Bratislava V</t>
+        </is>
+      </c>
+      <c r="C2980">
+        <v>124</v>
+      </c>
+      <c r="D2980">
+        <v>1</v>
+      </c>
+      <c r="E2980">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2981">
+      <c r="A2981" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2981" t="inlineStr">
+        <is>
+          <t>Okres Čadca</t>
+        </is>
+      </c>
+      <c r="C2981">
+        <v>452</v>
+      </c>
+      <c r="D2981">
+        <v>21</v>
+      </c>
+      <c r="E2981">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="2982">
+      <c r="A2982" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2982" t="inlineStr">
+        <is>
+          <t>Okres Dolný Kubín</t>
+        </is>
+      </c>
+      <c r="C2982">
+        <v>147</v>
+      </c>
+      <c r="D2982">
+        <v>12</v>
+      </c>
+      <c r="E2982">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2983">
+      <c r="A2983" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2983" t="inlineStr">
+        <is>
+          <t>Okres Dunajská Streda</t>
+        </is>
+      </c>
+      <c r="C2983">
+        <v>445</v>
+      </c>
+      <c r="D2983">
+        <v>24</v>
+      </c>
+      <c r="E2983">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2984">
+      <c r="A2984" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2984" t="inlineStr">
+        <is>
+          <t>Okres Galanta</t>
+        </is>
+      </c>
+      <c r="C2984">
+        <v>458</v>
+      </c>
+      <c r="D2984">
+        <v>24</v>
+      </c>
+      <c r="E2984">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="2985">
+      <c r="A2985" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2985" t="inlineStr">
+        <is>
+          <t>Okres Hlohovec</t>
+        </is>
+      </c>
+      <c r="C2985">
+        <v>3</v>
+      </c>
+      <c r="D2985">
+        <v>0</v>
+      </c>
+      <c r="E2985">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2986">
+      <c r="A2986" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2986" t="inlineStr">
+        <is>
+          <t>Okres Humenné</t>
+        </is>
+      </c>
+      <c r="C2986">
+        <v>336</v>
+      </c>
+      <c r="D2986">
+        <v>14</v>
+      </c>
+      <c r="E2986">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2987">
+      <c r="A2987" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2987" t="inlineStr">
+        <is>
+          <t>Okres Ilava</t>
+        </is>
+      </c>
+      <c r="C2987">
+        <v>282</v>
+      </c>
+      <c r="D2987">
+        <v>35</v>
+      </c>
+      <c r="E2987">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2988">
+      <c r="A2988" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2988" t="inlineStr">
+        <is>
+          <t>Okres Komárno</t>
+        </is>
+      </c>
+      <c r="C2988">
+        <v>385</v>
+      </c>
+      <c r="D2988">
+        <v>5</v>
+      </c>
+      <c r="E2988">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="2989">
+      <c r="A2989" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2989" t="inlineStr">
+        <is>
+          <t>Okres Košice I</t>
+        </is>
+      </c>
+      <c r="C2989">
+        <v>533</v>
+      </c>
+      <c r="D2989">
+        <v>32</v>
+      </c>
+      <c r="E2989">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="2990">
+      <c r="A2990" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2990" t="inlineStr">
+        <is>
+          <t>Okres Košice II</t>
+        </is>
+      </c>
+      <c r="C2990">
+        <v>577</v>
+      </c>
+      <c r="D2990">
+        <v>2</v>
+      </c>
+      <c r="E2990">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="2991">
+      <c r="A2991" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2991" t="inlineStr">
+        <is>
+          <t>Okres Košice IV</t>
+        </is>
+      </c>
+      <c r="C2991">
+        <v>184</v>
+      </c>
+      <c r="D2991">
+        <v>9</v>
+      </c>
+      <c r="E2991">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2992">
+      <c r="A2992" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2992" t="inlineStr">
+        <is>
+          <t>Okres Krupina</t>
+        </is>
+      </c>
+      <c r="C2992">
+        <v>0</v>
+      </c>
+      <c r="D2992">
+        <v>0</v>
+      </c>
+      <c r="E2992">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2993">
+      <c r="A2993" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2993" t="inlineStr">
+        <is>
+          <t>Okres Levice</t>
+        </is>
+      </c>
+      <c r="C2993">
+        <v>391</v>
+      </c>
+      <c r="D2993">
+        <v>21</v>
+      </c>
+      <c r="E2993">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="2994">
+      <c r="A2994" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2994" t="inlineStr">
+        <is>
+          <t>Okres Levoča</t>
+        </is>
+      </c>
+      <c r="C2994">
+        <v>229</v>
+      </c>
+      <c r="D2994">
+        <v>19</v>
+      </c>
+      <c r="E2994">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2995">
+      <c r="A2995" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2995" t="inlineStr">
+        <is>
+          <t>Okres Liptovský Mikuláš</t>
+        </is>
+      </c>
+      <c r="C2995">
+        <v>599</v>
+      </c>
+      <c r="D2995">
+        <v>44</v>
+      </c>
+      <c r="E2995">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="2996">
+      <c r="A2996" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2996" t="inlineStr">
+        <is>
+          <t>Okres Lučenec</t>
+        </is>
+      </c>
+      <c r="C2996">
+        <v>332</v>
+      </c>
+      <c r="D2996">
+        <v>18</v>
+      </c>
+      <c r="E2996">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2997">
+      <c r="A2997" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2997" t="inlineStr">
+        <is>
+          <t>Okres Martin</t>
+        </is>
+      </c>
+      <c r="C2997">
+        <v>91</v>
+      </c>
+      <c r="D2997">
+        <v>3</v>
+      </c>
+      <c r="E2997">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2998">
+      <c r="A2998" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2998" t="inlineStr">
+        <is>
+          <t>Okres Michalovce</t>
+        </is>
+      </c>
+      <c r="C2998">
+        <v>39</v>
+      </c>
+      <c r="D2998">
+        <v>3</v>
+      </c>
+      <c r="E2998">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2999">
+      <c r="A2999" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B2999" t="inlineStr">
+        <is>
+          <t>Okres Myjava</t>
+        </is>
+      </c>
+      <c r="C2999">
+        <v>347</v>
+      </c>
+      <c r="D2999">
+        <v>27</v>
+      </c>
+      <c r="E2999">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3000">
+      <c r="A3000" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3000" t="inlineStr">
+        <is>
+          <t>Okres Nitra</t>
+        </is>
+      </c>
+      <c r="C3000">
+        <v>279</v>
+      </c>
+      <c r="D3000">
+        <v>19</v>
+      </c>
+      <c r="E3000">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3001">
+      <c r="A3001" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3001" t="inlineStr">
+        <is>
+          <t>Okres Nové Mesto nad Váhom</t>
+        </is>
+      </c>
+      <c r="C3001">
+        <v>231</v>
+      </c>
+      <c r="D3001">
+        <v>34</v>
+      </c>
+      <c r="E3001">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3002">
+      <c r="A3002" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3002" t="inlineStr">
+        <is>
+          <t>Okres Partizánske</t>
+        </is>
+      </c>
+      <c r="C3002">
+        <v>271</v>
+      </c>
+      <c r="D3002">
+        <v>33</v>
+      </c>
+      <c r="E3002">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3003">
+      <c r="A3003" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3003" t="inlineStr">
+        <is>
+          <t>Okres Pezinok</t>
+        </is>
+      </c>
+      <c r="C3003">
+        <v>239</v>
+      </c>
+      <c r="D3003">
+        <v>24</v>
+      </c>
+      <c r="E3003">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3004">
+      <c r="A3004" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3004" t="inlineStr">
+        <is>
+          <t>Okres Piešťany</t>
+        </is>
+      </c>
+      <c r="C3004">
+        <v>319</v>
+      </c>
+      <c r="D3004">
+        <v>15</v>
+      </c>
+      <c r="E3004">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3005">
+      <c r="A3005" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3005" t="inlineStr">
+        <is>
+          <t>Okres Poprad</t>
+        </is>
+      </c>
+      <c r="C3005">
+        <v>37</v>
+      </c>
+      <c r="D3005">
+        <v>3</v>
+      </c>
+      <c r="E3005">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3006">
+      <c r="A3006" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3006" t="inlineStr">
+        <is>
+          <t>Okres Považská Bystrica</t>
+        </is>
+      </c>
+      <c r="C3006">
+        <v>282</v>
+      </c>
+      <c r="D3006">
+        <v>34</v>
+      </c>
+      <c r="E3006">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="3007">
+      <c r="A3007" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3007" t="inlineStr">
+        <is>
+          <t>Okres Prešov</t>
+        </is>
+      </c>
+      <c r="C3007">
+        <v>471</v>
+      </c>
+      <c r="D3007">
+        <v>19</v>
+      </c>
+      <c r="E3007">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="3008">
+      <c r="A3008" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3008" t="inlineStr">
+        <is>
+          <t>Okres Prievidza</t>
+        </is>
+      </c>
+      <c r="C3008">
+        <v>352</v>
+      </c>
+      <c r="D3008">
+        <v>32</v>
+      </c>
+      <c r="E3008">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="3009">
+      <c r="A3009" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3009" t="inlineStr">
+        <is>
+          <t>Okres Revúca</t>
+        </is>
+      </c>
+      <c r="C3009">
+        <v>326</v>
+      </c>
+      <c r="D3009">
+        <v>3</v>
+      </c>
+      <c r="E3009">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3010">
+      <c r="A3010" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3010" t="inlineStr">
+        <is>
+          <t>Okres Rimavská Sobota</t>
+        </is>
+      </c>
+      <c r="C3010">
+        <v>285</v>
+      </c>
+      <c r="D3010">
+        <v>8</v>
+      </c>
+      <c r="E3010">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3011">
+      <c r="A3011" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3011" t="inlineStr">
+        <is>
+          <t>Okres Rožňava</t>
+        </is>
+      </c>
+      <c r="C3011">
+        <v>198</v>
+      </c>
+      <c r="D3011">
+        <v>4</v>
+      </c>
+      <c r="E3011">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3012">
+      <c r="A3012" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3012" t="inlineStr">
+        <is>
+          <t>Okres Ružomberok</t>
+        </is>
+      </c>
+      <c r="C3012">
+        <v>104</v>
+      </c>
+      <c r="D3012">
+        <v>5</v>
+      </c>
+      <c r="E3012">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3013">
+      <c r="A3013" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3013" t="inlineStr">
+        <is>
+          <t>Okres Senec</t>
+        </is>
+      </c>
+      <c r="C3013">
+        <v>653</v>
+      </c>
+      <c r="D3013">
+        <v>25</v>
+      </c>
+      <c r="E3013">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="3014">
+      <c r="A3014" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3014" t="inlineStr">
+        <is>
+          <t>Okres Skalica</t>
+        </is>
+      </c>
+      <c r="C3014">
+        <v>569</v>
+      </c>
+      <c r="D3014">
+        <v>13</v>
+      </c>
+      <c r="E3014">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="3015">
+      <c r="A3015" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3015" t="inlineStr">
+        <is>
+          <t>Okres Snina</t>
+        </is>
+      </c>
+      <c r="C3015">
+        <v>13</v>
+      </c>
+      <c r="D3015">
+        <v>3</v>
+      </c>
+      <c r="E3015">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3016">
+      <c r="A3016" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3016" t="inlineStr">
+        <is>
+          <t>Okres Sobrance</t>
+        </is>
+      </c>
+      <c r="C3016">
+        <v>130</v>
+      </c>
+      <c r="D3016">
+        <v>9</v>
+      </c>
+      <c r="E3016">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3017">
+      <c r="A3017" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3017" t="inlineStr">
+        <is>
+          <t>Okres Spišská Nová Ves</t>
+        </is>
+      </c>
+      <c r="C3017">
+        <v>50</v>
+      </c>
+      <c r="D3017">
         <v>6</v>
       </c>
-      <c r="E2953">
-        <v>232</v>
+      <c r="E3017">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3018">
+      <c r="A3018" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3018" t="inlineStr">
+        <is>
+          <t>Okres Stará Ľubovňa</t>
+        </is>
+      </c>
+      <c r="C3018">
+        <v>208</v>
+      </c>
+      <c r="D3018">
+        <v>13</v>
+      </c>
+      <c r="E3018">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3019">
+      <c r="A3019" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3019" t="inlineStr">
+        <is>
+          <t>Okres Topoľčany</t>
+        </is>
+      </c>
+      <c r="C3019">
+        <v>370</v>
+      </c>
+      <c r="D3019">
+        <v>43</v>
+      </c>
+      <c r="E3019">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3020">
+      <c r="A3020" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3020" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C3020">
+        <v>290</v>
+      </c>
+      <c r="D3020">
+        <v>12</v>
+      </c>
+      <c r="E3020">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3021">
+      <c r="A3021" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3021" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C3021">
+        <v>241</v>
+      </c>
+      <c r="D3021">
+        <v>26</v>
+      </c>
+      <c r="E3021">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="3022">
+      <c r="A3022" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3022" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C3022">
+        <v>421</v>
+      </c>
+      <c r="D3022">
+        <v>43</v>
+      </c>
+      <c r="E3022">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="3023">
+      <c r="A3023" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3023" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C3023">
+        <v>32</v>
+      </c>
+      <c r="D3023">
+        <v>0</v>
+      </c>
+      <c r="E3023">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3024">
+      <c r="A3024" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3024" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C3024">
+        <v>274</v>
+      </c>
+      <c r="D3024">
+        <v>24</v>
+      </c>
+      <c r="E3024">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3025">
+      <c r="A3025" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3025" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C3025">
+        <v>199</v>
+      </c>
+      <c r="D3025">
+        <v>15</v>
+      </c>
+      <c r="E3025">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3026">
+      <c r="A3026" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3026" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C3026">
+        <v>356</v>
+      </c>
+      <c r="D3026">
+        <v>22</v>
+      </c>
+      <c r="E3026">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="3027">
+      <c r="A3027" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B3027" t="inlineStr">
+        <is>
+          <t>Okres Žilina</t>
+        </is>
+      </c>
+      <c r="C3027">
+        <v>179</v>
+      </c>
+      <c r="D3027">
+        <v>13</v>
+      </c>
+      <c r="E3027">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: pi 11. 12. 2020
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_AgTests_District.xlsx
+++ b/OpenData_Slovakia_Covid_AgTests_District.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3100"/>
+  <dimension ref="A1:E3163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -50129,13 +50129,13 @@
         </is>
       </c>
       <c r="C2629">
-        <v>20</v>
+        <v>122</v>
       </c>
       <c r="D2629">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2629">
-        <v>20</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2630">
@@ -52846,13 +52846,13 @@
         </is>
       </c>
       <c r="C2772">
-        <v>634</v>
+        <v>654</v>
       </c>
       <c r="D2772">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2772">
-        <v>639</v>
+        <v>660</v>
       </c>
     </row>
     <row r="2773">
@@ -54252,13 +54252,13 @@
         </is>
       </c>
       <c r="C2846">
-        <v>1132</v>
+        <v>1175</v>
       </c>
       <c r="D2846">
         <v>84</v>
       </c>
       <c r="E2846">
-        <v>1216</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="2847">
@@ -54727,13 +54727,13 @@
         </is>
       </c>
       <c r="C2871">
-        <v>315</v>
+        <v>546</v>
       </c>
       <c r="D2871">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E2871">
-        <v>327</v>
+        <v>580</v>
       </c>
     </row>
     <row r="2872">
@@ -55506,13 +55506,13 @@
         </is>
       </c>
       <c r="C2912">
-        <v>725</v>
+        <v>743</v>
       </c>
       <c r="D2912">
         <v>44</v>
       </c>
       <c r="E2912">
-        <v>769</v>
+        <v>787</v>
       </c>
     </row>
     <row r="2913">
@@ -55924,13 +55924,13 @@
         </is>
       </c>
       <c r="C2934">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D2934">
         <v>13</v>
       </c>
       <c r="E2934">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2935">
@@ -56000,13 +56000,13 @@
         </is>
       </c>
       <c r="C2938">
-        <v>182</v>
+        <v>371</v>
       </c>
       <c r="D2938">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E2938">
-        <v>187</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2939">
@@ -56171,13 +56171,13 @@
         </is>
       </c>
       <c r="C2947">
-        <v>971</v>
+        <v>997</v>
       </c>
       <c r="D2947">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E2947">
-        <v>1043</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="2948">
@@ -57197,13 +57197,13 @@
         </is>
       </c>
       <c r="C3001">
-        <v>692</v>
+        <v>699</v>
       </c>
       <c r="D3001">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E3001">
-        <v>715</v>
+        <v>723</v>
       </c>
     </row>
     <row r="3002">
@@ -57406,13 +57406,13 @@
         </is>
       </c>
       <c r="C3012">
-        <v>455</v>
+        <v>419</v>
       </c>
       <c r="D3012">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E3012">
-        <v>508</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3013">
@@ -57444,13 +57444,13 @@
         </is>
       </c>
       <c r="C3014">
-        <v>1783</v>
+        <v>1809</v>
       </c>
       <c r="D3014">
         <v>95</v>
       </c>
       <c r="E3014">
-        <v>1878</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="3015">
@@ -57862,13 +57862,13 @@
         </is>
       </c>
       <c r="C3036">
-        <v>2</v>
+        <v>150</v>
       </c>
       <c r="D3036">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E3036">
-        <v>2</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3037">
@@ -57900,13 +57900,13 @@
         </is>
       </c>
       <c r="C3038">
-        <v>792</v>
+        <v>2475</v>
       </c>
       <c r="D3038">
-        <v>69</v>
+        <v>205</v>
       </c>
       <c r="E3038">
-        <v>861</v>
+        <v>2680</v>
       </c>
     </row>
     <row r="3039">
@@ -57953,17 +57953,17 @@
       </c>
       <c r="B3041" t="inlineStr">
         <is>
-          <t>Okres Banská Bystrica</t>
+          <t>Okres Bánovce nad Bebravou</t>
         </is>
       </c>
       <c r="C3041">
-        <v>1122</v>
+        <v>216</v>
       </c>
       <c r="D3041">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E3041">
-        <v>1173</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3042">
@@ -57972,17 +57972,17 @@
       </c>
       <c r="B3042" t="inlineStr">
         <is>
-          <t>Okres Bardejov</t>
+          <t>Okres Banská Bystrica</t>
         </is>
       </c>
       <c r="C3042">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="D3042">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E3042">
-        <v>1</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="3043">
@@ -57991,17 +57991,17 @@
       </c>
       <c r="B3043" t="inlineStr">
         <is>
-          <t>Okres Bratislava I</t>
+          <t>Okres Bardejov</t>
         </is>
       </c>
       <c r="C3043">
-        <v>75</v>
+        <v>631</v>
       </c>
       <c r="D3043">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E3043">
-        <v>75</v>
+        <v>666</v>
       </c>
     </row>
     <row r="3044">
@@ -58010,17 +58010,17 @@
       </c>
       <c r="B3044" t="inlineStr">
         <is>
-          <t>Okres Bratislava II</t>
+          <t>Okres Bratislava I</t>
         </is>
       </c>
       <c r="C3044">
-        <v>680</v>
+        <v>314</v>
       </c>
       <c r="D3044">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E3044">
-        <v>714</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3045">
@@ -58029,17 +58029,17 @@
       </c>
       <c r="B3045" t="inlineStr">
         <is>
-          <t>Okres Bratislava III</t>
+          <t>Okres Bratislava II</t>
         </is>
       </c>
       <c r="C3045">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="D3045">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E3045">
-        <v>707</v>
+        <v>714</v>
       </c>
     </row>
     <row r="3046">
@@ -58048,17 +58048,17 @@
       </c>
       <c r="B3046" t="inlineStr">
         <is>
-          <t>Okres Bratislava V</t>
+          <t>Okres Bratislava III</t>
         </is>
       </c>
       <c r="C3046">
-        <v>266</v>
+        <v>683</v>
       </c>
       <c r="D3046">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E3046">
-        <v>278</v>
+        <v>707</v>
       </c>
     </row>
     <row r="3047">
@@ -58067,17 +58067,17 @@
       </c>
       <c r="B3047" t="inlineStr">
         <is>
-          <t>Okres Brezno</t>
+          <t>Okres Bratislava V</t>
         </is>
       </c>
       <c r="C3047">
-        <v>429</v>
+        <v>491</v>
       </c>
       <c r="D3047">
-        <v>116</v>
+        <v>26</v>
       </c>
       <c r="E3047">
-        <v>545</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3048">
@@ -58086,17 +58086,17 @@
       </c>
       <c r="B3048" t="inlineStr">
         <is>
-          <t>Okres Čadca</t>
+          <t>Okres Brezno</t>
         </is>
       </c>
       <c r="C3048">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D3048">
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="E3048">
-        <v>461</v>
+        <v>545</v>
       </c>
     </row>
     <row r="3049">
@@ -58105,17 +58105,17 @@
       </c>
       <c r="B3049" t="inlineStr">
         <is>
-          <t>Okres Dolný Kubín</t>
+          <t>Okres Čadca</t>
         </is>
       </c>
       <c r="C3049">
-        <v>35</v>
+        <v>432</v>
       </c>
       <c r="D3049">
-        <v>144</v>
+        <v>29</v>
       </c>
       <c r="E3049">
-        <v>179</v>
+        <v>461</v>
       </c>
     </row>
     <row r="3050">
@@ -58124,17 +58124,17 @@
       </c>
       <c r="B3050" t="inlineStr">
         <is>
-          <t>Okres Dunajská Streda</t>
+          <t>Okres Detva</t>
         </is>
       </c>
       <c r="C3050">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="D3050">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3050">
-        <v>373</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3051">
@@ -58143,17 +58143,17 @@
       </c>
       <c r="B3051" t="inlineStr">
         <is>
-          <t>Okres Galanta</t>
+          <t>Okres Dolný Kubín</t>
         </is>
       </c>
       <c r="C3051">
-        <v>574</v>
+        <v>35</v>
       </c>
       <c r="D3051">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="E3051">
-        <v>606</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3052">
@@ -58162,17 +58162,17 @@
       </c>
       <c r="B3052" t="inlineStr">
         <is>
-          <t>Okres Gelnica</t>
+          <t>Okres Dunajská Streda</t>
         </is>
       </c>
       <c r="C3052">
-        <v>214</v>
+        <v>428</v>
       </c>
       <c r="D3052">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E3052">
-        <v>222</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3053">
@@ -58181,17 +58181,17 @@
       </c>
       <c r="B3053" t="inlineStr">
         <is>
-          <t>Okres Hlohovec</t>
+          <t>Okres Galanta</t>
         </is>
       </c>
       <c r="C3053">
-        <v>19</v>
+        <v>582</v>
       </c>
       <c r="D3053">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E3053">
-        <v>21</v>
+        <v>614</v>
       </c>
     </row>
     <row r="3054">
@@ -58200,17 +58200,17 @@
       </c>
       <c r="B3054" t="inlineStr">
         <is>
-          <t>Okres Humenné</t>
+          <t>Okres Gelnica</t>
         </is>
       </c>
       <c r="C3054">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="D3054">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3054">
-        <v>241</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3055">
@@ -58219,17 +58219,17 @@
       </c>
       <c r="B3055" t="inlineStr">
         <is>
-          <t>Okres Ilava</t>
+          <t>Okres Hlohovec</t>
         </is>
       </c>
       <c r="C3055">
-        <v>355</v>
+        <v>20</v>
       </c>
       <c r="D3055">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E3055">
-        <v>399</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3056">
@@ -58238,17 +58238,17 @@
       </c>
       <c r="B3056" t="inlineStr">
         <is>
-          <t>Okres Kežmarok</t>
+          <t>Okres Humenné</t>
         </is>
       </c>
       <c r="C3056">
-        <v>220</v>
+        <v>441</v>
       </c>
       <c r="D3056">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E3056">
-        <v>236</v>
+        <v>474</v>
       </c>
     </row>
     <row r="3057">
@@ -58257,17 +58257,17 @@
       </c>
       <c r="B3057" t="inlineStr">
         <is>
-          <t>Okres Komárno</t>
+          <t>Okres Ilava</t>
         </is>
       </c>
       <c r="C3057">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="D3057">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="E3057">
-        <v>375</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3058">
@@ -58276,17 +58276,17 @@
       </c>
       <c r="B3058" t="inlineStr">
         <is>
-          <t>Okres Košice I</t>
+          <t>Okres Kežmarok</t>
         </is>
       </c>
       <c r="C3058">
-        <v>453</v>
+        <v>402</v>
       </c>
       <c r="D3058">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E3058">
-        <v>486</v>
+        <v>442</v>
       </c>
     </row>
     <row r="3059">
@@ -58295,17 +58295,17 @@
       </c>
       <c r="B3059" t="inlineStr">
         <is>
-          <t>Okres Košice II</t>
+          <t>Okres Komárno</t>
         </is>
       </c>
       <c r="C3059">
-        <v>619</v>
+        <v>610</v>
       </c>
       <c r="D3059">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E3059">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="3060">
@@ -58314,17 +58314,17 @@
       </c>
       <c r="B3060" t="inlineStr">
         <is>
-          <t>Okres Košice IV</t>
+          <t>Okres Košice I</t>
         </is>
       </c>
       <c r="C3060">
-        <v>198</v>
+        <v>453</v>
       </c>
       <c r="D3060">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="E3060">
-        <v>205</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3061">
@@ -58333,17 +58333,17 @@
       </c>
       <c r="B3061" t="inlineStr">
         <is>
-          <t>Okres Krupina</t>
+          <t>Okres Košice II</t>
         </is>
       </c>
       <c r="C3061">
-        <v>2</v>
+        <v>628</v>
       </c>
       <c r="D3061">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E3061">
-        <v>3</v>
+        <v>643</v>
       </c>
     </row>
     <row r="3062">
@@ -58352,17 +58352,17 @@
       </c>
       <c r="B3062" t="inlineStr">
         <is>
-          <t>Okres Levice</t>
+          <t>Okres Košice IV</t>
         </is>
       </c>
       <c r="C3062">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="D3062">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E3062">
-        <v>534</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3063">
@@ -58371,17 +58371,17 @@
       </c>
       <c r="B3063" t="inlineStr">
         <is>
-          <t>Okres Levoča</t>
+          <t>Okres Krupina</t>
         </is>
       </c>
       <c r="C3063">
-        <v>138</v>
+        <v>2</v>
       </c>
       <c r="D3063">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E3063">
-        <v>151</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3064">
@@ -58390,17 +58390,17 @@
       </c>
       <c r="B3064" t="inlineStr">
         <is>
-          <t>Okres Liptovský Mikuláš</t>
+          <t>Okres Levice</t>
         </is>
       </c>
       <c r="C3064">
-        <v>217</v>
+        <v>1192</v>
       </c>
       <c r="D3064">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="E3064">
-        <v>228</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="3065">
@@ -58409,17 +58409,17 @@
       </c>
       <c r="B3065" t="inlineStr">
         <is>
-          <t>Okres Lučenec</t>
+          <t>Okres Levoča</t>
         </is>
       </c>
       <c r="C3065">
-        <v>295</v>
+        <v>138</v>
       </c>
       <c r="D3065">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3065">
-        <v>311</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3066">
@@ -58428,17 +58428,17 @@
       </c>
       <c r="B3066" t="inlineStr">
         <is>
-          <t>Okres Malacky</t>
+          <t>Okres Liptovský Mikuláš</t>
         </is>
       </c>
       <c r="C3066">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="D3066">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E3066">
-        <v>205</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3067">
@@ -58447,17 +58447,17 @@
       </c>
       <c r="B3067" t="inlineStr">
         <is>
-          <t>Okres Martin</t>
+          <t>Okres Lučenec</t>
         </is>
       </c>
       <c r="C3067">
-        <v>506</v>
+        <v>374</v>
       </c>
       <c r="D3067">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="E3067">
-        <v>548</v>
+        <v>395</v>
       </c>
     </row>
     <row r="3068">
@@ -58466,17 +58466,17 @@
       </c>
       <c r="B3068" t="inlineStr">
         <is>
-          <t>Okres Michalovce</t>
+          <t>Okres Malacky</t>
         </is>
       </c>
       <c r="C3068">
-        <v>552</v>
+        <v>190</v>
       </c>
       <c r="D3068">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="E3068">
-        <v>594</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3069">
@@ -58485,17 +58485,17 @@
       </c>
       <c r="B3069" t="inlineStr">
         <is>
-          <t>Okres Myjava</t>
+          <t>Okres Martin</t>
         </is>
       </c>
       <c r="C3069">
-        <v>195</v>
+        <v>733</v>
       </c>
       <c r="D3069">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="E3069">
-        <v>224</v>
+        <v>788</v>
       </c>
     </row>
     <row r="3070">
@@ -58504,17 +58504,17 @@
       </c>
       <c r="B3070" t="inlineStr">
         <is>
-          <t>Okres Nitra</t>
+          <t>Okres Medzilaborce</t>
         </is>
       </c>
       <c r="C3070">
-        <v>602</v>
+        <v>48</v>
       </c>
       <c r="D3070">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="E3070">
-        <v>646</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3071">
@@ -58523,17 +58523,17 @@
       </c>
       <c r="B3071" t="inlineStr">
         <is>
-          <t>Okres Nové Mesto nad Váhom</t>
+          <t>Okres Michalovce</t>
         </is>
       </c>
       <c r="C3071">
-        <v>188</v>
+        <v>1241</v>
       </c>
       <c r="D3071">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="E3071">
-        <v>215</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="3072">
@@ -58542,17 +58542,17 @@
       </c>
       <c r="B3072" t="inlineStr">
         <is>
-          <t>Okres Partizánske</t>
+          <t>Okres Myjava</t>
         </is>
       </c>
       <c r="C3072">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D3072">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E3072">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3073">
@@ -58561,17 +58561,17 @@
       </c>
       <c r="B3073" t="inlineStr">
         <is>
-          <t>Okres Pezinok</t>
+          <t>Okres Námestovo</t>
         </is>
       </c>
       <c r="C3073">
-        <v>376</v>
+        <v>543</v>
       </c>
       <c r="D3073">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E3073">
-        <v>388</v>
+        <v>569</v>
       </c>
     </row>
     <row r="3074">
@@ -58580,17 +58580,17 @@
       </c>
       <c r="B3074" t="inlineStr">
         <is>
-          <t>Okres Piešťany</t>
+          <t>Okres Nitra</t>
         </is>
       </c>
       <c r="C3074">
-        <v>144</v>
+        <v>623</v>
       </c>
       <c r="D3074">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E3074">
-        <v>149</v>
+        <v>671</v>
       </c>
     </row>
     <row r="3075">
@@ -58599,17 +58599,17 @@
       </c>
       <c r="B3075" t="inlineStr">
         <is>
-          <t>Okres Poprad</t>
+          <t>Okres Nové Mesto nad Váhom</t>
         </is>
       </c>
       <c r="C3075">
-        <v>948</v>
+        <v>480</v>
       </c>
       <c r="D3075">
-        <v>113</v>
+        <v>49</v>
       </c>
       <c r="E3075">
-        <v>1061</v>
+        <v>529</v>
       </c>
     </row>
     <row r="3076">
@@ -58618,17 +58618,17 @@
       </c>
       <c r="B3076" t="inlineStr">
         <is>
-          <t>Okres Považská Bystrica</t>
+          <t>Okres Partizánske</t>
         </is>
       </c>
       <c r="C3076">
-        <v>290</v>
+        <v>204</v>
       </c>
       <c r="D3076">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="E3076">
-        <v>329</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3077">
@@ -58637,17 +58637,17 @@
       </c>
       <c r="B3077" t="inlineStr">
         <is>
-          <t>Okres Prešov</t>
+          <t>Okres Pezinok</t>
         </is>
       </c>
       <c r="C3077">
-        <v>233</v>
+        <v>376</v>
       </c>
       <c r="D3077">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3077">
-        <v>244</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3078">
@@ -58656,17 +58656,17 @@
       </c>
       <c r="B3078" t="inlineStr">
         <is>
-          <t>Okres Prievidza</t>
+          <t>Okres Piešťany</t>
         </is>
       </c>
       <c r="C3078">
-        <v>393</v>
+        <v>443</v>
       </c>
       <c r="D3078">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E3078">
-        <v>432</v>
+        <v>467</v>
       </c>
     </row>
     <row r="3079">
@@ -58675,17 +58675,17 @@
       </c>
       <c r="B3079" t="inlineStr">
         <is>
-          <t>Okres Púchov</t>
+          <t>Okres Poprad</t>
         </is>
       </c>
       <c r="C3079">
-        <v>4</v>
+        <v>1170</v>
       </c>
       <c r="D3079">
-        <v>1</v>
+        <v>126</v>
       </c>
       <c r="E3079">
-        <v>5</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="3080">
@@ -58694,17 +58694,17 @@
       </c>
       <c r="B3080" t="inlineStr">
         <is>
-          <t>Okres Revúca</t>
+          <t>Okres Považská Bystrica</t>
         </is>
       </c>
       <c r="C3080">
-        <v>259</v>
+        <v>290</v>
       </c>
       <c r="D3080">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E3080">
-        <v>264</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3081">
@@ -58713,17 +58713,17 @@
       </c>
       <c r="B3081" t="inlineStr">
         <is>
-          <t>Okres Rimavská Sobota</t>
+          <t>Okres Prešov</t>
         </is>
       </c>
       <c r="C3081">
-        <v>241</v>
+        <v>804</v>
       </c>
       <c r="D3081">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="E3081">
-        <v>251</v>
+        <v>849</v>
       </c>
     </row>
     <row r="3082">
@@ -58732,17 +58732,17 @@
       </c>
       <c r="B3082" t="inlineStr">
         <is>
-          <t>Okres Rožňava</t>
+          <t>Okres Prievidza</t>
         </is>
       </c>
       <c r="C3082">
-        <v>224</v>
+        <v>523</v>
       </c>
       <c r="D3082">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="E3082">
-        <v>227</v>
+        <v>582</v>
       </c>
     </row>
     <row r="3083">
@@ -58751,17 +58751,17 @@
       </c>
       <c r="B3083" t="inlineStr">
         <is>
-          <t>Okres Ružomberok</t>
+          <t>Okres Púchov</t>
         </is>
       </c>
       <c r="C3083">
-        <v>240</v>
+        <v>4</v>
       </c>
       <c r="D3083">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E3083">
-        <v>257</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3084">
@@ -58770,17 +58770,17 @@
       </c>
       <c r="B3084" t="inlineStr">
         <is>
-          <t>Okres Skalica</t>
+          <t>Okres Revúca</t>
         </is>
       </c>
       <c r="C3084">
-        <v>563</v>
+        <v>259</v>
       </c>
       <c r="D3084">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E3084">
-        <v>579</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3085">
@@ -58789,17 +58789,17 @@
       </c>
       <c r="B3085" t="inlineStr">
         <is>
-          <t>Okres Snina</t>
+          <t>Okres Rimavská Sobota</t>
         </is>
       </c>
       <c r="C3085">
-        <v>108</v>
+        <v>241</v>
       </c>
       <c r="D3085">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3085">
-        <v>119</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3086">
@@ -58808,17 +58808,17 @@
       </c>
       <c r="B3086" t="inlineStr">
         <is>
-          <t>Okres Sobrance</t>
+          <t>Okres Rožňava</t>
         </is>
       </c>
       <c r="C3086">
-        <v>107</v>
+        <v>329</v>
       </c>
       <c r="D3086">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3086">
-        <v>111</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3087">
@@ -58827,17 +58827,17 @@
       </c>
       <c r="B3087" t="inlineStr">
         <is>
-          <t>Okres Spišská Nová Ves</t>
+          <t>Okres Ružomberok</t>
         </is>
       </c>
       <c r="C3087">
-        <v>130</v>
+        <v>2541</v>
       </c>
       <c r="D3087">
-        <v>14</v>
+        <v>164</v>
       </c>
       <c r="E3087">
-        <v>144</v>
+        <v>2705</v>
       </c>
     </row>
     <row r="3088">
@@ -58846,17 +58846,17 @@
       </c>
       <c r="B3088" t="inlineStr">
         <is>
-          <t>Okres Stará Ľubovňa</t>
+          <t>Okres Sabinov</t>
         </is>
       </c>
       <c r="C3088">
-        <v>180</v>
+        <v>265</v>
       </c>
       <c r="D3088">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E3088">
-        <v>201</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3089">
@@ -58865,17 +58865,17 @@
       </c>
       <c r="B3089" t="inlineStr">
         <is>
-          <t>Okres Svidník</t>
+          <t>Okres Senec</t>
         </is>
       </c>
       <c r="C3089">
-        <v>39</v>
+        <v>452</v>
       </c>
       <c r="D3089">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3089">
-        <v>41</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3090">
@@ -58884,17 +58884,17 @@
       </c>
       <c r="B3090" t="inlineStr">
         <is>
-          <t>Okres Topoľčany</t>
+          <t>Okres Senica</t>
         </is>
       </c>
       <c r="C3090">
-        <v>181</v>
+        <v>267</v>
       </c>
       <c r="D3090">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E3090">
-        <v>190</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3091">
@@ -58903,17 +58903,17 @@
       </c>
       <c r="B3091" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Skalica</t>
         </is>
       </c>
       <c r="C3091">
-        <v>628</v>
+        <v>563</v>
       </c>
       <c r="D3091">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E3091">
-        <v>639</v>
+        <v>579</v>
       </c>
     </row>
     <row r="3092">
@@ -58922,17 +58922,17 @@
       </c>
       <c r="B3092" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Snina</t>
         </is>
       </c>
       <c r="C3092">
-        <v>275</v>
+        <v>108</v>
       </c>
       <c r="D3092">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="E3092">
-        <v>312</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3093">
@@ -58941,17 +58941,17 @@
       </c>
       <c r="B3093" t="inlineStr">
         <is>
-          <t>Okres Trnava</t>
+          <t>Okres Sobrance</t>
         </is>
       </c>
       <c r="C3093">
-        <v>603</v>
+        <v>159</v>
       </c>
       <c r="D3093">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E3093">
-        <v>633</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3094">
@@ -58960,17 +58960,17 @@
       </c>
       <c r="B3094" t="inlineStr">
         <is>
-          <t>Okres Tvrdošín</t>
+          <t>Okres Spišská Nová Ves</t>
         </is>
       </c>
       <c r="C3094">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="D3094">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E3094">
-        <v>51</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3095">
@@ -58979,17 +58979,17 @@
       </c>
       <c r="B3095" t="inlineStr">
         <is>
-          <t>Okres Veľký Krtíš</t>
+          <t>Okres Stará Ľubovňa</t>
         </is>
       </c>
       <c r="C3095">
-        <v>342</v>
+        <v>180</v>
       </c>
       <c r="D3095">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E3095">
-        <v>351</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3096">
@@ -58998,17 +58998,17 @@
       </c>
       <c r="B3096" t="inlineStr">
         <is>
-          <t>Okres Vranov nad Topľou</t>
+          <t>Okres Svidník</t>
         </is>
       </c>
       <c r="C3096">
-        <v>338</v>
+        <v>64</v>
       </c>
       <c r="D3096">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="E3096">
-        <v>370</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3097">
@@ -59017,17 +59017,17 @@
       </c>
       <c r="B3097" t="inlineStr">
         <is>
-          <t>Okres Zlaté Moravce</t>
+          <t>Okres Topoľčany</t>
         </is>
       </c>
       <c r="C3097">
-        <v>2</v>
+        <v>346</v>
       </c>
       <c r="D3097">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E3097">
-        <v>2</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3098">
@@ -59036,17 +59036,17 @@
       </c>
       <c r="B3098" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Trebišov</t>
         </is>
       </c>
       <c r="C3098">
-        <v>186</v>
+        <v>633</v>
       </c>
       <c r="D3098">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E3098">
-        <v>203</v>
+        <v>644</v>
       </c>
     </row>
     <row r="3099">
@@ -59055,17 +59055,17 @@
       </c>
       <c r="B3099" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Trenčín</t>
         </is>
       </c>
       <c r="C3099">
-        <v>710</v>
+        <v>502</v>
       </c>
       <c r="D3099">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="E3099">
-        <v>741</v>
+        <v>575</v>
       </c>
     </row>
     <row r="3100">
@@ -59074,17 +59074,1214 @@
       </c>
       <c r="B3100" t="inlineStr">
         <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C3100">
+        <v>916</v>
+      </c>
+      <c r="D3100">
+        <v>47</v>
+      </c>
+      <c r="E3100">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="3101">
+      <c r="A3101" s="2">
+        <v>44175</v>
+      </c>
+      <c r="B3101" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C3101">
+        <v>245</v>
+      </c>
+      <c r="D3101">
+        <v>18</v>
+      </c>
+      <c r="E3101">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3102">
+      <c r="A3102" s="2">
+        <v>44175</v>
+      </c>
+      <c r="B3102" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C3102">
+        <v>342</v>
+      </c>
+      <c r="D3102">
+        <v>9</v>
+      </c>
+      <c r="E3102">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3103">
+      <c r="A3103" s="2">
+        <v>44175</v>
+      </c>
+      <c r="B3103" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C3103">
+        <v>338</v>
+      </c>
+      <c r="D3103">
+        <v>32</v>
+      </c>
+      <c r="E3103">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="3104">
+      <c r="A3104" s="2">
+        <v>44175</v>
+      </c>
+      <c r="B3104" t="inlineStr">
+        <is>
+          <t>Okres Zlaté Moravce</t>
+        </is>
+      </c>
+      <c r="C3104">
+        <v>146</v>
+      </c>
+      <c r="D3104">
+        <v>9</v>
+      </c>
+      <c r="E3104">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3105">
+      <c r="A3105" s="2">
+        <v>44175</v>
+      </c>
+      <c r="B3105" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C3105">
+        <v>197</v>
+      </c>
+      <c r="D3105">
+        <v>17</v>
+      </c>
+      <c r="E3105">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3106">
+      <c r="A3106" s="2">
+        <v>44175</v>
+      </c>
+      <c r="B3106" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C3106">
+        <v>710</v>
+      </c>
+      <c r="D3106">
+        <v>31</v>
+      </c>
+      <c r="E3106">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="3107">
+      <c r="A3107" s="2">
+        <v>44175</v>
+      </c>
+      <c r="B3107" t="inlineStr">
+        <is>
           <t>Okres Žilina</t>
         </is>
       </c>
-      <c r="C3100">
-        <v>6740</v>
-      </c>
-      <c r="D3100">
-        <v>689</v>
-      </c>
-      <c r="E3100">
-        <v>7429</v>
+      <c r="C3107">
+        <v>6923</v>
+      </c>
+      <c r="D3107">
+        <v>697</v>
+      </c>
+      <c r="E3107">
+        <v>7620</v>
+      </c>
+    </row>
+    <row r="3108">
+      <c r="A3108" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3108" t="inlineStr">
+        <is>
+          <t>Okres Banská Bystrica</t>
+        </is>
+      </c>
+      <c r="C3108">
+        <v>633</v>
+      </c>
+      <c r="D3108">
+        <v>30</v>
+      </c>
+      <c r="E3108">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="3109">
+      <c r="A3109" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3109" t="inlineStr">
+        <is>
+          <t>Okres Banská Štiavnica</t>
+        </is>
+      </c>
+      <c r="C3109">
+        <v>5</v>
+      </c>
+      <c r="D3109">
+        <v>0</v>
+      </c>
+      <c r="E3109">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3110">
+      <c r="A3110" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3110" t="inlineStr">
+        <is>
+          <t>Okres Bardejov</t>
+        </is>
+      </c>
+      <c r="C3110">
+        <v>555</v>
+      </c>
+      <c r="D3110">
+        <v>30</v>
+      </c>
+      <c r="E3110">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="3111">
+      <c r="A3111" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3111" t="inlineStr">
+        <is>
+          <t>Okres Bratislava I</t>
+        </is>
+      </c>
+      <c r="C3111">
+        <v>77</v>
+      </c>
+      <c r="D3111">
+        <v>0</v>
+      </c>
+      <c r="E3111">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3112">
+      <c r="A3112" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3112" t="inlineStr">
+        <is>
+          <t>Okres Bratislava II</t>
+        </is>
+      </c>
+      <c r="C3112">
+        <v>1356</v>
+      </c>
+      <c r="D3112">
+        <v>51</v>
+      </c>
+      <c r="E3112">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="3113">
+      <c r="A3113" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3113" t="inlineStr">
+        <is>
+          <t>Okres Bratislava III</t>
+        </is>
+      </c>
+      <c r="C3113">
+        <v>517</v>
+      </c>
+      <c r="D3113">
+        <v>19</v>
+      </c>
+      <c r="E3113">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="3114">
+      <c r="A3114" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3114" t="inlineStr">
+        <is>
+          <t>Okres Bratislava IV</t>
+        </is>
+      </c>
+      <c r="C3114">
+        <v>92</v>
+      </c>
+      <c r="D3114">
+        <v>3</v>
+      </c>
+      <c r="E3114">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3115">
+      <c r="A3115" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3115" t="inlineStr">
+        <is>
+          <t>Okres Bratislava V</t>
+        </is>
+      </c>
+      <c r="C3115">
+        <v>843</v>
+      </c>
+      <c r="D3115">
+        <v>63</v>
+      </c>
+      <c r="E3115">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="3116">
+      <c r="A3116" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3116" t="inlineStr">
+        <is>
+          <t>Okres Brezno</t>
+        </is>
+      </c>
+      <c r="C3116">
+        <v>261</v>
+      </c>
+      <c r="D3116">
+        <v>31</v>
+      </c>
+      <c r="E3116">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3117">
+      <c r="A3117" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3117" t="inlineStr">
+        <is>
+          <t>Okres Čadca</t>
+        </is>
+      </c>
+      <c r="C3117">
+        <v>386</v>
+      </c>
+      <c r="D3117">
+        <v>34</v>
+      </c>
+      <c r="E3117">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="3118">
+      <c r="A3118" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3118" t="inlineStr">
+        <is>
+          <t>Okres Dolný Kubín</t>
+        </is>
+      </c>
+      <c r="C3118">
+        <v>184</v>
+      </c>
+      <c r="D3118">
+        <v>11</v>
+      </c>
+      <c r="E3118">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3119">
+      <c r="A3119" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3119" t="inlineStr">
+        <is>
+          <t>Okres Dunajská Streda</t>
+        </is>
+      </c>
+      <c r="C3119">
+        <v>306</v>
+      </c>
+      <c r="D3119">
+        <v>25</v>
+      </c>
+      <c r="E3119">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3120">
+      <c r="A3120" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3120" t="inlineStr">
+        <is>
+          <t>Okres Galanta</t>
+        </is>
+      </c>
+      <c r="C3120">
+        <v>420</v>
+      </c>
+      <c r="D3120">
+        <v>19</v>
+      </c>
+      <c r="E3120">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="3121">
+      <c r="A3121" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3121" t="inlineStr">
+        <is>
+          <t>Okres Hlohovec</t>
+        </is>
+      </c>
+      <c r="C3121">
+        <v>2</v>
+      </c>
+      <c r="D3121">
+        <v>0</v>
+      </c>
+      <c r="E3121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3122">
+      <c r="A3122" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3122" t="inlineStr">
+        <is>
+          <t>Okres Humenné</t>
+        </is>
+      </c>
+      <c r="C3122">
+        <v>86</v>
+      </c>
+      <c r="D3122">
+        <v>7</v>
+      </c>
+      <c r="E3122">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3123">
+      <c r="A3123" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3123" t="inlineStr">
+        <is>
+          <t>Okres Ilava</t>
+        </is>
+      </c>
+      <c r="C3123">
+        <v>262</v>
+      </c>
+      <c r="D3123">
+        <v>29</v>
+      </c>
+      <c r="E3123">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3124">
+      <c r="A3124" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3124" t="inlineStr">
+        <is>
+          <t>Okres Komárno</t>
+        </is>
+      </c>
+      <c r="C3124">
+        <v>286</v>
+      </c>
+      <c r="D3124">
+        <v>27</v>
+      </c>
+      <c r="E3124">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3125">
+      <c r="A3125" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3125" t="inlineStr">
+        <is>
+          <t>Okres Košice I</t>
+        </is>
+      </c>
+      <c r="C3125">
+        <v>564</v>
+      </c>
+      <c r="D3125">
+        <v>26</v>
+      </c>
+      <c r="E3125">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="3126">
+      <c r="A3126" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3126" t="inlineStr">
+        <is>
+          <t>Okres Košice II</t>
+        </is>
+      </c>
+      <c r="C3126">
+        <v>174</v>
+      </c>
+      <c r="D3126">
+        <v>0</v>
+      </c>
+      <c r="E3126">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3127">
+      <c r="A3127" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3127" t="inlineStr">
+        <is>
+          <t>Okres Košice IV</t>
+        </is>
+      </c>
+      <c r="C3127">
+        <v>507</v>
+      </c>
+      <c r="D3127">
+        <v>13</v>
+      </c>
+      <c r="E3127">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="3128">
+      <c r="A3128" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3128" t="inlineStr">
+        <is>
+          <t>Okres Krupina</t>
+        </is>
+      </c>
+      <c r="C3128">
+        <v>8</v>
+      </c>
+      <c r="D3128">
+        <v>0</v>
+      </c>
+      <c r="E3128">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3129">
+      <c r="A3129" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3129" t="inlineStr">
+        <is>
+          <t>Okres Levice</t>
+        </is>
+      </c>
+      <c r="C3129">
+        <v>418</v>
+      </c>
+      <c r="D3129">
+        <v>20</v>
+      </c>
+      <c r="E3129">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="3130">
+      <c r="A3130" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3130" t="inlineStr">
+        <is>
+          <t>Okres Levoča</t>
+        </is>
+      </c>
+      <c r="C3130">
+        <v>157</v>
+      </c>
+      <c r="D3130">
+        <v>24</v>
+      </c>
+      <c r="E3130">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3131">
+      <c r="A3131" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3131" t="inlineStr">
+        <is>
+          <t>Okres Liptovský Mikuláš</t>
+        </is>
+      </c>
+      <c r="C3131">
+        <v>229</v>
+      </c>
+      <c r="D3131">
+        <v>11</v>
+      </c>
+      <c r="E3131">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3132">
+      <c r="A3132" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3132" t="inlineStr">
+        <is>
+          <t>Okres Lučenec</t>
+        </is>
+      </c>
+      <c r="C3132">
+        <v>426</v>
+      </c>
+      <c r="D3132">
+        <v>16</v>
+      </c>
+      <c r="E3132">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="3133">
+      <c r="A3133" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3133" t="inlineStr">
+        <is>
+          <t>Okres Martin</t>
+        </is>
+      </c>
+      <c r="C3133">
+        <v>101</v>
+      </c>
+      <c r="D3133">
+        <v>13</v>
+      </c>
+      <c r="E3133">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3134">
+      <c r="A3134" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3134" t="inlineStr">
+        <is>
+          <t>Okres Michalovce</t>
+        </is>
+      </c>
+      <c r="C3134">
+        <v>457</v>
+      </c>
+      <c r="D3134">
+        <v>23</v>
+      </c>
+      <c r="E3134">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3135">
+      <c r="A3135" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3135" t="inlineStr">
+        <is>
+          <t>Okres Myjava</t>
+        </is>
+      </c>
+      <c r="C3135">
+        <v>200</v>
+      </c>
+      <c r="D3135">
+        <v>11</v>
+      </c>
+      <c r="E3135">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3136">
+      <c r="A3136" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3136" t="inlineStr">
+        <is>
+          <t>Okres Nitra</t>
+        </is>
+      </c>
+      <c r="C3136">
+        <v>28</v>
+      </c>
+      <c r="D3136">
+        <v>1</v>
+      </c>
+      <c r="E3136">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3137">
+      <c r="A3137" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3137" t="inlineStr">
+        <is>
+          <t>Okres Nové Mesto nad Váhom</t>
+        </is>
+      </c>
+      <c r="C3137">
+        <v>181</v>
+      </c>
+      <c r="D3137">
+        <v>36</v>
+      </c>
+      <c r="E3137">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3138">
+      <c r="A3138" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3138" t="inlineStr">
+        <is>
+          <t>Okres Nové Zámky</t>
+        </is>
+      </c>
+      <c r="C3138">
+        <v>671</v>
+      </c>
+      <c r="D3138">
+        <v>30</v>
+      </c>
+      <c r="E3138">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="3139">
+      <c r="A3139" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3139" t="inlineStr">
+        <is>
+          <t>Okres Partizánske</t>
+        </is>
+      </c>
+      <c r="C3139">
+        <v>230</v>
+      </c>
+      <c r="D3139">
+        <v>18</v>
+      </c>
+      <c r="E3139">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3140">
+      <c r="A3140" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3140" t="inlineStr">
+        <is>
+          <t>Okres Pezinok</t>
+        </is>
+      </c>
+      <c r="C3140">
+        <v>291</v>
+      </c>
+      <c r="D3140">
+        <v>14</v>
+      </c>
+      <c r="E3140">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3141">
+      <c r="A3141" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3141" t="inlineStr">
+        <is>
+          <t>Okres Piešťany</t>
+        </is>
+      </c>
+      <c r="C3141">
+        <v>35</v>
+      </c>
+      <c r="D3141">
+        <v>1</v>
+      </c>
+      <c r="E3141">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3142">
+      <c r="A3142" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3142" t="inlineStr">
+        <is>
+          <t>Okres Poprad</t>
+        </is>
+      </c>
+      <c r="C3142">
+        <v>437</v>
+      </c>
+      <c r="D3142">
+        <v>38</v>
+      </c>
+      <c r="E3142">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="3143">
+      <c r="A3143" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3143" t="inlineStr">
+        <is>
+          <t>Okres Považská Bystrica</t>
+        </is>
+      </c>
+      <c r="C3143">
+        <v>187</v>
+      </c>
+      <c r="D3143">
+        <v>37</v>
+      </c>
+      <c r="E3143">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3144">
+      <c r="A3144" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3144" t="inlineStr">
+        <is>
+          <t>Okres Prešov</t>
+        </is>
+      </c>
+      <c r="C3144">
+        <v>637</v>
+      </c>
+      <c r="D3144">
+        <v>20</v>
+      </c>
+      <c r="E3144">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="3145">
+      <c r="A3145" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3145" t="inlineStr">
+        <is>
+          <t>Okres Prievidza</t>
+        </is>
+      </c>
+      <c r="C3145">
+        <v>0</v>
+      </c>
+      <c r="D3145">
+        <v>0</v>
+      </c>
+      <c r="E3145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3146">
+      <c r="A3146" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3146" t="inlineStr">
+        <is>
+          <t>Okres Revúca</t>
+        </is>
+      </c>
+      <c r="C3146">
+        <v>407</v>
+      </c>
+      <c r="D3146">
+        <v>9</v>
+      </c>
+      <c r="E3146">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="3147">
+      <c r="A3147" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3147" t="inlineStr">
+        <is>
+          <t>Okres Rimavská Sobota</t>
+        </is>
+      </c>
+      <c r="C3147">
+        <v>442</v>
+      </c>
+      <c r="D3147">
+        <v>21</v>
+      </c>
+      <c r="E3147">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="3148">
+      <c r="A3148" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3148" t="inlineStr">
+        <is>
+          <t>Okres Rožňava</t>
+        </is>
+      </c>
+      <c r="C3148">
+        <v>135</v>
+      </c>
+      <c r="D3148">
+        <v>3</v>
+      </c>
+      <c r="E3148">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3149">
+      <c r="A3149" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3149" t="inlineStr">
+        <is>
+          <t>Okres Ružomberok</t>
+        </is>
+      </c>
+      <c r="C3149">
+        <v>38</v>
+      </c>
+      <c r="D3149">
+        <v>8</v>
+      </c>
+      <c r="E3149">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3150">
+      <c r="A3150" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3150" t="inlineStr">
+        <is>
+          <t>Okres Skalica</t>
+        </is>
+      </c>
+      <c r="C3150">
+        <v>345</v>
+      </c>
+      <c r="D3150">
+        <v>8</v>
+      </c>
+      <c r="E3150">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="3151">
+      <c r="A3151" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3151" t="inlineStr">
+        <is>
+          <t>Okres Sobrance</t>
+        </is>
+      </c>
+      <c r="C3151">
+        <v>70</v>
+      </c>
+      <c r="D3151">
+        <v>3</v>
+      </c>
+      <c r="E3151">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3152">
+      <c r="A3152" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3152" t="inlineStr">
+        <is>
+          <t>Okres Spišská Nová Ves</t>
+        </is>
+      </c>
+      <c r="C3152">
+        <v>90</v>
+      </c>
+      <c r="D3152">
+        <v>13</v>
+      </c>
+      <c r="E3152">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3153">
+      <c r="A3153" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3153" t="inlineStr">
+        <is>
+          <t>Okres Stará Ľubovňa</t>
+        </is>
+      </c>
+      <c r="C3153">
+        <v>172</v>
+      </c>
+      <c r="D3153">
+        <v>10</v>
+      </c>
+      <c r="E3153">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3154">
+      <c r="A3154" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3154" t="inlineStr">
+        <is>
+          <t>Okres Svidník</t>
+        </is>
+      </c>
+      <c r="C3154">
+        <v>45</v>
+      </c>
+      <c r="D3154">
+        <v>6</v>
+      </c>
+      <c r="E3154">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3155">
+      <c r="A3155" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3155" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C3155">
+        <v>419</v>
+      </c>
+      <c r="D3155">
+        <v>22</v>
+      </c>
+      <c r="E3155">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="3156">
+      <c r="A3156" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3156" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C3156">
+        <v>262</v>
+      </c>
+      <c r="D3156">
+        <v>22</v>
+      </c>
+      <c r="E3156">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3157">
+      <c r="A3157" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3157" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C3157">
+        <v>324</v>
+      </c>
+      <c r="D3157">
+        <v>10</v>
+      </c>
+      <c r="E3157">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3158">
+      <c r="A3158" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3158" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C3158">
+        <v>32</v>
+      </c>
+      <c r="D3158">
+        <v>0</v>
+      </c>
+      <c r="E3158">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3159">
+      <c r="A3159" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3159" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C3159">
+        <v>332</v>
+      </c>
+      <c r="D3159">
+        <v>23</v>
+      </c>
+      <c r="E3159">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="3160">
+      <c r="A3160" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3160" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C3160">
+        <v>283</v>
+      </c>
+      <c r="D3160">
+        <v>32</v>
+      </c>
+      <c r="E3160">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3161">
+      <c r="A3161" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3161" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C3161">
+        <v>257</v>
+      </c>
+      <c r="D3161">
+        <v>26</v>
+      </c>
+      <c r="E3161">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3162">
+      <c r="A3162" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3162" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C3162">
+        <v>297</v>
+      </c>
+      <c r="D3162">
+        <v>7</v>
+      </c>
+      <c r="E3162">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3163">
+      <c r="A3163" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B3163" t="inlineStr">
+        <is>
+          <t>Okres Žilina</t>
+        </is>
+      </c>
+      <c r="C3163">
+        <v>530</v>
+      </c>
+      <c r="D3163">
+        <v>33</v>
+      </c>
+      <c r="E3163">
+        <v>563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: ut 15. 12. 2020
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_AgTests_District.xlsx
+++ b/OpenData_Slovakia_Covid_AgTests_District.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3306"/>
+  <dimension ref="A1:E3382"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -47849,13 +47849,13 @@
         </is>
       </c>
       <c r="C2509">
-        <v>881</v>
+        <v>937</v>
       </c>
       <c r="D2509">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E2509">
-        <v>921</v>
+        <v>981</v>
       </c>
     </row>
     <row r="2510">
@@ -51573,13 +51573,13 @@
         </is>
       </c>
       <c r="C2705">
-        <v>708</v>
+        <v>898</v>
       </c>
       <c r="D2705">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E2705">
-        <v>719</v>
+        <v>913</v>
       </c>
     </row>
     <row r="2706">
@@ -58109,13 +58109,13 @@
         </is>
       </c>
       <c r="C3049">
-        <v>491</v>
+        <v>787</v>
       </c>
       <c r="D3049">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E3049">
-        <v>517</v>
+        <v>821</v>
       </c>
     </row>
     <row r="3050">
@@ -59382,13 +59382,13 @@
         </is>
       </c>
       <c r="C3116">
-        <v>1549</v>
+        <v>1668</v>
       </c>
       <c r="D3116">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E3116">
-        <v>1609</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="3117">
@@ -59439,13 +59439,13 @@
         </is>
       </c>
       <c r="C3119">
-        <v>843</v>
+        <v>1140</v>
       </c>
       <c r="D3119">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="E3119">
-        <v>906</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="3120">
@@ -59838,13 +59838,13 @@
         </is>
       </c>
       <c r="C3140">
-        <v>377</v>
+        <v>472</v>
       </c>
       <c r="D3140">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E3140">
-        <v>395</v>
+        <v>494</v>
       </c>
     </row>
     <row r="3141">
@@ -59857,13 +59857,13 @@
         </is>
       </c>
       <c r="C3141">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D3141">
         <v>38</v>
       </c>
       <c r="E3141">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="3142">
@@ -60218,13 +60218,13 @@
         </is>
       </c>
       <c r="C3160">
-        <v>3538</v>
+        <v>3443</v>
       </c>
       <c r="D3160">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E3160">
-        <v>3787</v>
+        <v>3688</v>
       </c>
     </row>
     <row r="3161">
@@ -60693,13 +60693,13 @@
         </is>
       </c>
       <c r="C3185">
-        <v>534</v>
+        <v>926</v>
       </c>
       <c r="D3185">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E3185">
-        <v>558</v>
+        <v>970</v>
       </c>
     </row>
     <row r="3186">
@@ -60750,13 +60750,13 @@
         </is>
       </c>
       <c r="C3188">
-        <v>736</v>
+        <v>1386</v>
       </c>
       <c r="D3188">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="E3188">
-        <v>764</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="3189">
@@ -60803,17 +60803,17 @@
       </c>
       <c r="B3191" t="inlineStr">
         <is>
-          <t>Okres Humenné</t>
+          <t>Okres Hlohovec</t>
         </is>
       </c>
       <c r="C3191">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D3191">
         <v>0</v>
       </c>
       <c r="E3191">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3192">
@@ -60822,17 +60822,17 @@
       </c>
       <c r="B3192" t="inlineStr">
         <is>
-          <t>Okres Komárno</t>
+          <t>Okres Humenné</t>
         </is>
       </c>
       <c r="C3192">
-        <v>408</v>
+        <v>32</v>
       </c>
       <c r="D3192">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="E3192">
-        <v>435</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3193">
@@ -60841,17 +60841,17 @@
       </c>
       <c r="B3193" t="inlineStr">
         <is>
-          <t>Okres Košice I</t>
+          <t>Okres Komárno</t>
         </is>
       </c>
       <c r="C3193">
-        <v>566</v>
+        <v>408</v>
       </c>
       <c r="D3193">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E3193">
-        <v>613</v>
+        <v>435</v>
       </c>
     </row>
     <row r="3194">
@@ -60860,17 +60860,17 @@
       </c>
       <c r="B3194" t="inlineStr">
         <is>
-          <t>Okres Košice II</t>
+          <t>Okres Košice I</t>
         </is>
       </c>
       <c r="C3194">
-        <v>130</v>
+        <v>566</v>
       </c>
       <c r="D3194">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="E3194">
-        <v>137</v>
+        <v>613</v>
       </c>
     </row>
     <row r="3195">
@@ -60879,17 +60879,17 @@
       </c>
       <c r="B3195" t="inlineStr">
         <is>
-          <t>Okres Košice IV</t>
+          <t>Okres Košice II</t>
         </is>
       </c>
       <c r="C3195">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="D3195">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3195">
-        <v>79</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3196">
@@ -60898,17 +60898,17 @@
       </c>
       <c r="B3196" t="inlineStr">
         <is>
-          <t>Okres Krupina</t>
+          <t>Okres Košice IV</t>
         </is>
       </c>
       <c r="C3196">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="D3196">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E3196">
-        <v>16</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3197">
@@ -60917,17 +60917,17 @@
       </c>
       <c r="B3197" t="inlineStr">
         <is>
-          <t>Okres Levice</t>
+          <t>Okres Krupina</t>
         </is>
       </c>
       <c r="C3197">
-        <v>436</v>
+        <v>0</v>
       </c>
       <c r="D3197">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E3197">
-        <v>443</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3198">
@@ -60936,17 +60936,17 @@
       </c>
       <c r="B3198" t="inlineStr">
         <is>
-          <t>Okres Levoča</t>
+          <t>Okres Levice</t>
         </is>
       </c>
       <c r="C3198">
-        <v>162</v>
+        <v>436</v>
       </c>
       <c r="D3198">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E3198">
-        <v>174</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3199">
@@ -60955,17 +60955,17 @@
       </c>
       <c r="B3199" t="inlineStr">
         <is>
-          <t>Okres Lučenec</t>
+          <t>Okres Levoča</t>
         </is>
       </c>
       <c r="C3199">
-        <v>411</v>
+        <v>162</v>
       </c>
       <c r="D3199">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3199">
-        <v>422</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3200">
@@ -60974,17 +60974,17 @@
       </c>
       <c r="B3200" t="inlineStr">
         <is>
-          <t>Okres Michalovce</t>
+          <t>Okres Lučenec</t>
         </is>
       </c>
       <c r="C3200">
-        <v>555</v>
+        <v>411</v>
       </c>
       <c r="D3200">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E3200">
-        <v>593</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3201">
@@ -60993,17 +60993,17 @@
       </c>
       <c r="B3201" t="inlineStr">
         <is>
-          <t>Okres Myjava</t>
+          <t>Okres Michalovce</t>
         </is>
       </c>
       <c r="C3201">
-        <v>189</v>
+        <v>555</v>
       </c>
       <c r="D3201">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="E3201">
-        <v>201</v>
+        <v>593</v>
       </c>
     </row>
     <row r="3202">
@@ -61012,17 +61012,17 @@
       </c>
       <c r="B3202" t="inlineStr">
         <is>
-          <t>Okres Nitra</t>
+          <t>Okres Myjava</t>
         </is>
       </c>
       <c r="C3202">
-        <v>613</v>
+        <v>189</v>
       </c>
       <c r="D3202">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="E3202">
-        <v>678</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3203">
@@ -61031,17 +61031,17 @@
       </c>
       <c r="B3203" t="inlineStr">
         <is>
-          <t>Okres Nové Mesto nad Váhom</t>
+          <t>Okres Nitra</t>
         </is>
       </c>
       <c r="C3203">
-        <v>215</v>
+        <v>613</v>
       </c>
       <c r="D3203">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="E3203">
-        <v>235</v>
+        <v>678</v>
       </c>
     </row>
     <row r="3204">
@@ -61050,17 +61050,17 @@
       </c>
       <c r="B3204" t="inlineStr">
         <is>
-          <t>Okres Partizánske</t>
+          <t>Okres Nové Mesto nad Váhom</t>
         </is>
       </c>
       <c r="C3204">
-        <v>309</v>
+        <v>215</v>
       </c>
       <c r="D3204">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="E3204">
-        <v>352</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3205">
@@ -61069,17 +61069,17 @@
       </c>
       <c r="B3205" t="inlineStr">
         <is>
-          <t>Okres Pezinok</t>
+          <t>Okres Partizánske</t>
         </is>
       </c>
       <c r="C3205">
-        <v>271</v>
+        <v>309</v>
       </c>
       <c r="D3205">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E3205">
-        <v>285</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3206">
@@ -61088,17 +61088,17 @@
       </c>
       <c r="B3206" t="inlineStr">
         <is>
-          <t>Okres Poprad</t>
+          <t>Okres Pezinok</t>
         </is>
       </c>
       <c r="C3206">
-        <v>1173</v>
+        <v>271</v>
       </c>
       <c r="D3206">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="E3206">
-        <v>1218</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3207">
@@ -61107,17 +61107,17 @@
       </c>
       <c r="B3207" t="inlineStr">
         <is>
-          <t>Okres Považská Bystrica</t>
+          <t>Okres Poprad</t>
         </is>
       </c>
       <c r="C3207">
-        <v>249</v>
+        <v>1173</v>
       </c>
       <c r="D3207">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E3207">
-        <v>291</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="3208">
@@ -61126,17 +61126,17 @@
       </c>
       <c r="B3208" t="inlineStr">
         <is>
-          <t>Okres Prešov</t>
+          <t>Okres Považská Bystrica</t>
         </is>
       </c>
       <c r="C3208">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="D3208">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="E3208">
-        <v>253</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3209">
@@ -61145,17 +61145,17 @@
       </c>
       <c r="B3209" t="inlineStr">
         <is>
-          <t>Okres Prievidza</t>
+          <t>Okres Prešov</t>
         </is>
       </c>
       <c r="C3209">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="D3209">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E3209">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3210">
@@ -61164,17 +61164,17 @@
       </c>
       <c r="B3210" t="inlineStr">
         <is>
-          <t>Okres Revúca</t>
+          <t>Okres Prievidza</t>
         </is>
       </c>
       <c r="C3210">
-        <v>1068</v>
+        <v>229</v>
       </c>
       <c r="D3210">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E3210">
-        <v>1096</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3211">
@@ -61183,17 +61183,17 @@
       </c>
       <c r="B3211" t="inlineStr">
         <is>
-          <t>Okres Ružomberok</t>
+          <t>Okres Revúca</t>
         </is>
       </c>
       <c r="C3211">
-        <v>68</v>
+        <v>1068</v>
       </c>
       <c r="D3211">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E3211">
-        <v>70</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="3212">
@@ -61202,17 +61202,17 @@
       </c>
       <c r="B3212" t="inlineStr">
         <is>
-          <t>Okres Senec</t>
+          <t>Okres Ružomberok</t>
         </is>
       </c>
       <c r="C3212">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="D3212">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3212">
-        <v>8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3213">
@@ -61221,17 +61221,17 @@
       </c>
       <c r="B3213" t="inlineStr">
         <is>
-          <t>Okres Senica</t>
+          <t>Okres Senec</t>
         </is>
       </c>
       <c r="C3213">
-        <v>300</v>
+        <v>8</v>
       </c>
       <c r="D3213">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E3213">
-        <v>321</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3214">
@@ -61240,17 +61240,17 @@
       </c>
       <c r="B3214" t="inlineStr">
         <is>
-          <t>Okres Skalica</t>
+          <t>Okres Senica</t>
         </is>
       </c>
       <c r="C3214">
-        <v>340</v>
+        <v>300</v>
       </c>
       <c r="D3214">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E3214">
-        <v>347</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3215">
@@ -61259,17 +61259,17 @@
       </c>
       <c r="B3215" t="inlineStr">
         <is>
-          <t>Okres Snina</t>
+          <t>Okres Skalica</t>
         </is>
       </c>
       <c r="C3215">
-        <v>4</v>
+        <v>340</v>
       </c>
       <c r="D3215">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E3215">
-        <v>4</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3216">
@@ -61278,17 +61278,17 @@
       </c>
       <c r="B3216" t="inlineStr">
         <is>
-          <t>Okres Sobrance</t>
+          <t>Okres Snina</t>
         </is>
       </c>
       <c r="C3216">
-        <v>121</v>
+        <v>4</v>
       </c>
       <c r="D3216">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3216">
-        <v>127</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3217">
@@ -61297,17 +61297,17 @@
       </c>
       <c r="B3217" t="inlineStr">
         <is>
-          <t>Okres Spišská Nová Ves</t>
+          <t>Okres Sobrance</t>
         </is>
       </c>
       <c r="C3217">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="D3217">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E3217">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3218">
@@ -61316,17 +61316,17 @@
       </c>
       <c r="B3218" t="inlineStr">
         <is>
-          <t>Okres Stará Ľubovňa</t>
+          <t>Okres Spišská Nová Ves</t>
         </is>
       </c>
       <c r="C3218">
-        <v>236</v>
+        <v>97</v>
       </c>
       <c r="D3218">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3218">
-        <v>253</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3219">
@@ -61335,17 +61335,17 @@
       </c>
       <c r="B3219" t="inlineStr">
         <is>
-          <t>Okres Svidník</t>
+          <t>Okres Stará Ľubovňa</t>
         </is>
       </c>
       <c r="C3219">
-        <v>59</v>
+        <v>236</v>
       </c>
       <c r="D3219">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E3219">
-        <v>64</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3220">
@@ -61354,17 +61354,17 @@
       </c>
       <c r="B3220" t="inlineStr">
         <is>
-          <t>Okres Topoľčany</t>
+          <t>Okres Svidník</t>
         </is>
       </c>
       <c r="C3220">
-        <v>375</v>
+        <v>59</v>
       </c>
       <c r="D3220">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="E3220">
-        <v>401</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3221">
@@ -61373,17 +61373,17 @@
       </c>
       <c r="B3221" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Topoľčany</t>
         </is>
       </c>
       <c r="C3221">
-        <v>12</v>
+        <v>375</v>
       </c>
       <c r="D3221">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E3221">
-        <v>12</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3222">
@@ -61392,17 +61392,17 @@
       </c>
       <c r="B3222" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Trebišov</t>
         </is>
       </c>
       <c r="C3222">
-        <v>208</v>
+        <v>12</v>
       </c>
       <c r="D3222">
+        <v>0</v>
+      </c>
+      <c r="E3222">
         <v>12</v>
-      </c>
-      <c r="E3222">
-        <v>220</v>
       </c>
     </row>
     <row r="3223">
@@ -61411,17 +61411,17 @@
       </c>
       <c r="B3223" t="inlineStr">
         <is>
-          <t>Okres Vranov nad Topľou</t>
+          <t>Okres Trenčín</t>
         </is>
       </c>
       <c r="C3223">
-        <v>354</v>
+        <v>208</v>
       </c>
       <c r="D3223">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="E3223">
-        <v>403</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3224">
@@ -61430,17 +61430,17 @@
       </c>
       <c r="B3224" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Vranov nad Topľou</t>
         </is>
       </c>
       <c r="C3224">
-        <v>218</v>
+        <v>354</v>
       </c>
       <c r="D3224">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="E3224">
-        <v>231</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3225">
@@ -61449,17 +61449,17 @@
       </c>
       <c r="B3225" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Zvolen</t>
         </is>
       </c>
       <c r="C3225">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="D3225">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3225">
-        <v>209</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3226">
@@ -61468,36 +61468,36 @@
       </c>
       <c r="B3226" t="inlineStr">
         <is>
-          <t>Okres Žilina</t>
+          <t>Okres Žiar nad Hronom</t>
         </is>
       </c>
       <c r="C3226">
-        <v>561</v>
+        <v>202</v>
       </c>
       <c r="D3226">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E3226">
-        <v>594</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3227">
       <c r="A3227" s="2">
-        <v>44178</v>
+        <v>44177</v>
       </c>
       <c r="B3227" t="inlineStr">
         <is>
-          <t>Okres Bratislava I</t>
+          <t>Okres Žilina</t>
         </is>
       </c>
       <c r="C3227">
-        <v>15</v>
+        <v>561</v>
       </c>
       <c r="D3227">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E3227">
-        <v>15</v>
+        <v>594</v>
       </c>
     </row>
     <row r="3228">
@@ -61506,17 +61506,17 @@
       </c>
       <c r="B3228" t="inlineStr">
         <is>
-          <t>Okres Bratislava II</t>
+          <t>Okres Bratislava I</t>
         </is>
       </c>
       <c r="C3228">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D3228">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3228">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3229">
@@ -61525,17 +61525,17 @@
       </c>
       <c r="B3229" t="inlineStr">
         <is>
-          <t>Okres Bratislava III</t>
+          <t>Okres Bratislava II</t>
         </is>
       </c>
       <c r="C3229">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="D3229">
         <v>3</v>
       </c>
       <c r="E3229">
-        <v>64</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3230">
@@ -61544,17 +61544,17 @@
       </c>
       <c r="B3230" t="inlineStr">
         <is>
-          <t>Okres Bratislava V</t>
+          <t>Okres Bratislava III</t>
         </is>
       </c>
       <c r="C3230">
-        <v>148</v>
+        <v>61</v>
       </c>
       <c r="D3230">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3230">
-        <v>152</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3231">
@@ -61563,17 +61563,17 @@
       </c>
       <c r="B3231" t="inlineStr">
         <is>
-          <t>Okres Čadca</t>
+          <t>Okres Bratislava V</t>
         </is>
       </c>
       <c r="C3231">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="D3231">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E3231">
-        <v>108</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3232">
@@ -61582,17 +61582,17 @@
       </c>
       <c r="B3232" t="inlineStr">
         <is>
-          <t>Okres Humenné</t>
+          <t>Okres Čadca</t>
         </is>
       </c>
       <c r="C3232">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D3232">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E3232">
-        <v>2</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3233">
@@ -61601,17 +61601,17 @@
       </c>
       <c r="B3233" t="inlineStr">
         <is>
-          <t>Okres Kežmarok</t>
+          <t>Okres Humenné</t>
         </is>
       </c>
       <c r="C3233">
-        <v>248</v>
+        <v>2</v>
       </c>
       <c r="D3233">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E3233">
-        <v>267</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3234">
@@ -61620,17 +61620,17 @@
       </c>
       <c r="B3234" t="inlineStr">
         <is>
-          <t>Okres Komárno</t>
+          <t>Okres Kežmarok</t>
         </is>
       </c>
       <c r="C3234">
-        <v>26</v>
+        <v>248</v>
       </c>
       <c r="D3234">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E3234">
-        <v>31</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3235">
@@ -61639,17 +61639,17 @@
       </c>
       <c r="B3235" t="inlineStr">
         <is>
-          <t>Okres Košice II</t>
+          <t>Okres Komárno</t>
         </is>
       </c>
       <c r="C3235">
-        <v>142</v>
+        <v>26</v>
       </c>
       <c r="D3235">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E3235">
-        <v>142</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3236">
@@ -61658,17 +61658,17 @@
       </c>
       <c r="B3236" t="inlineStr">
         <is>
-          <t>Okres Kysucké Nové Mesto</t>
+          <t>Okres Košice II</t>
         </is>
       </c>
       <c r="C3236">
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="D3236">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3236">
-        <v>1</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3237">
@@ -61677,17 +61677,17 @@
       </c>
       <c r="B3237" t="inlineStr">
         <is>
-          <t>Okres Levice</t>
+          <t>Okres Kysucké Nové Mesto</t>
         </is>
       </c>
       <c r="C3237">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D3237">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3237">
-        <v>34</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3238">
@@ -61696,17 +61696,17 @@
       </c>
       <c r="B3238" t="inlineStr">
         <is>
-          <t>Okres Lučenec</t>
+          <t>Okres Levice</t>
         </is>
       </c>
       <c r="C3238">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D3238">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3238">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3239">
@@ -61715,17 +61715,17 @@
       </c>
       <c r="B3239" t="inlineStr">
         <is>
-          <t>Okres Michalovce</t>
+          <t>Okres Lučenec</t>
         </is>
       </c>
       <c r="C3239">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D3239">
         <v>1</v>
       </c>
       <c r="E3239">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3240">
@@ -61734,17 +61734,17 @@
       </c>
       <c r="B3240" t="inlineStr">
         <is>
-          <t>Okres Myjava</t>
+          <t>Okres Michalovce</t>
         </is>
       </c>
       <c r="C3240">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D3240">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3240">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3241">
@@ -61753,17 +61753,17 @@
       </c>
       <c r="B3241" t="inlineStr">
         <is>
-          <t>Okres Nové Mesto nad Váhom</t>
+          <t>Okres Myjava</t>
         </is>
       </c>
       <c r="C3241">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D3241">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3241">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3242">
@@ -61772,17 +61772,17 @@
       </c>
       <c r="B3242" t="inlineStr">
         <is>
-          <t>Okres Partizánske</t>
+          <t>Okres Nové Mesto nad Váhom</t>
         </is>
       </c>
       <c r="C3242">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D3242">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3242">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3243">
@@ -61791,17 +61791,17 @@
       </c>
       <c r="B3243" t="inlineStr">
         <is>
-          <t>Okres Pezinok</t>
+          <t>Okres Partizánske</t>
         </is>
       </c>
       <c r="C3243">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D3243">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3243">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3244">
@@ -61810,17 +61810,17 @@
       </c>
       <c r="B3244" t="inlineStr">
         <is>
-          <t>Okres Piešťany</t>
+          <t>Okres Pezinok</t>
         </is>
       </c>
       <c r="C3244">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3244">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3244">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3245">
@@ -61829,17 +61829,17 @@
       </c>
       <c r="B3245" t="inlineStr">
         <is>
-          <t>Okres Poprad</t>
+          <t>Okres Piešťany</t>
         </is>
       </c>
       <c r="C3245">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D3245">
+        <v>0</v>
+      </c>
+      <c r="E3245">
         <v>2</v>
-      </c>
-      <c r="E3245">
-        <v>10</v>
       </c>
     </row>
     <row r="3246">
@@ -61848,17 +61848,17 @@
       </c>
       <c r="B3246" t="inlineStr">
         <is>
-          <t>Okres Prešov</t>
+          <t>Okres Poprad</t>
         </is>
       </c>
       <c r="C3246">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D3246">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3246">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3247">
@@ -61867,17 +61867,17 @@
       </c>
       <c r="B3247" t="inlineStr">
         <is>
-          <t>Okres Revúca</t>
+          <t>Okres Prešov</t>
         </is>
       </c>
       <c r="C3247">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D3247">
         <v>0</v>
       </c>
       <c r="E3247">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3248">
@@ -61886,17 +61886,17 @@
       </c>
       <c r="B3248" t="inlineStr">
         <is>
-          <t>Okres Ružomberok</t>
+          <t>Okres Revúca</t>
         </is>
       </c>
       <c r="C3248">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D3248">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3248">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3249">
@@ -61905,17 +61905,17 @@
       </c>
       <c r="B3249" t="inlineStr">
         <is>
-          <t>Okres Senec</t>
+          <t>Okres Ružomberok</t>
         </is>
       </c>
       <c r="C3249">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D3249">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3249">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3250">
@@ -61924,17 +61924,17 @@
       </c>
       <c r="B3250" t="inlineStr">
         <is>
-          <t>Okres Skalica</t>
+          <t>Okres Senec</t>
         </is>
       </c>
       <c r="C3250">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3250">
         <v>0</v>
       </c>
       <c r="E3250">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3251">
@@ -61943,17 +61943,17 @@
       </c>
       <c r="B3251" t="inlineStr">
         <is>
-          <t>Okres Snina</t>
+          <t>Okres Skalica</t>
         </is>
       </c>
       <c r="C3251">
         <v>5</v>
       </c>
       <c r="D3251">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3251">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3252">
@@ -61962,17 +61962,17 @@
       </c>
       <c r="B3252" t="inlineStr">
         <is>
-          <t>Okres Sobrance</t>
+          <t>Okres Snina</t>
         </is>
       </c>
       <c r="C3252">
+        <v>5</v>
+      </c>
+      <c r="D3252">
         <v>3</v>
       </c>
-      <c r="D3252">
-        <v>0</v>
-      </c>
       <c r="E3252">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3253">
@@ -61981,17 +61981,17 @@
       </c>
       <c r="B3253" t="inlineStr">
         <is>
-          <t>Okres Spišská Nová Ves</t>
+          <t>Okres Sobrance</t>
         </is>
       </c>
       <c r="C3253">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D3253">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3253">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3254">
@@ -62000,17 +62000,17 @@
       </c>
       <c r="B3254" t="inlineStr">
         <is>
-          <t>Okres Stará Ľubovňa</t>
+          <t>Okres Spišská Nová Ves</t>
         </is>
       </c>
       <c r="C3254">
+        <v>12</v>
+      </c>
+      <c r="D3254">
+        <v>1</v>
+      </c>
+      <c r="E3254">
         <v>13</v>
-      </c>
-      <c r="D3254">
-        <v>3</v>
-      </c>
-      <c r="E3254">
-        <v>16</v>
       </c>
     </row>
     <row r="3255">
@@ -62019,17 +62019,17 @@
       </c>
       <c r="B3255" t="inlineStr">
         <is>
-          <t>Okres Topoľčany</t>
+          <t>Okres Stará Ľubovňa</t>
         </is>
       </c>
       <c r="C3255">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3255">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3255">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3256">
@@ -62038,17 +62038,17 @@
       </c>
       <c r="B3256" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Topoľčany</t>
         </is>
       </c>
       <c r="C3256">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3256">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3256">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3257">
@@ -62057,17 +62057,17 @@
       </c>
       <c r="B3257" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Trebišov</t>
         </is>
       </c>
       <c r="C3257">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D3257">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3257">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3258">
@@ -62076,17 +62076,17 @@
       </c>
       <c r="B3258" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Trenčín</t>
         </is>
       </c>
       <c r="C3258">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3258">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3258">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3259">
@@ -62095,17 +62095,17 @@
       </c>
       <c r="B3259" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Zvolen</t>
         </is>
       </c>
       <c r="C3259">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D3259">
         <v>0</v>
       </c>
       <c r="E3259">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3260">
@@ -62114,36 +62114,36 @@
       </c>
       <c r="B3260" t="inlineStr">
         <is>
-          <t>Okres Žilina</t>
+          <t>Okres Žiar nad Hronom</t>
         </is>
       </c>
       <c r="C3260">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="D3260">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E3260">
-        <v>452</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3261">
       <c r="A3261" s="2">
-        <v>44179</v>
+        <v>44178</v>
       </c>
       <c r="B3261" t="inlineStr">
         <is>
-          <t>Okres Banská Bystrica</t>
+          <t>Okres Žilina</t>
         </is>
       </c>
       <c r="C3261">
-        <v>23</v>
+        <v>400</v>
       </c>
       <c r="D3261">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E3261">
-        <v>23</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3262">
@@ -62152,17 +62152,17 @@
       </c>
       <c r="B3262" t="inlineStr">
         <is>
-          <t>Okres Banská Štiavnica</t>
+          <t>Okres Bánovce nad Bebravou</t>
         </is>
       </c>
       <c r="C3262">
-        <v>14</v>
+        <v>249</v>
       </c>
       <c r="D3262">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="E3262">
-        <v>14</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3263">
@@ -62171,17 +62171,17 @@
       </c>
       <c r="B3263" t="inlineStr">
         <is>
-          <t>Okres Bardejov</t>
+          <t>Okres Banská Bystrica</t>
         </is>
       </c>
       <c r="C3263">
-        <v>24</v>
+        <v>282</v>
       </c>
       <c r="D3263">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E3263">
-        <v>26</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3264">
@@ -62190,17 +62190,17 @@
       </c>
       <c r="B3264" t="inlineStr">
         <is>
-          <t>Okres Bratislava I</t>
+          <t>Okres Banská Štiavnica</t>
         </is>
       </c>
       <c r="C3264">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D3264">
         <v>0</v>
       </c>
       <c r="E3264">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3265">
@@ -62209,17 +62209,17 @@
       </c>
       <c r="B3265" t="inlineStr">
         <is>
-          <t>Okres Bratislava II</t>
+          <t>Okres Bardejov</t>
         </is>
       </c>
       <c r="C3265">
-        <v>258</v>
+        <v>1016</v>
       </c>
       <c r="D3265">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="E3265">
-        <v>260</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="3266">
@@ -62228,17 +62228,17 @@
       </c>
       <c r="B3266" t="inlineStr">
         <is>
-          <t>Okres Bratislava III</t>
+          <t>Okres Bratislava I</t>
         </is>
       </c>
       <c r="C3266">
-        <v>81</v>
+        <v>394</v>
       </c>
       <c r="D3266">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E3266">
-        <v>83</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3267">
@@ -62247,17 +62247,17 @@
       </c>
       <c r="B3267" t="inlineStr">
         <is>
-          <t>Okres Bratislava IV</t>
+          <t>Okres Bratislava II</t>
         </is>
       </c>
       <c r="C3267">
-        <v>690</v>
+        <v>536</v>
       </c>
       <c r="D3267">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3267">
-        <v>704</v>
+        <v>552</v>
       </c>
     </row>
     <row r="3268">
@@ -62266,17 +62266,17 @@
       </c>
       <c r="B3268" t="inlineStr">
         <is>
-          <t>Okres Bratislava V</t>
+          <t>Okres Bratislava III</t>
         </is>
       </c>
       <c r="C3268">
-        <v>0</v>
+        <v>698</v>
       </c>
       <c r="D3268">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E3268">
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="3269">
@@ -62285,17 +62285,17 @@
       </c>
       <c r="B3269" t="inlineStr">
         <is>
-          <t>Okres Čadca</t>
+          <t>Okres Bratislava IV</t>
         </is>
       </c>
       <c r="C3269">
-        <v>62</v>
+        <v>690</v>
       </c>
       <c r="D3269">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3269">
-        <v>72</v>
+        <v>704</v>
       </c>
     </row>
     <row r="3270">
@@ -62304,17 +62304,17 @@
       </c>
       <c r="B3270" t="inlineStr">
         <is>
-          <t>Okres Dolný Kubín</t>
+          <t>Okres Bratislava V</t>
         </is>
       </c>
       <c r="C3270">
-        <v>276</v>
+        <v>690</v>
       </c>
       <c r="D3270">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="E3270">
-        <v>291</v>
+        <v>745</v>
       </c>
     </row>
     <row r="3271">
@@ -62323,17 +62323,17 @@
       </c>
       <c r="B3271" t="inlineStr">
         <is>
-          <t>Okres Dunajská Streda</t>
+          <t>Okres Čadca</t>
         </is>
       </c>
       <c r="C3271">
-        <v>343</v>
+        <v>65</v>
       </c>
       <c r="D3271">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3271">
-        <v>352</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3272">
@@ -62342,17 +62342,17 @@
       </c>
       <c r="B3272" t="inlineStr">
         <is>
-          <t>Okres Galanta</t>
+          <t>Okres Detva</t>
         </is>
       </c>
       <c r="C3272">
-        <v>3</v>
+        <v>231</v>
       </c>
       <c r="D3272">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E3272">
-        <v>3</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3273">
@@ -62361,17 +62361,17 @@
       </c>
       <c r="B3273" t="inlineStr">
         <is>
-          <t>Okres Hlohovec</t>
+          <t>Okres Dolný Kubín</t>
         </is>
       </c>
       <c r="C3273">
-        <v>9</v>
+        <v>286</v>
       </c>
       <c r="D3273">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E3273">
-        <v>10</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3274">
@@ -62380,17 +62380,17 @@
       </c>
       <c r="B3274" t="inlineStr">
         <is>
-          <t>Okres Humenné</t>
+          <t>Okres Dunajská Streda</t>
         </is>
       </c>
       <c r="C3274">
-        <v>113</v>
+        <v>393</v>
       </c>
       <c r="D3274">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E3274">
-        <v>118</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3275">
@@ -62399,17 +62399,17 @@
       </c>
       <c r="B3275" t="inlineStr">
         <is>
-          <t>Okres Ilava</t>
+          <t>Okres Galanta</t>
         </is>
       </c>
       <c r="C3275">
-        <v>361</v>
+        <v>119</v>
       </c>
       <c r="D3275">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="E3275">
-        <v>397</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3276">
@@ -62418,17 +62418,17 @@
       </c>
       <c r="B3276" t="inlineStr">
         <is>
-          <t>Okres Komárno</t>
+          <t>Okres Gelnica</t>
         </is>
       </c>
       <c r="C3276">
-        <v>17</v>
+        <v>247</v>
       </c>
       <c r="D3276">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E3276">
-        <v>17</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3277">
@@ -62437,17 +62437,17 @@
       </c>
       <c r="B3277" t="inlineStr">
         <is>
-          <t>Okres Košice II</t>
+          <t>Okres Hlohovec</t>
         </is>
       </c>
       <c r="C3277">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="D3277">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3277">
-        <v>88</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3278">
@@ -62456,17 +62456,17 @@
       </c>
       <c r="B3278" t="inlineStr">
         <is>
-          <t>Okres Levice</t>
+          <t>Okres Humenné</t>
         </is>
       </c>
       <c r="C3278">
-        <v>330</v>
+        <v>504</v>
       </c>
       <c r="D3278">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="E3278">
-        <v>334</v>
+        <v>574</v>
       </c>
     </row>
     <row r="3279">
@@ -62475,17 +62475,17 @@
       </c>
       <c r="B3279" t="inlineStr">
         <is>
-          <t>Okres Levoča</t>
+          <t>Okres Ilava</t>
         </is>
       </c>
       <c r="C3279">
-        <v>52</v>
+        <v>395</v>
       </c>
       <c r="D3279">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="E3279">
-        <v>57</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3280">
@@ -62494,17 +62494,17 @@
       </c>
       <c r="B3280" t="inlineStr">
         <is>
-          <t>Okres Liptovský Mikuláš</t>
+          <t>Okres Kežmarok</t>
         </is>
       </c>
       <c r="C3280">
-        <v>246</v>
+        <v>286</v>
       </c>
       <c r="D3280">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="E3280">
-        <v>254</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3281">
@@ -62513,17 +62513,17 @@
       </c>
       <c r="B3281" t="inlineStr">
         <is>
-          <t>Okres Lučenec</t>
+          <t>Okres Komárno</t>
         </is>
       </c>
       <c r="C3281">
-        <v>76</v>
+        <v>406</v>
       </c>
       <c r="D3281">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="E3281">
-        <v>80</v>
+        <v>448</v>
       </c>
     </row>
     <row r="3282">
@@ -62532,17 +62532,17 @@
       </c>
       <c r="B3282" t="inlineStr">
         <is>
-          <t>Okres Martin</t>
+          <t>Okres Košice I</t>
         </is>
       </c>
       <c r="C3282">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="D3282">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3282">
-        <v>55</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3283">
@@ -62551,17 +62551,17 @@
       </c>
       <c r="B3283" t="inlineStr">
         <is>
-          <t>Okres Michalovce</t>
+          <t>Okres Košice II</t>
         </is>
       </c>
       <c r="C3283">
-        <v>50</v>
+        <v>584</v>
       </c>
       <c r="D3283">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="E3283">
-        <v>54</v>
+        <v>612</v>
       </c>
     </row>
     <row r="3284">
@@ -62570,17 +62570,17 @@
       </c>
       <c r="B3284" t="inlineStr">
         <is>
-          <t>Okres Myjava</t>
+          <t>Okres Košice IV</t>
         </is>
       </c>
       <c r="C3284">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D3284">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3284">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3285">
@@ -62589,17 +62589,17 @@
       </c>
       <c r="B3285" t="inlineStr">
         <is>
-          <t>Okres Nitra</t>
+          <t>Okres Kysucké Nové Mesto</t>
         </is>
       </c>
       <c r="C3285">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D3285">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3285">
-        <v>43</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3286">
@@ -62608,17 +62608,17 @@
       </c>
       <c r="B3286" t="inlineStr">
         <is>
-          <t>Okres Nové Mesto nad Váhom</t>
+          <t>Okres Levice</t>
         </is>
       </c>
       <c r="C3286">
-        <v>0</v>
+        <v>1225</v>
       </c>
       <c r="D3286">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="E3286">
-        <v>0</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="3287">
@@ -62627,17 +62627,17 @@
       </c>
       <c r="B3287" t="inlineStr">
         <is>
-          <t>Okres Partizánske</t>
+          <t>Okres Levoča</t>
         </is>
       </c>
       <c r="C3287">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="D3287">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3287">
-        <v>19</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3288">
@@ -62646,17 +62646,17 @@
       </c>
       <c r="B3288" t="inlineStr">
         <is>
-          <t>Okres Pezinok</t>
+          <t>Okres Liptovský Mikuláš</t>
         </is>
       </c>
       <c r="C3288">
-        <v>12</v>
+        <v>246</v>
       </c>
       <c r="D3288">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E3288">
-        <v>14</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3289">
@@ -62665,17 +62665,17 @@
       </c>
       <c r="B3289" t="inlineStr">
         <is>
-          <t>Okres Poprad</t>
+          <t>Okres Lučenec</t>
         </is>
       </c>
       <c r="C3289">
-        <v>237</v>
+        <v>310</v>
       </c>
       <c r="D3289">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E3289">
-        <v>254</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3290">
@@ -62684,17 +62684,17 @@
       </c>
       <c r="B3290" t="inlineStr">
         <is>
-          <t>Okres Prešov</t>
+          <t>Okres Malacky</t>
         </is>
       </c>
       <c r="C3290">
-        <v>90</v>
+        <v>236</v>
       </c>
       <c r="D3290">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E3290">
-        <v>90</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3291">
@@ -62703,17 +62703,17 @@
       </c>
       <c r="B3291" t="inlineStr">
         <is>
-          <t>Okres Prievidza</t>
+          <t>Okres Martin</t>
         </is>
       </c>
       <c r="C3291">
-        <v>190</v>
+        <v>696</v>
       </c>
       <c r="D3291">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E3291">
-        <v>196</v>
+        <v>726</v>
       </c>
     </row>
     <row r="3292">
@@ -62722,17 +62722,17 @@
       </c>
       <c r="B3292" t="inlineStr">
         <is>
-          <t>Okres Revúca</t>
+          <t>Okres Medzilaborce</t>
         </is>
       </c>
       <c r="C3292">
-        <v>223</v>
+        <v>148</v>
       </c>
       <c r="D3292">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3292">
-        <v>235</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3293">
@@ -62741,17 +62741,17 @@
       </c>
       <c r="B3293" t="inlineStr">
         <is>
-          <t>Okres Rimavská Sobota</t>
+          <t>Okres Michalovce</t>
         </is>
       </c>
       <c r="C3293">
-        <v>357</v>
+        <v>831</v>
       </c>
       <c r="D3293">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="E3293">
-        <v>363</v>
+        <v>890</v>
       </c>
     </row>
     <row r="3294">
@@ -62760,17 +62760,17 @@
       </c>
       <c r="B3294" t="inlineStr">
         <is>
-          <t>Okres Rožňava</t>
+          <t>Okres Myjava</t>
         </is>
       </c>
       <c r="C3294">
-        <v>232</v>
+        <v>25</v>
       </c>
       <c r="D3294">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E3294">
-        <v>240</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3295">
@@ -62779,17 +62779,17 @@
       </c>
       <c r="B3295" t="inlineStr">
         <is>
-          <t>Okres Ružomberok</t>
+          <t>Okres Námestovo</t>
         </is>
       </c>
       <c r="C3295">
-        <v>4</v>
+        <v>577</v>
       </c>
       <c r="D3295">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="E3295">
-        <v>4</v>
+        <v>620</v>
       </c>
     </row>
     <row r="3296">
@@ -62798,17 +62798,17 @@
       </c>
       <c r="B3296" t="inlineStr">
         <is>
-          <t>Okres Skalica</t>
+          <t>Okres Nitra</t>
         </is>
       </c>
       <c r="C3296">
-        <v>10</v>
+        <v>2148</v>
       </c>
       <c r="D3296">
-        <v>2</v>
+        <v>251</v>
       </c>
       <c r="E3296">
-        <v>12</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="3297">
@@ -62817,17 +62817,17 @@
       </c>
       <c r="B3297" t="inlineStr">
         <is>
-          <t>Okres Sobrance</t>
+          <t>Okres Nové Mesto nad Váhom</t>
         </is>
       </c>
       <c r="C3297">
-        <v>4</v>
+        <v>220</v>
       </c>
       <c r="D3297">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E3297">
-        <v>4</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3298">
@@ -62836,17 +62836,17 @@
       </c>
       <c r="B3298" t="inlineStr">
         <is>
-          <t>Okres Topoľčany</t>
+          <t>Okres Nové Zámky</t>
         </is>
       </c>
       <c r="C3298">
-        <v>679</v>
+        <v>595</v>
       </c>
       <c r="D3298">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="E3298">
-        <v>745</v>
+        <v>646</v>
       </c>
     </row>
     <row r="3299">
@@ -62855,17 +62855,17 @@
       </c>
       <c r="B3299" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Partizánske</t>
         </is>
       </c>
       <c r="C3299">
-        <v>163</v>
+        <v>15</v>
       </c>
       <c r="D3299">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E3299">
-        <v>178</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3300">
@@ -62874,17 +62874,17 @@
       </c>
       <c r="B3300" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Pezinok</t>
         </is>
       </c>
       <c r="C3300">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="D3300">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="E3300">
-        <v>131</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3301">
@@ -62893,17 +62893,17 @@
       </c>
       <c r="B3301" t="inlineStr">
         <is>
-          <t>Okres Trnava</t>
+          <t>Okres Piešťany</t>
         </is>
       </c>
       <c r="C3301">
-        <v>137</v>
+        <v>462</v>
       </c>
       <c r="D3301">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E3301">
-        <v>145</v>
+        <v>502</v>
       </c>
     </row>
     <row r="3302">
@@ -62912,17 +62912,17 @@
       </c>
       <c r="B3302" t="inlineStr">
         <is>
-          <t>Okres Tvrdošín</t>
+          <t>Okres Poprad</t>
         </is>
       </c>
       <c r="C3302">
-        <v>24</v>
+        <v>707</v>
       </c>
       <c r="D3302">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="E3302">
-        <v>24</v>
+        <v>767</v>
       </c>
     </row>
     <row r="3303">
@@ -62931,17 +62931,17 @@
       </c>
       <c r="B3303" t="inlineStr">
         <is>
-          <t>Okres Veľký Krtíš</t>
+          <t>Okres Považská Bystrica</t>
         </is>
       </c>
       <c r="C3303">
-        <v>132</v>
+        <v>14</v>
       </c>
       <c r="D3303">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E3303">
-        <v>136</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3304">
@@ -62950,17 +62950,17 @@
       </c>
       <c r="B3304" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Prešov</t>
         </is>
       </c>
       <c r="C3304">
-        <v>66</v>
+        <v>2043</v>
       </c>
       <c r="D3304">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="E3304">
-        <v>68</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="3305">
@@ -62969,17 +62969,17 @@
       </c>
       <c r="B3305" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Prievidza</t>
         </is>
       </c>
       <c r="C3305">
-        <v>242</v>
+        <v>484</v>
       </c>
       <c r="D3305">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="E3305">
-        <v>251</v>
+        <v>550</v>
       </c>
     </row>
     <row r="3306">
@@ -62988,17 +62988,1461 @@
       </c>
       <c r="B3306" t="inlineStr">
         <is>
+          <t>Okres Púchov</t>
+        </is>
+      </c>
+      <c r="C3306">
+        <v>15</v>
+      </c>
+      <c r="D3306">
+        <v>1</v>
+      </c>
+      <c r="E3306">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3307">
+      <c r="A3307" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3307" t="inlineStr">
+        <is>
+          <t>Okres Revúca</t>
+        </is>
+      </c>
+      <c r="C3307">
+        <v>447</v>
+      </c>
+      <c r="D3307">
+        <v>19</v>
+      </c>
+      <c r="E3307">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="3308">
+      <c r="A3308" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3308" t="inlineStr">
+        <is>
+          <t>Okres Rimavská Sobota</t>
+        </is>
+      </c>
+      <c r="C3308">
+        <v>357</v>
+      </c>
+      <c r="D3308">
+        <v>6</v>
+      </c>
+      <c r="E3308">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3309">
+      <c r="A3309" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3309" t="inlineStr">
+        <is>
+          <t>Okres Rožňava</t>
+        </is>
+      </c>
+      <c r="C3309">
+        <v>232</v>
+      </c>
+      <c r="D3309">
+        <v>8</v>
+      </c>
+      <c r="E3309">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3310">
+      <c r="A3310" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3310" t="inlineStr">
+        <is>
+          <t>Okres Ružomberok</t>
+        </is>
+      </c>
+      <c r="C3310">
+        <v>4018</v>
+      </c>
+      <c r="D3310">
+        <v>498</v>
+      </c>
+      <c r="E3310">
+        <v>4516</v>
+      </c>
+    </row>
+    <row r="3311">
+      <c r="A3311" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3311" t="inlineStr">
+        <is>
+          <t>Okres Sabinov</t>
+        </is>
+      </c>
+      <c r="C3311">
+        <v>430</v>
+      </c>
+      <c r="D3311">
+        <v>25</v>
+      </c>
+      <c r="E3311">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="3312">
+      <c r="A3312" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3312" t="inlineStr">
+        <is>
+          <t>Okres Senec</t>
+        </is>
+      </c>
+      <c r="C3312">
+        <v>469</v>
+      </c>
+      <c r="D3312">
+        <v>17</v>
+      </c>
+      <c r="E3312">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="3313">
+      <c r="A3313" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3313" t="inlineStr">
+        <is>
+          <t>Okres Senica</t>
+        </is>
+      </c>
+      <c r="C3313">
+        <v>357</v>
+      </c>
+      <c r="D3313">
+        <v>32</v>
+      </c>
+      <c r="E3313">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="3314">
+      <c r="A3314" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3314" t="inlineStr">
+        <is>
+          <t>Okres Skalica</t>
+        </is>
+      </c>
+      <c r="C3314">
+        <v>11</v>
+      </c>
+      <c r="D3314">
+        <v>2</v>
+      </c>
+      <c r="E3314">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3315">
+      <c r="A3315" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3315" t="inlineStr">
+        <is>
+          <t>Okres Snina</t>
+        </is>
+      </c>
+      <c r="C3315">
+        <v>60</v>
+      </c>
+      <c r="D3315">
+        <v>4</v>
+      </c>
+      <c r="E3315">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3316">
+      <c r="A3316" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3316" t="inlineStr">
+        <is>
+          <t>Okres Sobrance</t>
+        </is>
+      </c>
+      <c r="C3316">
+        <v>79</v>
+      </c>
+      <c r="D3316">
+        <v>4</v>
+      </c>
+      <c r="E3316">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3317">
+      <c r="A3317" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3317" t="inlineStr">
+        <is>
+          <t>Okres Spišská Nová Ves</t>
+        </is>
+      </c>
+      <c r="C3317">
+        <v>310</v>
+      </c>
+      <c r="D3317">
+        <v>52</v>
+      </c>
+      <c r="E3317">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3318">
+      <c r="A3318" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3318" t="inlineStr">
+        <is>
+          <t>Okres Stará Ľubovňa</t>
+        </is>
+      </c>
+      <c r="C3318">
+        <v>90</v>
+      </c>
+      <c r="D3318">
+        <v>11</v>
+      </c>
+      <c r="E3318">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3319">
+      <c r="A3319" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3319" t="inlineStr">
+        <is>
+          <t>Okres Svidník</t>
+        </is>
+      </c>
+      <c r="C3319">
+        <v>64</v>
+      </c>
+      <c r="D3319">
+        <v>12</v>
+      </c>
+      <c r="E3319">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3320">
+      <c r="A3320" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3320" t="inlineStr">
+        <is>
+          <t>Okres Šaľa</t>
+        </is>
+      </c>
+      <c r="C3320">
+        <v>9</v>
+      </c>
+      <c r="D3320">
+        <v>2</v>
+      </c>
+      <c r="E3320">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3321">
+      <c r="A3321" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3321" t="inlineStr">
+        <is>
+          <t>Okres Topoľčany</t>
+        </is>
+      </c>
+      <c r="C3321">
+        <v>1075</v>
+      </c>
+      <c r="D3321">
+        <v>116</v>
+      </c>
+      <c r="E3321">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="3322">
+      <c r="A3322" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3322" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C3322">
+        <v>301</v>
+      </c>
+      <c r="D3322">
+        <v>17</v>
+      </c>
+      <c r="E3322">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3323">
+      <c r="A3323" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3323" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C3323">
+        <v>300</v>
+      </c>
+      <c r="D3323">
+        <v>127</v>
+      </c>
+      <c r="E3323">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="3324">
+      <c r="A3324" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3324" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C3324">
+        <v>217</v>
+      </c>
+      <c r="D3324">
+        <v>12</v>
+      </c>
+      <c r="E3324">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3325">
+      <c r="A3325" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3325" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C3325">
+        <v>337</v>
+      </c>
+      <c r="D3325">
+        <v>30</v>
+      </c>
+      <c r="E3325">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3326">
+      <c r="A3326" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3326" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C3326">
+        <v>910</v>
+      </c>
+      <c r="D3326">
+        <v>25</v>
+      </c>
+      <c r="E3326">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="3327">
+      <c r="A3327" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3327" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C3327">
+        <v>86</v>
+      </c>
+      <c r="D3327">
+        <v>2</v>
+      </c>
+      <c r="E3327">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3328">
+      <c r="A3328" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3328" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C3328">
+        <v>242</v>
+      </c>
+      <c r="D3328">
+        <v>9</v>
+      </c>
+      <c r="E3328">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3329">
+      <c r="A3329" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B3329" t="inlineStr">
+        <is>
           <t>Okres Žilina</t>
         </is>
       </c>
-      <c r="C3306">
-        <v>606</v>
-      </c>
-      <c r="D3306">
-        <v>51</v>
-      </c>
-      <c r="E3306">
-        <v>657</v>
+      <c r="C3329">
+        <v>1214</v>
+      </c>
+      <c r="D3329">
+        <v>132</v>
+      </c>
+      <c r="E3329">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="3330">
+      <c r="A3330" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3330" t="inlineStr">
+        <is>
+          <t>Okres Banská Bystrica</t>
+        </is>
+      </c>
+      <c r="C3330">
+        <v>862</v>
+      </c>
+      <c r="D3330">
+        <v>97</v>
+      </c>
+      <c r="E3330">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="3331">
+      <c r="A3331" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3331" t="inlineStr">
+        <is>
+          <t>Okres Bratislava I</t>
+        </is>
+      </c>
+      <c r="C3331">
+        <v>52</v>
+      </c>
+      <c r="D3331">
+        <v>0</v>
+      </c>
+      <c r="E3331">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3332">
+      <c r="A3332" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3332" t="inlineStr">
+        <is>
+          <t>Okres Bratislava II</t>
+        </is>
+      </c>
+      <c r="C3332">
+        <v>1015</v>
+      </c>
+      <c r="D3332">
+        <v>34</v>
+      </c>
+      <c r="E3332">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="3333">
+      <c r="A3333" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3333" t="inlineStr">
+        <is>
+          <t>Okres Bratislava III</t>
+        </is>
+      </c>
+      <c r="C3333">
+        <v>2050</v>
+      </c>
+      <c r="D3333">
+        <v>41</v>
+      </c>
+      <c r="E3333">
+        <v>2091</v>
+      </c>
+    </row>
+    <row r="3334">
+      <c r="A3334" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3334" t="inlineStr">
+        <is>
+          <t>Okres Bratislava IV</t>
+        </is>
+      </c>
+      <c r="C3334">
+        <v>318</v>
+      </c>
+      <c r="D3334">
+        <v>28</v>
+      </c>
+      <c r="E3334">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="3335">
+      <c r="A3335" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3335" t="inlineStr">
+        <is>
+          <t>Okres Bratislava V</t>
+        </is>
+      </c>
+      <c r="C3335">
+        <v>0</v>
+      </c>
+      <c r="D3335">
+        <v>0</v>
+      </c>
+      <c r="E3335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3336">
+      <c r="A3336" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3336" t="inlineStr">
+        <is>
+          <t>Okres Brezno</t>
+        </is>
+      </c>
+      <c r="C3336">
+        <v>494</v>
+      </c>
+      <c r="D3336">
+        <v>76</v>
+      </c>
+      <c r="E3336">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="3337">
+      <c r="A3337" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3337" t="inlineStr">
+        <is>
+          <t>Okres Čadca</t>
+        </is>
+      </c>
+      <c r="C3337">
+        <v>610</v>
+      </c>
+      <c r="D3337">
+        <v>82</v>
+      </c>
+      <c r="E3337">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="3338">
+      <c r="A3338" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3338" t="inlineStr">
+        <is>
+          <t>Okres Dolný Kubín</t>
+        </is>
+      </c>
+      <c r="C3338">
+        <v>156</v>
+      </c>
+      <c r="D3338">
+        <v>13</v>
+      </c>
+      <c r="E3338">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3339">
+      <c r="A3339" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3339" t="inlineStr">
+        <is>
+          <t>Okres Dunajská Streda</t>
+        </is>
+      </c>
+      <c r="C3339">
+        <v>348</v>
+      </c>
+      <c r="D3339">
+        <v>37</v>
+      </c>
+      <c r="E3339">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="3340">
+      <c r="A3340" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3340" t="inlineStr">
+        <is>
+          <t>Okres Galanta</t>
+        </is>
+      </c>
+      <c r="C3340">
+        <v>551</v>
+      </c>
+      <c r="D3340">
+        <v>60</v>
+      </c>
+      <c r="E3340">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="3341">
+      <c r="A3341" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3341" t="inlineStr">
+        <is>
+          <t>Okres Humenné</t>
+        </is>
+      </c>
+      <c r="C3341">
+        <v>125</v>
+      </c>
+      <c r="D3341">
+        <v>16</v>
+      </c>
+      <c r="E3341">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3342">
+      <c r="A3342" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3342" t="inlineStr">
+        <is>
+          <t>Okres Ilava</t>
+        </is>
+      </c>
+      <c r="C3342">
+        <v>271</v>
+      </c>
+      <c r="D3342">
+        <v>77</v>
+      </c>
+      <c r="E3342">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="3343">
+      <c r="A3343" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3343" t="inlineStr">
+        <is>
+          <t>Okres Komárno</t>
+        </is>
+      </c>
+      <c r="C3343">
+        <v>368</v>
+      </c>
+      <c r="D3343">
+        <v>27</v>
+      </c>
+      <c r="E3343">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="3344">
+      <c r="A3344" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3344" t="inlineStr">
+        <is>
+          <t>Okres Košice I</t>
+        </is>
+      </c>
+      <c r="C3344">
+        <v>460</v>
+      </c>
+      <c r="D3344">
+        <v>34</v>
+      </c>
+      <c r="E3344">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="3345">
+      <c r="A3345" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3345" t="inlineStr">
+        <is>
+          <t>Okres Košice II</t>
+        </is>
+      </c>
+      <c r="C3345">
+        <v>140</v>
+      </c>
+      <c r="D3345">
+        <v>3</v>
+      </c>
+      <c r="E3345">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3346">
+      <c r="A3346" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3346" t="inlineStr">
+        <is>
+          <t>Okres Košice IV</t>
+        </is>
+      </c>
+      <c r="C3346">
+        <v>333</v>
+      </c>
+      <c r="D3346">
+        <v>21</v>
+      </c>
+      <c r="E3346">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="3347">
+      <c r="A3347" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3347" t="inlineStr">
+        <is>
+          <t>Okres Krupina</t>
+        </is>
+      </c>
+      <c r="C3347">
+        <v>8</v>
+      </c>
+      <c r="D3347">
+        <v>3</v>
+      </c>
+      <c r="E3347">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3348">
+      <c r="A3348" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3348" t="inlineStr">
+        <is>
+          <t>Okres Levice</t>
+        </is>
+      </c>
+      <c r="C3348">
+        <v>165</v>
+      </c>
+      <c r="D3348">
+        <v>11</v>
+      </c>
+      <c r="E3348">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3349">
+      <c r="A3349" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3349" t="inlineStr">
+        <is>
+          <t>Okres Levoča</t>
+        </is>
+      </c>
+      <c r="C3349">
+        <v>252</v>
+      </c>
+      <c r="D3349">
+        <v>34</v>
+      </c>
+      <c r="E3349">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3350">
+      <c r="A3350" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3350" t="inlineStr">
+        <is>
+          <t>Okres Liptovský Mikuláš</t>
+        </is>
+      </c>
+      <c r="C3350">
+        <v>364</v>
+      </c>
+      <c r="D3350">
+        <v>19</v>
+      </c>
+      <c r="E3350">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="3351">
+      <c r="A3351" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3351" t="inlineStr">
+        <is>
+          <t>Okres Lučenec</t>
+        </is>
+      </c>
+      <c r="C3351">
+        <v>320</v>
+      </c>
+      <c r="D3351">
+        <v>16</v>
+      </c>
+      <c r="E3351">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3352">
+      <c r="A3352" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3352" t="inlineStr">
+        <is>
+          <t>Okres Martin</t>
+        </is>
+      </c>
+      <c r="C3352">
+        <v>107</v>
+      </c>
+      <c r="D3352">
+        <v>14</v>
+      </c>
+      <c r="E3352">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3353">
+      <c r="A3353" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3353" t="inlineStr">
+        <is>
+          <t>Okres Michalovce</t>
+        </is>
+      </c>
+      <c r="C3353">
+        <v>436</v>
+      </c>
+      <c r="D3353">
+        <v>32</v>
+      </c>
+      <c r="E3353">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="3354">
+      <c r="A3354" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3354" t="inlineStr">
+        <is>
+          <t>Okres Myjava</t>
+        </is>
+      </c>
+      <c r="C3354">
+        <v>239</v>
+      </c>
+      <c r="D3354">
+        <v>29</v>
+      </c>
+      <c r="E3354">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3355">
+      <c r="A3355" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3355" t="inlineStr">
+        <is>
+          <t>Okres Nitra</t>
+        </is>
+      </c>
+      <c r="C3355">
+        <v>419</v>
+      </c>
+      <c r="D3355">
+        <v>24</v>
+      </c>
+      <c r="E3355">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="3356">
+      <c r="A3356" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3356" t="inlineStr">
+        <is>
+          <t>Okres Nové Mesto nad Váhom</t>
+        </is>
+      </c>
+      <c r="C3356">
+        <v>191</v>
+      </c>
+      <c r="D3356">
+        <v>56</v>
+      </c>
+      <c r="E3356">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3357">
+      <c r="A3357" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3357" t="inlineStr">
+        <is>
+          <t>Okres Partizánske</t>
+        </is>
+      </c>
+      <c r="C3357">
+        <v>239</v>
+      </c>
+      <c r="D3357">
+        <v>55</v>
+      </c>
+      <c r="E3357">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3358">
+      <c r="A3358" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3358" t="inlineStr">
+        <is>
+          <t>Okres Pezinok</t>
+        </is>
+      </c>
+      <c r="C3358">
+        <v>367</v>
+      </c>
+      <c r="D3358">
+        <v>23</v>
+      </c>
+      <c r="E3358">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="3359">
+      <c r="A3359" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3359" t="inlineStr">
+        <is>
+          <t>Okres Piešťany</t>
+        </is>
+      </c>
+      <c r="C3359">
+        <v>1</v>
+      </c>
+      <c r="D3359">
+        <v>0</v>
+      </c>
+      <c r="E3359">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3360">
+      <c r="A3360" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3360" t="inlineStr">
+        <is>
+          <t>Okres Poprad</t>
+        </is>
+      </c>
+      <c r="C3360">
+        <v>392</v>
+      </c>
+      <c r="D3360">
+        <v>49</v>
+      </c>
+      <c r="E3360">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="3361">
+      <c r="A3361" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3361" t="inlineStr">
+        <is>
+          <t>Okres Považská Bystrica</t>
+        </is>
+      </c>
+      <c r="C3361">
+        <v>213</v>
+      </c>
+      <c r="D3361">
+        <v>42</v>
+      </c>
+      <c r="E3361">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3362">
+      <c r="A3362" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3362" t="inlineStr">
+        <is>
+          <t>Okres Prievidza</t>
+        </is>
+      </c>
+      <c r="C3362">
+        <v>336</v>
+      </c>
+      <c r="D3362">
+        <v>31</v>
+      </c>
+      <c r="E3362">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3363">
+      <c r="A3363" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3363" t="inlineStr">
+        <is>
+          <t>Okres Revúca</t>
+        </is>
+      </c>
+      <c r="C3363">
+        <v>366</v>
+      </c>
+      <c r="D3363">
+        <v>23</v>
+      </c>
+      <c r="E3363">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="3364">
+      <c r="A3364" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3364" t="inlineStr">
+        <is>
+          <t>Okres Rimavská Sobota</t>
+        </is>
+      </c>
+      <c r="C3364">
+        <v>268</v>
+      </c>
+      <c r="D3364">
+        <v>22</v>
+      </c>
+      <c r="E3364">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3365">
+      <c r="A3365" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3365" t="inlineStr">
+        <is>
+          <t>Okres Rožňava</t>
+        </is>
+      </c>
+      <c r="C3365">
+        <v>303</v>
+      </c>
+      <c r="D3365">
+        <v>21</v>
+      </c>
+      <c r="E3365">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="3366">
+      <c r="A3366" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3366" t="inlineStr">
+        <is>
+          <t>Okres Ružomberok</t>
+        </is>
+      </c>
+      <c r="C3366">
+        <v>95</v>
+      </c>
+      <c r="D3366">
+        <v>2</v>
+      </c>
+      <c r="E3366">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3367">
+      <c r="A3367" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3367" t="inlineStr">
+        <is>
+          <t>Okres Senica</t>
+        </is>
+      </c>
+      <c r="C3367">
+        <v>2</v>
+      </c>
+      <c r="D3367">
+        <v>0</v>
+      </c>
+      <c r="E3367">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3368">
+      <c r="A3368" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3368" t="inlineStr">
+        <is>
+          <t>Okres Skalica</t>
+        </is>
+      </c>
+      <c r="C3368">
+        <v>346</v>
+      </c>
+      <c r="D3368">
+        <v>20</v>
+      </c>
+      <c r="E3368">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3369">
+      <c r="A3369" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3369" t="inlineStr">
+        <is>
+          <t>Okres Snina</t>
+        </is>
+      </c>
+      <c r="C3369">
+        <v>23</v>
+      </c>
+      <c r="D3369">
+        <v>3</v>
+      </c>
+      <c r="E3369">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3370">
+      <c r="A3370" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3370" t="inlineStr">
+        <is>
+          <t>Okres Sobrance</t>
+        </is>
+      </c>
+      <c r="C3370">
+        <v>112</v>
+      </c>
+      <c r="D3370">
+        <v>7</v>
+      </c>
+      <c r="E3370">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3371">
+      <c r="A3371" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3371" t="inlineStr">
+        <is>
+          <t>Okres Spišská Nová Ves</t>
+        </is>
+      </c>
+      <c r="C3371">
+        <v>215</v>
+      </c>
+      <c r="D3371">
+        <v>34</v>
+      </c>
+      <c r="E3371">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3372">
+      <c r="A3372" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3372" t="inlineStr">
+        <is>
+          <t>Okres Stará Ľubovňa</t>
+        </is>
+      </c>
+      <c r="C3372">
+        <v>249</v>
+      </c>
+      <c r="D3372">
+        <v>35</v>
+      </c>
+      <c r="E3372">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3373">
+      <c r="A3373" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3373" t="inlineStr">
+        <is>
+          <t>Okres Topoľčany</t>
+        </is>
+      </c>
+      <c r="C3373">
+        <v>328</v>
+      </c>
+      <c r="D3373">
+        <v>26</v>
+      </c>
+      <c r="E3373">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="3374">
+      <c r="A3374" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3374" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C3374">
+        <v>713</v>
+      </c>
+      <c r="D3374">
+        <v>49</v>
+      </c>
+      <c r="E3374">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="3375">
+      <c r="A3375" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3375" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C3375">
+        <v>293</v>
+      </c>
+      <c r="D3375">
+        <v>48</v>
+      </c>
+      <c r="E3375">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3376">
+      <c r="A3376" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3376" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C3376">
+        <v>630</v>
+      </c>
+      <c r="D3376">
+        <v>74</v>
+      </c>
+      <c r="E3376">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="3377">
+      <c r="A3377" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3377" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C3377">
+        <v>24</v>
+      </c>
+      <c r="D3377">
+        <v>2</v>
+      </c>
+      <c r="E3377">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3378">
+      <c r="A3378" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3378" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C3378">
+        <v>120</v>
+      </c>
+      <c r="D3378">
+        <v>7</v>
+      </c>
+      <c r="E3378">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3379">
+      <c r="A3379" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3379" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C3379">
+        <v>297</v>
+      </c>
+      <c r="D3379">
+        <v>74</v>
+      </c>
+      <c r="E3379">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3380">
+      <c r="A3380" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3380" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C3380">
+        <v>218</v>
+      </c>
+      <c r="D3380">
+        <v>14</v>
+      </c>
+      <c r="E3380">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3381">
+      <c r="A3381" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3381" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C3381">
+        <v>317</v>
+      </c>
+      <c r="D3381">
+        <v>33</v>
+      </c>
+      <c r="E3381">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="3382">
+      <c r="A3382" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B3382" t="inlineStr">
+        <is>
+          <t>Okres Žilina</t>
+        </is>
+      </c>
+      <c r="C3382">
+        <v>572</v>
+      </c>
+      <c r="D3382">
+        <v>57</v>
+      </c>
+      <c r="E3382">
+        <v>629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: st 23. 12. 2020
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_AgTests_District.xlsx
+++ b/OpenData_Slovakia_Covid_AgTests_District.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3841"/>
+  <dimension ref="A1:E3916"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -47678,13 +47678,13 @@
         </is>
       </c>
       <c r="C2500">
-        <v>104</v>
+        <v>445</v>
       </c>
       <c r="D2500">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E2500">
-        <v>107</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2501">
@@ -48210,13 +48210,13 @@
         </is>
       </c>
       <c r="C2528">
-        <v>1032</v>
+        <v>891</v>
       </c>
       <c r="D2528">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E2528">
-        <v>1092</v>
+        <v>946</v>
       </c>
     </row>
     <row r="2529">
@@ -48837,13 +48837,13 @@
         </is>
       </c>
       <c r="C2561">
-        <v>899</v>
+        <v>1199</v>
       </c>
       <c r="D2561">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E2561">
-        <v>939</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="2562">
@@ -49483,13 +49483,13 @@
         </is>
       </c>
       <c r="C2595">
-        <v>706</v>
+        <v>608</v>
       </c>
       <c r="D2595">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E2595">
-        <v>749</v>
+        <v>642</v>
       </c>
     </row>
     <row r="2596">
@@ -50072,13 +50072,13 @@
         </is>
       </c>
       <c r="C2626">
-        <v>2212</v>
+        <v>2477</v>
       </c>
       <c r="D2626">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E2626">
-        <v>2245</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="2627">
@@ -50680,13 +50680,13 @@
         </is>
       </c>
       <c r="C2658">
-        <v>1089</v>
+        <v>900</v>
       </c>
       <c r="D2658">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E2658">
-        <v>1133</v>
+        <v>942</v>
       </c>
     </row>
     <row r="2659">
@@ -51307,13 +51307,13 @@
         </is>
       </c>
       <c r="C2691">
-        <v>557</v>
+        <v>820</v>
       </c>
       <c r="D2691">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E2691">
-        <v>596</v>
+        <v>874</v>
       </c>
     </row>
     <row r="2692">
@@ -51915,13 +51915,13 @@
         </is>
       </c>
       <c r="C2723">
-        <v>1076</v>
+        <v>875</v>
       </c>
       <c r="D2723">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E2723">
-        <v>1112</v>
+        <v>905</v>
       </c>
     </row>
     <row r="2724">
@@ -52618,13 +52618,13 @@
         </is>
       </c>
       <c r="C2760">
-        <v>861</v>
+        <v>1200</v>
       </c>
       <c r="D2760">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E2760">
-        <v>901</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="2761">
@@ -53017,13 +53017,13 @@
         </is>
       </c>
       <c r="C2781">
-        <v>1549</v>
+        <v>987</v>
       </c>
       <c r="D2781">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E2781">
-        <v>1572</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="2782">
@@ -53758,13 +53758,13 @@
         </is>
       </c>
       <c r="C2820">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="D2820">
         <v>0</v>
       </c>
       <c r="E2820">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2821">
@@ -55886,13 +55886,13 @@
         </is>
       </c>
       <c r="C2932">
-        <v>2473</v>
+        <v>2089</v>
       </c>
       <c r="D2932">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="E2932">
-        <v>2659</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="2933">
@@ -57178,13 +57178,13 @@
         </is>
       </c>
       <c r="C3000">
-        <v>2019</v>
+        <v>1635</v>
       </c>
       <c r="D3000">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="E3000">
-        <v>2138</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="3001">
@@ -58489,13 +58489,13 @@
         </is>
       </c>
       <c r="C3069">
-        <v>1505</v>
+        <v>1332</v>
       </c>
       <c r="D3069">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="E3069">
-        <v>1619</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="3070">
@@ -59192,13 +59192,13 @@
         </is>
       </c>
       <c r="C3106">
-        <v>1747</v>
+        <v>2077</v>
       </c>
       <c r="D3106">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="E3106">
-        <v>1880</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="3107">
@@ -59838,13 +59838,13 @@
         </is>
       </c>
       <c r="C3140">
-        <v>1642</v>
+        <v>1513</v>
       </c>
       <c r="D3140">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E3140">
-        <v>1753</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="3141">
@@ -60541,13 +60541,13 @@
         </is>
       </c>
       <c r="C3177">
-        <v>1105</v>
+        <v>1373</v>
       </c>
       <c r="D3177">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="E3177">
-        <v>1170</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="3178">
@@ -61016,13 +61016,13 @@
         </is>
       </c>
       <c r="C3202">
-        <v>574</v>
+        <v>436</v>
       </c>
       <c r="D3202">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E3202">
-        <v>588</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3203">
@@ -63410,13 +63410,13 @@
         </is>
       </c>
       <c r="C3328">
-        <v>766</v>
+        <v>1063</v>
       </c>
       <c r="D3328">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="E3328">
-        <v>833</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="3329">
@@ -63562,13 +63562,13 @@
         </is>
       </c>
       <c r="C3336">
-        <v>885</v>
+        <v>900</v>
       </c>
       <c r="D3336">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E3336">
-        <v>984</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3337">
@@ -63581,13 +63581,13 @@
         </is>
       </c>
       <c r="C3337">
-        <v>715</v>
+        <v>747</v>
       </c>
       <c r="D3337">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E3337">
-        <v>749</v>
+        <v>784</v>
       </c>
     </row>
     <row r="3338">
@@ -64018,13 +64018,13 @@
         </is>
       </c>
       <c r="C3360">
-        <v>3543</v>
+        <v>3390</v>
       </c>
       <c r="D3360">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E3360">
-        <v>3742</v>
+        <v>3578</v>
       </c>
     </row>
     <row r="3361">
@@ -64721,13 +64721,13 @@
         </is>
       </c>
       <c r="C3397">
-        <v>647</v>
+        <v>908</v>
       </c>
       <c r="D3397">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="E3397">
-        <v>724</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="3398">
@@ -65367,13 +65367,13 @@
         </is>
       </c>
       <c r="C3431">
-        <v>2326</v>
+        <v>2234</v>
       </c>
       <c r="D3431">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E3431">
-        <v>2436</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="3432">
@@ -66089,13 +66089,13 @@
         </is>
       </c>
       <c r="C3469">
-        <v>1785</v>
+        <v>2097</v>
       </c>
       <c r="D3469">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="E3469">
-        <v>1942</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="3470">
@@ -66355,13 +66355,13 @@
         </is>
       </c>
       <c r="C3483">
-        <v>1836</v>
+        <v>2117</v>
       </c>
       <c r="D3483">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E3483">
-        <v>1903</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="3484">
@@ -66735,13 +66735,13 @@
         </is>
       </c>
       <c r="C3503">
-        <v>1538</v>
+        <v>1471</v>
       </c>
       <c r="D3503">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E3503">
-        <v>1639</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="3504">
@@ -68084,13 +68084,13 @@
         </is>
       </c>
       <c r="C3574">
-        <v>2191</v>
+        <v>2102</v>
       </c>
       <c r="D3574">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E3574">
-        <v>2311</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="3575">
@@ -68806,13 +68806,13 @@
         </is>
       </c>
       <c r="C3612">
-        <v>1570</v>
+        <v>1880</v>
       </c>
       <c r="D3612">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="E3612">
-        <v>1714</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="3613">
@@ -70687,13 +70687,13 @@
         </is>
       </c>
       <c r="C3711">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="D3711">
         <v>36</v>
       </c>
       <c r="E3711">
-        <v>878</v>
+        <v>881</v>
       </c>
     </row>
     <row r="3712">
@@ -70782,13 +70782,13 @@
         </is>
       </c>
       <c r="C3716">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D3716">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E3716">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="3717">
@@ -70877,13 +70877,13 @@
         </is>
       </c>
       <c r="C3721">
-        <v>696</v>
+        <v>944</v>
       </c>
       <c r="D3721">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="E3721">
-        <v>745</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="3722">
@@ -71298,10 +71298,10 @@
         <v>319</v>
       </c>
       <c r="D3743">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E3743">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3744">
@@ -71390,13 +71390,13 @@
         </is>
       </c>
       <c r="C3748">
-        <v>1803</v>
+        <v>1974</v>
       </c>
       <c r="D3748">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="E3748">
-        <v>1899</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="3749">
@@ -71428,13 +71428,13 @@
         </is>
       </c>
       <c r="C3750">
-        <v>1960</v>
+        <v>2022</v>
       </c>
       <c r="D3750">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E3750">
-        <v>2096</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="3751">
@@ -71542,13 +71542,13 @@
         </is>
       </c>
       <c r="C3756">
-        <v>6046</v>
+        <v>6383</v>
       </c>
       <c r="D3756">
-        <v>648</v>
+        <v>706</v>
       </c>
       <c r="E3756">
-        <v>6694</v>
+        <v>7089</v>
       </c>
     </row>
     <row r="3757">
@@ -71770,13 +71770,13 @@
         </is>
       </c>
       <c r="C3768">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="D3768">
         <v>46</v>
       </c>
       <c r="E3768">
-        <v>558</v>
+        <v>561</v>
       </c>
     </row>
     <row r="3769">
@@ -71808,13 +71808,13 @@
         </is>
       </c>
       <c r="C3770">
-        <v>1342</v>
+        <v>1649</v>
       </c>
       <c r="D3770">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="E3770">
-        <v>1442</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="3771">
@@ -71884,13 +71884,13 @@
         </is>
       </c>
       <c r="C3774">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="D3774">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="E3774">
-        <v>25</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3775">
@@ -71975,17 +71975,17 @@
       </c>
       <c r="B3779" t="inlineStr">
         <is>
-          <t>Okres Banská Bystrica</t>
+          <t>Okres Bánovce nad Bebravou</t>
         </is>
       </c>
       <c r="C3779">
-        <v>1059</v>
+        <v>399</v>
       </c>
       <c r="D3779">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="E3779">
-        <v>1154</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3780">
@@ -71994,17 +71994,17 @@
       </c>
       <c r="B3780" t="inlineStr">
         <is>
-          <t>Okres Banská Štiavnica</t>
+          <t>Okres Banská Bystrica</t>
         </is>
       </c>
       <c r="C3780">
-        <v>335</v>
+        <v>1286</v>
       </c>
       <c r="D3780">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="E3780">
-        <v>366</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="3781">
@@ -72013,17 +72013,17 @@
       </c>
       <c r="B3781" t="inlineStr">
         <is>
-          <t>Okres Bardejov</t>
+          <t>Okres Banská Štiavnica</t>
         </is>
       </c>
       <c r="C3781">
-        <v>141</v>
+        <v>689</v>
       </c>
       <c r="D3781">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="E3781">
-        <v>170</v>
+        <v>743</v>
       </c>
     </row>
     <row r="3782">
@@ -72032,17 +72032,17 @@
       </c>
       <c r="B3782" t="inlineStr">
         <is>
-          <t>Okres Bratislava I</t>
+          <t>Okres Bardejov</t>
         </is>
       </c>
       <c r="C3782">
-        <v>100</v>
+        <v>887</v>
       </c>
       <c r="D3782">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="E3782">
-        <v>102</v>
+        <v>968</v>
       </c>
     </row>
     <row r="3783">
@@ -72051,17 +72051,17 @@
       </c>
       <c r="B3783" t="inlineStr">
         <is>
-          <t>Okres Bratislava II</t>
+          <t>Okres Bratislava I</t>
         </is>
       </c>
       <c r="C3783">
-        <v>522</v>
+        <v>1694</v>
       </c>
       <c r="D3783">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E3783">
-        <v>537</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="3784">
@@ -72070,17 +72070,17 @@
       </c>
       <c r="B3784" t="inlineStr">
         <is>
-          <t>Okres Bratislava III</t>
+          <t>Okres Bratislava II</t>
         </is>
       </c>
       <c r="C3784">
-        <v>555</v>
+        <v>3601</v>
       </c>
       <c r="D3784">
-        <v>11</v>
+        <v>213</v>
       </c>
       <c r="E3784">
-        <v>566</v>
+        <v>3814</v>
       </c>
     </row>
     <row r="3785">
@@ -72089,17 +72089,17 @@
       </c>
       <c r="B3785" t="inlineStr">
         <is>
-          <t>Okres Bratislava IV</t>
+          <t>Okres Bratislava III</t>
         </is>
       </c>
       <c r="C3785">
-        <v>4</v>
+        <v>772</v>
       </c>
       <c r="D3785">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E3785">
-        <v>4</v>
+        <v>790</v>
       </c>
     </row>
     <row r="3786">
@@ -72108,17 +72108,17 @@
       </c>
       <c r="B3786" t="inlineStr">
         <is>
-          <t>Okres Bratislava V</t>
+          <t>Okres Bratislava IV</t>
         </is>
       </c>
       <c r="C3786">
-        <v>449</v>
+        <v>919</v>
       </c>
       <c r="D3786">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E3786">
-        <v>492</v>
+        <v>965</v>
       </c>
     </row>
     <row r="3787">
@@ -72127,17 +72127,17 @@
       </c>
       <c r="B3787" t="inlineStr">
         <is>
-          <t>Okres Brezno</t>
+          <t>Okres Bratislava V</t>
         </is>
       </c>
       <c r="C3787">
-        <v>8</v>
+        <v>1870</v>
       </c>
       <c r="D3787">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="E3787">
-        <v>18</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="3788">
@@ -72146,17 +72146,17 @@
       </c>
       <c r="B3788" t="inlineStr">
         <is>
-          <t>Okres Bytča</t>
+          <t>Okres Brezno</t>
         </is>
       </c>
       <c r="C3788">
-        <v>262</v>
+        <v>486</v>
       </c>
       <c r="D3788">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="E3788">
-        <v>305</v>
+        <v>549</v>
       </c>
     </row>
     <row r="3789">
@@ -72165,17 +72165,17 @@
       </c>
       <c r="B3789" t="inlineStr">
         <is>
-          <t>Okres Čadca</t>
+          <t>Okres Bytča</t>
         </is>
       </c>
       <c r="C3789">
-        <v>681</v>
+        <v>262</v>
       </c>
       <c r="D3789">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E3789">
-        <v>737</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3790">
@@ -72184,17 +72184,17 @@
       </c>
       <c r="B3790" t="inlineStr">
         <is>
-          <t>Okres Detva</t>
+          <t>Okres Čadca</t>
         </is>
       </c>
       <c r="C3790">
-        <v>3</v>
+        <v>1312</v>
       </c>
       <c r="D3790">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="E3790">
-        <v>5</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="3791">
@@ -72203,17 +72203,17 @@
       </c>
       <c r="B3791" t="inlineStr">
         <is>
-          <t>Okres Dolný Kubín</t>
+          <t>Okres Detva</t>
         </is>
       </c>
       <c r="C3791">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="D3791">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E3791">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3792">
@@ -72222,17 +72222,17 @@
       </c>
       <c r="B3792" t="inlineStr">
         <is>
-          <t>Okres Dunajská Streda</t>
+          <t>Okres Dolný Kubín</t>
         </is>
       </c>
       <c r="C3792">
-        <v>407</v>
+        <v>319</v>
       </c>
       <c r="D3792">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E3792">
-        <v>450</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3793">
@@ -72241,17 +72241,17 @@
       </c>
       <c r="B3793" t="inlineStr">
         <is>
-          <t>Okres Galanta</t>
+          <t>Okres Dunajská Streda</t>
         </is>
       </c>
       <c r="C3793">
-        <v>956</v>
+        <v>592</v>
       </c>
       <c r="D3793">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="E3793">
-        <v>1068</v>
+        <v>658</v>
       </c>
     </row>
     <row r="3794">
@@ -72260,17 +72260,17 @@
       </c>
       <c r="B3794" t="inlineStr">
         <is>
-          <t>Okres Hlohovec</t>
+          <t>Okres Galanta</t>
         </is>
       </c>
       <c r="C3794">
-        <v>13</v>
+        <v>1069</v>
       </c>
       <c r="D3794">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="E3794">
-        <v>13</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="3795">
@@ -72279,17 +72279,17 @@
       </c>
       <c r="B3795" t="inlineStr">
         <is>
-          <t>Okres Humenné</t>
+          <t>Okres Gelnica</t>
         </is>
       </c>
       <c r="C3795">
-        <v>219</v>
+        <v>306</v>
       </c>
       <c r="D3795">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E3795">
-        <v>245</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3796">
@@ -72298,17 +72298,17 @@
       </c>
       <c r="B3796" t="inlineStr">
         <is>
-          <t>Okres Ilava</t>
+          <t>Okres Hlohovec</t>
         </is>
       </c>
       <c r="C3796">
-        <v>330</v>
+        <v>375</v>
       </c>
       <c r="D3796">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E3796">
-        <v>378</v>
+        <v>408</v>
       </c>
     </row>
     <row r="3797">
@@ -72317,17 +72317,17 @@
       </c>
       <c r="B3797" t="inlineStr">
         <is>
-          <t>Okres Komárno</t>
+          <t>Okres Humenné</t>
         </is>
       </c>
       <c r="C3797">
-        <v>509</v>
+        <v>1165</v>
       </c>
       <c r="D3797">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="E3797">
-        <v>544</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="3798">
@@ -72336,17 +72336,17 @@
       </c>
       <c r="B3798" t="inlineStr">
         <is>
-          <t>Okres Košice I</t>
+          <t>Okres Ilava</t>
         </is>
       </c>
       <c r="C3798">
-        <v>577</v>
+        <v>417</v>
       </c>
       <c r="D3798">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="E3798">
-        <v>597</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3799">
@@ -72355,17 +72355,17 @@
       </c>
       <c r="B3799" t="inlineStr">
         <is>
-          <t>Okres Košice II</t>
+          <t>Okres Kežmarok</t>
         </is>
       </c>
       <c r="C3799">
-        <v>126</v>
+        <v>8</v>
       </c>
       <c r="D3799">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E3799">
-        <v>134</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3800">
@@ -72374,17 +72374,17 @@
       </c>
       <c r="B3800" t="inlineStr">
         <is>
-          <t>Okres Košice IV</t>
+          <t>Okres Komárno</t>
         </is>
       </c>
       <c r="C3800">
-        <v>381</v>
+        <v>754</v>
       </c>
       <c r="D3800">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="E3800">
-        <v>419</v>
+        <v>803</v>
       </c>
     </row>
     <row r="3801">
@@ -72393,17 +72393,17 @@
       </c>
       <c r="B3801" t="inlineStr">
         <is>
-          <t>Okres Kysucké Nové Mesto</t>
+          <t>Okres Košice I</t>
         </is>
       </c>
       <c r="C3801">
-        <v>3079</v>
+        <v>577</v>
       </c>
       <c r="D3801">
-        <v>374</v>
+        <v>20</v>
       </c>
       <c r="E3801">
-        <v>3453</v>
+        <v>597</v>
       </c>
     </row>
     <row r="3802">
@@ -72412,17 +72412,17 @@
       </c>
       <c r="B3802" t="inlineStr">
         <is>
-          <t>Okres Levice</t>
+          <t>Okres Košice II</t>
         </is>
       </c>
       <c r="C3802">
-        <v>450</v>
+        <v>987</v>
       </c>
       <c r="D3802">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="E3802">
-        <v>467</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="3803">
@@ -72431,17 +72431,17 @@
       </c>
       <c r="B3803" t="inlineStr">
         <is>
-          <t>Okres Levoča</t>
+          <t>Okres Košice IV</t>
         </is>
       </c>
       <c r="C3803">
-        <v>263</v>
+        <v>390</v>
       </c>
       <c r="D3803">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E3803">
-        <v>290</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3804">
@@ -72450,17 +72450,17 @@
       </c>
       <c r="B3804" t="inlineStr">
         <is>
-          <t>Okres Liptovský Mikuláš</t>
+          <t>Okres Krupina</t>
         </is>
       </c>
       <c r="C3804">
-        <v>427</v>
+        <v>3</v>
       </c>
       <c r="D3804">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E3804">
-        <v>459</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3805">
@@ -72469,17 +72469,17 @@
       </c>
       <c r="B3805" t="inlineStr">
         <is>
-          <t>Okres Lučenec</t>
+          <t>Okres Kysucké Nové Mesto</t>
         </is>
       </c>
       <c r="C3805">
-        <v>353</v>
+        <v>3084</v>
       </c>
       <c r="D3805">
-        <v>24</v>
+        <v>376</v>
       </c>
       <c r="E3805">
-        <v>377</v>
+        <v>3460</v>
       </c>
     </row>
     <row r="3806">
@@ -72488,17 +72488,17 @@
       </c>
       <c r="B3806" t="inlineStr">
         <is>
-          <t>Okres Michalovce</t>
+          <t>Okres Levice</t>
         </is>
       </c>
       <c r="C3806">
-        <v>907</v>
+        <v>2532</v>
       </c>
       <c r="D3806">
-        <v>61</v>
+        <v>172</v>
       </c>
       <c r="E3806">
-        <v>968</v>
+        <v>2704</v>
       </c>
     </row>
     <row r="3807">
@@ -72507,17 +72507,17 @@
       </c>
       <c r="B3807" t="inlineStr">
         <is>
-          <t>Okres Myjava</t>
+          <t>Okres Levoča</t>
         </is>
       </c>
       <c r="C3807">
-        <v>329</v>
+        <v>1693</v>
       </c>
       <c r="D3807">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="E3807">
-        <v>350</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="3808">
@@ -72526,17 +72526,17 @@
       </c>
       <c r="B3808" t="inlineStr">
         <is>
-          <t>Okres Námestovo</t>
+          <t>Okres Liptovský Mikuláš</t>
         </is>
       </c>
       <c r="C3808">
-        <v>272</v>
+        <v>427</v>
       </c>
       <c r="D3808">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E3808">
-        <v>294</v>
+        <v>459</v>
       </c>
     </row>
     <row r="3809">
@@ -72545,17 +72545,17 @@
       </c>
       <c r="B3809" t="inlineStr">
         <is>
-          <t>Okres Nitra</t>
+          <t>Okres Lučenec</t>
         </is>
       </c>
       <c r="C3809">
-        <v>223</v>
+        <v>609</v>
       </c>
       <c r="D3809">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E3809">
-        <v>267</v>
+        <v>648</v>
       </c>
     </row>
     <row r="3810">
@@ -72564,17 +72564,17 @@
       </c>
       <c r="B3810" t="inlineStr">
         <is>
-          <t>Okres Nové Mesto nad Váhom</t>
+          <t>Okres Martin</t>
         </is>
       </c>
       <c r="C3810">
-        <v>212</v>
+        <v>1222</v>
       </c>
       <c r="D3810">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="E3810">
-        <v>243</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="3811">
@@ -72583,17 +72583,17 @@
       </c>
       <c r="B3811" t="inlineStr">
         <is>
-          <t>Okres Partizánske</t>
+          <t>Okres Medzilaborce</t>
         </is>
       </c>
       <c r="C3811">
-        <v>355</v>
+        <v>148</v>
       </c>
       <c r="D3811">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E3811">
-        <v>435</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3812">
@@ -72602,17 +72602,17 @@
       </c>
       <c r="B3812" t="inlineStr">
         <is>
-          <t>Okres Pezinok</t>
+          <t>Okres Michalovce</t>
         </is>
       </c>
       <c r="C3812">
-        <v>458</v>
+        <v>2398</v>
       </c>
       <c r="D3812">
-        <v>39</v>
+        <v>152</v>
       </c>
       <c r="E3812">
-        <v>497</v>
+        <v>2550</v>
       </c>
     </row>
     <row r="3813">
@@ -72621,17 +72621,17 @@
       </c>
       <c r="B3813" t="inlineStr">
         <is>
-          <t>Okres Piešťany</t>
+          <t>Okres Myjava</t>
         </is>
       </c>
       <c r="C3813">
-        <v>294</v>
+        <v>329</v>
       </c>
       <c r="D3813">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E3813">
-        <v>304</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3814">
@@ -72640,17 +72640,17 @@
       </c>
       <c r="B3814" t="inlineStr">
         <is>
-          <t>Okres Poprad</t>
+          <t>Okres Námestovo</t>
         </is>
       </c>
       <c r="C3814">
-        <v>535</v>
+        <v>790</v>
       </c>
       <c r="D3814">
         <v>61</v>
       </c>
       <c r="E3814">
-        <v>596</v>
+        <v>851</v>
       </c>
     </row>
     <row r="3815">
@@ -72659,17 +72659,17 @@
       </c>
       <c r="B3815" t="inlineStr">
         <is>
-          <t>Okres Považská Bystrica</t>
+          <t>Okres Nitra</t>
         </is>
       </c>
       <c r="C3815">
-        <v>497</v>
+        <v>866</v>
       </c>
       <c r="D3815">
-        <v>104</v>
+        <v>164</v>
       </c>
       <c r="E3815">
-        <v>601</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="3816">
@@ -72678,17 +72678,17 @@
       </c>
       <c r="B3816" t="inlineStr">
         <is>
-          <t>Okres Prešov</t>
+          <t>Okres Nové Mesto nad Váhom</t>
         </is>
       </c>
       <c r="C3816">
-        <v>518</v>
+        <v>607</v>
       </c>
       <c r="D3816">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="E3816">
-        <v>555</v>
+        <v>677</v>
       </c>
     </row>
     <row r="3817">
@@ -72697,17 +72697,17 @@
       </c>
       <c r="B3817" t="inlineStr">
         <is>
-          <t>Okres Prievidza</t>
+          <t>Okres Nové Zámky</t>
         </is>
       </c>
       <c r="C3817">
-        <v>381</v>
+        <v>1186</v>
       </c>
       <c r="D3817">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="E3817">
-        <v>403</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="3818">
@@ -72716,17 +72716,17 @@
       </c>
       <c r="B3818" t="inlineStr">
         <is>
-          <t>Okres Revúca</t>
+          <t>Okres Partizánske</t>
         </is>
       </c>
       <c r="C3818">
-        <v>532</v>
+        <v>358</v>
       </c>
       <c r="D3818">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="E3818">
-        <v>554</v>
+        <v>441</v>
       </c>
     </row>
     <row r="3819">
@@ -72735,17 +72735,17 @@
       </c>
       <c r="B3819" t="inlineStr">
         <is>
-          <t>Okres Rimavská Sobota</t>
+          <t>Okres Pezinok</t>
         </is>
       </c>
       <c r="C3819">
-        <v>623</v>
+        <v>1115</v>
       </c>
       <c r="D3819">
-        <v>39</v>
+        <v>173</v>
       </c>
       <c r="E3819">
-        <v>662</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="3820">
@@ -72754,17 +72754,17 @@
       </c>
       <c r="B3820" t="inlineStr">
         <is>
-          <t>Okres Rožňava</t>
+          <t>Okres Piešťany</t>
         </is>
       </c>
       <c r="C3820">
-        <v>327</v>
+        <v>931</v>
       </c>
       <c r="D3820">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E3820">
-        <v>343</v>
+        <v>987</v>
       </c>
     </row>
     <row r="3821">
@@ -72773,17 +72773,17 @@
       </c>
       <c r="B3821" t="inlineStr">
         <is>
-          <t>Okres Ružomberok</t>
+          <t>Okres Poprad</t>
         </is>
       </c>
       <c r="C3821">
-        <v>1539</v>
+        <v>852</v>
       </c>
       <c r="D3821">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E3821">
-        <v>1612</v>
+        <v>922</v>
       </c>
     </row>
     <row r="3822">
@@ -72792,17 +72792,17 @@
       </c>
       <c r="B3822" t="inlineStr">
         <is>
-          <t>Okres Senica</t>
+          <t>Okres Považská Bystrica</t>
         </is>
       </c>
       <c r="C3822">
-        <v>17</v>
+        <v>819</v>
       </c>
       <c r="D3822">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="E3822">
-        <v>17</v>
+        <v>945</v>
       </c>
     </row>
     <row r="3823">
@@ -72811,17 +72811,17 @@
       </c>
       <c r="B3823" t="inlineStr">
         <is>
-          <t>Okres Skalica</t>
+          <t>Okres Prešov</t>
         </is>
       </c>
       <c r="C3823">
-        <v>288</v>
+        <v>1790</v>
       </c>
       <c r="D3823">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="E3823">
-        <v>313</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="3824">
@@ -72830,17 +72830,17 @@
       </c>
       <c r="B3824" t="inlineStr">
         <is>
-          <t>Okres Snina</t>
+          <t>Okres Prievidza</t>
         </is>
       </c>
       <c r="C3824">
-        <v>19</v>
+        <v>931</v>
       </c>
       <c r="D3824">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="E3824">
-        <v>21</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="3825">
@@ -72849,17 +72849,17 @@
       </c>
       <c r="B3825" t="inlineStr">
         <is>
-          <t>Okres Sobrance</t>
+          <t>Okres Púchov</t>
         </is>
       </c>
       <c r="C3825">
-        <v>165</v>
+        <v>289</v>
       </c>
       <c r="D3825">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E3825">
-        <v>182</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3826">
@@ -72868,17 +72868,17 @@
       </c>
       <c r="B3826" t="inlineStr">
         <is>
-          <t>Okres Spišská Nová Ves</t>
+          <t>Okres Revúca</t>
         </is>
       </c>
       <c r="C3826">
-        <v>99</v>
+        <v>1427</v>
       </c>
       <c r="D3826">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="E3826">
-        <v>109</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="3827">
@@ -72887,17 +72887,17 @@
       </c>
       <c r="B3827" t="inlineStr">
         <is>
-          <t>Okres Stará Ľubovňa</t>
+          <t>Okres Rimavská Sobota</t>
         </is>
       </c>
       <c r="C3827">
-        <v>255</v>
+        <v>623</v>
       </c>
       <c r="D3827">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E3827">
-        <v>283</v>
+        <v>662</v>
       </c>
     </row>
     <row r="3828">
@@ -72906,17 +72906,17 @@
       </c>
       <c r="B3828" t="inlineStr">
         <is>
-          <t>Okres Svidník</t>
+          <t>Okres Rožňava</t>
         </is>
       </c>
       <c r="C3828">
-        <v>129</v>
+        <v>536</v>
       </c>
       <c r="D3828">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E3828">
-        <v>151</v>
+        <v>553</v>
       </c>
     </row>
     <row r="3829">
@@ -72925,17 +72925,17 @@
       </c>
       <c r="B3829" t="inlineStr">
         <is>
-          <t>Okres Šaľa</t>
+          <t>Okres Ružomberok</t>
         </is>
       </c>
       <c r="C3829">
-        <v>1</v>
+        <v>8088</v>
       </c>
       <c r="D3829">
-        <v>0</v>
+        <v>515</v>
       </c>
       <c r="E3829">
-        <v>1</v>
+        <v>8603</v>
       </c>
     </row>
     <row r="3830">
@@ -72944,17 +72944,17 @@
       </c>
       <c r="B3830" t="inlineStr">
         <is>
-          <t>Okres Topoľčany</t>
+          <t>Okres Sabinov</t>
         </is>
       </c>
       <c r="C3830">
-        <v>402</v>
+        <v>344</v>
       </c>
       <c r="D3830">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="E3830">
-        <v>468</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3831">
@@ -72963,17 +72963,17 @@
       </c>
       <c r="B3831" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Senec</t>
         </is>
       </c>
       <c r="C3831">
-        <v>631</v>
+        <v>466</v>
       </c>
       <c r="D3831">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E3831">
-        <v>660</v>
+        <v>483</v>
       </c>
     </row>
     <row r="3832">
@@ -72982,17 +72982,17 @@
       </c>
       <c r="B3832" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Senica</t>
         </is>
       </c>
       <c r="C3832">
-        <v>259</v>
+        <v>382</v>
       </c>
       <c r="D3832">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E3832">
-        <v>291</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3833">
@@ -73001,17 +73001,17 @@
       </c>
       <c r="B3833" t="inlineStr">
         <is>
-          <t>Okres Trnava</t>
+          <t>Okres Skalica</t>
         </is>
       </c>
       <c r="C3833">
-        <v>54</v>
+        <v>297</v>
       </c>
       <c r="D3833">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="E3833">
-        <v>60</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3834">
@@ -73020,17 +73020,17 @@
       </c>
       <c r="B3834" t="inlineStr">
         <is>
-          <t>Okres Turčianske Teplice</t>
+          <t>Okres Snina</t>
         </is>
       </c>
       <c r="C3834">
-        <v>174</v>
+        <v>664</v>
       </c>
       <c r="D3834">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="E3834">
-        <v>193</v>
+        <v>704</v>
       </c>
     </row>
     <row r="3835">
@@ -73039,17 +73039,17 @@
       </c>
       <c r="B3835" t="inlineStr">
         <is>
-          <t>Okres Tvrdošín</t>
+          <t>Okres Sobrance</t>
         </is>
       </c>
       <c r="C3835">
-        <v>36</v>
+        <v>353</v>
       </c>
       <c r="D3835">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E3835">
-        <v>38</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3836">
@@ -73058,17 +73058,17 @@
       </c>
       <c r="B3836" t="inlineStr">
         <is>
-          <t>Okres Veľký Krtíš</t>
+          <t>Okres Spišská Nová Ves</t>
         </is>
       </c>
       <c r="C3836">
-        <v>411</v>
+        <v>493</v>
       </c>
       <c r="D3836">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E3836">
-        <v>444</v>
+        <v>527</v>
       </c>
     </row>
     <row r="3837">
@@ -73077,17 +73077,17 @@
       </c>
       <c r="B3837" t="inlineStr">
         <is>
-          <t>Okres Vranov nad Topľou</t>
+          <t>Okres Stará Ľubovňa</t>
         </is>
       </c>
       <c r="C3837">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="D3837">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E3837">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3838">
@@ -73096,17 +73096,17 @@
       </c>
       <c r="B3838" t="inlineStr">
         <is>
-          <t>Okres Zlaté Moravce</t>
+          <t>Okres Stropkov</t>
         </is>
       </c>
       <c r="C3838">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3838">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3838">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3839">
@@ -73115,17 +73115,17 @@
       </c>
       <c r="B3839" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Svidník</t>
         </is>
       </c>
       <c r="C3839">
-        <v>427</v>
+        <v>335</v>
       </c>
       <c r="D3839">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E3839">
-        <v>457</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3840">
@@ -73134,17 +73134,17 @@
       </c>
       <c r="B3840" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Šaľa</t>
         </is>
       </c>
       <c r="C3840">
-        <v>94</v>
+        <v>1315</v>
       </c>
       <c r="D3840">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="E3840">
-        <v>95</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="3841">
@@ -73153,17 +73153,1442 @@
       </c>
       <c r="B3841" t="inlineStr">
         <is>
+          <t>Okres Topoľčany</t>
+        </is>
+      </c>
+      <c r="C3841">
+        <v>1441</v>
+      </c>
+      <c r="D3841">
+        <v>199</v>
+      </c>
+      <c r="E3841">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="3842">
+      <c r="A3842" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B3842" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C3842">
+        <v>767</v>
+      </c>
+      <c r="D3842">
+        <v>46</v>
+      </c>
+      <c r="E3842">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="3843">
+      <c r="A3843" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B3843" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C3843">
+        <v>730</v>
+      </c>
+      <c r="D3843">
+        <v>102</v>
+      </c>
+      <c r="E3843">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="3844">
+      <c r="A3844" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B3844" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C3844">
+        <v>371</v>
+      </c>
+      <c r="D3844">
+        <v>43</v>
+      </c>
+      <c r="E3844">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="3845">
+      <c r="A3845" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B3845" t="inlineStr">
+        <is>
+          <t>Okres Turčianske Teplice</t>
+        </is>
+      </c>
+      <c r="C3845">
+        <v>174</v>
+      </c>
+      <c r="D3845">
+        <v>19</v>
+      </c>
+      <c r="E3845">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3846">
+      <c r="A3846" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B3846" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C3846">
+        <v>646</v>
+      </c>
+      <c r="D3846">
+        <v>30</v>
+      </c>
+      <c r="E3846">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="3847">
+      <c r="A3847" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B3847" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C3847">
+        <v>411</v>
+      </c>
+      <c r="D3847">
+        <v>30</v>
+      </c>
+      <c r="E3847">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="3848">
+      <c r="A3848" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B3848" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C3848">
+        <v>384</v>
+      </c>
+      <c r="D3848">
+        <v>63</v>
+      </c>
+      <c r="E3848">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="3849">
+      <c r="A3849" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B3849" t="inlineStr">
+        <is>
+          <t>Okres Zlaté Moravce</t>
+        </is>
+      </c>
+      <c r="C3849">
+        <v>260</v>
+      </c>
+      <c r="D3849">
+        <v>31</v>
+      </c>
+      <c r="E3849">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3850">
+      <c r="A3850" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B3850" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C3850">
+        <v>433</v>
+      </c>
+      <c r="D3850">
+        <v>31</v>
+      </c>
+      <c r="E3850">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="3851">
+      <c r="A3851" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B3851" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C3851">
+        <v>372</v>
+      </c>
+      <c r="D3851">
+        <v>20</v>
+      </c>
+      <c r="E3851">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="3852">
+      <c r="A3852" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B3852" t="inlineStr">
+        <is>
           <t>Okres Žilina</t>
         </is>
       </c>
-      <c r="C3841">
-        <v>1009</v>
-      </c>
-      <c r="D3841">
-        <v>107</v>
-      </c>
-      <c r="E3841">
-        <v>1116</v>
+      <c r="C3852">
+        <v>2660</v>
+      </c>
+      <c r="D3852">
+        <v>229</v>
+      </c>
+      <c r="E3852">
+        <v>2889</v>
+      </c>
+    </row>
+    <row r="3853">
+      <c r="A3853" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3853" t="inlineStr">
+        <is>
+          <t>Okres Banská Bystrica</t>
+        </is>
+      </c>
+      <c r="C3853">
+        <v>325</v>
+      </c>
+      <c r="D3853">
+        <v>10</v>
+      </c>
+      <c r="E3853">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3854">
+      <c r="A3854" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3854" t="inlineStr">
+        <is>
+          <t>Okres Bardejov</t>
+        </is>
+      </c>
+      <c r="C3854">
+        <v>6</v>
+      </c>
+      <c r="D3854">
+        <v>1</v>
+      </c>
+      <c r="E3854">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3855">
+      <c r="A3855" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3855" t="inlineStr">
+        <is>
+          <t>Okres Bratislava I</t>
+        </is>
+      </c>
+      <c r="C3855">
+        <v>61</v>
+      </c>
+      <c r="D3855">
+        <v>0</v>
+      </c>
+      <c r="E3855">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3856">
+      <c r="A3856" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3856" t="inlineStr">
+        <is>
+          <t>Okres Bratislava II</t>
+        </is>
+      </c>
+      <c r="C3856">
+        <v>1808</v>
+      </c>
+      <c r="D3856">
+        <v>75</v>
+      </c>
+      <c r="E3856">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="3857">
+      <c r="A3857" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3857" t="inlineStr">
+        <is>
+          <t>Okres Bratislava III</t>
+        </is>
+      </c>
+      <c r="C3857">
+        <v>287</v>
+      </c>
+      <c r="D3857">
+        <v>5</v>
+      </c>
+      <c r="E3857">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3858">
+      <c r="A3858" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3858" t="inlineStr">
+        <is>
+          <t>Okres Bratislava IV</t>
+        </is>
+      </c>
+      <c r="C3858">
+        <v>389</v>
+      </c>
+      <c r="D3858">
+        <v>11</v>
+      </c>
+      <c r="E3858">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3859">
+      <c r="A3859" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3859" t="inlineStr">
+        <is>
+          <t>Okres Bratislava V</t>
+        </is>
+      </c>
+      <c r="C3859">
+        <v>1</v>
+      </c>
+      <c r="D3859">
+        <v>1</v>
+      </c>
+      <c r="E3859">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3860">
+      <c r="A3860" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3860" t="inlineStr">
+        <is>
+          <t>Okres Brezno</t>
+        </is>
+      </c>
+      <c r="C3860">
+        <v>4</v>
+      </c>
+      <c r="D3860">
+        <v>1</v>
+      </c>
+      <c r="E3860">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3861">
+      <c r="A3861" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3861" t="inlineStr">
+        <is>
+          <t>Okres Bytča</t>
+        </is>
+      </c>
+      <c r="C3861">
+        <v>177</v>
+      </c>
+      <c r="D3861">
+        <v>38</v>
+      </c>
+      <c r="E3861">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3862">
+      <c r="A3862" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3862" t="inlineStr">
+        <is>
+          <t>Okres Čadca</t>
+        </is>
+      </c>
+      <c r="C3862">
+        <v>2218</v>
+      </c>
+      <c r="D3862">
+        <v>161</v>
+      </c>
+      <c r="E3862">
+        <v>2379</v>
+      </c>
+    </row>
+    <row r="3863">
+      <c r="A3863" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3863" t="inlineStr">
+        <is>
+          <t>Okres Detva</t>
+        </is>
+      </c>
+      <c r="C3863">
+        <v>1</v>
+      </c>
+      <c r="D3863">
+        <v>4</v>
+      </c>
+      <c r="E3863">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3864">
+      <c r="A3864" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3864" t="inlineStr">
+        <is>
+          <t>Okres Dolný Kubín</t>
+        </is>
+      </c>
+      <c r="C3864">
+        <v>334</v>
+      </c>
+      <c r="D3864">
+        <v>11</v>
+      </c>
+      <c r="E3864">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3865">
+      <c r="A3865" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3865" t="inlineStr">
+        <is>
+          <t>Okres Dunajská Streda</t>
+        </is>
+      </c>
+      <c r="C3865">
+        <v>762</v>
+      </c>
+      <c r="D3865">
+        <v>36</v>
+      </c>
+      <c r="E3865">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="3866">
+      <c r="A3866" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3866" t="inlineStr">
+        <is>
+          <t>Okres Galanta</t>
+        </is>
+      </c>
+      <c r="C3866">
+        <v>824</v>
+      </c>
+      <c r="D3866">
+        <v>67</v>
+      </c>
+      <c r="E3866">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="3867">
+      <c r="A3867" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3867" t="inlineStr">
+        <is>
+          <t>Okres Humenné</t>
+        </is>
+      </c>
+      <c r="C3867">
+        <v>374</v>
+      </c>
+      <c r="D3867">
+        <v>16</v>
+      </c>
+      <c r="E3867">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="3868">
+      <c r="A3868" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3868" t="inlineStr">
+        <is>
+          <t>Okres Ilava</t>
+        </is>
+      </c>
+      <c r="C3868">
+        <v>373</v>
+      </c>
+      <c r="D3868">
+        <v>40</v>
+      </c>
+      <c r="E3868">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3869">
+      <c r="A3869" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3869" t="inlineStr">
+        <is>
+          <t>Okres Kežmarok</t>
+        </is>
+      </c>
+      <c r="C3869">
+        <v>264</v>
+      </c>
+      <c r="D3869">
+        <v>37</v>
+      </c>
+      <c r="E3869">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3870">
+      <c r="A3870" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3870" t="inlineStr">
+        <is>
+          <t>Okres Komárno</t>
+        </is>
+      </c>
+      <c r="C3870">
+        <v>503</v>
+      </c>
+      <c r="D3870">
+        <v>30</v>
+      </c>
+      <c r="E3870">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="3871">
+      <c r="A3871" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3871" t="inlineStr">
+        <is>
+          <t>Okres Košice I</t>
+        </is>
+      </c>
+      <c r="C3871">
+        <v>627</v>
+      </c>
+      <c r="D3871">
+        <v>14</v>
+      </c>
+      <c r="E3871">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="3872">
+      <c r="A3872" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3872" t="inlineStr">
+        <is>
+          <t>Okres Košice II</t>
+        </is>
+      </c>
+      <c r="C3872">
+        <v>452</v>
+      </c>
+      <c r="D3872">
+        <v>6</v>
+      </c>
+      <c r="E3872">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="3873">
+      <c r="A3873" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3873" t="inlineStr">
+        <is>
+          <t>Okres Košice IV</t>
+        </is>
+      </c>
+      <c r="C3873">
+        <v>324</v>
+      </c>
+      <c r="D3873">
+        <v>17</v>
+      </c>
+      <c r="E3873">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3874">
+      <c r="A3874" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3874" t="inlineStr">
+        <is>
+          <t>Okres Kysucké Nové Mesto</t>
+        </is>
+      </c>
+      <c r="C3874">
+        <v>232</v>
+      </c>
+      <c r="D3874">
+        <v>39</v>
+      </c>
+      <c r="E3874">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3875">
+      <c r="A3875" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3875" t="inlineStr">
+        <is>
+          <t>Okres Levice</t>
+        </is>
+      </c>
+      <c r="C3875">
+        <v>568</v>
+      </c>
+      <c r="D3875">
+        <v>37</v>
+      </c>
+      <c r="E3875">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="3876">
+      <c r="A3876" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3876" t="inlineStr">
+        <is>
+          <t>Okres Levoča</t>
+        </is>
+      </c>
+      <c r="C3876">
+        <v>293</v>
+      </c>
+      <c r="D3876">
+        <v>22</v>
+      </c>
+      <c r="E3876">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3877">
+      <c r="A3877" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3877" t="inlineStr">
+        <is>
+          <t>Okres Liptovský Mikuláš</t>
+        </is>
+      </c>
+      <c r="C3877">
+        <v>1813</v>
+      </c>
+      <c r="D3877">
+        <v>114</v>
+      </c>
+      <c r="E3877">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="3878">
+      <c r="A3878" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3878" t="inlineStr">
+        <is>
+          <t>Okres Lučenec</t>
+        </is>
+      </c>
+      <c r="C3878">
+        <v>306</v>
+      </c>
+      <c r="D3878">
+        <v>22</v>
+      </c>
+      <c r="E3878">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3879">
+      <c r="A3879" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3879" t="inlineStr">
+        <is>
+          <t>Okres Malacky</t>
+        </is>
+      </c>
+      <c r="C3879">
+        <v>9</v>
+      </c>
+      <c r="D3879">
+        <v>2</v>
+      </c>
+      <c r="E3879">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3880">
+      <c r="A3880" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3880" t="inlineStr">
+        <is>
+          <t>Okres Michalovce</t>
+        </is>
+      </c>
+      <c r="C3880">
+        <v>336</v>
+      </c>
+      <c r="D3880">
+        <v>24</v>
+      </c>
+      <c r="E3880">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3881">
+      <c r="A3881" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3881" t="inlineStr">
+        <is>
+          <t>Okres Myjava</t>
+        </is>
+      </c>
+      <c r="C3881">
+        <v>382</v>
+      </c>
+      <c r="D3881">
+        <v>23</v>
+      </c>
+      <c r="E3881">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="3882">
+      <c r="A3882" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3882" t="inlineStr">
+        <is>
+          <t>Okres Námestovo</t>
+        </is>
+      </c>
+      <c r="C3882">
+        <v>10</v>
+      </c>
+      <c r="D3882">
+        <v>0</v>
+      </c>
+      <c r="E3882">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3883">
+      <c r="A3883" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3883" t="inlineStr">
+        <is>
+          <t>Okres Nitra</t>
+        </is>
+      </c>
+      <c r="C3883">
+        <v>91</v>
+      </c>
+      <c r="D3883">
+        <v>12</v>
+      </c>
+      <c r="E3883">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3884">
+      <c r="A3884" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3884" t="inlineStr">
+        <is>
+          <t>Okres Nové Mesto nad Váhom</t>
+        </is>
+      </c>
+      <c r="C3884">
+        <v>271</v>
+      </c>
+      <c r="D3884">
+        <v>30</v>
+      </c>
+      <c r="E3884">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3885">
+      <c r="A3885" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3885" t="inlineStr">
+        <is>
+          <t>Okres Nové Zámky</t>
+        </is>
+      </c>
+      <c r="C3885">
+        <v>1371</v>
+      </c>
+      <c r="D3885">
+        <v>68</v>
+      </c>
+      <c r="E3885">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="3886">
+      <c r="A3886" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3886" t="inlineStr">
+        <is>
+          <t>Okres Partizánske</t>
+        </is>
+      </c>
+      <c r="C3886">
+        <v>530</v>
+      </c>
+      <c r="D3886">
+        <v>97</v>
+      </c>
+      <c r="E3886">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="3887">
+      <c r="A3887" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3887" t="inlineStr">
+        <is>
+          <t>Okres Pezinok</t>
+        </is>
+      </c>
+      <c r="C3887">
+        <v>383</v>
+      </c>
+      <c r="D3887">
+        <v>13</v>
+      </c>
+      <c r="E3887">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="3888">
+      <c r="A3888" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3888" t="inlineStr">
+        <is>
+          <t>Okres Piešťany</t>
+        </is>
+      </c>
+      <c r="C3888">
+        <v>58</v>
+      </c>
+      <c r="D3888">
+        <v>0</v>
+      </c>
+      <c r="E3888">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3889">
+      <c r="A3889" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3889" t="inlineStr">
+        <is>
+          <t>Okres Poprad</t>
+        </is>
+      </c>
+      <c r="C3889">
+        <v>686</v>
+      </c>
+      <c r="D3889">
+        <v>53</v>
+      </c>
+      <c r="E3889">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="3890">
+      <c r="A3890" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3890" t="inlineStr">
+        <is>
+          <t>Okres Považská Bystrica</t>
+        </is>
+      </c>
+      <c r="C3890">
+        <v>540</v>
+      </c>
+      <c r="D3890">
+        <v>70</v>
+      </c>
+      <c r="E3890">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="3891">
+      <c r="A3891" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3891" t="inlineStr">
+        <is>
+          <t>Okres Prešov</t>
+        </is>
+      </c>
+      <c r="C3891">
+        <v>537</v>
+      </c>
+      <c r="D3891">
+        <v>28</v>
+      </c>
+      <c r="E3891">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="3892">
+      <c r="A3892" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3892" t="inlineStr">
+        <is>
+          <t>Okres Prievidza</t>
+        </is>
+      </c>
+      <c r="C3892">
+        <v>431</v>
+      </c>
+      <c r="D3892">
+        <v>26</v>
+      </c>
+      <c r="E3892">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="3893">
+      <c r="A3893" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3893" t="inlineStr">
+        <is>
+          <t>Okres Púchov</t>
+        </is>
+      </c>
+      <c r="C3893">
+        <v>6</v>
+      </c>
+      <c r="D3893">
+        <v>0</v>
+      </c>
+      <c r="E3893">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3894">
+      <c r="A3894" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3894" t="inlineStr">
+        <is>
+          <t>Okres Revúca</t>
+        </is>
+      </c>
+      <c r="C3894">
+        <v>365</v>
+      </c>
+      <c r="D3894">
+        <v>18</v>
+      </c>
+      <c r="E3894">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="3895">
+      <c r="A3895" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3895" t="inlineStr">
+        <is>
+          <t>Okres Rimavská Sobota</t>
+        </is>
+      </c>
+      <c r="C3895">
+        <v>363</v>
+      </c>
+      <c r="D3895">
+        <v>13</v>
+      </c>
+      <c r="E3895">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="3896">
+      <c r="A3896" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3896" t="inlineStr">
+        <is>
+          <t>Okres Rožňava</t>
+        </is>
+      </c>
+      <c r="C3896">
+        <v>281</v>
+      </c>
+      <c r="D3896">
+        <v>9</v>
+      </c>
+      <c r="E3896">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3897">
+      <c r="A3897" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3897" t="inlineStr">
+        <is>
+          <t>Okres Ružomberok</t>
+        </is>
+      </c>
+      <c r="C3897">
+        <v>16</v>
+      </c>
+      <c r="D3897">
+        <v>3</v>
+      </c>
+      <c r="E3897">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3898">
+      <c r="A3898" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3898" t="inlineStr">
+        <is>
+          <t>Okres Senica</t>
+        </is>
+      </c>
+      <c r="C3898">
+        <v>14</v>
+      </c>
+      <c r="D3898">
+        <v>2</v>
+      </c>
+      <c r="E3898">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3899">
+      <c r="A3899" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3899" t="inlineStr">
+        <is>
+          <t>Okres Skalica</t>
+        </is>
+      </c>
+      <c r="C3899">
+        <v>429</v>
+      </c>
+      <c r="D3899">
+        <v>17</v>
+      </c>
+      <c r="E3899">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="3900">
+      <c r="A3900" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3900" t="inlineStr">
+        <is>
+          <t>Okres Snina</t>
+        </is>
+      </c>
+      <c r="C3900">
+        <v>3</v>
+      </c>
+      <c r="D3900">
+        <v>1</v>
+      </c>
+      <c r="E3900">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3901">
+      <c r="A3901" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3901" t="inlineStr">
+        <is>
+          <t>Okres Sobrance</t>
+        </is>
+      </c>
+      <c r="C3901">
+        <v>125</v>
+      </c>
+      <c r="D3901">
+        <v>16</v>
+      </c>
+      <c r="E3901">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3902">
+      <c r="A3902" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3902" t="inlineStr">
+        <is>
+          <t>Okres Spišská Nová Ves</t>
+        </is>
+      </c>
+      <c r="C3902">
+        <v>60</v>
+      </c>
+      <c r="D3902">
+        <v>5</v>
+      </c>
+      <c r="E3902">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3903">
+      <c r="A3903" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3903" t="inlineStr">
+        <is>
+          <t>Okres Stará Ľubovňa</t>
+        </is>
+      </c>
+      <c r="C3903">
+        <v>54</v>
+      </c>
+      <c r="D3903">
+        <v>225</v>
+      </c>
+      <c r="E3903">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3904">
+      <c r="A3904" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3904" t="inlineStr">
+        <is>
+          <t>Okres Stropkov</t>
+        </is>
+      </c>
+      <c r="C3904">
+        <v>1</v>
+      </c>
+      <c r="D3904">
+        <v>0</v>
+      </c>
+      <c r="E3904">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3905">
+      <c r="A3905" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3905" t="inlineStr">
+        <is>
+          <t>Okres Svidník</t>
+        </is>
+      </c>
+      <c r="C3905">
+        <v>139</v>
+      </c>
+      <c r="D3905">
+        <v>16</v>
+      </c>
+      <c r="E3905">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3906">
+      <c r="A3906" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3906" t="inlineStr">
+        <is>
+          <t>Okres Šaľa</t>
+        </is>
+      </c>
+      <c r="C3906">
+        <v>1</v>
+      </c>
+      <c r="D3906">
+        <v>0</v>
+      </c>
+      <c r="E3906">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3907">
+      <c r="A3907" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3907" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C3907">
+        <v>595</v>
+      </c>
+      <c r="D3907">
+        <v>39</v>
+      </c>
+      <c r="E3907">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="3908">
+      <c r="A3908" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3908" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C3908">
+        <v>491</v>
+      </c>
+      <c r="D3908">
+        <v>27</v>
+      </c>
+      <c r="E3908">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3909">
+      <c r="A3909" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3909" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C3909">
+        <v>557</v>
+      </c>
+      <c r="D3909">
+        <v>29</v>
+      </c>
+      <c r="E3909">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="3910">
+      <c r="A3910" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3910" t="inlineStr">
+        <is>
+          <t>Okres Turčianske Teplice</t>
+        </is>
+      </c>
+      <c r="C3910">
+        <v>183</v>
+      </c>
+      <c r="D3910">
+        <v>6</v>
+      </c>
+      <c r="E3910">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3911">
+      <c r="A3911" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3911" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C3911">
+        <v>54</v>
+      </c>
+      <c r="D3911">
+        <v>4</v>
+      </c>
+      <c r="E3911">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3912">
+      <c r="A3912" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3912" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C3912">
+        <v>464</v>
+      </c>
+      <c r="D3912">
+        <v>19</v>
+      </c>
+      <c r="E3912">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="3913">
+      <c r="A3913" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3913" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C3913">
+        <v>279</v>
+      </c>
+      <c r="D3913">
+        <v>33</v>
+      </c>
+      <c r="E3913">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3914">
+      <c r="A3914" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3914" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C3914">
+        <v>358</v>
+      </c>
+      <c r="D3914">
+        <v>20</v>
+      </c>
+      <c r="E3914">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="3915">
+      <c r="A3915" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3915" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C3915">
+        <v>594</v>
+      </c>
+      <c r="D3915">
+        <v>30</v>
+      </c>
+      <c r="E3915">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="3916">
+      <c r="A3916" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B3916" t="inlineStr">
+        <is>
+          <t>Okres Žilina</t>
+        </is>
+      </c>
+      <c r="C3916">
+        <v>853</v>
+      </c>
+      <c r="D3916">
+        <v>53</v>
+      </c>
+      <c r="E3916">
+        <v>906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: pi 08. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_AgTests_District.xlsx
+++ b/OpenData_Slovakia_Covid_AgTests_District.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4875"/>
+  <dimension ref="A1:E4955"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -70910,13 +70910,13 @@
         </is>
       </c>
       <c r="C3713">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3713">
         <v>7</v>
       </c>
       <c r="E3713">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3714">
@@ -71708,13 +71708,13 @@
         </is>
       </c>
       <c r="C3755">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D3755">
         <v>91</v>
       </c>
       <c r="E3755">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="3756">
@@ -74501,13 +74501,13 @@
         </is>
       </c>
       <c r="C3902">
-        <v>1343</v>
+        <v>1348</v>
       </c>
       <c r="D3902">
         <v>38</v>
       </c>
       <c r="E3902">
-        <v>1381</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="3903">
@@ -81227,13 +81227,13 @@
         </is>
       </c>
       <c r="C4256">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="D4256">
         <v>110</v>
       </c>
       <c r="E4256">
-        <v>921</v>
+        <v>917</v>
       </c>
     </row>
     <row r="4257">
@@ -82595,13 +82595,13 @@
         </is>
       </c>
       <c r="C4328">
-        <v>3432</v>
+        <v>3436</v>
       </c>
       <c r="D4328">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E4328">
-        <v>3679</v>
+        <v>3684</v>
       </c>
     </row>
     <row r="4329">
@@ -85426,13 +85426,13 @@
         </is>
       </c>
       <c r="C4477">
-        <v>1655</v>
+        <v>1657</v>
       </c>
       <c r="D4477">
         <v>80</v>
       </c>
       <c r="E4477">
-        <v>1735</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="4478">
@@ -88238,13 +88238,13 @@
         </is>
       </c>
       <c r="C4625">
-        <v>2215</v>
+        <v>2234</v>
       </c>
       <c r="D4625">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E4625">
-        <v>2435</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="4626">
@@ -89644,13 +89644,13 @@
         </is>
       </c>
       <c r="C4699">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="D4699">
         <v>73</v>
       </c>
       <c r="E4699">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="4700">
@@ -89663,13 +89663,13 @@
         </is>
       </c>
       <c r="C4700">
-        <v>1494</v>
+        <v>1509</v>
       </c>
       <c r="D4700">
         <v>85</v>
       </c>
       <c r="E4700">
-        <v>1579</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="4701">
@@ -90100,13 +90100,13 @@
         </is>
       </c>
       <c r="C4723">
-        <v>871</v>
+        <v>995</v>
       </c>
       <c r="D4723">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E4723">
-        <v>933</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="4724">
@@ -90974,13 +90974,13 @@
         </is>
       </c>
       <c r="C4769">
-        <v>950</v>
+        <v>957</v>
       </c>
       <c r="D4769">
         <v>56</v>
       </c>
       <c r="E4769">
-        <v>1006</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="4770">
@@ -91506,13 +91506,13 @@
         </is>
       </c>
       <c r="C4797">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D4797">
         <v>19</v>
       </c>
       <c r="E4797">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4798">
@@ -91958,17 +91958,17 @@
       </c>
       <c r="B4821" t="inlineStr">
         <is>
-          <t>Okres Banská Bystrica</t>
+          <t>Okres Bánovce nad Bebravou</t>
         </is>
       </c>
       <c r="C4821">
-        <v>339</v>
+        <v>252</v>
       </c>
       <c r="D4821">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E4821">
-        <v>356</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4822">
@@ -91977,17 +91977,17 @@
       </c>
       <c r="B4822" t="inlineStr">
         <is>
-          <t>Okres Bardejov</t>
+          <t>Okres Banská Bystrica</t>
         </is>
       </c>
       <c r="C4822">
-        <v>58</v>
+        <v>588</v>
       </c>
       <c r="D4822">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E4822">
-        <v>59</v>
+        <v>606</v>
       </c>
     </row>
     <row r="4823">
@@ -91996,17 +91996,17 @@
       </c>
       <c r="B4823" t="inlineStr">
         <is>
-          <t>Okres Bratislava I</t>
+          <t>Okres Banská Štiavnica</t>
         </is>
       </c>
       <c r="C4823">
-        <v>213</v>
+        <v>20</v>
       </c>
       <c r="D4823">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4823">
-        <v>216</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4824">
@@ -92015,17 +92015,17 @@
       </c>
       <c r="B4824" t="inlineStr">
         <is>
-          <t>Okres Bratislava II</t>
+          <t>Okres Bardejov</t>
         </is>
       </c>
       <c r="C4824">
-        <v>124</v>
+        <v>796</v>
       </c>
       <c r="D4824">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E4824">
-        <v>144</v>
+        <v>820</v>
       </c>
     </row>
     <row r="4825">
@@ -92034,17 +92034,17 @@
       </c>
       <c r="B4825" t="inlineStr">
         <is>
-          <t>Okres Bratislava III</t>
+          <t>Okres Bratislava I</t>
         </is>
       </c>
       <c r="C4825">
-        <v>296</v>
+        <v>956</v>
       </c>
       <c r="D4825">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="E4825">
-        <v>302</v>
+        <v>997</v>
       </c>
     </row>
     <row r="4826">
@@ -92053,17 +92053,17 @@
       </c>
       <c r="B4826" t="inlineStr">
         <is>
-          <t>Okres Bratislava IV</t>
+          <t>Okres Bratislava II</t>
         </is>
       </c>
       <c r="C4826">
-        <v>231</v>
+        <v>721</v>
       </c>
       <c r="D4826">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E4826">
-        <v>262</v>
+        <v>756</v>
       </c>
     </row>
     <row r="4827">
@@ -92072,17 +92072,17 @@
       </c>
       <c r="B4827" t="inlineStr">
         <is>
-          <t>Okres Bratislava V</t>
+          <t>Okres Bratislava III</t>
         </is>
       </c>
       <c r="C4827">
-        <v>101</v>
+        <v>512</v>
       </c>
       <c r="D4827">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E4827">
-        <v>106</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4828">
@@ -92091,17 +92091,17 @@
       </c>
       <c r="B4828" t="inlineStr">
         <is>
-          <t>Okres Brezno</t>
+          <t>Okres Bratislava IV</t>
         </is>
       </c>
       <c r="C4828">
-        <v>99</v>
+        <v>238</v>
       </c>
       <c r="D4828">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E4828">
-        <v>136</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4829">
@@ -92110,17 +92110,17 @@
       </c>
       <c r="B4829" t="inlineStr">
         <is>
-          <t>Okres Čadca</t>
+          <t>Okres Bratislava V</t>
         </is>
       </c>
       <c r="C4829">
-        <v>106</v>
+        <v>382</v>
       </c>
       <c r="D4829">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E4829">
-        <v>113</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4830">
@@ -92129,17 +92129,17 @@
       </c>
       <c r="B4830" t="inlineStr">
         <is>
-          <t>Okres Dolný Kubín</t>
+          <t>Okres Brezno</t>
         </is>
       </c>
       <c r="C4830">
-        <v>289</v>
+        <v>385</v>
       </c>
       <c r="D4830">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="E4830">
-        <v>310</v>
+        <v>462</v>
       </c>
     </row>
     <row r="4831">
@@ -92148,17 +92148,17 @@
       </c>
       <c r="B4831" t="inlineStr">
         <is>
-          <t>Okres Dunajská Streda</t>
+          <t>Okres Bytča</t>
         </is>
       </c>
       <c r="C4831">
-        <v>462</v>
+        <v>248</v>
       </c>
       <c r="D4831">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E4831">
-        <v>499</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4832">
@@ -92167,17 +92167,17 @@
       </c>
       <c r="B4832" t="inlineStr">
         <is>
-          <t>Okres Hlohovec</t>
+          <t>Okres Čadca</t>
         </is>
       </c>
       <c r="C4832">
-        <v>1</v>
+        <v>909</v>
       </c>
       <c r="D4832">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="E4832">
-        <v>1</v>
+        <v>968</v>
       </c>
     </row>
     <row r="4833">
@@ -92186,17 +92186,17 @@
       </c>
       <c r="B4833" t="inlineStr">
         <is>
-          <t>Okres Humenné</t>
+          <t>Okres Detva</t>
         </is>
       </c>
       <c r="C4833">
-        <v>342</v>
+        <v>284</v>
       </c>
       <c r="D4833">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="E4833">
-        <v>355</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4834">
@@ -92205,17 +92205,17 @@
       </c>
       <c r="B4834" t="inlineStr">
         <is>
-          <t>Okres Ilava</t>
+          <t>Okres Dolný Kubín</t>
         </is>
       </c>
       <c r="C4834">
-        <v>182</v>
+        <v>314</v>
       </c>
       <c r="D4834">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E4834">
-        <v>212</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4835">
@@ -92224,17 +92224,17 @@
       </c>
       <c r="B4835" t="inlineStr">
         <is>
-          <t>Okres Kežmarok</t>
+          <t>Okres Dunajská Streda</t>
         </is>
       </c>
       <c r="C4835">
-        <v>14</v>
+        <v>906</v>
       </c>
       <c r="D4835">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="E4835">
-        <v>15</v>
+        <v>986</v>
       </c>
     </row>
     <row r="4836">
@@ -92243,17 +92243,17 @@
       </c>
       <c r="B4836" t="inlineStr">
         <is>
-          <t>Okres Komárno</t>
+          <t>Okres Galanta</t>
         </is>
       </c>
       <c r="C4836">
-        <v>59</v>
+        <v>125</v>
       </c>
       <c r="D4836">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4836">
-        <v>73</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4837">
@@ -92262,17 +92262,17 @@
       </c>
       <c r="B4837" t="inlineStr">
         <is>
-          <t>Okres Košice II</t>
+          <t>Okres Gelnica</t>
         </is>
       </c>
       <c r="C4837">
-        <v>235</v>
+        <v>277</v>
       </c>
       <c r="D4837">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E4837">
-        <v>241</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4838">
@@ -92281,17 +92281,17 @@
       </c>
       <c r="B4838" t="inlineStr">
         <is>
-          <t>Okres Krupina</t>
+          <t>Okres Hlohovec</t>
         </is>
       </c>
       <c r="C4838">
-        <v>3</v>
+        <v>410</v>
       </c>
       <c r="D4838">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E4838">
-        <v>3</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4839">
@@ -92300,17 +92300,17 @@
       </c>
       <c r="B4839" t="inlineStr">
         <is>
-          <t>Okres Levice</t>
+          <t>Okres Humenné</t>
         </is>
       </c>
       <c r="C4839">
-        <v>1280</v>
+        <v>982</v>
       </c>
       <c r="D4839">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E4839">
-        <v>1352</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="4840">
@@ -92319,17 +92319,17 @@
       </c>
       <c r="B4840" t="inlineStr">
         <is>
-          <t>Okres Liptovský Mikuláš</t>
+          <t>Okres Ilava</t>
         </is>
       </c>
       <c r="C4840">
-        <v>239</v>
+        <v>200</v>
       </c>
       <c r="D4840">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E4840">
-        <v>248</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4841">
@@ -92338,17 +92338,17 @@
       </c>
       <c r="B4841" t="inlineStr">
         <is>
-          <t>Okres Lučenec</t>
+          <t>Okres Kežmarok</t>
         </is>
       </c>
       <c r="C4841">
-        <v>32</v>
+        <v>406</v>
       </c>
       <c r="D4841">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="E4841">
-        <v>32</v>
+        <v>482</v>
       </c>
     </row>
     <row r="4842">
@@ -92357,17 +92357,17 @@
       </c>
       <c r="B4842" t="inlineStr">
         <is>
-          <t>Okres Malacky</t>
+          <t>Okres Komárno</t>
         </is>
       </c>
       <c r="C4842">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="D4842">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E4842">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4843">
@@ -92376,17 +92376,17 @@
       </c>
       <c r="B4843" t="inlineStr">
         <is>
-          <t>Okres Martin</t>
+          <t>Okres Košice I</t>
         </is>
       </c>
       <c r="C4843">
-        <v>81</v>
+        <v>576</v>
       </c>
       <c r="D4843">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="E4843">
-        <v>83</v>
+        <v>619</v>
       </c>
     </row>
     <row r="4844">
@@ -92395,17 +92395,17 @@
       </c>
       <c r="B4844" t="inlineStr">
         <is>
-          <t>Okres Myjava</t>
+          <t>Okres Košice II</t>
         </is>
       </c>
       <c r="C4844">
-        <v>43</v>
+        <v>885</v>
       </c>
       <c r="D4844">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="E4844">
-        <v>44</v>
+        <v>954</v>
       </c>
     </row>
     <row r="4845">
@@ -92414,17 +92414,17 @@
       </c>
       <c r="B4845" t="inlineStr">
         <is>
-          <t>Okres Námestovo</t>
+          <t>Okres Košice IV</t>
         </is>
       </c>
       <c r="C4845">
-        <v>10</v>
+        <v>837</v>
       </c>
       <c r="D4845">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E4845">
-        <v>10</v>
+        <v>870</v>
       </c>
     </row>
     <row r="4846">
@@ -92433,17 +92433,17 @@
       </c>
       <c r="B4846" t="inlineStr">
         <is>
-          <t>Okres Nitra</t>
+          <t>Okres Krupina</t>
         </is>
       </c>
       <c r="C4846">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="D4846">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E4846">
-        <v>86</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4847">
@@ -92452,17 +92452,17 @@
       </c>
       <c r="B4847" t="inlineStr">
         <is>
-          <t>Okres Partizánske</t>
+          <t>Okres Kysucké Nové Mesto</t>
         </is>
       </c>
       <c r="C4847">
-        <v>626</v>
+        <v>206</v>
       </c>
       <c r="D4847">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="E4847">
-        <v>720</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4848">
@@ -92471,17 +92471,17 @@
       </c>
       <c r="B4848" t="inlineStr">
         <is>
-          <t>Okres Pezinok</t>
+          <t>Okres Levice</t>
         </is>
       </c>
       <c r="C4848">
-        <v>43</v>
+        <v>2872</v>
       </c>
       <c r="D4848">
-        <v>0</v>
+        <v>247</v>
       </c>
       <c r="E4848">
-        <v>43</v>
+        <v>3119</v>
       </c>
     </row>
     <row r="4849">
@@ -92490,17 +92490,17 @@
       </c>
       <c r="B4849" t="inlineStr">
         <is>
-          <t>Okres Piešťany</t>
+          <t>Okres Levoča</t>
         </is>
       </c>
       <c r="C4849">
-        <v>1</v>
+        <v>203</v>
       </c>
       <c r="D4849">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E4849">
-        <v>1</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4850">
@@ -92509,17 +92509,17 @@
       </c>
       <c r="B4850" t="inlineStr">
         <is>
-          <t>Okres Poprad</t>
+          <t>Okres Liptovský Mikuláš</t>
         </is>
       </c>
       <c r="C4850">
-        <v>48</v>
+        <v>563</v>
       </c>
       <c r="D4850">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E4850">
-        <v>48</v>
+        <v>592</v>
       </c>
     </row>
     <row r="4851">
@@ -92528,17 +92528,17 @@
       </c>
       <c r="B4851" t="inlineStr">
         <is>
-          <t>Okres Považská Bystrica</t>
+          <t>Okres Lučenec</t>
         </is>
       </c>
       <c r="C4851">
-        <v>507</v>
+        <v>460</v>
       </c>
       <c r="D4851">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="E4851">
-        <v>594</v>
+        <v>476</v>
       </c>
     </row>
     <row r="4852">
@@ -92547,17 +92547,17 @@
       </c>
       <c r="B4852" t="inlineStr">
         <is>
-          <t>Okres Prešov</t>
+          <t>Okres Malacky</t>
         </is>
       </c>
       <c r="C4852">
-        <v>1</v>
+        <v>363</v>
       </c>
       <c r="D4852">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E4852">
-        <v>1</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4853">
@@ -92566,17 +92566,17 @@
       </c>
       <c r="B4853" t="inlineStr">
         <is>
-          <t>Okres Prievidza</t>
+          <t>Okres Martin</t>
         </is>
       </c>
       <c r="C4853">
-        <v>218</v>
+        <v>1468</v>
       </c>
       <c r="D4853">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="E4853">
-        <v>231</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="4854">
@@ -92585,17 +92585,17 @@
       </c>
       <c r="B4854" t="inlineStr">
         <is>
-          <t>Okres Púchov</t>
+          <t>Okres Medzilaborce</t>
         </is>
       </c>
       <c r="C4854">
-        <v>0</v>
+        <v>222</v>
       </c>
       <c r="D4854">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E4854">
-        <v>0</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4855">
@@ -92604,17 +92604,17 @@
       </c>
       <c r="B4855" t="inlineStr">
         <is>
-          <t>Okres Revúca</t>
+          <t>Okres Michalovce</t>
         </is>
       </c>
       <c r="C4855">
-        <v>101</v>
+        <v>893</v>
       </c>
       <c r="D4855">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E4855">
-        <v>103</v>
+        <v>953</v>
       </c>
     </row>
     <row r="4856">
@@ -92623,17 +92623,17 @@
       </c>
       <c r="B4856" t="inlineStr">
         <is>
-          <t>Okres Rimavská Sobota</t>
+          <t>Okres Myjava</t>
         </is>
       </c>
       <c r="C4856">
-        <v>316</v>
+        <v>121</v>
       </c>
       <c r="D4856">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E4856">
-        <v>338</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4857">
@@ -92642,17 +92642,17 @@
       </c>
       <c r="B4857" t="inlineStr">
         <is>
-          <t>Okres Ružomberok</t>
+          <t>Okres Námestovo</t>
         </is>
       </c>
       <c r="C4857">
-        <v>53</v>
+        <v>383</v>
       </c>
       <c r="D4857">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E4857">
-        <v>60</v>
+        <v>409</v>
       </c>
     </row>
     <row r="4858">
@@ -92661,17 +92661,17 @@
       </c>
       <c r="B4858" t="inlineStr">
         <is>
-          <t>Okres Skalica</t>
+          <t>Okres Nitra</t>
         </is>
       </c>
       <c r="C4858">
-        <v>17</v>
+        <v>3491</v>
       </c>
       <c r="D4858">
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="E4858">
-        <v>17</v>
+        <v>3647</v>
       </c>
     </row>
     <row r="4859">
@@ -92680,17 +92680,17 @@
       </c>
       <c r="B4859" t="inlineStr">
         <is>
-          <t>Okres Sobrance</t>
+          <t>Okres Nové Mesto nad Váhom</t>
         </is>
       </c>
       <c r="C4859">
-        <v>7</v>
+        <v>521</v>
       </c>
       <c r="D4859">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="E4859">
-        <v>7</v>
+        <v>592</v>
       </c>
     </row>
     <row r="4860">
@@ -92699,17 +92699,17 @@
       </c>
       <c r="B4860" t="inlineStr">
         <is>
-          <t>Okres Spišská Nová Ves</t>
+          <t>Okres Nové Zámky</t>
         </is>
       </c>
       <c r="C4860">
-        <v>33</v>
+        <v>3379</v>
       </c>
       <c r="D4860">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="E4860">
-        <v>36</v>
+        <v>3502</v>
       </c>
     </row>
     <row r="4861">
@@ -92718,17 +92718,17 @@
       </c>
       <c r="B4861" t="inlineStr">
         <is>
-          <t>Okres Stará Ľubovňa</t>
+          <t>Okres Partizánske</t>
         </is>
       </c>
       <c r="C4861">
-        <v>66</v>
+        <v>643</v>
       </c>
       <c r="D4861">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="E4861">
-        <v>75</v>
+        <v>738</v>
       </c>
     </row>
     <row r="4862">
@@ -92737,17 +92737,17 @@
       </c>
       <c r="B4862" t="inlineStr">
         <is>
-          <t>Okres Stropkov</t>
+          <t>Okres Pezinok</t>
         </is>
       </c>
       <c r="C4862">
-        <v>1</v>
+        <v>493</v>
       </c>
       <c r="D4862">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E4862">
-        <v>1</v>
+        <v>507</v>
       </c>
     </row>
     <row r="4863">
@@ -92756,17 +92756,17 @@
       </c>
       <c r="B4863" t="inlineStr">
         <is>
-          <t>Okres Svidník</t>
+          <t>Okres Piešťany</t>
         </is>
       </c>
       <c r="C4863">
-        <v>14</v>
+        <v>765</v>
       </c>
       <c r="D4863">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="E4863">
-        <v>16</v>
+        <v>816</v>
       </c>
     </row>
     <row r="4864">
@@ -92775,17 +92775,17 @@
       </c>
       <c r="B4864" t="inlineStr">
         <is>
-          <t>Okres Topoľčany</t>
+          <t>Okres Poprad</t>
         </is>
       </c>
       <c r="C4864">
-        <v>1</v>
+        <v>820</v>
       </c>
       <c r="D4864">
-        <v>1</v>
+        <v>68</v>
       </c>
       <c r="E4864">
-        <v>1</v>
+        <v>888</v>
       </c>
     </row>
     <row r="4865">
@@ -92794,17 +92794,17 @@
       </c>
       <c r="B4865" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Považská Bystrica</t>
         </is>
       </c>
       <c r="C4865">
-        <v>255</v>
+        <v>753</v>
       </c>
       <c r="D4865">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E4865">
-        <v>265</v>
+        <v>860</v>
       </c>
     </row>
     <row r="4866">
@@ -92813,17 +92813,17 @@
       </c>
       <c r="B4866" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Prešov</t>
         </is>
       </c>
       <c r="C4866">
-        <v>127</v>
+        <v>1965</v>
       </c>
       <c r="D4866">
-        <v>27</v>
+        <v>120</v>
       </c>
       <c r="E4866">
-        <v>154</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="4867">
@@ -92832,17 +92832,17 @@
       </c>
       <c r="B4867" t="inlineStr">
         <is>
-          <t>Okres Trnava</t>
+          <t>Okres Prievidza</t>
         </is>
       </c>
       <c r="C4867">
-        <v>131</v>
+        <v>746</v>
       </c>
       <c r="D4867">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="E4867">
-        <v>163</v>
+        <v>816</v>
       </c>
     </row>
     <row r="4868">
@@ -92851,17 +92851,17 @@
       </c>
       <c r="B4868" t="inlineStr">
         <is>
-          <t>Okres Tvrdošín</t>
+          <t>Okres Púchov</t>
         </is>
       </c>
       <c r="C4868">
+        <v>191</v>
+      </c>
+      <c r="D4868">
         <v>21</v>
       </c>
-      <c r="D4868">
-        <v>0</v>
-      </c>
       <c r="E4868">
-        <v>21</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4869">
@@ -92870,17 +92870,17 @@
       </c>
       <c r="B4869" t="inlineStr">
         <is>
-          <t>Okres Veľký Krtíš</t>
+          <t>Okres Revúca</t>
         </is>
       </c>
       <c r="C4869">
-        <v>341</v>
+        <v>474</v>
       </c>
       <c r="D4869">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4869">
-        <v>353</v>
+        <v>482</v>
       </c>
     </row>
     <row r="4870">
@@ -92889,17 +92889,17 @@
       </c>
       <c r="B4870" t="inlineStr">
         <is>
-          <t>Okres Vranov nad Topľou</t>
+          <t>Okres Rimavská Sobota</t>
         </is>
       </c>
       <c r="C4870">
-        <v>1</v>
+        <v>577</v>
       </c>
       <c r="D4870">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E4870">
-        <v>1</v>
+        <v>611</v>
       </c>
     </row>
     <row r="4871">
@@ -92908,17 +92908,17 @@
       </c>
       <c r="B4871" t="inlineStr">
         <is>
-          <t>Okres Zlaté Moravce</t>
+          <t>Okres Rožňava</t>
         </is>
       </c>
       <c r="C4871">
-        <v>2</v>
+        <v>793</v>
       </c>
       <c r="D4871">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="E4871">
-        <v>3</v>
+        <v>849</v>
       </c>
     </row>
     <row r="4872">
@@ -92927,17 +92927,17 @@
       </c>
       <c r="B4872" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Ružomberok</t>
         </is>
       </c>
       <c r="C4872">
-        <v>284</v>
+        <v>1573</v>
       </c>
       <c r="D4872">
-        <v>17</v>
+        <v>147</v>
       </c>
       <c r="E4872">
-        <v>301</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="4873">
@@ -92946,17 +92946,17 @@
       </c>
       <c r="B4873" t="inlineStr">
         <is>
-          <t>Okres Žarnovica</t>
+          <t>Okres Sabinov</t>
         </is>
       </c>
       <c r="C4873">
-        <v>10</v>
+        <v>771</v>
       </c>
       <c r="D4873">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E4873">
-        <v>10</v>
+        <v>871</v>
       </c>
     </row>
     <row r="4874">
@@ -92965,17 +92965,17 @@
       </c>
       <c r="B4874" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Senec</t>
         </is>
       </c>
       <c r="C4874">
-        <v>314</v>
+        <v>447</v>
       </c>
       <c r="D4874">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E4874">
-        <v>336</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4875">
@@ -92984,17 +92984,1537 @@
       </c>
       <c r="B4875" t="inlineStr">
         <is>
+          <t>Okres Senica</t>
+        </is>
+      </c>
+      <c r="C4875">
+        <v>274</v>
+      </c>
+      <c r="D4875">
+        <v>28</v>
+      </c>
+      <c r="E4875">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="4876">
+      <c r="A4876" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4876" t="inlineStr">
+        <is>
+          <t>Okres Skalica</t>
+        </is>
+      </c>
+      <c r="C4876">
+        <v>27</v>
+      </c>
+      <c r="D4876">
+        <v>1</v>
+      </c>
+      <c r="E4876">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4877">
+      <c r="A4877" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4877" t="inlineStr">
+        <is>
+          <t>Okres Snina</t>
+        </is>
+      </c>
+      <c r="C4877">
+        <v>496</v>
+      </c>
+      <c r="D4877">
+        <v>39</v>
+      </c>
+      <c r="E4877">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="4878">
+      <c r="A4878" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4878" t="inlineStr">
+        <is>
+          <t>Okres Sobrance</t>
+        </is>
+      </c>
+      <c r="C4878">
+        <v>163</v>
+      </c>
+      <c r="D4878">
+        <v>6</v>
+      </c>
+      <c r="E4878">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4879">
+      <c r="A4879" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4879" t="inlineStr">
+        <is>
+          <t>Okres Spišská Nová Ves</t>
+        </is>
+      </c>
+      <c r="C4879">
+        <v>916</v>
+      </c>
+      <c r="D4879">
+        <v>67</v>
+      </c>
+      <c r="E4879">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="4880">
+      <c r="A4880" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4880" t="inlineStr">
+        <is>
+          <t>Okres Stará Ľubovňa</t>
+        </is>
+      </c>
+      <c r="C4880">
+        <v>87</v>
+      </c>
+      <c r="D4880">
+        <v>9</v>
+      </c>
+      <c r="E4880">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4881">
+      <c r="A4881" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4881" t="inlineStr">
+        <is>
+          <t>Okres Stropkov</t>
+        </is>
+      </c>
+      <c r="C4881">
+        <v>1</v>
+      </c>
+      <c r="D4881">
+        <v>0</v>
+      </c>
+      <c r="E4881">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4882">
+      <c r="A4882" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4882" t="inlineStr">
+        <is>
+          <t>Okres Svidník</t>
+        </is>
+      </c>
+      <c r="C4882">
+        <v>131</v>
+      </c>
+      <c r="D4882">
+        <v>11</v>
+      </c>
+      <c r="E4882">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4883">
+      <c r="A4883" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4883" t="inlineStr">
+        <is>
+          <t>Okres Šaľa</t>
+        </is>
+      </c>
+      <c r="C4883">
+        <v>232</v>
+      </c>
+      <c r="D4883">
+        <v>25</v>
+      </c>
+      <c r="E4883">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4884">
+      <c r="A4884" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4884" t="inlineStr">
+        <is>
+          <t>Okres Topoľčany</t>
+        </is>
+      </c>
+      <c r="C4884">
+        <v>484</v>
+      </c>
+      <c r="D4884">
+        <v>66</v>
+      </c>
+      <c r="E4884">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="4885">
+      <c r="A4885" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4885" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C4885">
+        <v>651</v>
+      </c>
+      <c r="D4885">
+        <v>33</v>
+      </c>
+      <c r="E4885">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="4886">
+      <c r="A4886" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4886" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C4886">
+        <v>2404</v>
+      </c>
+      <c r="D4886">
+        <v>117</v>
+      </c>
+      <c r="E4886">
+        <v>2521</v>
+      </c>
+    </row>
+    <row r="4887">
+      <c r="A4887" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4887" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C4887">
+        <v>990</v>
+      </c>
+      <c r="D4887">
+        <v>125</v>
+      </c>
+      <c r="E4887">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="4888">
+      <c r="A4888" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4888" t="inlineStr">
+        <is>
+          <t>Okres Turčianske Teplice</t>
+        </is>
+      </c>
+      <c r="C4888">
+        <v>148</v>
+      </c>
+      <c r="D4888">
+        <v>14</v>
+      </c>
+      <c r="E4888">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4889">
+      <c r="A4889" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4889" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C4889">
+        <v>561</v>
+      </c>
+      <c r="D4889">
+        <v>29</v>
+      </c>
+      <c r="E4889">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="4890">
+      <c r="A4890" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4890" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C4890">
+        <v>341</v>
+      </c>
+      <c r="D4890">
+        <v>12</v>
+      </c>
+      <c r="E4890">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4891">
+      <c r="A4891" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4891" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C4891">
+        <v>227</v>
+      </c>
+      <c r="D4891">
+        <v>28</v>
+      </c>
+      <c r="E4891">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4892">
+      <c r="A4892" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4892" t="inlineStr">
+        <is>
+          <t>Okres Zlaté Moravce</t>
+        </is>
+      </c>
+      <c r="C4892">
+        <v>222</v>
+      </c>
+      <c r="D4892">
+        <v>25</v>
+      </c>
+      <c r="E4892">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4893">
+      <c r="A4893" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4893" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C4893">
+        <v>324</v>
+      </c>
+      <c r="D4893">
+        <v>17</v>
+      </c>
+      <c r="E4893">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4894">
+      <c r="A4894" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4894" t="inlineStr">
+        <is>
+          <t>Okres Žarnovica</t>
+        </is>
+      </c>
+      <c r="C4894">
+        <v>10</v>
+      </c>
+      <c r="D4894">
+        <v>0</v>
+      </c>
+      <c r="E4894">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4895">
+      <c r="A4895" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4895" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C4895">
+        <v>563</v>
+      </c>
+      <c r="D4895">
+        <v>39</v>
+      </c>
+      <c r="E4895">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="4896">
+      <c r="A4896" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B4896" t="inlineStr">
+        <is>
           <t>Okres Žilina</t>
         </is>
       </c>
-      <c r="C4875">
-        <v>839</v>
-      </c>
-      <c r="D4875">
+      <c r="C4896">
+        <v>1474</v>
+      </c>
+      <c r="D4896">
+        <v>156</v>
+      </c>
+      <c r="E4896">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="4897">
+      <c r="A4897" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4897" t="inlineStr">
+        <is>
+          <t>Okres Banská Bystrica</t>
+        </is>
+      </c>
+      <c r="C4897">
+        <v>1067</v>
+      </c>
+      <c r="D4897">
         <v>79</v>
       </c>
-      <c r="E4875">
-        <v>918</v>
+      <c r="E4897">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="4898">
+      <c r="A4898" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4898" t="inlineStr">
+        <is>
+          <t>Okres Banská Štiavnica</t>
+        </is>
+      </c>
+      <c r="C4898">
+        <v>242</v>
+      </c>
+      <c r="D4898">
+        <v>13</v>
+      </c>
+      <c r="E4898">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4899">
+      <c r="A4899" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4899" t="inlineStr">
+        <is>
+          <t>Okres Bardejov</t>
+        </is>
+      </c>
+      <c r="C4899">
+        <v>30</v>
+      </c>
+      <c r="D4899">
+        <v>1</v>
+      </c>
+      <c r="E4899">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4900">
+      <c r="A4900" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4900" t="inlineStr">
+        <is>
+          <t>Okres Bratislava I</t>
+        </is>
+      </c>
+      <c r="C4900">
+        <v>643</v>
+      </c>
+      <c r="D4900">
+        <v>4</v>
+      </c>
+      <c r="E4900">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="4901">
+      <c r="A4901" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4901" t="inlineStr">
+        <is>
+          <t>Okres Bratislava II</t>
+        </is>
+      </c>
+      <c r="C4901">
+        <v>1411</v>
+      </c>
+      <c r="D4901">
+        <v>90</v>
+      </c>
+      <c r="E4901">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="4902">
+      <c r="A4902" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4902" t="inlineStr">
+        <is>
+          <t>Okres Bratislava III</t>
+        </is>
+      </c>
+      <c r="C4902">
+        <v>394</v>
+      </c>
+      <c r="D4902">
+        <v>12</v>
+      </c>
+      <c r="E4902">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="4903">
+      <c r="A4903" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4903" t="inlineStr">
+        <is>
+          <t>Okres Bratislava IV</t>
+        </is>
+      </c>
+      <c r="C4903">
+        <v>258</v>
+      </c>
+      <c r="D4903">
+        <v>28</v>
+      </c>
+      <c r="E4903">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4904">
+      <c r="A4904" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4904" t="inlineStr">
+        <is>
+          <t>Okres Bratislava V</t>
+        </is>
+      </c>
+      <c r="C4904">
+        <v>127</v>
+      </c>
+      <c r="D4904">
+        <v>4</v>
+      </c>
+      <c r="E4904">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4905">
+      <c r="A4905" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4905" t="inlineStr">
+        <is>
+          <t>Okres Brezno</t>
+        </is>
+      </c>
+      <c r="C4905">
+        <v>0</v>
+      </c>
+      <c r="D4905">
+        <v>0</v>
+      </c>
+      <c r="E4905">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4906">
+      <c r="A4906" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4906" t="inlineStr">
+        <is>
+          <t>Okres Bytča</t>
+        </is>
+      </c>
+      <c r="C4906">
+        <v>258</v>
+      </c>
+      <c r="D4906">
+        <v>33</v>
+      </c>
+      <c r="E4906">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="4907">
+      <c r="A4907" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4907" t="inlineStr">
+        <is>
+          <t>Okres Čadca</t>
+        </is>
+      </c>
+      <c r="C4907">
+        <v>438</v>
+      </c>
+      <c r="D4907">
+        <v>35</v>
+      </c>
+      <c r="E4907">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="4908">
+      <c r="A4908" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4908" t="inlineStr">
+        <is>
+          <t>Okres Dolný Kubín</t>
+        </is>
+      </c>
+      <c r="C4908">
+        <v>247</v>
+      </c>
+      <c r="D4908">
+        <v>24</v>
+      </c>
+      <c r="E4908">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4909">
+      <c r="A4909" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4909" t="inlineStr">
+        <is>
+          <t>Okres Dunajská Streda</t>
+        </is>
+      </c>
+      <c r="C4909">
+        <v>477</v>
+      </c>
+      <c r="D4909">
+        <v>77</v>
+      </c>
+      <c r="E4909">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="4910">
+      <c r="A4910" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4910" t="inlineStr">
+        <is>
+          <t>Okres Galanta</t>
+        </is>
+      </c>
+      <c r="C4910">
+        <v>635</v>
+      </c>
+      <c r="D4910">
+        <v>101</v>
+      </c>
+      <c r="E4910">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="4911">
+      <c r="A4911" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4911" t="inlineStr">
+        <is>
+          <t>Okres Humenné</t>
+        </is>
+      </c>
+      <c r="C4911">
+        <v>149</v>
+      </c>
+      <c r="D4911">
+        <v>8</v>
+      </c>
+      <c r="E4911">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4912">
+      <c r="A4912" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4912" t="inlineStr">
+        <is>
+          <t>Okres Ilava</t>
+        </is>
+      </c>
+      <c r="C4912">
+        <v>329</v>
+      </c>
+      <c r="D4912">
+        <v>39</v>
+      </c>
+      <c r="E4912">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="4913">
+      <c r="A4913" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4913" t="inlineStr">
+        <is>
+          <t>Okres Kežmarok</t>
+        </is>
+      </c>
+      <c r="C4913">
+        <v>183</v>
+      </c>
+      <c r="D4913">
+        <v>14</v>
+      </c>
+      <c r="E4913">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4914">
+      <c r="A4914" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4914" t="inlineStr">
+        <is>
+          <t>Okres Komárno</t>
+        </is>
+      </c>
+      <c r="C4914">
+        <v>646</v>
+      </c>
+      <c r="D4914">
+        <v>40</v>
+      </c>
+      <c r="E4914">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="4915">
+      <c r="A4915" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4915" t="inlineStr">
+        <is>
+          <t>Okres Košice I</t>
+        </is>
+      </c>
+      <c r="C4915">
+        <v>69</v>
+      </c>
+      <c r="D4915">
+        <v>2</v>
+      </c>
+      <c r="E4915">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4916">
+      <c r="A4916" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4916" t="inlineStr">
+        <is>
+          <t>Okres Košice II</t>
+        </is>
+      </c>
+      <c r="C4916">
+        <v>119</v>
+      </c>
+      <c r="D4916">
+        <v>16</v>
+      </c>
+      <c r="E4916">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4917">
+      <c r="A4917" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4917" t="inlineStr">
+        <is>
+          <t>Okres Košice IV</t>
+        </is>
+      </c>
+      <c r="C4917">
+        <v>183</v>
+      </c>
+      <c r="D4917">
+        <v>7</v>
+      </c>
+      <c r="E4917">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4918">
+      <c r="A4918" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4918" t="inlineStr">
+        <is>
+          <t>Okres Kysucké Nové Mesto</t>
+        </is>
+      </c>
+      <c r="C4918">
+        <v>264</v>
+      </c>
+      <c r="D4918">
+        <v>41</v>
+      </c>
+      <c r="E4918">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4919">
+      <c r="A4919" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4919" t="inlineStr">
+        <is>
+          <t>Okres Levice</t>
+        </is>
+      </c>
+      <c r="C4919">
+        <v>586</v>
+      </c>
+      <c r="D4919">
+        <v>54</v>
+      </c>
+      <c r="E4919">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="4920">
+      <c r="A4920" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4920" t="inlineStr">
+        <is>
+          <t>Okres Levoča</t>
+        </is>
+      </c>
+      <c r="C4920">
+        <v>241</v>
+      </c>
+      <c r="D4920">
+        <v>18</v>
+      </c>
+      <c r="E4920">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4921">
+      <c r="A4921" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4921" t="inlineStr">
+        <is>
+          <t>Okres Liptovský Mikuláš</t>
+        </is>
+      </c>
+      <c r="C4921">
+        <v>451</v>
+      </c>
+      <c r="D4921">
+        <v>23</v>
+      </c>
+      <c r="E4921">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="4922">
+      <c r="A4922" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4922" t="inlineStr">
+        <is>
+          <t>Okres Lučenec</t>
+        </is>
+      </c>
+      <c r="C4922">
+        <v>319</v>
+      </c>
+      <c r="D4922">
+        <v>24</v>
+      </c>
+      <c r="E4922">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4923">
+      <c r="A4923" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4923" t="inlineStr">
+        <is>
+          <t>Okres Martin</t>
+        </is>
+      </c>
+      <c r="C4923">
+        <v>90</v>
+      </c>
+      <c r="D4923">
+        <v>3</v>
+      </c>
+      <c r="E4923">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4924">
+      <c r="A4924" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4924" t="inlineStr">
+        <is>
+          <t>Okres Michalovce</t>
+        </is>
+      </c>
+      <c r="C4924">
+        <v>211</v>
+      </c>
+      <c r="D4924">
+        <v>19</v>
+      </c>
+      <c r="E4924">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4925">
+      <c r="A4925" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4925" t="inlineStr">
+        <is>
+          <t>Okres Myjava</t>
+        </is>
+      </c>
+      <c r="C4925">
+        <v>93</v>
+      </c>
+      <c r="D4925">
+        <v>3</v>
+      </c>
+      <c r="E4925">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4926">
+      <c r="A4926" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4926" t="inlineStr">
+        <is>
+          <t>Okres Nitra</t>
+        </is>
+      </c>
+      <c r="C4926">
+        <v>651</v>
+      </c>
+      <c r="D4926">
+        <v>40</v>
+      </c>
+      <c r="E4926">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="4927">
+      <c r="A4927" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4927" t="inlineStr">
+        <is>
+          <t>Okres Partizánske</t>
+        </is>
+      </c>
+      <c r="C4927">
+        <v>423</v>
+      </c>
+      <c r="D4927">
+        <v>15</v>
+      </c>
+      <c r="E4927">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="4928">
+      <c r="A4928" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4928" t="inlineStr">
+        <is>
+          <t>Okres Pezinok</t>
+        </is>
+      </c>
+      <c r="C4928">
+        <v>333</v>
+      </c>
+      <c r="D4928">
+        <v>17</v>
+      </c>
+      <c r="E4928">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4929">
+      <c r="A4929" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4929" t="inlineStr">
+        <is>
+          <t>Okres Piešťany</t>
+        </is>
+      </c>
+      <c r="C4929">
+        <v>252</v>
+      </c>
+      <c r="D4929">
+        <v>6</v>
+      </c>
+      <c r="E4929">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4930">
+      <c r="A4930" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4930" t="inlineStr">
+        <is>
+          <t>Okres Poprad</t>
+        </is>
+      </c>
+      <c r="C4930">
+        <v>405</v>
+      </c>
+      <c r="D4930">
+        <v>14</v>
+      </c>
+      <c r="E4930">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="4931">
+      <c r="A4931" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4931" t="inlineStr">
+        <is>
+          <t>Okres Považská Bystrica</t>
+        </is>
+      </c>
+      <c r="C4931">
+        <v>547</v>
+      </c>
+      <c r="D4931">
+        <v>50</v>
+      </c>
+      <c r="E4931">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="4932">
+      <c r="A4932" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4932" t="inlineStr">
+        <is>
+          <t>Okres Prievidza</t>
+        </is>
+      </c>
+      <c r="C4932">
+        <v>461</v>
+      </c>
+      <c r="D4932">
+        <v>30</v>
+      </c>
+      <c r="E4932">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="4933">
+      <c r="A4933" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4933" t="inlineStr">
+        <is>
+          <t>Okres Púchov</t>
+        </is>
+      </c>
+      <c r="C4933">
+        <v>4</v>
+      </c>
+      <c r="D4933">
+        <v>0</v>
+      </c>
+      <c r="E4933">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4934">
+      <c r="A4934" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4934" t="inlineStr">
+        <is>
+          <t>Okres Revúca</t>
+        </is>
+      </c>
+      <c r="C4934">
+        <v>409</v>
+      </c>
+      <c r="D4934">
+        <v>28</v>
+      </c>
+      <c r="E4934">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="4935">
+      <c r="A4935" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4935" t="inlineStr">
+        <is>
+          <t>Okres Rimavská Sobota</t>
+        </is>
+      </c>
+      <c r="C4935">
+        <v>402</v>
+      </c>
+      <c r="D4935">
+        <v>17</v>
+      </c>
+      <c r="E4935">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="4936">
+      <c r="A4936" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4936" t="inlineStr">
+        <is>
+          <t>Okres Rožňava</t>
+        </is>
+      </c>
+      <c r="C4936">
+        <v>426</v>
+      </c>
+      <c r="D4936">
+        <v>20</v>
+      </c>
+      <c r="E4936">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="4937">
+      <c r="A4937" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4937" t="inlineStr">
+        <is>
+          <t>Okres Ružomberok</t>
+        </is>
+      </c>
+      <c r="C4937">
+        <v>132</v>
+      </c>
+      <c r="D4937">
+        <v>7</v>
+      </c>
+      <c r="E4937">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4938">
+      <c r="A4938" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4938" t="inlineStr">
+        <is>
+          <t>Okres Sabinov</t>
+        </is>
+      </c>
+      <c r="C4938">
+        <v>4</v>
+      </c>
+      <c r="D4938">
+        <v>0</v>
+      </c>
+      <c r="E4938">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4939">
+      <c r="A4939" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4939" t="inlineStr">
+        <is>
+          <t>Okres Senec</t>
+        </is>
+      </c>
+      <c r="C4939">
+        <v>1</v>
+      </c>
+      <c r="D4939">
+        <v>0</v>
+      </c>
+      <c r="E4939">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4940">
+      <c r="A4940" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4940" t="inlineStr">
+        <is>
+          <t>Okres Skalica</t>
+        </is>
+      </c>
+      <c r="C4940">
+        <v>364</v>
+      </c>
+      <c r="D4940">
+        <v>15</v>
+      </c>
+      <c r="E4940">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="4941">
+      <c r="A4941" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4941" t="inlineStr">
+        <is>
+          <t>Okres Sobrance</t>
+        </is>
+      </c>
+      <c r="C4941">
+        <v>142</v>
+      </c>
+      <c r="D4941">
+        <v>13</v>
+      </c>
+      <c r="E4941">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4942">
+      <c r="A4942" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4942" t="inlineStr">
+        <is>
+          <t>Okres Spišská Nová Ves</t>
+        </is>
+      </c>
+      <c r="C4942">
+        <v>22</v>
+      </c>
+      <c r="D4942">
+        <v>6</v>
+      </c>
+      <c r="E4942">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4943">
+      <c r="A4943" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4943" t="inlineStr">
+        <is>
+          <t>Okres Stará Ľubovňa</t>
+        </is>
+      </c>
+      <c r="C4943">
+        <v>259</v>
+      </c>
+      <c r="D4943">
+        <v>66</v>
+      </c>
+      <c r="E4943">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4944">
+      <c r="A4944" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4944" t="inlineStr">
+        <is>
+          <t>Okres Stropkov</t>
+        </is>
+      </c>
+      <c r="C4944">
+        <v>2</v>
+      </c>
+      <c r="D4944">
+        <v>0</v>
+      </c>
+      <c r="E4944">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4945">
+      <c r="A4945" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4945" t="inlineStr">
+        <is>
+          <t>Okres Topoľčany</t>
+        </is>
+      </c>
+      <c r="C4945">
+        <v>424</v>
+      </c>
+      <c r="D4945">
+        <v>62</v>
+      </c>
+      <c r="E4945">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="4946">
+      <c r="A4946" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4946" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C4946">
+        <v>777</v>
+      </c>
+      <c r="D4946">
+        <v>56</v>
+      </c>
+      <c r="E4946">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="4947">
+      <c r="A4947" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4947" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C4947">
+        <v>406</v>
+      </c>
+      <c r="D4947">
+        <v>29</v>
+      </c>
+      <c r="E4947">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="4948">
+      <c r="A4948" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4948" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C4948">
+        <v>161</v>
+      </c>
+      <c r="D4948">
+        <v>8</v>
+      </c>
+      <c r="E4948">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4949">
+      <c r="A4949" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4949" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C4949">
+        <v>45</v>
+      </c>
+      <c r="D4949">
+        <v>3</v>
+      </c>
+      <c r="E4949">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4950">
+      <c r="A4950" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4950" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C4950">
+        <v>495</v>
+      </c>
+      <c r="D4950">
+        <v>16</v>
+      </c>
+      <c r="E4950">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="4951">
+      <c r="A4951" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4951" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C4951">
+        <v>302</v>
+      </c>
+      <c r="D4951">
+        <v>18</v>
+      </c>
+      <c r="E4951">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4952">
+      <c r="A4952" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4952" t="inlineStr">
+        <is>
+          <t>Okres Zlaté Moravce</t>
+        </is>
+      </c>
+      <c r="C4952">
+        <v>1</v>
+      </c>
+      <c r="D4952">
+        <v>0</v>
+      </c>
+      <c r="E4952">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4953">
+      <c r="A4953" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4953" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C4953">
+        <v>451</v>
+      </c>
+      <c r="D4953">
+        <v>22</v>
+      </c>
+      <c r="E4953">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="4954">
+      <c r="A4954" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4954" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C4954">
+        <v>325</v>
+      </c>
+      <c r="D4954">
+        <v>15</v>
+      </c>
+      <c r="E4954">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="4955">
+      <c r="A4955" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B4955" t="inlineStr">
+        <is>
+          <t>Okres Žilina</t>
+        </is>
+      </c>
+      <c r="C4955">
+        <v>955</v>
+      </c>
+      <c r="D4955">
+        <v>64</v>
+      </c>
+      <c r="E4955">
+        <v>1019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: ut 12. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_AgTests_District.xlsx
+++ b/OpenData_Slovakia_Covid_AgTests_District.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5138"/>
+  <dimension ref="A1:E5219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -88371,13 +88371,13 @@
         </is>
       </c>
       <c r="C4632">
-        <v>2234</v>
+        <v>2436</v>
       </c>
       <c r="D4632">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="E4632">
-        <v>2455</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="4633">
@@ -89055,13 +89055,13 @@
         </is>
       </c>
       <c r="C4668">
-        <v>794</v>
+        <v>800</v>
       </c>
       <c r="D4668">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E4668">
-        <v>866</v>
+        <v>873</v>
       </c>
     </row>
     <row r="4669">
@@ -89777,13 +89777,13 @@
         </is>
       </c>
       <c r="C4706">
-        <v>949</v>
+        <v>954</v>
       </c>
       <c r="D4706">
         <v>45</v>
       </c>
       <c r="E4706">
-        <v>994</v>
+        <v>999</v>
       </c>
     </row>
     <row r="4707">
@@ -89815,13 +89815,13 @@
         </is>
       </c>
       <c r="C4708">
-        <v>1509</v>
+        <v>1658</v>
       </c>
       <c r="D4708">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E4708">
-        <v>1594</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="4709">
@@ -92266,13 +92266,13 @@
         </is>
       </c>
       <c r="C4837">
-        <v>721</v>
+        <v>836</v>
       </c>
       <c r="D4837">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E4837">
-        <v>756</v>
+        <v>880</v>
       </c>
     </row>
     <row r="4838">
@@ -92513,13 +92513,13 @@
         </is>
       </c>
       <c r="C4850">
-        <v>1315</v>
+        <v>982</v>
       </c>
       <c r="D4850">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E4850">
-        <v>1409</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="4851">
@@ -93710,13 +93710,13 @@
         </is>
       </c>
       <c r="C4913">
-        <v>1078</v>
+        <v>1357</v>
       </c>
       <c r="D4913">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E4913">
-        <v>1091</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="4914">
@@ -93729,13 +93729,13 @@
         </is>
       </c>
       <c r="C4914">
-        <v>2388</v>
+        <v>2496</v>
       </c>
       <c r="D4914">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E4914">
-        <v>2517</v>
+        <v>2629</v>
       </c>
     </row>
     <row r="4915">
@@ -93786,13 +93786,13 @@
         </is>
       </c>
       <c r="C4917">
-        <v>385</v>
+        <v>456</v>
       </c>
       <c r="D4917">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4917">
-        <v>404</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4918">
@@ -93900,13 +93900,13 @@
         </is>
       </c>
       <c r="C4923">
-        <v>817</v>
+        <v>823</v>
       </c>
       <c r="D4923">
         <v>108</v>
       </c>
       <c r="E4923">
-        <v>925</v>
+        <v>931</v>
       </c>
     </row>
     <row r="4924">
@@ -93976,13 +93976,13 @@
         </is>
       </c>
       <c r="C4927">
-        <v>716</v>
+        <v>1049</v>
       </c>
       <c r="D4927">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="E4927">
-        <v>764</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="4928">
@@ -94318,13 +94318,13 @@
         </is>
       </c>
       <c r="C4945">
-        <v>5084</v>
+        <v>5295</v>
       </c>
       <c r="D4945">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="E4945">
-        <v>5223</v>
+        <v>5446</v>
       </c>
     </row>
     <row r="4946">
@@ -94413,13 +94413,13 @@
         </is>
       </c>
       <c r="C4950">
-        <v>1251</v>
+        <v>1253</v>
       </c>
       <c r="D4950">
         <v>55</v>
       </c>
       <c r="E4950">
-        <v>1306</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="4951">
@@ -94432,13 +94432,13 @@
         </is>
       </c>
       <c r="C4951">
-        <v>1481</v>
+        <v>1493</v>
       </c>
       <c r="D4951">
         <v>70</v>
       </c>
       <c r="E4951">
-        <v>1551</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="4952">
@@ -94584,13 +94584,13 @@
         </is>
       </c>
       <c r="C4959">
-        <v>7925</v>
+        <v>8244</v>
       </c>
       <c r="D4959">
-        <v>723</v>
+        <v>751</v>
       </c>
       <c r="E4959">
-        <v>8648</v>
+        <v>8995</v>
       </c>
     </row>
     <row r="4960">
@@ -94812,13 +94812,13 @@
         </is>
       </c>
       <c r="C4971">
-        <v>1512</v>
+        <v>1514</v>
       </c>
       <c r="D4971">
         <v>173</v>
       </c>
       <c r="E4971">
-        <v>1685</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="4972">
@@ -95173,13 +95173,13 @@
         </is>
       </c>
       <c r="C4990">
-        <v>1447</v>
+        <v>1458</v>
       </c>
       <c r="D4990">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E4990">
-        <v>1602</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="4991">
@@ -95530,17 +95530,17 @@
       </c>
       <c r="B5009" t="inlineStr">
         <is>
-          <t>Okres Michalovce</t>
+          <t>Okres Martin</t>
         </is>
       </c>
       <c r="C5009">
-        <v>343</v>
+        <v>0</v>
       </c>
       <c r="D5009">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E5009">
-        <v>368</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5010">
@@ -95549,17 +95549,17 @@
       </c>
       <c r="B5010" t="inlineStr">
         <is>
-          <t>Okres Myjava</t>
+          <t>Okres Michalovce</t>
         </is>
       </c>
       <c r="C5010">
-        <v>306</v>
+        <v>343</v>
       </c>
       <c r="D5010">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="E5010">
-        <v>313</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5011">
@@ -95568,17 +95568,17 @@
       </c>
       <c r="B5011" t="inlineStr">
         <is>
-          <t>Okres Nitra</t>
+          <t>Okres Myjava</t>
         </is>
       </c>
       <c r="C5011">
-        <v>1385</v>
+        <v>306</v>
       </c>
       <c r="D5011">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E5011">
-        <v>1424</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5012">
@@ -95587,17 +95587,17 @@
       </c>
       <c r="B5012" t="inlineStr">
         <is>
-          <t>Okres Nové Mesto nad Váhom</t>
+          <t>Okres Nitra</t>
         </is>
       </c>
       <c r="C5012">
-        <v>3</v>
+        <v>2477</v>
       </c>
       <c r="D5012">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E5012">
-        <v>3</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="5013">
@@ -95606,17 +95606,17 @@
       </c>
       <c r="B5013" t="inlineStr">
         <is>
-          <t>Okres Nové Zámky</t>
+          <t>Okres Nové Mesto nad Váhom</t>
         </is>
       </c>
       <c r="C5013">
-        <v>234</v>
+        <v>3</v>
       </c>
       <c r="D5013">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E5013">
-        <v>240</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5014">
@@ -95625,17 +95625,17 @@
       </c>
       <c r="B5014" t="inlineStr">
         <is>
-          <t>Okres Partizánske</t>
+          <t>Okres Nové Zámky</t>
         </is>
       </c>
       <c r="C5014">
-        <v>41</v>
+        <v>921</v>
       </c>
       <c r="D5014">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E5014">
-        <v>54</v>
+        <v>944</v>
       </c>
     </row>
     <row r="5015">
@@ -95644,17 +95644,17 @@
       </c>
       <c r="B5015" t="inlineStr">
         <is>
-          <t>Okres Pezinok</t>
+          <t>Okres Partizánske</t>
         </is>
       </c>
       <c r="C5015">
-        <v>871</v>
+        <v>41</v>
       </c>
       <c r="D5015">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E5015">
-        <v>897</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5016">
@@ -95663,17 +95663,17 @@
       </c>
       <c r="B5016" t="inlineStr">
         <is>
-          <t>Okres Piešťany</t>
+          <t>Okres Pezinok</t>
         </is>
       </c>
       <c r="C5016">
-        <v>410</v>
+        <v>871</v>
       </c>
       <c r="D5016">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E5016">
-        <v>430</v>
+        <v>897</v>
       </c>
     </row>
     <row r="5017">
@@ -95682,17 +95682,17 @@
       </c>
       <c r="B5017" t="inlineStr">
         <is>
-          <t>Okres Poprad</t>
+          <t>Okres Piešťany</t>
         </is>
       </c>
       <c r="C5017">
-        <v>1029</v>
+        <v>410</v>
       </c>
       <c r="D5017">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="E5017">
-        <v>1070</v>
+        <v>430</v>
       </c>
     </row>
     <row r="5018">
@@ -95701,17 +95701,17 @@
       </c>
       <c r="B5018" t="inlineStr">
         <is>
-          <t>Okres Považská Bystrica</t>
+          <t>Okres Poprad</t>
         </is>
       </c>
       <c r="C5018">
-        <v>554</v>
+        <v>1029</v>
       </c>
       <c r="D5018">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E5018">
-        <v>578</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="5019">
@@ -95720,17 +95720,17 @@
       </c>
       <c r="B5019" t="inlineStr">
         <is>
-          <t>Okres Prešov</t>
+          <t>Okres Považská Bystrica</t>
         </is>
       </c>
       <c r="C5019">
-        <v>17</v>
+        <v>554</v>
       </c>
       <c r="D5019">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E5019">
-        <v>17</v>
+        <v>578</v>
       </c>
     </row>
     <row r="5020">
@@ -95739,17 +95739,17 @@
       </c>
       <c r="B5020" t="inlineStr">
         <is>
-          <t>Okres Prievidza</t>
+          <t>Okres Prešov</t>
         </is>
       </c>
       <c r="C5020">
-        <v>502</v>
+        <v>17</v>
       </c>
       <c r="D5020">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E5020">
-        <v>524</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5021">
@@ -95758,17 +95758,17 @@
       </c>
       <c r="B5021" t="inlineStr">
         <is>
-          <t>Okres Púchov</t>
+          <t>Okres Prievidza</t>
         </is>
       </c>
       <c r="C5021">
-        <v>1</v>
+        <v>502</v>
       </c>
       <c r="D5021">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E5021">
-        <v>3</v>
+        <v>524</v>
       </c>
     </row>
     <row r="5022">
@@ -95777,17 +95777,17 @@
       </c>
       <c r="B5022" t="inlineStr">
         <is>
-          <t>Okres Revúca</t>
+          <t>Okres Púchov</t>
         </is>
       </c>
       <c r="C5022">
-        <v>609</v>
+        <v>1</v>
       </c>
       <c r="D5022">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E5022">
-        <v>635</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5023">
@@ -95796,17 +95796,17 @@
       </c>
       <c r="B5023" t="inlineStr">
         <is>
-          <t>Okres Rožňava</t>
+          <t>Okres Revúca</t>
         </is>
       </c>
       <c r="C5023">
-        <v>5</v>
+        <v>609</v>
       </c>
       <c r="D5023">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E5023">
-        <v>5</v>
+        <v>635</v>
       </c>
     </row>
     <row r="5024">
@@ -95815,17 +95815,17 @@
       </c>
       <c r="B5024" t="inlineStr">
         <is>
-          <t>Okres Ružomberok</t>
+          <t>Okres Rožňava</t>
         </is>
       </c>
       <c r="C5024">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D5024">
+        <v>0</v>
+      </c>
+      <c r="E5024">
         <v>5</v>
-      </c>
-      <c r="E5024">
-        <v>25</v>
       </c>
     </row>
     <row r="5025">
@@ -95834,17 +95834,17 @@
       </c>
       <c r="B5025" t="inlineStr">
         <is>
-          <t>Okres Sabinov</t>
+          <t>Okres Ružomberok</t>
         </is>
       </c>
       <c r="C5025">
-        <v>1</v>
+        <v>266</v>
       </c>
       <c r="D5025">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E5025">
-        <v>1</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5026">
@@ -95853,17 +95853,17 @@
       </c>
       <c r="B5026" t="inlineStr">
         <is>
-          <t>Okres Senec</t>
+          <t>Okres Sabinov</t>
         </is>
       </c>
       <c r="C5026">
-        <v>518</v>
+        <v>1</v>
       </c>
       <c r="D5026">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E5026">
-        <v>547</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5027">
@@ -95872,17 +95872,17 @@
       </c>
       <c r="B5027" t="inlineStr">
         <is>
-          <t>Okres Senica</t>
+          <t>Okres Senec</t>
         </is>
       </c>
       <c r="C5027">
-        <v>246</v>
+        <v>518</v>
       </c>
       <c r="D5027">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E5027">
-        <v>265</v>
+        <v>547</v>
       </c>
     </row>
     <row r="5028">
@@ -95891,17 +95891,17 @@
       </c>
       <c r="B5028" t="inlineStr">
         <is>
-          <t>Okres Skalica</t>
+          <t>Okres Senica</t>
         </is>
       </c>
       <c r="C5028">
-        <v>6</v>
+        <v>246</v>
       </c>
       <c r="D5028">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E5028">
-        <v>7</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5029">
@@ -95910,17 +95910,17 @@
       </c>
       <c r="B5029" t="inlineStr">
         <is>
-          <t>Okres Snina</t>
+          <t>Okres Skalica</t>
         </is>
       </c>
       <c r="C5029">
-        <v>269</v>
+        <v>6</v>
       </c>
       <c r="D5029">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="E5029">
-        <v>290</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5030">
@@ -95929,17 +95929,17 @@
       </c>
       <c r="B5030" t="inlineStr">
         <is>
-          <t>Okres Sobrance</t>
+          <t>Okres Snina</t>
         </is>
       </c>
       <c r="C5030">
-        <v>200</v>
+        <v>269</v>
       </c>
       <c r="D5030">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E5030">
-        <v>203</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5031">
@@ -95948,17 +95948,17 @@
       </c>
       <c r="B5031" t="inlineStr">
         <is>
-          <t>Okres Spišská Nová Ves</t>
+          <t>Okres Sobrance</t>
         </is>
       </c>
       <c r="C5031">
-        <v>96</v>
+        <v>200</v>
       </c>
       <c r="D5031">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E5031">
-        <v>102</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5032">
@@ -95967,17 +95967,17 @@
       </c>
       <c r="B5032" t="inlineStr">
         <is>
-          <t>Okres Stará Ľubovňa</t>
+          <t>Okres Spišská Nová Ves</t>
         </is>
       </c>
       <c r="C5032">
-        <v>310</v>
+        <v>96</v>
       </c>
       <c r="D5032">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="E5032">
-        <v>347</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5033">
@@ -95986,17 +95986,17 @@
       </c>
       <c r="B5033" t="inlineStr">
         <is>
-          <t>Okres Šaľa</t>
+          <t>Okres Stará Ľubovňa</t>
         </is>
       </c>
       <c r="C5033">
-        <v>226</v>
+        <v>310</v>
       </c>
       <c r="D5033">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E5033">
-        <v>242</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5034">
@@ -96005,17 +96005,17 @@
       </c>
       <c r="B5034" t="inlineStr">
         <is>
-          <t>Okres Topoľčany</t>
+          <t>Okres Šaľa</t>
         </is>
       </c>
       <c r="C5034">
-        <v>635</v>
+        <v>226</v>
       </c>
       <c r="D5034">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E5034">
-        <v>682</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5035">
@@ -96024,17 +96024,17 @@
       </c>
       <c r="B5035" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Topoľčany</t>
         </is>
       </c>
       <c r="C5035">
-        <v>49</v>
+        <v>635</v>
       </c>
       <c r="D5035">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="E5035">
-        <v>51</v>
+        <v>682</v>
       </c>
     </row>
     <row r="5036">
@@ -96043,17 +96043,17 @@
       </c>
       <c r="B5036" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Trebišov</t>
         </is>
       </c>
       <c r="C5036">
-        <v>366</v>
+        <v>49</v>
       </c>
       <c r="D5036">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E5036">
-        <v>383</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5037">
@@ -96062,17 +96062,17 @@
       </c>
       <c r="B5037" t="inlineStr">
         <is>
-          <t>Okres Trnava</t>
+          <t>Okres Trenčín</t>
         </is>
       </c>
       <c r="C5037">
-        <v>929</v>
+        <v>366</v>
       </c>
       <c r="D5037">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E5037">
-        <v>959</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5038">
@@ -96081,17 +96081,17 @@
       </c>
       <c r="B5038" t="inlineStr">
         <is>
-          <t>Okres Tvrdošín</t>
+          <t>Okres Trnava</t>
         </is>
       </c>
       <c r="C5038">
-        <v>316</v>
+        <v>929</v>
       </c>
       <c r="D5038">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E5038">
-        <v>322</v>
+        <v>959</v>
       </c>
     </row>
     <row r="5039">
@@ -96100,17 +96100,17 @@
       </c>
       <c r="B5039" t="inlineStr">
         <is>
-          <t>Okres Vranov nad Topľou</t>
+          <t>Okres Tvrdošín</t>
         </is>
       </c>
       <c r="C5039">
-        <v>371</v>
+        <v>316</v>
       </c>
       <c r="D5039">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E5039">
-        <v>386</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5040">
@@ -96119,17 +96119,17 @@
       </c>
       <c r="B5040" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Vranov nad Topľou</t>
         </is>
       </c>
       <c r="C5040">
-        <v>46</v>
+        <v>371</v>
       </c>
       <c r="D5040">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E5040">
-        <v>46</v>
+        <v>386</v>
       </c>
     </row>
     <row r="5041">
@@ -96138,17 +96138,17 @@
       </c>
       <c r="B5041" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Zvolen</t>
         </is>
       </c>
       <c r="C5041">
-        <v>281</v>
+        <v>46</v>
       </c>
       <c r="D5041">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E5041">
-        <v>290</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5042">
@@ -96157,36 +96157,36 @@
       </c>
       <c r="B5042" t="inlineStr">
         <is>
-          <t>Okres Žilina</t>
+          <t>Okres Žiar nad Hronom</t>
         </is>
       </c>
       <c r="C5042">
-        <v>902</v>
+        <v>281</v>
       </c>
       <c r="D5042">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="E5042">
-        <v>957</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5043">
       <c r="A5043" s="2">
-        <v>44206</v>
+        <v>44205</v>
       </c>
       <c r="B5043" t="inlineStr">
         <is>
-          <t>Okres Banská Bystrica</t>
+          <t>Okres Žilina</t>
         </is>
       </c>
       <c r="C5043">
-        <v>22</v>
+        <v>902</v>
       </c>
       <c r="D5043">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="E5043">
-        <v>22</v>
+        <v>957</v>
       </c>
     </row>
     <row r="5044">
@@ -96195,17 +96195,17 @@
       </c>
       <c r="B5044" t="inlineStr">
         <is>
-          <t>Okres Bardejov</t>
+          <t>Okres Banská Bystrica</t>
         </is>
       </c>
       <c r="C5044">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="D5044">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5044">
-        <v>65</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5045">
@@ -96214,17 +96214,17 @@
       </c>
       <c r="B5045" t="inlineStr">
         <is>
-          <t>Okres Bratislava I</t>
+          <t>Okres Bardejov</t>
         </is>
       </c>
       <c r="C5045">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="D5045">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E5045">
-        <v>15</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5046">
@@ -96233,17 +96233,17 @@
       </c>
       <c r="B5046" t="inlineStr">
         <is>
-          <t>Okres Bratislava II</t>
+          <t>Okres Bratislava I</t>
         </is>
       </c>
       <c r="C5046">
-        <v>393</v>
+        <v>14</v>
       </c>
       <c r="D5046">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E5046">
-        <v>412</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5047">
@@ -96252,17 +96252,17 @@
       </c>
       <c r="B5047" t="inlineStr">
         <is>
-          <t>Okres Bratislava III</t>
+          <t>Okres Bratislava II</t>
         </is>
       </c>
       <c r="C5047">
-        <v>202</v>
+        <v>393</v>
       </c>
       <c r="D5047">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E5047">
-        <v>238</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5048">
@@ -96271,17 +96271,17 @@
       </c>
       <c r="B5048" t="inlineStr">
         <is>
-          <t>Okres Bratislava V</t>
+          <t>Okres Bratislava III</t>
         </is>
       </c>
       <c r="C5048">
-        <v>1</v>
+        <v>202</v>
       </c>
       <c r="D5048">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E5048">
-        <v>1</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5049">
@@ -96290,17 +96290,17 @@
       </c>
       <c r="B5049" t="inlineStr">
         <is>
-          <t>Okres Čadca</t>
+          <t>Okres Bratislava V</t>
         </is>
       </c>
       <c r="C5049">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="D5049">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5049">
-        <v>85</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5050">
@@ -96309,17 +96309,17 @@
       </c>
       <c r="B5050" t="inlineStr">
         <is>
-          <t>Okres Humenné</t>
+          <t>Okres Čadca</t>
         </is>
       </c>
       <c r="C5050">
-        <v>336</v>
+        <v>81</v>
       </c>
       <c r="D5050">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E5050">
-        <v>352</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5051">
@@ -96328,17 +96328,17 @@
       </c>
       <c r="B5051" t="inlineStr">
         <is>
-          <t>Okres Kežmarok</t>
+          <t>Okres Humenné</t>
         </is>
       </c>
       <c r="C5051">
-        <v>4</v>
+        <v>336</v>
       </c>
       <c r="D5051">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E5051">
-        <v>4</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5052">
@@ -96347,17 +96347,17 @@
       </c>
       <c r="B5052" t="inlineStr">
         <is>
-          <t>Okres Komárno</t>
+          <t>Okres Kežmarok</t>
         </is>
       </c>
       <c r="C5052">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D5052">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E5052">
-        <v>30</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5053">
@@ -96366,17 +96366,17 @@
       </c>
       <c r="B5053" t="inlineStr">
         <is>
-          <t>Okres Košice II</t>
+          <t>Okres Komárno</t>
         </is>
       </c>
       <c r="C5053">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D5053">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5053">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5054">
@@ -96385,17 +96385,17 @@
       </c>
       <c r="B5054" t="inlineStr">
         <is>
-          <t>Okres Košice IV</t>
+          <t>Okres Košice II</t>
         </is>
       </c>
       <c r="C5054">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="D5054">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5054">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5055">
@@ -96404,17 +96404,17 @@
       </c>
       <c r="B5055" t="inlineStr">
         <is>
-          <t>Okres Levice</t>
+          <t>Okres Košice IV</t>
         </is>
       </c>
       <c r="C5055">
-        <v>403</v>
+        <v>2</v>
       </c>
       <c r="D5055">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E5055">
-        <v>429</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5056">
@@ -96423,17 +96423,17 @@
       </c>
       <c r="B5056" t="inlineStr">
         <is>
-          <t>Okres Levoča</t>
+          <t>Okres Levice</t>
         </is>
       </c>
       <c r="C5056">
-        <v>0</v>
+        <v>403</v>
       </c>
       <c r="D5056">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E5056">
-        <v>0</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5057">
@@ -96442,17 +96442,17 @@
       </c>
       <c r="B5057" t="inlineStr">
         <is>
-          <t>Okres Lučenec</t>
+          <t>Okres Levoča</t>
         </is>
       </c>
       <c r="C5057">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D5057">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5057">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5058">
@@ -96461,17 +96461,17 @@
       </c>
       <c r="B5058" t="inlineStr">
         <is>
-          <t>Okres Martin</t>
+          <t>Okres Lučenec</t>
         </is>
       </c>
       <c r="C5058">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D5058">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5058">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5059">
@@ -96480,17 +96480,17 @@
       </c>
       <c r="B5059" t="inlineStr">
         <is>
-          <t>Okres Michalovce</t>
+          <t>Okres Martin</t>
         </is>
       </c>
       <c r="C5059">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D5059">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5059">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5060">
@@ -96499,17 +96499,17 @@
       </c>
       <c r="B5060" t="inlineStr">
         <is>
-          <t>Okres Myjava</t>
+          <t>Okres Michalovce</t>
         </is>
       </c>
       <c r="C5060">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D5060">
         <v>1</v>
       </c>
       <c r="E5060">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5061">
@@ -96518,17 +96518,17 @@
       </c>
       <c r="B5061" t="inlineStr">
         <is>
-          <t>Okres Nitra</t>
+          <t>Okres Myjava</t>
         </is>
       </c>
       <c r="C5061">
-        <v>27188</v>
+        <v>29</v>
       </c>
       <c r="D5061">
-        <v>713</v>
+        <v>1</v>
       </c>
       <c r="E5061">
-        <v>27901</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5062">
@@ -96537,17 +96537,17 @@
       </c>
       <c r="B5062" t="inlineStr">
         <is>
-          <t>Okres Nové Mesto nad Váhom</t>
+          <t>Okres Nitra</t>
         </is>
       </c>
       <c r="C5062">
-        <v>2</v>
+        <v>28103</v>
       </c>
       <c r="D5062">
-        <v>0</v>
+        <v>738</v>
       </c>
       <c r="E5062">
-        <v>2</v>
+        <v>28841</v>
       </c>
     </row>
     <row r="5063">
@@ -96556,17 +96556,17 @@
       </c>
       <c r="B5063" t="inlineStr">
         <is>
-          <t>Okres Partizánske</t>
+          <t>Okres Nové Mesto nad Váhom</t>
         </is>
       </c>
       <c r="C5063">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5063">
         <v>0</v>
       </c>
       <c r="E5063">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5064">
@@ -96575,17 +96575,17 @@
       </c>
       <c r="B5064" t="inlineStr">
         <is>
-          <t>Okres Pezinok</t>
+          <t>Okres Nové Zámky</t>
         </is>
       </c>
       <c r="C5064">
-        <v>53</v>
+        <v>563</v>
       </c>
       <c r="D5064">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E5064">
-        <v>55</v>
+        <v>584</v>
       </c>
     </row>
     <row r="5065">
@@ -96594,17 +96594,17 @@
       </c>
       <c r="B5065" t="inlineStr">
         <is>
-          <t>Okres Poprad</t>
+          <t>Okres Partizánske</t>
         </is>
       </c>
       <c r="C5065">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D5065">
+        <v>0</v>
+      </c>
+      <c r="E5065">
         <v>1</v>
-      </c>
-      <c r="E5065">
-        <v>42</v>
       </c>
     </row>
     <row r="5066">
@@ -96613,17 +96613,17 @@
       </c>
       <c r="B5066" t="inlineStr">
         <is>
-          <t>Okres Prešov</t>
+          <t>Okres Pezinok</t>
         </is>
       </c>
       <c r="C5066">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="D5066">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5066">
-        <v>12</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5067">
@@ -96632,17 +96632,17 @@
       </c>
       <c r="B5067" t="inlineStr">
         <is>
-          <t>Okres Púchov</t>
+          <t>Okres Poprad</t>
         </is>
       </c>
       <c r="C5067">
+        <v>41</v>
+      </c>
+      <c r="D5067">
         <v>1</v>
       </c>
-      <c r="D5067">
-        <v>0</v>
-      </c>
       <c r="E5067">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5068">
@@ -96651,17 +96651,17 @@
       </c>
       <c r="B5068" t="inlineStr">
         <is>
-          <t>Okres Revúca</t>
+          <t>Okres Prešov</t>
         </is>
       </c>
       <c r="C5068">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D5068">
         <v>0</v>
       </c>
       <c r="E5068">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5069">
@@ -96670,17 +96670,17 @@
       </c>
       <c r="B5069" t="inlineStr">
         <is>
-          <t>Okres Ružomberok</t>
+          <t>Okres Púchov</t>
         </is>
       </c>
       <c r="C5069">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D5069">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5069">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5070">
@@ -96689,17 +96689,17 @@
       </c>
       <c r="B5070" t="inlineStr">
         <is>
-          <t>Okres Sabinov</t>
+          <t>Okres Revúca</t>
         </is>
       </c>
       <c r="C5070">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D5070">
         <v>0</v>
       </c>
       <c r="E5070">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5071">
@@ -96708,17 +96708,17 @@
       </c>
       <c r="B5071" t="inlineStr">
         <is>
-          <t>Okres Senec</t>
+          <t>Okres Ružomberok</t>
         </is>
       </c>
       <c r="C5071">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D5071">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5071">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5072">
@@ -96727,17 +96727,17 @@
       </c>
       <c r="B5072" t="inlineStr">
         <is>
-          <t>Okres Snina</t>
+          <t>Okres Sabinov</t>
         </is>
       </c>
       <c r="C5072">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D5072">
+        <v>0</v>
+      </c>
+      <c r="E5072">
         <v>1</v>
-      </c>
-      <c r="E5072">
-        <v>17</v>
       </c>
     </row>
     <row r="5073">
@@ -96746,17 +96746,17 @@
       </c>
       <c r="B5073" t="inlineStr">
         <is>
-          <t>Okres Sobrance</t>
+          <t>Okres Senec</t>
         </is>
       </c>
       <c r="C5073">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5073">
         <v>0</v>
       </c>
       <c r="E5073">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5074">
@@ -96765,17 +96765,17 @@
       </c>
       <c r="B5074" t="inlineStr">
         <is>
-          <t>Okres Spišská Nová Ves</t>
+          <t>Okres Snina</t>
         </is>
       </c>
       <c r="C5074">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D5074">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5074">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5075">
@@ -96784,17 +96784,17 @@
       </c>
       <c r="B5075" t="inlineStr">
         <is>
-          <t>Okres Stará Ľubovňa</t>
+          <t>Okres Sobrance</t>
         </is>
       </c>
       <c r="C5075">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D5075">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5075">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5076">
@@ -96803,17 +96803,17 @@
       </c>
       <c r="B5076" t="inlineStr">
         <is>
-          <t>Okres Šaľa</t>
+          <t>Okres Spišská Nová Ves</t>
         </is>
       </c>
       <c r="C5076">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D5076">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5076">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5077">
@@ -96822,17 +96822,17 @@
       </c>
       <c r="B5077" t="inlineStr">
         <is>
-          <t>Okres Topoľčany</t>
+          <t>Okres Stará Ľubovňa</t>
         </is>
       </c>
       <c r="C5077">
-        <v>1131</v>
+        <v>15</v>
       </c>
       <c r="D5077">
-        <v>164</v>
+        <v>1</v>
       </c>
       <c r="E5077">
-        <v>1295</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5078">
@@ -96841,17 +96841,17 @@
       </c>
       <c r="B5078" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Šaľa</t>
         </is>
       </c>
       <c r="C5078">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D5078">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5078">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5079">
@@ -96860,17 +96860,17 @@
       </c>
       <c r="B5079" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Topoľčany</t>
         </is>
       </c>
       <c r="C5079">
-        <v>15</v>
+        <v>1131</v>
       </c>
       <c r="D5079">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E5079">
-        <v>19</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="5080">
@@ -96879,17 +96879,17 @@
       </c>
       <c r="B5080" t="inlineStr">
         <is>
-          <t>Okres Trnava</t>
+          <t>Okres Trebišov</t>
         </is>
       </c>
       <c r="C5080">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D5080">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5080">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5081">
@@ -96898,17 +96898,17 @@
       </c>
       <c r="B5081" t="inlineStr">
         <is>
-          <t>Okres Tvrdošín</t>
+          <t>Okres Trenčín</t>
         </is>
       </c>
       <c r="C5081">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D5081">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5081">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5082">
@@ -96917,17 +96917,17 @@
       </c>
       <c r="B5082" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Trnava</t>
         </is>
       </c>
       <c r="C5082">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D5082">
         <v>0</v>
       </c>
       <c r="E5082">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5083">
@@ -96936,17 +96936,17 @@
       </c>
       <c r="B5083" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Tvrdošín</t>
         </is>
       </c>
       <c r="C5083">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="D5083">
         <v>0</v>
       </c>
       <c r="E5083">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5084">
@@ -96955,55 +96955,55 @@
       </c>
       <c r="B5084" t="inlineStr">
         <is>
-          <t>Okres Žilina</t>
+          <t>Okres Zvolen</t>
         </is>
       </c>
       <c r="C5084">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="D5084">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5084">
-        <v>94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5085">
       <c r="A5085" s="2">
-        <v>44207</v>
+        <v>44206</v>
       </c>
       <c r="B5085" t="inlineStr">
         <is>
-          <t>Okres Banská Bystrica</t>
+          <t>Okres Žiar nad Hronom</t>
         </is>
       </c>
       <c r="C5085">
-        <v>352</v>
+        <v>28</v>
       </c>
       <c r="D5085">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E5085">
-        <v>367</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5086">
       <c r="A5086" s="2">
-        <v>44207</v>
+        <v>44206</v>
       </c>
       <c r="B5086" t="inlineStr">
         <is>
-          <t>Okres Banská Štiavnica</t>
+          <t>Okres Žilina</t>
         </is>
       </c>
       <c r="C5086">
-        <v>387</v>
+        <v>93</v>
       </c>
       <c r="D5086">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E5086">
-        <v>400</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5087">
@@ -97012,17 +97012,17 @@
       </c>
       <c r="B5087" t="inlineStr">
         <is>
-          <t>Okres Bardejov</t>
+          <t>Okres Bánovce nad Bebravou</t>
         </is>
       </c>
       <c r="C5087">
-        <v>13</v>
+        <v>250</v>
       </c>
       <c r="D5087">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="E5087">
-        <v>14</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5088">
@@ -97031,17 +97031,17 @@
       </c>
       <c r="B5088" t="inlineStr">
         <is>
-          <t>Okres Bratislava I</t>
+          <t>Okres Banská Bystrica</t>
         </is>
       </c>
       <c r="C5088">
-        <v>25</v>
+        <v>533</v>
       </c>
       <c r="D5088">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E5088">
-        <v>25</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5089">
@@ -97050,17 +97050,17 @@
       </c>
       <c r="B5089" t="inlineStr">
         <is>
-          <t>Okres Bratislava II</t>
+          <t>Okres Banská Štiavnica</t>
         </is>
       </c>
       <c r="C5089">
-        <v>71</v>
+        <v>634</v>
       </c>
       <c r="D5089">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="E5089">
-        <v>74</v>
+        <v>669</v>
       </c>
     </row>
     <row r="5090">
@@ -97069,17 +97069,17 @@
       </c>
       <c r="B5090" t="inlineStr">
         <is>
-          <t>Okres Bratislava III</t>
+          <t>Okres Bardejov</t>
         </is>
       </c>
       <c r="C5090">
-        <v>305</v>
+        <v>401</v>
       </c>
       <c r="D5090">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E5090">
-        <v>311</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5091">
@@ -97088,17 +97088,17 @@
       </c>
       <c r="B5091" t="inlineStr">
         <is>
-          <t>Okres Bratislava IV</t>
+          <t>Okres Bratislava I</t>
         </is>
       </c>
       <c r="C5091">
-        <v>11</v>
+        <v>1940</v>
       </c>
       <c r="D5091">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E5091">
-        <v>11</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="5092">
@@ -97107,17 +97107,17 @@
       </c>
       <c r="B5092" t="inlineStr">
         <is>
-          <t>Okres Bratislava V</t>
+          <t>Okres Bratislava II</t>
         </is>
       </c>
       <c r="C5092">
-        <v>263</v>
+        <v>2267</v>
       </c>
       <c r="D5092">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E5092">
-        <v>274</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="5093">
@@ -97126,17 +97126,17 @@
       </c>
       <c r="B5093" t="inlineStr">
         <is>
-          <t>Okres Bytča</t>
+          <t>Okres Bratislava III</t>
         </is>
       </c>
       <c r="C5093">
-        <v>276</v>
+        <v>729</v>
       </c>
       <c r="D5093">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E5093">
-        <v>299</v>
+        <v>755</v>
       </c>
     </row>
     <row r="5094">
@@ -97145,17 +97145,17 @@
       </c>
       <c r="B5094" t="inlineStr">
         <is>
-          <t>Okres Čadca</t>
+          <t>Okres Bratislava IV</t>
         </is>
       </c>
       <c r="C5094">
-        <v>704</v>
+        <v>559</v>
       </c>
       <c r="D5094">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="E5094">
-        <v>717</v>
+        <v>610</v>
       </c>
     </row>
     <row r="5095">
@@ -97164,17 +97164,17 @@
       </c>
       <c r="B5095" t="inlineStr">
         <is>
-          <t>Okres Detva</t>
+          <t>Okres Bratislava V</t>
         </is>
       </c>
       <c r="C5095">
-        <v>14</v>
+        <v>575</v>
       </c>
       <c r="D5095">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E5095">
-        <v>15</v>
+        <v>593</v>
       </c>
     </row>
     <row r="5096">
@@ -97183,17 +97183,17 @@
       </c>
       <c r="B5096" t="inlineStr">
         <is>
-          <t>Okres Dolný Kubín</t>
+          <t>Okres Brezno</t>
         </is>
       </c>
       <c r="C5096">
-        <v>446</v>
+        <v>773</v>
       </c>
       <c r="D5096">
-        <v>26</v>
+        <v>153</v>
       </c>
       <c r="E5096">
-        <v>472</v>
+        <v>926</v>
       </c>
     </row>
     <row r="5097">
@@ -97202,17 +97202,17 @@
       </c>
       <c r="B5097" t="inlineStr">
         <is>
-          <t>Okres Dunajská Streda</t>
+          <t>Okres Bytča</t>
         </is>
       </c>
       <c r="C5097">
-        <v>596</v>
+        <v>276</v>
       </c>
       <c r="D5097">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="E5097">
-        <v>654</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5098">
@@ -97221,17 +97221,17 @@
       </c>
       <c r="B5098" t="inlineStr">
         <is>
-          <t>Okres Galanta</t>
+          <t>Okres Čadca</t>
         </is>
       </c>
       <c r="C5098">
-        <v>19</v>
+        <v>1436</v>
       </c>
       <c r="D5098">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E5098">
-        <v>23</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="5099">
@@ -97240,17 +97240,17 @@
       </c>
       <c r="B5099" t="inlineStr">
         <is>
-          <t>Okres Humenné</t>
+          <t>Okres Detva</t>
         </is>
       </c>
       <c r="C5099">
-        <v>196</v>
+        <v>409</v>
       </c>
       <c r="D5099">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E5099">
-        <v>213</v>
+        <v>435</v>
       </c>
     </row>
     <row r="5100">
@@ -97259,17 +97259,17 @@
       </c>
       <c r="B5100" t="inlineStr">
         <is>
-          <t>Okres Ilava</t>
+          <t>Okres Dolný Kubín</t>
         </is>
       </c>
       <c r="C5100">
-        <v>245</v>
+        <v>474</v>
       </c>
       <c r="D5100">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E5100">
-        <v>260</v>
+        <v>502</v>
       </c>
     </row>
     <row r="5101">
@@ -97278,17 +97278,17 @@
       </c>
       <c r="B5101" t="inlineStr">
         <is>
-          <t>Okres Kežmarok</t>
+          <t>Okres Dunajská Streda</t>
         </is>
       </c>
       <c r="C5101">
-        <v>6</v>
+        <v>1226</v>
       </c>
       <c r="D5101">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="E5101">
-        <v>6</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="5102">
@@ -97297,17 +97297,17 @@
       </c>
       <c r="B5102" t="inlineStr">
         <is>
-          <t>Okres Komárno</t>
+          <t>Okres Galanta</t>
         </is>
       </c>
       <c r="C5102">
-        <v>150</v>
+        <v>671</v>
       </c>
       <c r="D5102">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E5102">
-        <v>163</v>
+        <v>717</v>
       </c>
     </row>
     <row r="5103">
@@ -97316,17 +97316,17 @@
       </c>
       <c r="B5103" t="inlineStr">
         <is>
-          <t>Okres Košice II</t>
+          <t>Okres Gelnica</t>
         </is>
       </c>
       <c r="C5103">
-        <v>58</v>
+        <v>305</v>
       </c>
       <c r="D5103">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E5103">
-        <v>59</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5104">
@@ -97335,17 +97335,17 @@
       </c>
       <c r="B5104" t="inlineStr">
         <is>
-          <t>Okres Kysucké Nové Mesto</t>
+          <t>Okres Hlohovec</t>
         </is>
       </c>
       <c r="C5104">
-        <v>271</v>
+        <v>682</v>
       </c>
       <c r="D5104">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="E5104">
-        <v>289</v>
+        <v>750</v>
       </c>
     </row>
     <row r="5105">
@@ -97354,17 +97354,17 @@
       </c>
       <c r="B5105" t="inlineStr">
         <is>
-          <t>Okres Levice</t>
+          <t>Okres Humenné</t>
         </is>
       </c>
       <c r="C5105">
-        <v>48</v>
+        <v>708</v>
       </c>
       <c r="D5105">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E5105">
-        <v>48</v>
+        <v>761</v>
       </c>
     </row>
     <row r="5106">
@@ -97373,17 +97373,17 @@
       </c>
       <c r="B5106" t="inlineStr">
         <is>
-          <t>Okres Levoča</t>
+          <t>Okres Ilava</t>
         </is>
       </c>
       <c r="C5106">
-        <v>38</v>
+        <v>315</v>
       </c>
       <c r="D5106">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E5106">
-        <v>41</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5107">
@@ -97392,17 +97392,17 @@
       </c>
       <c r="B5107" t="inlineStr">
         <is>
-          <t>Okres Liptovský Mikuláš</t>
+          <t>Okres Kežmarok</t>
         </is>
       </c>
       <c r="C5107">
-        <v>409</v>
+        <v>485</v>
       </c>
       <c r="D5107">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="E5107">
-        <v>420</v>
+        <v>546</v>
       </c>
     </row>
     <row r="5108">
@@ -97411,17 +97411,17 @@
       </c>
       <c r="B5108" t="inlineStr">
         <is>
-          <t>Okres Lučenec</t>
+          <t>Okres Komárno</t>
         </is>
       </c>
       <c r="C5108">
-        <v>132</v>
+        <v>671</v>
       </c>
       <c r="D5108">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="E5108">
-        <v>137</v>
+        <v>720</v>
       </c>
     </row>
     <row r="5109">
@@ -97430,17 +97430,17 @@
       </c>
       <c r="B5109" t="inlineStr">
         <is>
-          <t>Okres Malacky</t>
+          <t>Okres Košice I</t>
         </is>
       </c>
       <c r="C5109">
-        <v>5</v>
+        <v>565</v>
       </c>
       <c r="D5109">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E5109">
-        <v>5</v>
+        <v>588</v>
       </c>
     </row>
     <row r="5110">
@@ -97449,17 +97449,17 @@
       </c>
       <c r="B5110" t="inlineStr">
         <is>
-          <t>Okres Martin</t>
+          <t>Okres Košice II</t>
         </is>
       </c>
       <c r="C5110">
-        <v>4</v>
+        <v>1712</v>
       </c>
       <c r="D5110">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E5110">
-        <v>4</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="5111">
@@ -97468,17 +97468,17 @@
       </c>
       <c r="B5111" t="inlineStr">
         <is>
-          <t>Okres Michalovce</t>
+          <t>Okres Košice IV</t>
         </is>
       </c>
       <c r="C5111">
-        <v>12</v>
+        <v>326</v>
       </c>
       <c r="D5111">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E5111">
-        <v>12</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5112">
@@ -97487,17 +97487,17 @@
       </c>
       <c r="B5112" t="inlineStr">
         <is>
-          <t>Okres Myjava</t>
+          <t>Okres Kysucké Nové Mesto</t>
         </is>
       </c>
       <c r="C5112">
-        <v>34</v>
+        <v>278</v>
       </c>
       <c r="D5112">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E5112">
-        <v>35</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5113">
@@ -97506,17 +97506,17 @@
       </c>
       <c r="B5113" t="inlineStr">
         <is>
-          <t>Okres Nitra</t>
+          <t>Okres Levice</t>
         </is>
       </c>
       <c r="C5113">
-        <v>441</v>
+        <v>14910</v>
       </c>
       <c r="D5113">
-        <v>19</v>
+        <v>528</v>
       </c>
       <c r="E5113">
-        <v>460</v>
+        <v>15438</v>
       </c>
     </row>
     <row r="5114">
@@ -97525,17 +97525,17 @@
       </c>
       <c r="B5114" t="inlineStr">
         <is>
-          <t>Okres Partizánske</t>
+          <t>Okres Levoča</t>
         </is>
       </c>
       <c r="C5114">
-        <v>69</v>
+        <v>265</v>
       </c>
       <c r="D5114">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E5114">
-        <v>87</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5115">
@@ -97544,17 +97544,17 @@
       </c>
       <c r="B5115" t="inlineStr">
         <is>
-          <t>Okres Piešťany</t>
+          <t>Okres Liptovský Mikuláš</t>
         </is>
       </c>
       <c r="C5115">
-        <v>94</v>
+        <v>924</v>
       </c>
       <c r="D5115">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="E5115">
-        <v>100</v>
+        <v>952</v>
       </c>
     </row>
     <row r="5116">
@@ -97563,17 +97563,17 @@
       </c>
       <c r="B5116" t="inlineStr">
         <is>
-          <t>Okres Poprad</t>
+          <t>Okres Lučenec</t>
         </is>
       </c>
       <c r="C5116">
-        <v>350</v>
+        <v>789</v>
       </c>
       <c r="D5116">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5116">
-        <v>366</v>
+        <v>804</v>
       </c>
     </row>
     <row r="5117">
@@ -97582,17 +97582,17 @@
       </c>
       <c r="B5117" t="inlineStr">
         <is>
-          <t>Okres Považská Bystrica</t>
+          <t>Okres Malacky</t>
         </is>
       </c>
       <c r="C5117">
-        <v>71</v>
+        <v>645</v>
       </c>
       <c r="D5117">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E5117">
-        <v>72</v>
+        <v>675</v>
       </c>
     </row>
     <row r="5118">
@@ -97601,17 +97601,17 @@
       </c>
       <c r="B5118" t="inlineStr">
         <is>
-          <t>Okres Prešov</t>
+          <t>Okres Martin</t>
         </is>
       </c>
       <c r="C5118">
-        <v>3</v>
+        <v>1293</v>
       </c>
       <c r="D5118">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E5118">
-        <v>3</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="5119">
@@ -97620,17 +97620,17 @@
       </c>
       <c r="B5119" t="inlineStr">
         <is>
-          <t>Okres Prievidza</t>
+          <t>Okres Medzilaborce</t>
         </is>
       </c>
       <c r="C5119">
-        <v>203</v>
+        <v>234</v>
       </c>
       <c r="D5119">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E5119">
-        <v>212</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5120">
@@ -97639,17 +97639,17 @@
       </c>
       <c r="B5120" t="inlineStr">
         <is>
-          <t>Okres Púchov</t>
+          <t>Okres Michalovce</t>
         </is>
       </c>
       <c r="C5120">
-        <v>1</v>
+        <v>858</v>
       </c>
       <c r="D5120">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E5120">
-        <v>1</v>
+        <v>898</v>
       </c>
     </row>
     <row r="5121">
@@ -97658,17 +97658,17 @@
       </c>
       <c r="B5121" t="inlineStr">
         <is>
-          <t>Okres Revúca</t>
+          <t>Okres Myjava</t>
         </is>
       </c>
       <c r="C5121">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D5121">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5121">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5122">
@@ -97677,17 +97677,17 @@
       </c>
       <c r="B5122" t="inlineStr">
         <is>
-          <t>Okres Rimavská Sobota</t>
+          <t>Okres Námestovo</t>
         </is>
       </c>
       <c r="C5122">
-        <v>533</v>
+        <v>594</v>
       </c>
       <c r="D5122">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E5122">
-        <v>551</v>
+        <v>621</v>
       </c>
     </row>
     <row r="5123">
@@ -97696,17 +97696,17 @@
       </c>
       <c r="B5123" t="inlineStr">
         <is>
-          <t>Okres Rožňava</t>
+          <t>Okres Nitra</t>
         </is>
       </c>
       <c r="C5123">
-        <v>422</v>
+        <v>950</v>
       </c>
       <c r="D5123">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="E5123">
-        <v>429</v>
+        <v>996</v>
       </c>
     </row>
     <row r="5124">
@@ -97715,17 +97715,17 @@
       </c>
       <c r="B5124" t="inlineStr">
         <is>
-          <t>Okres Ružomberok</t>
+          <t>Okres Nové Mesto nad Váhom</t>
         </is>
       </c>
       <c r="C5124">
-        <v>16</v>
+        <v>530</v>
       </c>
       <c r="D5124">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="E5124">
-        <v>17</v>
+        <v>579</v>
       </c>
     </row>
     <row r="5125">
@@ -97734,17 +97734,17 @@
       </c>
       <c r="B5125" t="inlineStr">
         <is>
-          <t>Okres Senica</t>
+          <t>Okres Nové Zámky</t>
         </is>
       </c>
       <c r="C5125">
-        <v>1</v>
+        <v>1186</v>
       </c>
       <c r="D5125">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E5125">
-        <v>1</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="5126">
@@ -97753,17 +97753,17 @@
       </c>
       <c r="B5126" t="inlineStr">
         <is>
-          <t>Okres Skalica</t>
+          <t>Okres Partizánske</t>
         </is>
       </c>
       <c r="C5126">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="D5126">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E5126">
-        <v>15</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5127">
@@ -97772,17 +97772,17 @@
       </c>
       <c r="B5127" t="inlineStr">
         <is>
-          <t>Okres Sobrance</t>
+          <t>Okres Pezinok</t>
         </is>
       </c>
       <c r="C5127">
-        <v>8</v>
+        <v>389</v>
       </c>
       <c r="D5127">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E5127">
-        <v>8</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5128">
@@ -97791,17 +97791,17 @@
       </c>
       <c r="B5128" t="inlineStr">
         <is>
-          <t>Okres Spišská Nová Ves</t>
+          <t>Okres Piešťany</t>
         </is>
       </c>
       <c r="C5128">
-        <v>174</v>
+        <v>610</v>
       </c>
       <c r="D5128">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E5128">
-        <v>174</v>
+        <v>655</v>
       </c>
     </row>
     <row r="5129">
@@ -97810,17 +97810,17 @@
       </c>
       <c r="B5129" t="inlineStr">
         <is>
-          <t>Okres Šaľa</t>
+          <t>Okres Poprad</t>
         </is>
       </c>
       <c r="C5129">
-        <v>12</v>
+        <v>1041</v>
       </c>
       <c r="D5129">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="E5129">
-        <v>15</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="5130">
@@ -97829,17 +97829,17 @@
       </c>
       <c r="B5130" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Považská Bystrica</t>
         </is>
       </c>
       <c r="C5130">
-        <v>499</v>
+        <v>333</v>
       </c>
       <c r="D5130">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5130">
-        <v>522</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5131">
@@ -97848,17 +97848,17 @@
       </c>
       <c r="B5131" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Prešov</t>
         </is>
       </c>
       <c r="C5131">
-        <v>209</v>
+        <v>2474</v>
       </c>
       <c r="D5131">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="E5131">
-        <v>230</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="5132">
@@ -97867,17 +97867,17 @@
       </c>
       <c r="B5132" t="inlineStr">
         <is>
-          <t>Okres Trnava</t>
+          <t>Okres Prievidza</t>
         </is>
       </c>
       <c r="C5132">
-        <v>445</v>
+        <v>591</v>
       </c>
       <c r="D5132">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E5132">
-        <v>487</v>
+        <v>629</v>
       </c>
     </row>
     <row r="5133">
@@ -97886,17 +97886,17 @@
       </c>
       <c r="B5133" t="inlineStr">
         <is>
-          <t>Okres Turčianske Teplice</t>
+          <t>Okres Púchov</t>
         </is>
       </c>
       <c r="C5133">
-        <v>162</v>
+        <v>114</v>
       </c>
       <c r="D5133">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5133">
-        <v>169</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5134">
@@ -97905,17 +97905,17 @@
       </c>
       <c r="B5134" t="inlineStr">
         <is>
-          <t>Okres Tvrdošín</t>
+          <t>Okres Revúca</t>
         </is>
       </c>
       <c r="C5134">
-        <v>51</v>
+        <v>514</v>
       </c>
       <c r="D5134">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E5134">
-        <v>52</v>
+        <v>535</v>
       </c>
     </row>
     <row r="5135">
@@ -97924,17 +97924,17 @@
       </c>
       <c r="B5135" t="inlineStr">
         <is>
-          <t>Okres Veľký Krtíš</t>
+          <t>Okres Rimavská Sobota</t>
         </is>
       </c>
       <c r="C5135">
-        <v>346</v>
+        <v>774</v>
       </c>
       <c r="D5135">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E5135">
-        <v>358</v>
+        <v>801</v>
       </c>
     </row>
     <row r="5136">
@@ -97943,17 +97943,17 @@
       </c>
       <c r="B5136" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Rožňava</t>
         </is>
       </c>
       <c r="C5136">
-        <v>0</v>
+        <v>984</v>
       </c>
       <c r="D5136">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="E5136">
-        <v>0</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="5137">
@@ -97962,17 +97962,17 @@
       </c>
       <c r="B5137" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Ružomberok</t>
         </is>
       </c>
       <c r="C5137">
-        <v>66</v>
+        <v>924</v>
       </c>
       <c r="D5137">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="E5137">
-        <v>69</v>
+        <v>993</v>
       </c>
     </row>
     <row r="5138">
@@ -97981,17 +97981,1556 @@
       </c>
       <c r="B5138" t="inlineStr">
         <is>
+          <t>Okres Sabinov</t>
+        </is>
+      </c>
+      <c r="C5138">
+        <v>665</v>
+      </c>
+      <c r="D5138">
+        <v>45</v>
+      </c>
+      <c r="E5138">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="5139">
+      <c r="A5139" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5139" t="inlineStr">
+        <is>
+          <t>Okres Senec</t>
+        </is>
+      </c>
+      <c r="C5139">
+        <v>446</v>
+      </c>
+      <c r="D5139">
+        <v>28</v>
+      </c>
+      <c r="E5139">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="5140">
+      <c r="A5140" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5140" t="inlineStr">
+        <is>
+          <t>Okres Senica</t>
+        </is>
+      </c>
+      <c r="C5140">
+        <v>241</v>
+      </c>
+      <c r="D5140">
+        <v>13</v>
+      </c>
+      <c r="E5140">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5141">
+      <c r="A5141" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5141" t="inlineStr">
+        <is>
+          <t>Okres Skalica</t>
+        </is>
+      </c>
+      <c r="C5141">
+        <v>19</v>
+      </c>
+      <c r="D5141">
+        <v>2</v>
+      </c>
+      <c r="E5141">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5142">
+      <c r="A5142" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5142" t="inlineStr">
+        <is>
+          <t>Okres Snina</t>
+        </is>
+      </c>
+      <c r="C5142">
+        <v>449</v>
+      </c>
+      <c r="D5142">
+        <v>40</v>
+      </c>
+      <c r="E5142">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="5143">
+      <c r="A5143" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5143" t="inlineStr">
+        <is>
+          <t>Okres Sobrance</t>
+        </is>
+      </c>
+      <c r="C5143">
+        <v>211</v>
+      </c>
+      <c r="D5143">
+        <v>13</v>
+      </c>
+      <c r="E5143">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5144">
+      <c r="A5144" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5144" t="inlineStr">
+        <is>
+          <t>Okres Spišská Nová Ves</t>
+        </is>
+      </c>
+      <c r="C5144">
+        <v>1143</v>
+      </c>
+      <c r="D5144">
+        <v>48</v>
+      </c>
+      <c r="E5144">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="5145">
+      <c r="A5145" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5145" t="inlineStr">
+        <is>
+          <t>Okres Stará Ľubovňa</t>
+        </is>
+      </c>
+      <c r="C5145">
+        <v>59</v>
+      </c>
+      <c r="D5145">
+        <v>4</v>
+      </c>
+      <c r="E5145">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5146">
+      <c r="A5146" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5146" t="inlineStr">
+        <is>
+          <t>Okres Stropkov</t>
+        </is>
+      </c>
+      <c r="C5146">
+        <v>1</v>
+      </c>
+      <c r="D5146">
+        <v>0</v>
+      </c>
+      <c r="E5146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5147">
+      <c r="A5147" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5147" t="inlineStr">
+        <is>
+          <t>Okres Svidník</t>
+        </is>
+      </c>
+      <c r="C5147">
+        <v>170</v>
+      </c>
+      <c r="D5147">
+        <v>21</v>
+      </c>
+      <c r="E5147">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5148">
+      <c r="A5148" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5148" t="inlineStr">
+        <is>
+          <t>Okres Šaľa</t>
+        </is>
+      </c>
+      <c r="C5148">
+        <v>221</v>
+      </c>
+      <c r="D5148">
+        <v>20</v>
+      </c>
+      <c r="E5148">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5149">
+      <c r="A5149" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5149" t="inlineStr">
+        <is>
+          <t>Okres Topoľčany</t>
+        </is>
+      </c>
+      <c r="C5149">
+        <v>733</v>
+      </c>
+      <c r="D5149">
+        <v>88</v>
+      </c>
+      <c r="E5149">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="5150">
+      <c r="A5150" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5150" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C5150">
+        <v>833</v>
+      </c>
+      <c r="D5150">
+        <v>47</v>
+      </c>
+      <c r="E5150">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="5151">
+      <c r="A5151" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5151" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C5151">
+        <v>1267</v>
+      </c>
+      <c r="D5151">
+        <v>89</v>
+      </c>
+      <c r="E5151">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="5152">
+      <c r="A5152" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5152" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C5152">
+        <v>1268</v>
+      </c>
+      <c r="D5152">
+        <v>87</v>
+      </c>
+      <c r="E5152">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="5153">
+      <c r="A5153" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5153" t="inlineStr">
+        <is>
+          <t>Okres Turčianske Teplice</t>
+        </is>
+      </c>
+      <c r="C5153">
+        <v>168</v>
+      </c>
+      <c r="D5153">
+        <v>7</v>
+      </c>
+      <c r="E5153">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5154">
+      <c r="A5154" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5154" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C5154">
+        <v>638</v>
+      </c>
+      <c r="D5154">
+        <v>33</v>
+      </c>
+      <c r="E5154">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="5155">
+      <c r="A5155" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5155" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C5155">
+        <v>346</v>
+      </c>
+      <c r="D5155">
+        <v>9</v>
+      </c>
+      <c r="E5155">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="5156">
+      <c r="A5156" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5156" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C5156">
+        <v>69</v>
+      </c>
+      <c r="D5156">
+        <v>2</v>
+      </c>
+      <c r="E5156">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5157">
+      <c r="A5157" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5157" t="inlineStr">
+        <is>
+          <t>Okres Zlaté Moravce</t>
+        </is>
+      </c>
+      <c r="C5157">
+        <v>223</v>
+      </c>
+      <c r="D5157">
+        <v>13</v>
+      </c>
+      <c r="E5157">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5158">
+      <c r="A5158" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5158" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C5158">
+        <v>736</v>
+      </c>
+      <c r="D5158">
+        <v>31</v>
+      </c>
+      <c r="E5158">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="5159">
+      <c r="A5159" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5159" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C5159">
+        <v>235</v>
+      </c>
+      <c r="D5159">
+        <v>19</v>
+      </c>
+      <c r="E5159">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5160">
+      <c r="A5160" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B5160" t="inlineStr">
+        <is>
           <t>Okres Žilina</t>
         </is>
       </c>
-      <c r="C5138">
-        <v>2072</v>
-      </c>
-      <c r="D5138">
+      <c r="C5160">
+        <v>2433</v>
+      </c>
+      <c r="D5160">
+        <v>95</v>
+      </c>
+      <c r="E5160">
+        <v>2528</v>
+      </c>
+    </row>
+    <row r="5161">
+      <c r="A5161" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5161" t="inlineStr">
+        <is>
+          <t>Okres Banská Bystrica</t>
+        </is>
+      </c>
+      <c r="C5161">
+        <v>1173</v>
+      </c>
+      <c r="D5161">
+        <v>191</v>
+      </c>
+      <c r="E5161">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="5162">
+      <c r="A5162" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5162" t="inlineStr">
+        <is>
+          <t>Okres Banská Štiavnica</t>
+        </is>
+      </c>
+      <c r="C5162">
+        <v>2</v>
+      </c>
+      <c r="D5162">
+        <v>2</v>
+      </c>
+      <c r="E5162">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5163">
+      <c r="A5163" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5163" t="inlineStr">
+        <is>
+          <t>Okres Bardejov</t>
+        </is>
+      </c>
+      <c r="C5163">
+        <v>7</v>
+      </c>
+      <c r="D5163">
+        <v>1</v>
+      </c>
+      <c r="E5163">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5164">
+      <c r="A5164" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5164" t="inlineStr">
+        <is>
+          <t>Okres Bratislava I</t>
+        </is>
+      </c>
+      <c r="C5164">
+        <v>156</v>
+      </c>
+      <c r="D5164">
+        <v>4</v>
+      </c>
+      <c r="E5164">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5165">
+      <c r="A5165" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5165" t="inlineStr">
+        <is>
+          <t>Okres Bratislava II</t>
+        </is>
+      </c>
+      <c r="C5165">
+        <v>2447</v>
+      </c>
+      <c r="D5165">
+        <v>95</v>
+      </c>
+      <c r="E5165">
+        <v>2542</v>
+      </c>
+    </row>
+    <row r="5166">
+      <c r="A5166" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5166" t="inlineStr">
+        <is>
+          <t>Okres Bratislava III</t>
+        </is>
+      </c>
+      <c r="C5166">
+        <v>1830</v>
+      </c>
+      <c r="D5166">
+        <v>53</v>
+      </c>
+      <c r="E5166">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="5167">
+      <c r="A5167" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5167" t="inlineStr">
+        <is>
+          <t>Okres Bratislava IV</t>
+        </is>
+      </c>
+      <c r="C5167">
+        <v>279</v>
+      </c>
+      <c r="D5167">
+        <v>30</v>
+      </c>
+      <c r="E5167">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="5168">
+      <c r="A5168" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5168" t="inlineStr">
+        <is>
+          <t>Okres Bratislava V</t>
+        </is>
+      </c>
+      <c r="C5168">
+        <v>59</v>
+      </c>
+      <c r="D5168">
+        <v>7</v>
+      </c>
+      <c r="E5168">
         <v>66</v>
       </c>
-      <c r="E5138">
-        <v>2138</v>
+    </row>
+    <row r="5169">
+      <c r="A5169" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5169" t="inlineStr">
+        <is>
+          <t>Okres Brezno</t>
+        </is>
+      </c>
+      <c r="C5169">
+        <v>51</v>
+      </c>
+      <c r="D5169">
+        <v>7</v>
+      </c>
+      <c r="E5169">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5170">
+      <c r="A5170" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5170" t="inlineStr">
+        <is>
+          <t>Okres Bytča</t>
+        </is>
+      </c>
+      <c r="C5170">
+        <v>254</v>
+      </c>
+      <c r="D5170">
+        <v>21</v>
+      </c>
+      <c r="E5170">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5171">
+      <c r="A5171" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5171" t="inlineStr">
+        <is>
+          <t>Okres Čadca</t>
+        </is>
+      </c>
+      <c r="C5171">
+        <v>882</v>
+      </c>
+      <c r="D5171">
+        <v>37</v>
+      </c>
+      <c r="E5171">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="5172">
+      <c r="A5172" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5172" t="inlineStr">
+        <is>
+          <t>Okres Dolný Kubín</t>
+        </is>
+      </c>
+      <c r="C5172">
+        <v>702</v>
+      </c>
+      <c r="D5172">
+        <v>29</v>
+      </c>
+      <c r="E5172">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="5173">
+      <c r="A5173" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5173" t="inlineStr">
+        <is>
+          <t>Okres Dunajská Streda</t>
+        </is>
+      </c>
+      <c r="C5173">
+        <v>710</v>
+      </c>
+      <c r="D5173">
+        <v>86</v>
+      </c>
+      <c r="E5173">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="5174">
+      <c r="A5174" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5174" t="inlineStr">
+        <is>
+          <t>Okres Galanta</t>
+        </is>
+      </c>
+      <c r="C5174">
+        <v>682</v>
+      </c>
+      <c r="D5174">
+        <v>60</v>
+      </c>
+      <c r="E5174">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="5175">
+      <c r="A5175" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5175" t="inlineStr">
+        <is>
+          <t>Okres Humenné</t>
+        </is>
+      </c>
+      <c r="C5175">
+        <v>553</v>
+      </c>
+      <c r="D5175">
+        <v>43</v>
+      </c>
+      <c r="E5175">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="5176">
+      <c r="A5176" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5176" t="inlineStr">
+        <is>
+          <t>Okres Ilava</t>
+        </is>
+      </c>
+      <c r="C5176">
+        <v>217</v>
+      </c>
+      <c r="D5176">
+        <v>23</v>
+      </c>
+      <c r="E5176">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5177">
+      <c r="A5177" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5177" t="inlineStr">
+        <is>
+          <t>Okres Kežmarok</t>
+        </is>
+      </c>
+      <c r="C5177">
+        <v>229</v>
+      </c>
+      <c r="D5177">
+        <v>13</v>
+      </c>
+      <c r="E5177">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5178">
+      <c r="A5178" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5178" t="inlineStr">
+        <is>
+          <t>Okres Komárno</t>
+        </is>
+      </c>
+      <c r="C5178">
+        <v>577</v>
+      </c>
+      <c r="D5178">
+        <v>38</v>
+      </c>
+      <c r="E5178">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="5179">
+      <c r="A5179" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5179" t="inlineStr">
+        <is>
+          <t>Okres Košice I</t>
+        </is>
+      </c>
+      <c r="C5179">
+        <v>43</v>
+      </c>
+      <c r="D5179">
+        <v>0</v>
+      </c>
+      <c r="E5179">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5180">
+      <c r="A5180" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5180" t="inlineStr">
+        <is>
+          <t>Okres Košice II</t>
+        </is>
+      </c>
+      <c r="C5180">
+        <v>149</v>
+      </c>
+      <c r="D5180">
+        <v>4</v>
+      </c>
+      <c r="E5180">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5181">
+      <c r="A5181" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5181" t="inlineStr">
+        <is>
+          <t>Okres Košice IV</t>
+        </is>
+      </c>
+      <c r="C5181">
+        <v>265</v>
+      </c>
+      <c r="D5181">
+        <v>4</v>
+      </c>
+      <c r="E5181">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5182">
+      <c r="A5182" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5182" t="inlineStr">
+        <is>
+          <t>Okres Kysucké Nové Mesto</t>
+        </is>
+      </c>
+      <c r="C5182">
+        <v>331</v>
+      </c>
+      <c r="D5182">
+        <v>26</v>
+      </c>
+      <c r="E5182">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="5183">
+      <c r="A5183" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5183" t="inlineStr">
+        <is>
+          <t>Okres Levice</t>
+        </is>
+      </c>
+      <c r="C5183">
+        <v>831</v>
+      </c>
+      <c r="D5183">
+        <v>44</v>
+      </c>
+      <c r="E5183">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="5184">
+      <c r="A5184" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5184" t="inlineStr">
+        <is>
+          <t>Okres Levoča</t>
+        </is>
+      </c>
+      <c r="C5184">
+        <v>251</v>
+      </c>
+      <c r="D5184">
+        <v>7</v>
+      </c>
+      <c r="E5184">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5185">
+      <c r="A5185" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5185" t="inlineStr">
+        <is>
+          <t>Okres Liptovský Mikuláš</t>
+        </is>
+      </c>
+      <c r="C5185">
+        <v>429</v>
+      </c>
+      <c r="D5185">
+        <v>20</v>
+      </c>
+      <c r="E5185">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="5186">
+      <c r="A5186" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5186" t="inlineStr">
+        <is>
+          <t>Okres Lučenec</t>
+        </is>
+      </c>
+      <c r="C5186">
+        <v>427</v>
+      </c>
+      <c r="D5186">
+        <v>21</v>
+      </c>
+      <c r="E5186">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="5187">
+      <c r="A5187" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5187" t="inlineStr">
+        <is>
+          <t>Okres Malacky</t>
+        </is>
+      </c>
+      <c r="C5187">
+        <v>397</v>
+      </c>
+      <c r="D5187">
+        <v>26</v>
+      </c>
+      <c r="E5187">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="5188">
+      <c r="A5188" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5188" t="inlineStr">
+        <is>
+          <t>Okres Martin</t>
+        </is>
+      </c>
+      <c r="C5188">
+        <v>350</v>
+      </c>
+      <c r="D5188">
+        <v>40</v>
+      </c>
+      <c r="E5188">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="5189">
+      <c r="A5189" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5189" t="inlineStr">
+        <is>
+          <t>Okres Michalovce</t>
+        </is>
+      </c>
+      <c r="C5189">
+        <v>263</v>
+      </c>
+      <c r="D5189">
+        <v>4</v>
+      </c>
+      <c r="E5189">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5190">
+      <c r="A5190" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5190" t="inlineStr">
+        <is>
+          <t>Okres Myjava</t>
+        </is>
+      </c>
+      <c r="C5190">
+        <v>271</v>
+      </c>
+      <c r="D5190">
+        <v>12</v>
+      </c>
+      <c r="E5190">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5191">
+      <c r="A5191" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5191" t="inlineStr">
+        <is>
+          <t>Okres Nitra</t>
+        </is>
+      </c>
+      <c r="C5191">
+        <v>132</v>
+      </c>
+      <c r="D5191">
+        <v>14</v>
+      </c>
+      <c r="E5191">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5192">
+      <c r="A5192" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5192" t="inlineStr">
+        <is>
+          <t>Okres Partizánske</t>
+        </is>
+      </c>
+      <c r="C5192">
+        <v>9</v>
+      </c>
+      <c r="D5192">
+        <v>0</v>
+      </c>
+      <c r="E5192">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5193">
+      <c r="A5193" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5193" t="inlineStr">
+        <is>
+          <t>Okres Pezinok</t>
+        </is>
+      </c>
+      <c r="C5193">
+        <v>837</v>
+      </c>
+      <c r="D5193">
+        <v>56</v>
+      </c>
+      <c r="E5193">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="5194">
+      <c r="A5194" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5194" t="inlineStr">
+        <is>
+          <t>Okres Piešťany</t>
+        </is>
+      </c>
+      <c r="C5194">
+        <v>291</v>
+      </c>
+      <c r="D5194">
+        <v>7</v>
+      </c>
+      <c r="E5194">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5195">
+      <c r="A5195" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5195" t="inlineStr">
+        <is>
+          <t>Okres Poprad</t>
+        </is>
+      </c>
+      <c r="C5195">
+        <v>1603</v>
+      </c>
+      <c r="D5195">
+        <v>23</v>
+      </c>
+      <c r="E5195">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="5196">
+      <c r="A5196" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5196" t="inlineStr">
+        <is>
+          <t>Okres Prešov</t>
+        </is>
+      </c>
+      <c r="C5196">
+        <v>135</v>
+      </c>
+      <c r="D5196">
+        <v>9</v>
+      </c>
+      <c r="E5196">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5197">
+      <c r="A5197" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5197" t="inlineStr">
+        <is>
+          <t>Okres Prievidza</t>
+        </is>
+      </c>
+      <c r="C5197">
+        <v>483</v>
+      </c>
+      <c r="D5197">
+        <v>15</v>
+      </c>
+      <c r="E5197">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="5198">
+      <c r="A5198" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5198" t="inlineStr">
+        <is>
+          <t>Okres Púchov</t>
+        </is>
+      </c>
+      <c r="C5198">
+        <v>1</v>
+      </c>
+      <c r="D5198">
+        <v>0</v>
+      </c>
+      <c r="E5198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5199">
+      <c r="A5199" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5199" t="inlineStr">
+        <is>
+          <t>Okres Revúca</t>
+        </is>
+      </c>
+      <c r="C5199">
+        <v>623</v>
+      </c>
+      <c r="D5199">
+        <v>36</v>
+      </c>
+      <c r="E5199">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="5200">
+      <c r="A5200" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5200" t="inlineStr">
+        <is>
+          <t>Okres Rimavská Sobota</t>
+        </is>
+      </c>
+      <c r="C5200">
+        <v>375</v>
+      </c>
+      <c r="D5200">
+        <v>13</v>
+      </c>
+      <c r="E5200">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="5201">
+      <c r="A5201" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5201" t="inlineStr">
+        <is>
+          <t>Okres Ružomberok</t>
+        </is>
+      </c>
+      <c r="C5201">
+        <v>978</v>
+      </c>
+      <c r="D5201">
+        <v>10</v>
+      </c>
+      <c r="E5201">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="5202">
+      <c r="A5202" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5202" t="inlineStr">
+        <is>
+          <t>Okres Senec</t>
+        </is>
+      </c>
+      <c r="C5202">
+        <v>450</v>
+      </c>
+      <c r="D5202">
+        <v>28</v>
+      </c>
+      <c r="E5202">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="5203">
+      <c r="A5203" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5203" t="inlineStr">
+        <is>
+          <t>Okres Senica</t>
+        </is>
+      </c>
+      <c r="C5203">
+        <v>25</v>
+      </c>
+      <c r="D5203">
+        <v>1</v>
+      </c>
+      <c r="E5203">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5204">
+      <c r="A5204" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5204" t="inlineStr">
+        <is>
+          <t>Okres Skalica</t>
+        </is>
+      </c>
+      <c r="C5204">
+        <v>399</v>
+      </c>
+      <c r="D5204">
+        <v>16</v>
+      </c>
+      <c r="E5204">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="5205">
+      <c r="A5205" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5205" t="inlineStr">
+        <is>
+          <t>Okres Snina</t>
+        </is>
+      </c>
+      <c r="C5205">
+        <v>44</v>
+      </c>
+      <c r="D5205">
+        <v>5</v>
+      </c>
+      <c r="E5205">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5206">
+      <c r="A5206" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5206" t="inlineStr">
+        <is>
+          <t>Okres Sobrance</t>
+        </is>
+      </c>
+      <c r="C5206">
+        <v>150</v>
+      </c>
+      <c r="D5206">
+        <v>12</v>
+      </c>
+      <c r="E5206">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5207">
+      <c r="A5207" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5207" t="inlineStr">
+        <is>
+          <t>Okres Spišská Nová Ves</t>
+        </is>
+      </c>
+      <c r="C5207">
+        <v>166</v>
+      </c>
+      <c r="D5207">
+        <v>5</v>
+      </c>
+      <c r="E5207">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5208">
+      <c r="A5208" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5208" t="inlineStr">
+        <is>
+          <t>Okres Stará Ľubovňa</t>
+        </is>
+      </c>
+      <c r="C5208">
+        <v>290</v>
+      </c>
+      <c r="D5208">
+        <v>40</v>
+      </c>
+      <c r="E5208">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5209">
+      <c r="A5209" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5209" t="inlineStr">
+        <is>
+          <t>Okres Topoľčany</t>
+        </is>
+      </c>
+      <c r="C5209">
+        <v>241</v>
+      </c>
+      <c r="D5209">
+        <v>30</v>
+      </c>
+      <c r="E5209">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5210">
+      <c r="A5210" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5210" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C5210">
+        <v>564</v>
+      </c>
+      <c r="D5210">
+        <v>47</v>
+      </c>
+      <c r="E5210">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="5211">
+      <c r="A5211" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5211" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C5211">
+        <v>750</v>
+      </c>
+      <c r="D5211">
+        <v>12</v>
+      </c>
+      <c r="E5211">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="5212">
+      <c r="A5212" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5212" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C5212">
+        <v>676</v>
+      </c>
+      <c r="D5212">
+        <v>27</v>
+      </c>
+      <c r="E5212">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="5213">
+      <c r="A5213" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5213" t="inlineStr">
+        <is>
+          <t>Okres Turčianske Teplice</t>
+        </is>
+      </c>
+      <c r="C5213">
+        <v>149</v>
+      </c>
+      <c r="D5213">
+        <v>12</v>
+      </c>
+      <c r="E5213">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5214">
+      <c r="A5214" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5214" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C5214">
+        <v>33</v>
+      </c>
+      <c r="D5214">
+        <v>1</v>
+      </c>
+      <c r="E5214">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5215">
+      <c r="A5215" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5215" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C5215">
+        <v>527</v>
+      </c>
+      <c r="D5215">
+        <v>14</v>
+      </c>
+      <c r="E5215">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="5216">
+      <c r="A5216" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5216" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C5216">
+        <v>333</v>
+      </c>
+      <c r="D5216">
+        <v>22</v>
+      </c>
+      <c r="E5216">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="5217">
+      <c r="A5217" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5217" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C5217">
+        <v>172</v>
+      </c>
+      <c r="D5217">
+        <v>7</v>
+      </c>
+      <c r="E5217">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5218">
+      <c r="A5218" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5218" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C5218">
+        <v>304</v>
+      </c>
+      <c r="D5218">
+        <v>21</v>
+      </c>
+      <c r="E5218">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5219">
+      <c r="A5219" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B5219" t="inlineStr">
+        <is>
+          <t>Okres Žilina</t>
+        </is>
+      </c>
+      <c r="C5219">
+        <v>858</v>
+      </c>
+      <c r="D5219">
+        <v>54</v>
+      </c>
+      <c r="E5219">
+        <v>912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: št 14. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_AgTests_District.xlsx
+++ b/OpenData_Slovakia_Covid_AgTests_District.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5306"/>
+  <dimension ref="A1:E5381"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -68763,13 +68763,13 @@
         </is>
       </c>
       <c r="C3600">
-        <v>6</v>
+        <v>229</v>
       </c>
       <c r="D3600">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E3600">
-        <v>7</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3601">
@@ -73988,13 +73988,13 @@
         </is>
       </c>
       <c r="C3875">
-        <v>835</v>
+        <v>1002</v>
       </c>
       <c r="D3875">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E3875">
-        <v>867</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="3876">
@@ -75451,13 +75451,13 @@
         </is>
       </c>
       <c r="C3952">
-        <v>635</v>
+        <v>794</v>
       </c>
       <c r="D3952">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E3952">
-        <v>673</v>
+        <v>837</v>
       </c>
     </row>
     <row r="3953">
@@ -80144,13 +80144,13 @@
         </is>
       </c>
       <c r="C4199">
-        <v>1925</v>
+        <v>2053</v>
       </c>
       <c r="D4199">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="E4199">
-        <v>2226</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="4200">
@@ -80638,13 +80638,13 @@
         </is>
       </c>
       <c r="C4225">
-        <v>749</v>
+        <v>1007</v>
       </c>
       <c r="D4225">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="E4225">
-        <v>853</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="4226">
@@ -82101,13 +82101,13 @@
         </is>
       </c>
       <c r="C4302">
-        <v>643</v>
+        <v>789</v>
       </c>
       <c r="D4302">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="E4302">
-        <v>701</v>
+        <v>873</v>
       </c>
     </row>
     <row r="4303">
@@ -83564,13 +83564,13 @@
         </is>
       </c>
       <c r="C4379">
-        <v>654</v>
+        <v>815</v>
       </c>
       <c r="D4379">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="E4379">
-        <v>718</v>
+        <v>904</v>
       </c>
     </row>
     <row r="4380">
@@ -85027,13 +85027,13 @@
         </is>
       </c>
       <c r="C4456">
-        <v>656</v>
+        <v>928</v>
       </c>
       <c r="D4456">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="E4456">
-        <v>716</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="4457">
@@ -89264,13 +89264,13 @@
         </is>
       </c>
       <c r="C4679">
-        <v>537</v>
+        <v>807</v>
       </c>
       <c r="D4679">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="E4679">
-        <v>601</v>
+        <v>894</v>
       </c>
     </row>
     <row r="4680">
@@ -90727,13 +90727,13 @@
         </is>
       </c>
       <c r="C4756">
-        <v>880</v>
+        <v>1065</v>
       </c>
       <c r="D4756">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="E4756">
-        <v>983</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="4757">
@@ -93178,13 +93178,13 @@
         </is>
       </c>
       <c r="C4885">
-        <v>959</v>
+        <v>1209</v>
       </c>
       <c r="D4885">
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="E4885">
-        <v>1080</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="4886">
@@ -94337,13 +94337,13 @@
         </is>
       </c>
       <c r="C4946">
-        <v>5295</v>
+        <v>5681</v>
       </c>
       <c r="D4946">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="E4946">
-        <v>5446</v>
+        <v>5846</v>
       </c>
     </row>
     <row r="4947">
@@ -94641,13 +94641,13 @@
         </is>
       </c>
       <c r="C4962">
-        <v>597</v>
+        <v>718</v>
       </c>
       <c r="D4962">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E4962">
-        <v>630</v>
+        <v>766</v>
       </c>
     </row>
     <row r="4963">
@@ -95363,13 +95363,13 @@
         </is>
       </c>
       <c r="C5000">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D5000">
         <v>0</v>
       </c>
       <c r="E5000">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5001">
@@ -95629,13 +95629,13 @@
         </is>
       </c>
       <c r="C5014">
-        <v>2477</v>
+        <v>7653</v>
       </c>
       <c r="D5014">
-        <v>80</v>
+        <v>231</v>
       </c>
       <c r="E5014">
-        <v>2557</v>
+        <v>7884</v>
       </c>
     </row>
     <row r="5015">
@@ -96579,13 +96579,13 @@
         </is>
       </c>
       <c r="C5064">
-        <v>28103</v>
+        <v>30683</v>
       </c>
       <c r="D5064">
-        <v>738</v>
+        <v>833</v>
       </c>
       <c r="E5064">
-        <v>28841</v>
+        <v>31516</v>
       </c>
     </row>
     <row r="5065">
@@ -97092,13 +97092,13 @@
         </is>
       </c>
       <c r="C5091">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="D5091">
         <v>35</v>
       </c>
       <c r="E5091">
-        <v>669</v>
+        <v>672</v>
       </c>
     </row>
     <row r="5092">
@@ -97187,13 +97187,13 @@
         </is>
       </c>
       <c r="C5096">
-        <v>782</v>
+        <v>813</v>
       </c>
       <c r="D5096">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="E5096">
-        <v>842</v>
+        <v>885</v>
       </c>
     </row>
     <row r="5097">
@@ -98061,13 +98061,13 @@
         </is>
       </c>
       <c r="C5142">
-        <v>665</v>
+        <v>896</v>
       </c>
       <c r="D5142">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="E5142">
-        <v>710</v>
+        <v>955</v>
       </c>
     </row>
     <row r="5143">
@@ -98631,13 +98631,13 @@
         </is>
       </c>
       <c r="C5172">
-        <v>2773</v>
+        <v>3119</v>
       </c>
       <c r="D5172">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="E5172">
-        <v>2884</v>
+        <v>3247</v>
       </c>
     </row>
     <row r="5173">
@@ -99011,13 +99011,13 @@
         </is>
       </c>
       <c r="C5192">
-        <v>2</v>
+        <v>212</v>
       </c>
       <c r="D5192">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E5192">
-        <v>3</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5193">
@@ -99049,13 +99049,13 @@
         </is>
       </c>
       <c r="C5194">
-        <v>3224</v>
+        <v>3436</v>
       </c>
       <c r="D5194">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="E5194">
-        <v>3420</v>
+        <v>3651</v>
       </c>
     </row>
     <row r="5195">
@@ -99182,13 +99182,13 @@
         </is>
       </c>
       <c r="C5201">
-        <v>1322</v>
+        <v>1324</v>
       </c>
       <c r="D5201">
         <v>30</v>
       </c>
       <c r="E5201">
-        <v>1352</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="5202">
@@ -99353,13 +99353,13 @@
         </is>
       </c>
       <c r="C5210">
-        <v>2150</v>
+        <v>2250</v>
       </c>
       <c r="D5210">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E5210">
-        <v>2186</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="5211">
@@ -99524,13 +99524,13 @@
         </is>
       </c>
       <c r="C5219">
-        <v>424</v>
+        <v>537</v>
       </c>
       <c r="D5219">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E5219">
-        <v>444</v>
+        <v>567</v>
       </c>
     </row>
     <row r="5220">
@@ -99885,13 +99885,13 @@
         </is>
       </c>
       <c r="C5238">
-        <v>180</v>
+        <v>435</v>
       </c>
       <c r="D5238">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E5238">
-        <v>191</v>
+        <v>462</v>
       </c>
     </row>
     <row r="5239">
@@ -99923,13 +99923,13 @@
         </is>
       </c>
       <c r="C5240">
-        <v>14</v>
+        <v>323</v>
       </c>
       <c r="D5240">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E5240">
-        <v>15</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5241">
@@ -99976,17 +99976,17 @@
       </c>
       <c r="B5243" t="inlineStr">
         <is>
-          <t>Okres Banská Bystrica</t>
+          <t>Okres Bánovce nad Bebravou</t>
         </is>
       </c>
       <c r="C5243">
-        <v>988</v>
+        <v>142</v>
       </c>
       <c r="D5243">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E5243">
-        <v>1016</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5244">
@@ -99995,17 +99995,17 @@
       </c>
       <c r="B5244" t="inlineStr">
         <is>
-          <t>Okres Banská Štiavnica</t>
+          <t>Okres Banská Bystrica</t>
         </is>
       </c>
       <c r="C5244">
-        <v>7</v>
+        <v>1150</v>
       </c>
       <c r="D5244">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E5244">
-        <v>8</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="5245">
@@ -100014,17 +100014,17 @@
       </c>
       <c r="B5245" t="inlineStr">
         <is>
-          <t>Okres Bardejov</t>
+          <t>Okres Banská Štiavnica</t>
         </is>
       </c>
       <c r="C5245">
-        <v>42</v>
+        <v>259</v>
       </c>
       <c r="D5245">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E5245">
-        <v>42</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5246">
@@ -100033,17 +100033,17 @@
       </c>
       <c r="B5246" t="inlineStr">
         <is>
-          <t>Okres Bratislava I</t>
+          <t>Okres Bardejov</t>
         </is>
       </c>
       <c r="C5246">
-        <v>65</v>
+        <v>699</v>
       </c>
       <c r="D5246">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E5246">
-        <v>68</v>
+        <v>712</v>
       </c>
     </row>
     <row r="5247">
@@ -100052,17 +100052,17 @@
       </c>
       <c r="B5247" t="inlineStr">
         <is>
-          <t>Okres Bratislava II</t>
+          <t>Okres Bratislava I</t>
         </is>
       </c>
       <c r="C5247">
-        <v>1711</v>
+        <v>851</v>
       </c>
       <c r="D5247">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="E5247">
-        <v>1778</v>
+        <v>988</v>
       </c>
     </row>
     <row r="5248">
@@ -100071,17 +100071,17 @@
       </c>
       <c r="B5248" t="inlineStr">
         <is>
-          <t>Okres Bratislava III</t>
+          <t>Okres Bratislava II</t>
         </is>
       </c>
       <c r="C5248">
-        <v>663</v>
+        <v>2275</v>
       </c>
       <c r="D5248">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="E5248">
-        <v>671</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="5249">
@@ -100090,17 +100090,17 @@
       </c>
       <c r="B5249" t="inlineStr">
         <is>
-          <t>Okres Bratislava IV</t>
+          <t>Okres Bratislava III</t>
         </is>
       </c>
       <c r="C5249">
-        <v>246</v>
+        <v>11670</v>
       </c>
       <c r="D5249">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="E5249">
-        <v>264</v>
+        <v>11800</v>
       </c>
     </row>
     <row r="5250">
@@ -100109,17 +100109,17 @@
       </c>
       <c r="B5250" t="inlineStr">
         <is>
-          <t>Okres Bratislava V</t>
+          <t>Okres Bratislava IV</t>
         </is>
       </c>
       <c r="C5250">
-        <v>130</v>
+        <v>463</v>
       </c>
       <c r="D5250">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E5250">
-        <v>140</v>
+        <v>496</v>
       </c>
     </row>
     <row r="5251">
@@ -100128,17 +100128,17 @@
       </c>
       <c r="B5251" t="inlineStr">
         <is>
-          <t>Okres Brezno</t>
+          <t>Okres Bratislava V</t>
         </is>
       </c>
       <c r="C5251">
-        <v>3</v>
+        <v>480</v>
       </c>
       <c r="D5251">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E5251">
-        <v>3</v>
+        <v>499</v>
       </c>
     </row>
     <row r="5252">
@@ -100147,17 +100147,17 @@
       </c>
       <c r="B5252" t="inlineStr">
         <is>
-          <t>Okres Bytča</t>
+          <t>Okres Brezno</t>
         </is>
       </c>
       <c r="C5252">
-        <v>153</v>
+        <v>270</v>
       </c>
       <c r="D5252">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E5252">
-        <v>162</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5253">
@@ -100166,17 +100166,17 @@
       </c>
       <c r="B5253" t="inlineStr">
         <is>
-          <t>Okres Čadca</t>
+          <t>Okres Bytča</t>
         </is>
       </c>
       <c r="C5253">
-        <v>661</v>
+        <v>153</v>
       </c>
       <c r="D5253">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E5253">
-        <v>676</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5254">
@@ -100185,17 +100185,17 @@
       </c>
       <c r="B5254" t="inlineStr">
         <is>
-          <t>Okres Detva</t>
+          <t>Okres Čadca</t>
         </is>
       </c>
       <c r="C5254">
-        <v>11</v>
+        <v>1099</v>
       </c>
       <c r="D5254">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E5254">
-        <v>13</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="5255">
@@ -100204,17 +100204,17 @@
       </c>
       <c r="B5255" t="inlineStr">
         <is>
-          <t>Okres Dolný Kubín</t>
+          <t>Okres Detva</t>
         </is>
       </c>
       <c r="C5255">
-        <v>102</v>
+        <v>254</v>
       </c>
       <c r="D5255">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E5255">
-        <v>104</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5256">
@@ -100223,17 +100223,17 @@
       </c>
       <c r="B5256" t="inlineStr">
         <is>
-          <t>Okres Dunajská Streda</t>
+          <t>Okres Dolný Kubín</t>
         </is>
       </c>
       <c r="C5256">
-        <v>504</v>
+        <v>145</v>
       </c>
       <c r="D5256">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="E5256">
-        <v>566</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5257">
@@ -100242,17 +100242,17 @@
       </c>
       <c r="B5257" t="inlineStr">
         <is>
-          <t>Okres Galanta</t>
+          <t>Okres Dunajská Streda</t>
         </is>
       </c>
       <c r="C5257">
-        <v>500</v>
+        <v>1013</v>
       </c>
       <c r="D5257">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="E5257">
-        <v>571</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="5258">
@@ -100261,17 +100261,17 @@
       </c>
       <c r="B5258" t="inlineStr">
         <is>
-          <t>Okres Humenné</t>
+          <t>Okres Galanta</t>
         </is>
       </c>
       <c r="C5258">
-        <v>148</v>
+        <v>864</v>
       </c>
       <c r="D5258">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="E5258">
-        <v>156</v>
+        <v>972</v>
       </c>
     </row>
     <row r="5259">
@@ -100280,17 +100280,17 @@
       </c>
       <c r="B5259" t="inlineStr">
         <is>
-          <t>Okres Ilava</t>
+          <t>Okres Gelnica</t>
         </is>
       </c>
       <c r="C5259">
-        <v>167</v>
+        <v>204</v>
       </c>
       <c r="D5259">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E5259">
-        <v>172</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5260">
@@ -100299,17 +100299,17 @@
       </c>
       <c r="B5260" t="inlineStr">
         <is>
-          <t>Okres Kežmarok</t>
+          <t>Okres Hlohovec</t>
         </is>
       </c>
       <c r="C5260">
-        <v>108</v>
+        <v>296</v>
       </c>
       <c r="D5260">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E5260">
-        <v>119</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5261">
@@ -100318,17 +100318,17 @@
       </c>
       <c r="B5261" t="inlineStr">
         <is>
-          <t>Okres Komárno</t>
+          <t>Okres Humenné</t>
         </is>
       </c>
       <c r="C5261">
-        <v>90</v>
+        <v>596</v>
       </c>
       <c r="D5261">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E5261">
-        <v>92</v>
+        <v>624</v>
       </c>
     </row>
     <row r="5262">
@@ -100337,17 +100337,17 @@
       </c>
       <c r="B5262" t="inlineStr">
         <is>
-          <t>Okres Košice II</t>
+          <t>Okres Ilava</t>
         </is>
       </c>
       <c r="C5262">
-        <v>85</v>
+        <v>208</v>
       </c>
       <c r="D5262">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E5262">
-        <v>85</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5263">
@@ -100356,17 +100356,17 @@
       </c>
       <c r="B5263" t="inlineStr">
         <is>
-          <t>Okres Košice IV</t>
+          <t>Okres Kežmarok</t>
         </is>
       </c>
       <c r="C5263">
-        <v>185</v>
+        <v>379</v>
       </c>
       <c r="D5263">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E5263">
-        <v>187</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5264">
@@ -100375,17 +100375,17 @@
       </c>
       <c r="B5264" t="inlineStr">
         <is>
-          <t>Okres Kysucké Nové Mesto</t>
+          <t>Okres Komárno</t>
         </is>
       </c>
       <c r="C5264">
-        <v>202</v>
+        <v>1104</v>
       </c>
       <c r="D5264">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E5264">
-        <v>216</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="5265">
@@ -100394,17 +100394,17 @@
       </c>
       <c r="B5265" t="inlineStr">
         <is>
-          <t>Okres Levice</t>
+          <t>Okres Košice I</t>
         </is>
       </c>
       <c r="C5265">
-        <v>186</v>
+        <v>349</v>
       </c>
       <c r="D5265">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E5265">
-        <v>195</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5266">
@@ -100413,17 +100413,17 @@
       </c>
       <c r="B5266" t="inlineStr">
         <is>
-          <t>Okres Levoča</t>
+          <t>Okres Košice II</t>
         </is>
       </c>
       <c r="C5266">
-        <v>132</v>
+        <v>450</v>
       </c>
       <c r="D5266">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E5266">
-        <v>136</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5267">
@@ -100432,17 +100432,17 @@
       </c>
       <c r="B5267" t="inlineStr">
         <is>
-          <t>Okres Liptovský Mikuláš</t>
+          <t>Okres Košice III</t>
         </is>
       </c>
       <c r="C5267">
-        <v>6070</v>
+        <v>3</v>
       </c>
       <c r="D5267">
-        <v>351</v>
+        <v>0</v>
       </c>
       <c r="E5267">
-        <v>6421</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5268">
@@ -100451,17 +100451,17 @@
       </c>
       <c r="B5268" t="inlineStr">
         <is>
-          <t>Okres Lučenec</t>
+          <t>Okres Košice IV</t>
         </is>
       </c>
       <c r="C5268">
-        <v>271</v>
+        <v>624</v>
       </c>
       <c r="D5268">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E5268">
-        <v>278</v>
+        <v>644</v>
       </c>
     </row>
     <row r="5269">
@@ -100470,17 +100470,17 @@
       </c>
       <c r="B5269" t="inlineStr">
         <is>
-          <t>Okres Malacky</t>
+          <t>Okres Kysucké Nové Mesto</t>
         </is>
       </c>
       <c r="C5269">
-        <v>246</v>
+        <v>202</v>
       </c>
       <c r="D5269">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E5269">
-        <v>257</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5270">
@@ -100489,17 +100489,17 @@
       </c>
       <c r="B5270" t="inlineStr">
         <is>
-          <t>Okres Martin</t>
+          <t>Okres Levice</t>
         </is>
       </c>
       <c r="C5270">
-        <v>246</v>
+        <v>1861</v>
       </c>
       <c r="D5270">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="E5270">
-        <v>247</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="5271">
@@ -100508,17 +100508,17 @@
       </c>
       <c r="B5271" t="inlineStr">
         <is>
-          <t>Okres Michalovce</t>
+          <t>Okres Levoča</t>
         </is>
       </c>
       <c r="C5271">
-        <v>345</v>
+        <v>225</v>
       </c>
       <c r="D5271">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E5271">
-        <v>351</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5272">
@@ -100527,17 +100527,17 @@
       </c>
       <c r="B5272" t="inlineStr">
         <is>
-          <t>Okres Myjava</t>
+          <t>Okres Liptovský Mikuláš</t>
         </is>
       </c>
       <c r="C5272">
-        <v>157</v>
+        <v>6339</v>
       </c>
       <c r="D5272">
-        <v>6</v>
+        <v>358</v>
       </c>
       <c r="E5272">
-        <v>163</v>
+        <v>6697</v>
       </c>
     </row>
     <row r="5273">
@@ -100546,17 +100546,17 @@
       </c>
       <c r="B5273" t="inlineStr">
         <is>
-          <t>Okres Nitra</t>
+          <t>Okres Lučenec</t>
         </is>
       </c>
       <c r="C5273">
-        <v>135</v>
+        <v>1017</v>
       </c>
       <c r="D5273">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E5273">
-        <v>152</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="5274">
@@ -100565,17 +100565,17 @@
       </c>
       <c r="B5274" t="inlineStr">
         <is>
-          <t>Okres Nové Mesto nad Váhom</t>
+          <t>Okres Malacky</t>
         </is>
       </c>
       <c r="C5274">
-        <v>81</v>
+        <v>586</v>
       </c>
       <c r="D5274">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="E5274">
-        <v>82</v>
+        <v>626</v>
       </c>
     </row>
     <row r="5275">
@@ -100584,17 +100584,17 @@
       </c>
       <c r="B5275" t="inlineStr">
         <is>
-          <t>Okres Partizánske</t>
+          <t>Okres Martin</t>
         </is>
       </c>
       <c r="C5275">
-        <v>337</v>
+        <v>823</v>
       </c>
       <c r="D5275">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="E5275">
-        <v>383</v>
+        <v>838</v>
       </c>
     </row>
     <row r="5276">
@@ -100603,17 +100603,17 @@
       </c>
       <c r="B5276" t="inlineStr">
         <is>
-          <t>Okres Pezinok</t>
+          <t>Okres Medzilaborce</t>
         </is>
       </c>
       <c r="C5276">
-        <v>480</v>
+        <v>103</v>
       </c>
       <c r="D5276">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E5276">
-        <v>496</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5277">
@@ -100622,17 +100622,17 @@
       </c>
       <c r="B5277" t="inlineStr">
         <is>
-          <t>Okres Poprad</t>
+          <t>Okres Michalovce</t>
         </is>
       </c>
       <c r="C5277">
-        <v>168</v>
+        <v>829</v>
       </c>
       <c r="D5277">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E5277">
-        <v>170</v>
+        <v>856</v>
       </c>
     </row>
     <row r="5278">
@@ -100641,17 +100641,17 @@
       </c>
       <c r="B5278" t="inlineStr">
         <is>
-          <t>Okres Považská Bystrica</t>
+          <t>Okres Myjava</t>
         </is>
       </c>
       <c r="C5278">
-        <v>542</v>
+        <v>162</v>
       </c>
       <c r="D5278">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="E5278">
-        <v>574</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5279">
@@ -100660,17 +100660,17 @@
       </c>
       <c r="B5279" t="inlineStr">
         <is>
-          <t>Okres Prešov</t>
+          <t>Okres Námestovo</t>
         </is>
       </c>
       <c r="C5279">
-        <v>138</v>
+        <v>189</v>
       </c>
       <c r="D5279">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E5279">
-        <v>143</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5280">
@@ -100679,17 +100679,17 @@
       </c>
       <c r="B5280" t="inlineStr">
         <is>
-          <t>Okres Prievidza</t>
+          <t>Okres Nitra</t>
         </is>
       </c>
       <c r="C5280">
-        <v>16</v>
+        <v>438</v>
       </c>
       <c r="D5280">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E5280">
-        <v>16</v>
+        <v>483</v>
       </c>
     </row>
     <row r="5281">
@@ -100698,17 +100698,17 @@
       </c>
       <c r="B5281" t="inlineStr">
         <is>
-          <t>Okres Púchov</t>
+          <t>Okres Nové Mesto nad Váhom</t>
         </is>
       </c>
       <c r="C5281">
-        <v>4</v>
+        <v>510</v>
       </c>
       <c r="D5281">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E5281">
-        <v>4</v>
+        <v>533</v>
       </c>
     </row>
     <row r="5282">
@@ -100717,17 +100717,17 @@
       </c>
       <c r="B5282" t="inlineStr">
         <is>
-          <t>Okres Revúca</t>
+          <t>Okres Nové Zámky</t>
         </is>
       </c>
       <c r="C5282">
-        <v>438</v>
+        <v>2668</v>
       </c>
       <c r="D5282">
-        <v>18</v>
+        <v>355</v>
       </c>
       <c r="E5282">
-        <v>456</v>
+        <v>3023</v>
       </c>
     </row>
     <row r="5283">
@@ -100736,17 +100736,17 @@
       </c>
       <c r="B5283" t="inlineStr">
         <is>
-          <t>Okres Rimavská Sobota</t>
+          <t>Okres Partizánske</t>
         </is>
       </c>
       <c r="C5283">
-        <v>236</v>
+        <v>357</v>
       </c>
       <c r="D5283">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="E5283">
-        <v>243</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5284">
@@ -100755,17 +100755,17 @@
       </c>
       <c r="B5284" t="inlineStr">
         <is>
-          <t>Okres Rožňava</t>
+          <t>Okres Pezinok</t>
         </is>
       </c>
       <c r="C5284">
-        <v>217</v>
+        <v>788</v>
       </c>
       <c r="D5284">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E5284">
-        <v>226</v>
+        <v>817</v>
       </c>
     </row>
     <row r="5285">
@@ -100774,17 +100774,17 @@
       </c>
       <c r="B5285" t="inlineStr">
         <is>
-          <t>Okres Ružomberok</t>
+          <t>Okres Piešťany</t>
         </is>
       </c>
       <c r="C5285">
-        <v>91</v>
+        <v>627</v>
       </c>
       <c r="D5285">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E5285">
-        <v>94</v>
+        <v>654</v>
       </c>
     </row>
     <row r="5286">
@@ -100793,17 +100793,17 @@
       </c>
       <c r="B5286" t="inlineStr">
         <is>
-          <t>Okres Senec</t>
+          <t>Okres Poprad</t>
         </is>
       </c>
       <c r="C5286">
-        <v>335</v>
+        <v>808</v>
       </c>
       <c r="D5286">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5286">
-        <v>352</v>
+        <v>824</v>
       </c>
     </row>
     <row r="5287">
@@ -100812,17 +100812,17 @@
       </c>
       <c r="B5287" t="inlineStr">
         <is>
-          <t>Okres Senica</t>
+          <t>Okres Považská Bystrica</t>
         </is>
       </c>
       <c r="C5287">
-        <v>6</v>
+        <v>662</v>
       </c>
       <c r="D5287">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="E5287">
-        <v>7</v>
+        <v>701</v>
       </c>
     </row>
     <row r="5288">
@@ -100831,17 +100831,17 @@
       </c>
       <c r="B5288" t="inlineStr">
         <is>
-          <t>Okres Skalica</t>
+          <t>Okres Prešov</t>
         </is>
       </c>
       <c r="C5288">
-        <v>378</v>
+        <v>1215</v>
       </c>
       <c r="D5288">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="E5288">
-        <v>385</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="5289">
@@ -100850,17 +100850,17 @@
       </c>
       <c r="B5289" t="inlineStr">
         <is>
-          <t>Okres Sobrance</t>
+          <t>Okres Prievidza</t>
         </is>
       </c>
       <c r="C5289">
-        <v>60</v>
+        <v>844</v>
       </c>
       <c r="D5289">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E5289">
-        <v>64</v>
+        <v>888</v>
       </c>
     </row>
     <row r="5290">
@@ -100869,17 +100869,17 @@
       </c>
       <c r="B5290" t="inlineStr">
         <is>
-          <t>Okres Spišská Nová Ves</t>
+          <t>Okres Púchov</t>
         </is>
       </c>
       <c r="C5290">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="D5290">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E5290">
-        <v>77</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5291">
@@ -100888,17 +100888,17 @@
       </c>
       <c r="B5291" t="inlineStr">
         <is>
-          <t>Okres Stará Ľubovňa</t>
+          <t>Okres Revúca</t>
         </is>
       </c>
       <c r="C5291">
-        <v>153</v>
+        <v>638</v>
       </c>
       <c r="D5291">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E5291">
-        <v>164</v>
+        <v>669</v>
       </c>
     </row>
     <row r="5292">
@@ -100907,17 +100907,17 @@
       </c>
       <c r="B5292" t="inlineStr">
         <is>
-          <t>Okres Stropkov</t>
+          <t>Okres Rimavská Sobota</t>
         </is>
       </c>
       <c r="C5292">
-        <v>6</v>
+        <v>362</v>
       </c>
       <c r="D5292">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E5292">
-        <v>6</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5293">
@@ -100926,17 +100926,17 @@
       </c>
       <c r="B5293" t="inlineStr">
         <is>
-          <t>Okres Svidník</t>
+          <t>Okres Rožňava</t>
         </is>
       </c>
       <c r="C5293">
-        <v>39</v>
+        <v>778</v>
       </c>
       <c r="D5293">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E5293">
-        <v>40</v>
+        <v>804</v>
       </c>
     </row>
     <row r="5294">
@@ -100945,17 +100945,17 @@
       </c>
       <c r="B5294" t="inlineStr">
         <is>
-          <t>Okres Topoľčany</t>
+          <t>Okres Ružomberok</t>
         </is>
       </c>
       <c r="C5294">
-        <v>653</v>
+        <v>507</v>
       </c>
       <c r="D5294">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E5294">
-        <v>677</v>
+        <v>533</v>
       </c>
     </row>
     <row r="5295">
@@ -100964,17 +100964,17 @@
       </c>
       <c r="B5295" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Sabinov</t>
         </is>
       </c>
       <c r="C5295">
-        <v>493</v>
+        <v>207</v>
       </c>
       <c r="D5295">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E5295">
-        <v>533</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5296">
@@ -100983,17 +100983,17 @@
       </c>
       <c r="B5296" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Senec</t>
         </is>
       </c>
       <c r="C5296">
-        <v>766</v>
+        <v>685</v>
       </c>
       <c r="D5296">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E5296">
-        <v>779</v>
+        <v>716</v>
       </c>
     </row>
     <row r="5297">
@@ -101002,17 +101002,17 @@
       </c>
       <c r="B5297" t="inlineStr">
         <is>
-          <t>Okres Trnava</t>
+          <t>Okres Senica</t>
         </is>
       </c>
       <c r="C5297">
-        <v>85</v>
+        <v>241</v>
       </c>
       <c r="D5297">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E5297">
-        <v>95</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5298">
@@ -101021,17 +101021,17 @@
       </c>
       <c r="B5298" t="inlineStr">
         <is>
-          <t>Okres Turčianske Teplice</t>
+          <t>Okres Skalica</t>
         </is>
       </c>
       <c r="C5298">
-        <v>97</v>
+        <v>685</v>
       </c>
       <c r="D5298">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E5298">
-        <v>104</v>
+        <v>694</v>
       </c>
     </row>
     <row r="5299">
@@ -101040,17 +101040,17 @@
       </c>
       <c r="B5299" t="inlineStr">
         <is>
-          <t>Okres Tvrdošín</t>
+          <t>Okres Snina</t>
         </is>
       </c>
       <c r="C5299">
+        <v>275</v>
+      </c>
+      <c r="D5299">
         <v>13</v>
       </c>
-      <c r="D5299">
-        <v>0</v>
-      </c>
       <c r="E5299">
-        <v>13</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5300">
@@ -101059,17 +101059,17 @@
       </c>
       <c r="B5300" t="inlineStr">
         <is>
-          <t>Okres Veľký Krtíš</t>
+          <t>Okres Sobrance</t>
         </is>
       </c>
       <c r="C5300">
-        <v>303</v>
+        <v>169</v>
       </c>
       <c r="D5300">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E5300">
-        <v>303</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5301">
@@ -101078,17 +101078,17 @@
       </c>
       <c r="B5301" t="inlineStr">
         <is>
-          <t>Okres Vranov nad Topľou</t>
+          <t>Okres Spišská Nová Ves</t>
         </is>
       </c>
       <c r="C5301">
-        <v>262</v>
+        <v>505</v>
       </c>
       <c r="D5301">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E5301">
-        <v>275</v>
+        <v>530</v>
       </c>
     </row>
     <row r="5302">
@@ -101097,17 +101097,17 @@
       </c>
       <c r="B5302" t="inlineStr">
         <is>
-          <t>Okres Zlaté Moravce</t>
+          <t>Okres Stará Ľubovňa</t>
         </is>
       </c>
       <c r="C5302">
-        <v>5</v>
+        <v>158</v>
       </c>
       <c r="D5302">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E5302">
-        <v>7</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5303">
@@ -101116,17 +101116,17 @@
       </c>
       <c r="B5303" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Stropkov</t>
         </is>
       </c>
       <c r="C5303">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="D5303">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5303">
-        <v>78</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5304">
@@ -101135,17 +101135,17 @@
       </c>
       <c r="B5304" t="inlineStr">
         <is>
-          <t>Okres Žarnovica</t>
+          <t>Okres Svidník</t>
         </is>
       </c>
       <c r="C5304">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="D5304">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5304">
-        <v>2</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5305">
@@ -101154,17 +101154,17 @@
       </c>
       <c r="B5305" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Šaľa</t>
         </is>
       </c>
       <c r="C5305">
-        <v>403</v>
+        <v>172</v>
       </c>
       <c r="D5305">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E5305">
-        <v>422</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5306">
@@ -101173,17 +101173,1442 @@
       </c>
       <c r="B5306" t="inlineStr">
         <is>
+          <t>Okres Topoľčany</t>
+        </is>
+      </c>
+      <c r="C5306">
+        <v>2067</v>
+      </c>
+      <c r="D5306">
+        <v>151</v>
+      </c>
+      <c r="E5306">
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="5307">
+      <c r="A5307" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B5307" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C5307">
+        <v>727</v>
+      </c>
+      <c r="D5307">
+        <v>59</v>
+      </c>
+      <c r="E5307">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="5308">
+      <c r="A5308" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B5308" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C5308">
+        <v>1114</v>
+      </c>
+      <c r="D5308">
+        <v>27</v>
+      </c>
+      <c r="E5308">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="5309">
+      <c r="A5309" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B5309" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C5309">
+        <v>746</v>
+      </c>
+      <c r="D5309">
+        <v>47</v>
+      </c>
+      <c r="E5309">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="5310">
+      <c r="A5310" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B5310" t="inlineStr">
+        <is>
+          <t>Okres Turčianske Teplice</t>
+        </is>
+      </c>
+      <c r="C5310">
+        <v>97</v>
+      </c>
+      <c r="D5310">
+        <v>7</v>
+      </c>
+      <c r="E5310">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5311">
+      <c r="A5311" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B5311" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C5311">
+        <v>243</v>
+      </c>
+      <c r="D5311">
+        <v>2</v>
+      </c>
+      <c r="E5311">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5312">
+      <c r="A5312" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B5312" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C5312">
+        <v>494</v>
+      </c>
+      <c r="D5312">
+        <v>0</v>
+      </c>
+      <c r="E5312">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="5313">
+      <c r="A5313" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B5313" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C5313">
+        <v>283</v>
+      </c>
+      <c r="D5313">
+        <v>14</v>
+      </c>
+      <c r="E5313">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5314">
+      <c r="A5314" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B5314" t="inlineStr">
+        <is>
+          <t>Okres Zlaté Moravce</t>
+        </is>
+      </c>
+      <c r="C5314">
+        <v>131</v>
+      </c>
+      <c r="D5314">
+        <v>5</v>
+      </c>
+      <c r="E5314">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5315">
+      <c r="A5315" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B5315" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C5315">
+        <v>322</v>
+      </c>
+      <c r="D5315">
+        <v>12</v>
+      </c>
+      <c r="E5315">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5316">
+      <c r="A5316" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B5316" t="inlineStr">
+        <is>
+          <t>Okres Žarnovica</t>
+        </is>
+      </c>
+      <c r="C5316">
+        <v>3</v>
+      </c>
+      <c r="D5316">
+        <v>0</v>
+      </c>
+      <c r="E5316">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5317">
+      <c r="A5317" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B5317" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C5317">
+        <v>575</v>
+      </c>
+      <c r="D5317">
+        <v>31</v>
+      </c>
+      <c r="E5317">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="5318">
+      <c r="A5318" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B5318" t="inlineStr">
+        <is>
           <t>Okres Žilina</t>
         </is>
       </c>
-      <c r="C5306">
+      <c r="C5318">
+        <v>833</v>
+      </c>
+      <c r="D5318">
+        <v>61</v>
+      </c>
+      <c r="E5318">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="5319">
+      <c r="A5319" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5319" t="inlineStr">
+        <is>
+          <t>Okres Banská Bystrica</t>
+        </is>
+      </c>
+      <c r="C5319">
+        <v>967</v>
+      </c>
+      <c r="D5319">
+        <v>44</v>
+      </c>
+      <c r="E5319">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="5320">
+      <c r="A5320" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5320" t="inlineStr">
+        <is>
+          <t>Okres Banská Štiavnica</t>
+        </is>
+      </c>
+      <c r="C5320">
+        <v>20</v>
+      </c>
+      <c r="D5320">
+        <v>0</v>
+      </c>
+      <c r="E5320">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5321">
+      <c r="A5321" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5321" t="inlineStr">
+        <is>
+          <t>Okres Bardejov</t>
+        </is>
+      </c>
+      <c r="C5321">
+        <v>32</v>
+      </c>
+      <c r="D5321">
+        <v>0</v>
+      </c>
+      <c r="E5321">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5322">
+      <c r="A5322" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5322" t="inlineStr">
+        <is>
+          <t>Okres Bratislava I</t>
+        </is>
+      </c>
+      <c r="C5322">
+        <v>114</v>
+      </c>
+      <c r="D5322">
+        <v>5</v>
+      </c>
+      <c r="E5322">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5323">
+      <c r="A5323" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5323" t="inlineStr">
+        <is>
+          <t>Okres Bratislava II</t>
+        </is>
+      </c>
+      <c r="C5323">
+        <v>294</v>
+      </c>
+      <c r="D5323">
+        <v>10</v>
+      </c>
+      <c r="E5323">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5324">
+      <c r="A5324" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5324" t="inlineStr">
+        <is>
+          <t>Okres Bratislava III</t>
+        </is>
+      </c>
+      <c r="C5324">
+        <v>359</v>
+      </c>
+      <c r="D5324">
+        <v>14</v>
+      </c>
+      <c r="E5324">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5325">
+      <c r="A5325" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5325" t="inlineStr">
+        <is>
+          <t>Okres Bratislava IV</t>
+        </is>
+      </c>
+      <c r="C5325">
+        <v>12</v>
+      </c>
+      <c r="D5325">
+        <v>0</v>
+      </c>
+      <c r="E5325">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5326">
+      <c r="A5326" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5326" t="inlineStr">
+        <is>
+          <t>Okres Bratislava V</t>
+        </is>
+      </c>
+      <c r="C5326">
+        <v>251</v>
+      </c>
+      <c r="D5326">
+        <v>2</v>
+      </c>
+      <c r="E5326">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5327">
+      <c r="A5327" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5327" t="inlineStr">
+        <is>
+          <t>Okres Brezno</t>
+        </is>
+      </c>
+      <c r="C5327">
+        <v>67</v>
+      </c>
+      <c r="D5327">
+        <v>80</v>
+      </c>
+      <c r="E5327">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5328">
+      <c r="A5328" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5328" t="inlineStr">
+        <is>
+          <t>Okres Bytča</t>
+        </is>
+      </c>
+      <c r="C5328">
+        <v>151</v>
+      </c>
+      <c r="D5328">
+        <v>14</v>
+      </c>
+      <c r="E5328">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5329">
+      <c r="A5329" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5329" t="inlineStr">
+        <is>
+          <t>Okres Čadca</t>
+        </is>
+      </c>
+      <c r="C5329">
+        <v>679</v>
+      </c>
+      <c r="D5329">
+        <v>17</v>
+      </c>
+      <c r="E5329">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="5330">
+      <c r="A5330" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5330" t="inlineStr">
+        <is>
+          <t>Okres Detva</t>
+        </is>
+      </c>
+      <c r="C5330">
+        <v>7</v>
+      </c>
+      <c r="D5330">
+        <v>1</v>
+      </c>
+      <c r="E5330">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5331">
+      <c r="A5331" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5331" t="inlineStr">
+        <is>
+          <t>Okres Dolný Kubín</t>
+        </is>
+      </c>
+      <c r="C5331">
+        <v>99</v>
+      </c>
+      <c r="D5331">
+        <v>3</v>
+      </c>
+      <c r="E5331">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5332">
+      <c r="A5332" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5332" t="inlineStr">
+        <is>
+          <t>Okres Dunajská Streda</t>
+        </is>
+      </c>
+      <c r="C5332">
+        <v>499</v>
+      </c>
+      <c r="D5332">
+        <v>57</v>
+      </c>
+      <c r="E5332">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="5333">
+      <c r="A5333" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5333" t="inlineStr">
+        <is>
+          <t>Okres Galanta</t>
+        </is>
+      </c>
+      <c r="C5333">
+        <v>559</v>
+      </c>
+      <c r="D5333">
+        <v>73</v>
+      </c>
+      <c r="E5333">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="5334">
+      <c r="A5334" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5334" t="inlineStr">
+        <is>
+          <t>Okres Hlohovec</t>
+        </is>
+      </c>
+      <c r="C5334">
+        <v>82</v>
+      </c>
+      <c r="D5334">
+        <v>17</v>
+      </c>
+      <c r="E5334">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5335">
+      <c r="A5335" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5335" t="inlineStr">
+        <is>
+          <t>Okres Humenné</t>
+        </is>
+      </c>
+      <c r="C5335">
+        <v>95</v>
+      </c>
+      <c r="D5335">
+        <v>3</v>
+      </c>
+      <c r="E5335">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5336">
+      <c r="A5336" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5336" t="inlineStr">
+        <is>
+          <t>Okres Ilava</t>
+        </is>
+      </c>
+      <c r="C5336">
+        <v>168</v>
+      </c>
+      <c r="D5336">
+        <v>6</v>
+      </c>
+      <c r="E5336">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5337">
+      <c r="A5337" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5337" t="inlineStr">
+        <is>
+          <t>Okres Kežmarok</t>
+        </is>
+      </c>
+      <c r="C5337">
+        <v>108</v>
+      </c>
+      <c r="D5337">
+        <v>8</v>
+      </c>
+      <c r="E5337">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5338">
+      <c r="A5338" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5338" t="inlineStr">
+        <is>
+          <t>Okres Komárno</t>
+        </is>
+      </c>
+      <c r="C5338">
+        <v>351</v>
+      </c>
+      <c r="D5338">
+        <v>27</v>
+      </c>
+      <c r="E5338">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="5339">
+      <c r="A5339" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5339" t="inlineStr">
+        <is>
+          <t>Okres Košice I</t>
+        </is>
+      </c>
+      <c r="C5339">
+        <v>5</v>
+      </c>
+      <c r="D5339">
+        <v>0</v>
+      </c>
+      <c r="E5339">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5340">
+      <c r="A5340" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5340" t="inlineStr">
+        <is>
+          <t>Okres Košice II</t>
+        </is>
+      </c>
+      <c r="C5340">
+        <v>33</v>
+      </c>
+      <c r="D5340">
+        <v>0</v>
+      </c>
+      <c r="E5340">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5341">
+      <c r="A5341" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5341" t="inlineStr">
+        <is>
+          <t>Okres Košice IV</t>
+        </is>
+      </c>
+      <c r="C5341">
+        <v>123</v>
+      </c>
+      <c r="D5341">
+        <v>5</v>
+      </c>
+      <c r="E5341">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5342">
+      <c r="A5342" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5342" t="inlineStr">
+        <is>
+          <t>Okres Kysucké Nové Mesto</t>
+        </is>
+      </c>
+      <c r="C5342">
+        <v>178</v>
+      </c>
+      <c r="D5342">
+        <v>13</v>
+      </c>
+      <c r="E5342">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5343">
+      <c r="A5343" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5343" t="inlineStr">
+        <is>
+          <t>Okres Levice</t>
+        </is>
+      </c>
+      <c r="C5343">
+        <v>144</v>
+      </c>
+      <c r="D5343">
+        <v>14</v>
+      </c>
+      <c r="E5343">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5344">
+      <c r="A5344" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5344" t="inlineStr">
+        <is>
+          <t>Okres Levoča</t>
+        </is>
+      </c>
+      <c r="C5344">
+        <v>154</v>
+      </c>
+      <c r="D5344">
+        <v>16</v>
+      </c>
+      <c r="E5344">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5345">
+      <c r="A5345" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5345" t="inlineStr">
+        <is>
+          <t>Okres Liptovský Mikuláš</t>
+        </is>
+      </c>
+      <c r="C5345">
+        <v>315</v>
+      </c>
+      <c r="D5345">
+        <v>22</v>
+      </c>
+      <c r="E5345">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="5346">
+      <c r="A5346" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5346" t="inlineStr">
+        <is>
+          <t>Okres Lučenec</t>
+        </is>
+      </c>
+      <c r="C5346">
+        <v>236</v>
+      </c>
+      <c r="D5346">
+        <v>6</v>
+      </c>
+      <c r="E5346">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5347">
+      <c r="A5347" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5347" t="inlineStr">
+        <is>
+          <t>Okres Malacky</t>
+        </is>
+      </c>
+      <c r="C5347">
+        <v>4</v>
+      </c>
+      <c r="D5347">
+        <v>1</v>
+      </c>
+      <c r="E5347">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5348">
+      <c r="A5348" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5348" t="inlineStr">
+        <is>
+          <t>Okres Michalovce</t>
+        </is>
+      </c>
+      <c r="C5348">
+        <v>126</v>
+      </c>
+      <c r="D5348">
+        <v>4</v>
+      </c>
+      <c r="E5348">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5349">
+      <c r="A5349" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5349" t="inlineStr">
+        <is>
+          <t>Okres Myjava</t>
+        </is>
+      </c>
+      <c r="C5349">
+        <v>178</v>
+      </c>
+      <c r="D5349">
+        <v>1</v>
+      </c>
+      <c r="E5349">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5350">
+      <c r="A5350" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5350" t="inlineStr">
+        <is>
+          <t>Okres Nitra</t>
+        </is>
+      </c>
+      <c r="C5350">
+        <v>88</v>
+      </c>
+      <c r="D5350">
+        <v>6</v>
+      </c>
+      <c r="E5350">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5351">
+      <c r="A5351" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5351" t="inlineStr">
+        <is>
+          <t>Okres Partizánske</t>
+        </is>
+      </c>
+      <c r="C5351">
+        <v>53</v>
+      </c>
+      <c r="D5351">
+        <v>12</v>
+      </c>
+      <c r="E5351">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5352">
+      <c r="A5352" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5352" t="inlineStr">
+        <is>
+          <t>Okres Pezinok</t>
+        </is>
+      </c>
+      <c r="C5352">
+        <v>416</v>
+      </c>
+      <c r="D5352">
+        <v>15</v>
+      </c>
+      <c r="E5352">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="5353">
+      <c r="A5353" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5353" t="inlineStr">
+        <is>
+          <t>Okres Piešťany</t>
+        </is>
+      </c>
+      <c r="C5353">
+        <v>29</v>
+      </c>
+      <c r="D5353">
+        <v>2</v>
+      </c>
+      <c r="E5353">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5354">
+      <c r="A5354" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5354" t="inlineStr">
+        <is>
+          <t>Okres Poprad</t>
+        </is>
+      </c>
+      <c r="C5354">
+        <v>307</v>
+      </c>
+      <c r="D5354">
+        <v>6</v>
+      </c>
+      <c r="E5354">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5355">
+      <c r="A5355" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5355" t="inlineStr">
+        <is>
+          <t>Okres Považská Bystrica</t>
+        </is>
+      </c>
+      <c r="C5355">
+        <v>92</v>
+      </c>
+      <c r="D5355">
+        <v>0</v>
+      </c>
+      <c r="E5355">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5356">
+      <c r="A5356" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5356" t="inlineStr">
+        <is>
+          <t>Okres Prešov</t>
+        </is>
+      </c>
+      <c r="C5356">
+        <v>78</v>
+      </c>
+      <c r="D5356">
+        <v>3</v>
+      </c>
+      <c r="E5356">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5357">
+      <c r="A5357" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5357" t="inlineStr">
+        <is>
+          <t>Okres Prievidza</t>
+        </is>
+      </c>
+      <c r="C5357">
+        <v>380</v>
+      </c>
+      <c r="D5357">
+        <v>14</v>
+      </c>
+      <c r="E5357">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="5358">
+      <c r="A5358" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5358" t="inlineStr">
+        <is>
+          <t>Okres Revúca</t>
+        </is>
+      </c>
+      <c r="C5358">
+        <v>396</v>
+      </c>
+      <c r="D5358">
+        <v>21</v>
+      </c>
+      <c r="E5358">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5359">
+      <c r="A5359" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5359" t="inlineStr">
+        <is>
+          <t>Okres Rimavská Sobota</t>
+        </is>
+      </c>
+      <c r="C5359">
+        <v>190</v>
+      </c>
+      <c r="D5359">
+        <v>6</v>
+      </c>
+      <c r="E5359">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5360">
+      <c r="A5360" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5360" t="inlineStr">
+        <is>
+          <t>Okres Rožňava</t>
+        </is>
+      </c>
+      <c r="C5360">
+        <v>247</v>
+      </c>
+      <c r="D5360">
+        <v>8</v>
+      </c>
+      <c r="E5360">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5361">
+      <c r="A5361" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5361" t="inlineStr">
+        <is>
+          <t>Okres Ružomberok</t>
+        </is>
+      </c>
+      <c r="C5361">
+        <v>53</v>
+      </c>
+      <c r="D5361">
+        <v>2</v>
+      </c>
+      <c r="E5361">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5362">
+      <c r="A5362" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5362" t="inlineStr">
+        <is>
+          <t>Okres Sabinov</t>
+        </is>
+      </c>
+      <c r="C5362">
+        <v>131</v>
+      </c>
+      <c r="D5362">
+        <v>2</v>
+      </c>
+      <c r="E5362">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5363">
+      <c r="A5363" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5363" t="inlineStr">
+        <is>
+          <t>Okres Senec</t>
+        </is>
+      </c>
+      <c r="C5363">
+        <v>169</v>
+      </c>
+      <c r="D5363">
+        <v>7</v>
+      </c>
+      <c r="E5363">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5364">
+      <c r="A5364" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5364" t="inlineStr">
+        <is>
+          <t>Okres Senica</t>
+        </is>
+      </c>
+      <c r="C5364">
+        <v>1</v>
+      </c>
+      <c r="D5364">
+        <v>1</v>
+      </c>
+      <c r="E5364">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5365">
+      <c r="A5365" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5365" t="inlineStr">
+        <is>
+          <t>Okres Skalica</t>
+        </is>
+      </c>
+      <c r="C5365">
+        <v>313</v>
+      </c>
+      <c r="D5365">
+        <v>11</v>
+      </c>
+      <c r="E5365">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5366">
+      <c r="A5366" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5366" t="inlineStr">
+        <is>
+          <t>Okres Spišská Nová Ves</t>
+        </is>
+      </c>
+      <c r="C5366">
+        <v>33</v>
+      </c>
+      <c r="D5366">
+        <v>1</v>
+      </c>
+      <c r="E5366">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5367">
+      <c r="A5367" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5367" t="inlineStr">
+        <is>
+          <t>Okres Stará Ľubovňa</t>
+        </is>
+      </c>
+      <c r="C5367">
+        <v>133</v>
+      </c>
+      <c r="D5367">
+        <v>14</v>
+      </c>
+      <c r="E5367">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5368">
+      <c r="A5368" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5368" t="inlineStr">
+        <is>
+          <t>Okres Stropkov</t>
+        </is>
+      </c>
+      <c r="C5368">
+        <v>3</v>
+      </c>
+      <c r="D5368">
+        <v>0</v>
+      </c>
+      <c r="E5368">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5369">
+      <c r="A5369" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5369" t="inlineStr">
+        <is>
+          <t>Okres Svidník</t>
+        </is>
+      </c>
+      <c r="C5369">
+        <v>39</v>
+      </c>
+      <c r="D5369">
+        <v>1</v>
+      </c>
+      <c r="E5369">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5370">
+      <c r="A5370" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5370" t="inlineStr">
+        <is>
+          <t>Okres Topoľčany</t>
+        </is>
+      </c>
+      <c r="C5370">
+        <v>439</v>
+      </c>
+      <c r="D5370">
+        <v>25</v>
+      </c>
+      <c r="E5370">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="5371">
+      <c r="A5371" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5371" t="inlineStr">
+        <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C5371">
+        <v>346</v>
+      </c>
+      <c r="D5371">
+        <v>15</v>
+      </c>
+      <c r="E5371">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="5372">
+      <c r="A5372" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5372" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C5372">
         <v>576</v>
       </c>
-      <c r="D5306">
-        <v>32</v>
-      </c>
-      <c r="E5306">
-        <v>608</v>
+      <c r="D5372">
+        <v>19</v>
+      </c>
+      <c r="E5372">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="5373">
+      <c r="A5373" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5373" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C5373">
+        <v>145</v>
+      </c>
+      <c r="D5373">
+        <v>11</v>
+      </c>
+      <c r="E5373">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5374">
+      <c r="A5374" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5374" t="inlineStr">
+        <is>
+          <t>Okres Turčianske Teplice</t>
+        </is>
+      </c>
+      <c r="C5374">
+        <v>60</v>
+      </c>
+      <c r="D5374">
+        <v>2</v>
+      </c>
+      <c r="E5374">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5375">
+      <c r="A5375" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5375" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C5375">
+        <v>21</v>
+      </c>
+      <c r="D5375">
+        <v>0</v>
+      </c>
+      <c r="E5375">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5376">
+      <c r="A5376" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5376" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C5376">
+        <v>261</v>
+      </c>
+      <c r="D5376">
+        <v>1</v>
+      </c>
+      <c r="E5376">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5377">
+      <c r="A5377" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5377" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C5377">
+        <v>194</v>
+      </c>
+      <c r="D5377">
+        <v>18</v>
+      </c>
+      <c r="E5377">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5378">
+      <c r="A5378" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5378" t="inlineStr">
+        <is>
+          <t>Okres Zlaté Moravce</t>
+        </is>
+      </c>
+      <c r="C5378">
+        <v>2</v>
+      </c>
+      <c r="D5378">
+        <v>0</v>
+      </c>
+      <c r="E5378">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5379">
+      <c r="A5379" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5379" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C5379">
+        <v>292</v>
+      </c>
+      <c r="D5379">
+        <v>33</v>
+      </c>
+      <c r="E5379">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5380">
+      <c r="A5380" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5380" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C5380">
+        <v>297</v>
+      </c>
+      <c r="D5380">
+        <v>17</v>
+      </c>
+      <c r="E5380">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5381">
+      <c r="A5381" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B5381" t="inlineStr">
+        <is>
+          <t>Okres Žilina</t>
+        </is>
+      </c>
+      <c r="C5381">
+        <v>396</v>
+      </c>
+      <c r="D5381">
+        <v>31</v>
+      </c>
+      <c r="E5381">
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: st 20. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_AgTests_District.xlsx
+++ b/OpenData_Slovakia_Covid_AgTests_District.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5723"/>
+  <dimension ref="A1:E5732"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -97168,13 +97168,13 @@
         </is>
       </c>
       <c r="C5095">
-        <v>2427</v>
+        <v>2431</v>
       </c>
       <c r="D5095">
         <v>39</v>
       </c>
       <c r="E5095">
-        <v>2466</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="5096">
@@ -98631,13 +98631,13 @@
         </is>
       </c>
       <c r="C5172">
-        <v>2764</v>
+        <v>2772</v>
       </c>
       <c r="D5172">
         <v>124</v>
       </c>
       <c r="E5172">
-        <v>2888</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="5173">
@@ -100132,13 +100132,13 @@
         </is>
       </c>
       <c r="C5251">
-        <v>2275</v>
+        <v>2278</v>
       </c>
       <c r="D5251">
         <v>103</v>
       </c>
       <c r="E5251">
-        <v>2378</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="5252">
@@ -101614,13 +101614,13 @@
         </is>
       </c>
       <c r="C5329">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="D5329">
         <v>68</v>
       </c>
       <c r="E5329">
-        <v>1740</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="5330">
@@ -102146,13 +102146,13 @@
         </is>
       </c>
       <c r="C5357">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="D5357">
         <v>27</v>
       </c>
       <c r="E5357">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="5358">
@@ -103096,13 +103096,13 @@
         </is>
       </c>
       <c r="C5407">
-        <v>1672</v>
+        <v>1676</v>
       </c>
       <c r="D5407">
         <v>61</v>
       </c>
       <c r="E5407">
-        <v>1733</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="5408">
@@ -103438,13 +103438,13 @@
         </is>
       </c>
       <c r="C5425">
-        <v>773</v>
+        <v>788</v>
       </c>
       <c r="D5425">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E5425">
-        <v>806</v>
+        <v>824</v>
       </c>
     </row>
     <row r="5426">
@@ -106592,13 +106592,13 @@
         </is>
       </c>
       <c r="C5591">
-        <v>940</v>
+        <v>1157</v>
       </c>
       <c r="D5591">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E5591">
-        <v>973</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="5592">
@@ -106820,13 +106820,13 @@
         </is>
       </c>
       <c r="C5603">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D5603">
         <v>55</v>
       </c>
       <c r="E5603">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="5604">
@@ -107485,13 +107485,13 @@
         </is>
       </c>
       <c r="C5638">
-        <v>327</v>
+        <v>73</v>
       </c>
       <c r="D5638">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E5638">
-        <v>333</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5639">
@@ -107656,13 +107656,13 @@
         </is>
       </c>
       <c r="C5647">
-        <v>1033</v>
+        <v>1037</v>
       </c>
       <c r="D5647">
         <v>33</v>
       </c>
       <c r="E5647">
-        <v>1066</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="5648">
@@ -107789,13 +107789,13 @@
         </is>
       </c>
       <c r="C5654">
-        <v>1330</v>
+        <v>1323</v>
       </c>
       <c r="D5654">
         <v>38</v>
       </c>
       <c r="E5654">
-        <v>1368</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="5655">
@@ -107994,17 +107994,17 @@
       </c>
       <c r="B5665" t="inlineStr">
         <is>
-          <t>Okres Banská Bystrica</t>
+          <t>Okres Bánovce nad Bebravou</t>
         </is>
       </c>
       <c r="C5665">
-        <v>1788</v>
+        <v>0</v>
       </c>
       <c r="D5665">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="E5665">
-        <v>1825</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5666">
@@ -108013,17 +108013,17 @@
       </c>
       <c r="B5666" t="inlineStr">
         <is>
-          <t>Okres Banská Štiavnica</t>
+          <t>Okres Banská Bystrica</t>
         </is>
       </c>
       <c r="C5666">
-        <v>378</v>
+        <v>1823</v>
       </c>
       <c r="D5666">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="E5666">
-        <v>401</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="5667">
@@ -108032,17 +108032,17 @@
       </c>
       <c r="B5667" t="inlineStr">
         <is>
-          <t>Okres Bardejov</t>
+          <t>Okres Banská Štiavnica</t>
         </is>
       </c>
       <c r="C5667">
-        <v>84</v>
+        <v>378</v>
       </c>
       <c r="D5667">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E5667">
-        <v>85</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5668">
@@ -108051,17 +108051,17 @@
       </c>
       <c r="B5668" t="inlineStr">
         <is>
-          <t>Okres Bratislava I</t>
+          <t>Okres Bardejov</t>
         </is>
       </c>
       <c r="C5668">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="D5668">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5668">
-        <v>160</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5669">
@@ -108070,17 +108070,17 @@
       </c>
       <c r="B5669" t="inlineStr">
         <is>
-          <t>Okres Bratislava II</t>
+          <t>Okres Bratislava I</t>
         </is>
       </c>
       <c r="C5669">
-        <v>1258</v>
+        <v>232</v>
       </c>
       <c r="D5669">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E5669">
-        <v>1325</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5670">
@@ -108089,17 +108089,17 @@
       </c>
       <c r="B5670" t="inlineStr">
         <is>
-          <t>Okres Bratislava III</t>
+          <t>Okres Bratislava II</t>
         </is>
       </c>
       <c r="C5670">
-        <v>806</v>
+        <v>1542</v>
       </c>
       <c r="D5670">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="E5670">
-        <v>817</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="5671">
@@ -108108,17 +108108,17 @@
       </c>
       <c r="B5671" t="inlineStr">
         <is>
-          <t>Okres Bratislava V</t>
+          <t>Okres Bratislava III</t>
         </is>
       </c>
       <c r="C5671">
-        <v>105</v>
+        <v>879</v>
       </c>
       <c r="D5671">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E5671">
-        <v>114</v>
+        <v>901</v>
       </c>
     </row>
     <row r="5672">
@@ -108127,17 +108127,17 @@
       </c>
       <c r="B5672" t="inlineStr">
         <is>
-          <t>Okres Brezno</t>
+          <t>Okres Bratislava IV</t>
         </is>
       </c>
       <c r="C5672">
-        <v>29</v>
+        <v>252</v>
       </c>
       <c r="D5672">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E5672">
-        <v>34</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5673">
@@ -108146,17 +108146,17 @@
       </c>
       <c r="B5673" t="inlineStr">
         <is>
-          <t>Okres Bytča</t>
+          <t>Okres Bratislava V</t>
         </is>
       </c>
       <c r="C5673">
-        <v>303</v>
+        <v>365</v>
       </c>
       <c r="D5673">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E5673">
-        <v>334</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5674">
@@ -108165,17 +108165,17 @@
       </c>
       <c r="B5674" t="inlineStr">
         <is>
-          <t>Okres Čadca</t>
+          <t>Okres Brezno</t>
         </is>
       </c>
       <c r="C5674">
-        <v>554</v>
+        <v>29</v>
       </c>
       <c r="D5674">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E5674">
-        <v>565</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5675">
@@ -108184,17 +108184,17 @@
       </c>
       <c r="B5675" t="inlineStr">
         <is>
-          <t>Okres Detva</t>
+          <t>Okres Bytča</t>
         </is>
       </c>
       <c r="C5675">
-        <v>3</v>
+        <v>303</v>
       </c>
       <c r="D5675">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E5675">
-        <v>3</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5676">
@@ -108203,17 +108203,17 @@
       </c>
       <c r="B5676" t="inlineStr">
         <is>
-          <t>Okres Dolný Kubín</t>
+          <t>Okres Čadca</t>
         </is>
       </c>
       <c r="C5676">
-        <v>207</v>
+        <v>1094</v>
       </c>
       <c r="D5676">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E5676">
-        <v>215</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="5677">
@@ -108222,17 +108222,17 @@
       </c>
       <c r="B5677" t="inlineStr">
         <is>
-          <t>Okres Dunajská Streda</t>
+          <t>Okres Detva</t>
         </is>
       </c>
       <c r="C5677">
-        <v>356</v>
+        <v>31</v>
       </c>
       <c r="D5677">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E5677">
-        <v>409</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5678">
@@ -108241,17 +108241,17 @@
       </c>
       <c r="B5678" t="inlineStr">
         <is>
-          <t>Okres Galanta</t>
+          <t>Okres Dolný Kubín</t>
         </is>
       </c>
       <c r="C5678">
-        <v>9</v>
+        <v>225</v>
       </c>
       <c r="D5678">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E5678">
-        <v>9</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5679">
@@ -108260,17 +108260,17 @@
       </c>
       <c r="B5679" t="inlineStr">
         <is>
-          <t>Okres Gelnica</t>
+          <t>Okres Dunajská Streda</t>
         </is>
       </c>
       <c r="C5679">
-        <v>1</v>
+        <v>418</v>
       </c>
       <c r="D5679">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="E5679">
-        <v>1</v>
+        <v>477</v>
       </c>
     </row>
     <row r="5680">
@@ -108279,17 +108279,17 @@
       </c>
       <c r="B5680" t="inlineStr">
         <is>
-          <t>Okres Humenné</t>
+          <t>Okres Galanta</t>
         </is>
       </c>
       <c r="C5680">
-        <v>260</v>
+        <v>9</v>
       </c>
       <c r="D5680">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E5680">
-        <v>274</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5681">
@@ -108298,17 +108298,17 @@
       </c>
       <c r="B5681" t="inlineStr">
         <is>
-          <t>Okres Ilava</t>
+          <t>Okres Gelnica</t>
         </is>
       </c>
       <c r="C5681">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5681">
         <v>0</v>
       </c>
       <c r="E5681">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5682">
@@ -108317,17 +108317,17 @@
       </c>
       <c r="B5682" t="inlineStr">
         <is>
-          <t>Okres Kežmarok</t>
+          <t>Okres Hlohovec</t>
         </is>
       </c>
       <c r="C5682">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D5682">
         <v>0</v>
       </c>
       <c r="E5682">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5683">
@@ -108336,17 +108336,17 @@
       </c>
       <c r="B5683" t="inlineStr">
         <is>
-          <t>Okres Komárno</t>
+          <t>Okres Humenné</t>
         </is>
       </c>
       <c r="C5683">
-        <v>488</v>
+        <v>261</v>
       </c>
       <c r="D5683">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="E5683">
-        <v>533</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5684">
@@ -108355,17 +108355,17 @@
       </c>
       <c r="B5684" t="inlineStr">
         <is>
-          <t>Okres Košice I</t>
+          <t>Okres Ilava</t>
         </is>
       </c>
       <c r="C5684">
-        <v>38</v>
+        <v>280</v>
       </c>
       <c r="D5684">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E5684">
-        <v>39</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5685">
@@ -108374,17 +108374,17 @@
       </c>
       <c r="B5685" t="inlineStr">
         <is>
-          <t>Okres Košice II</t>
+          <t>Okres Kežmarok</t>
         </is>
       </c>
       <c r="C5685">
-        <v>807</v>
+        <v>179</v>
       </c>
       <c r="D5685">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E5685">
-        <v>813</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5686">
@@ -108393,17 +108393,17 @@
       </c>
       <c r="B5686" t="inlineStr">
         <is>
-          <t>Okres Košice IV</t>
+          <t>Okres Komárno</t>
         </is>
       </c>
       <c r="C5686">
-        <v>186</v>
+        <v>489</v>
       </c>
       <c r="D5686">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="E5686">
-        <v>189</v>
+        <v>534</v>
       </c>
     </row>
     <row r="5687">
@@ -108412,17 +108412,17 @@
       </c>
       <c r="B5687" t="inlineStr">
         <is>
-          <t>Okres Kysucké Nové Mesto</t>
+          <t>Okres Košice I</t>
         </is>
       </c>
       <c r="C5687">
-        <v>274</v>
+        <v>54</v>
       </c>
       <c r="D5687">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E5687">
-        <v>288</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5688">
@@ -108431,17 +108431,17 @@
       </c>
       <c r="B5688" t="inlineStr">
         <is>
-          <t>Okres Levice</t>
+          <t>Okres Košice II</t>
         </is>
       </c>
       <c r="C5688">
-        <v>1181</v>
+        <v>808</v>
       </c>
       <c r="D5688">
-        <v>132</v>
+        <v>6</v>
       </c>
       <c r="E5688">
-        <v>1313</v>
+        <v>814</v>
       </c>
     </row>
     <row r="5689">
@@ -108450,17 +108450,17 @@
       </c>
       <c r="B5689" t="inlineStr">
         <is>
-          <t>Okres Levoča</t>
+          <t>Okres Košice IV</t>
         </is>
       </c>
       <c r="C5689">
-        <v>213</v>
+        <v>286</v>
       </c>
       <c r="D5689">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E5689">
-        <v>218</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5690">
@@ -108469,17 +108469,17 @@
       </c>
       <c r="B5690" t="inlineStr">
         <is>
-          <t>Okres Liptovský Mikuláš</t>
+          <t>Okres Kysucké Nové Mesto</t>
         </is>
       </c>
       <c r="C5690">
-        <v>691</v>
+        <v>287</v>
       </c>
       <c r="D5690">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E5690">
-        <v>711</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5691">
@@ -108488,17 +108488,17 @@
       </c>
       <c r="B5691" t="inlineStr">
         <is>
-          <t>Okres Lučenec</t>
+          <t>Okres Levice</t>
         </is>
       </c>
       <c r="C5691">
-        <v>514</v>
+        <v>1644</v>
       </c>
       <c r="D5691">
-        <v>6</v>
+        <v>156</v>
       </c>
       <c r="E5691">
-        <v>520</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="5692">
@@ -108507,17 +108507,17 @@
       </c>
       <c r="B5692" t="inlineStr">
         <is>
-          <t>Okres Malacky</t>
+          <t>Okres Levoča</t>
         </is>
       </c>
       <c r="C5692">
-        <v>13</v>
+        <v>213</v>
       </c>
       <c r="D5692">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5692">
-        <v>15</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5693">
@@ -108526,17 +108526,17 @@
       </c>
       <c r="B5693" t="inlineStr">
         <is>
-          <t>Okres Martin</t>
+          <t>Okres Liptovský Mikuláš</t>
         </is>
       </c>
       <c r="C5693">
-        <v>168</v>
+        <v>691</v>
       </c>
       <c r="D5693">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E5693">
-        <v>168</v>
+        <v>711</v>
       </c>
     </row>
     <row r="5694">
@@ -108545,17 +108545,17 @@
       </c>
       <c r="B5694" t="inlineStr">
         <is>
-          <t>Okres Michalovce</t>
+          <t>Okres Lučenec</t>
         </is>
       </c>
       <c r="C5694">
-        <v>460</v>
+        <v>519</v>
       </c>
       <c r="D5694">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E5694">
-        <v>470</v>
+        <v>525</v>
       </c>
     </row>
     <row r="5695">
@@ -108564,17 +108564,17 @@
       </c>
       <c r="B5695" t="inlineStr">
         <is>
-          <t>Okres Myjava</t>
+          <t>Okres Malacky</t>
         </is>
       </c>
       <c r="C5695">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="D5695">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5695">
-        <v>80</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5696">
@@ -108583,17 +108583,17 @@
       </c>
       <c r="B5696" t="inlineStr">
         <is>
-          <t>Okres Nitra</t>
+          <t>Okres Martin</t>
         </is>
       </c>
       <c r="C5696">
-        <v>149</v>
+        <v>4383</v>
       </c>
       <c r="D5696">
-        <v>9</v>
+        <v>158</v>
       </c>
       <c r="E5696">
-        <v>158</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="5697">
@@ -108602,17 +108602,17 @@
       </c>
       <c r="B5697" t="inlineStr">
         <is>
-          <t>Okres Nové Mesto nad Váhom</t>
+          <t>Okres Michalovce</t>
         </is>
       </c>
       <c r="C5697">
-        <v>4</v>
+        <v>460</v>
       </c>
       <c r="D5697">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E5697">
-        <v>5</v>
+        <v>470</v>
       </c>
     </row>
     <row r="5698">
@@ -108621,17 +108621,17 @@
       </c>
       <c r="B5698" t="inlineStr">
         <is>
-          <t>Okres Partizánske</t>
+          <t>Okres Myjava</t>
         </is>
       </c>
       <c r="C5698">
-        <v>417</v>
+        <v>80</v>
       </c>
       <c r="D5698">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E5698">
-        <v>493</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5699">
@@ -108640,17 +108640,17 @@
       </c>
       <c r="B5699" t="inlineStr">
         <is>
-          <t>Okres Pezinok</t>
+          <t>Okres Námestovo</t>
         </is>
       </c>
       <c r="C5699">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="D5699">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E5699">
-        <v>298</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5700">
@@ -108659,17 +108659,17 @@
       </c>
       <c r="B5700" t="inlineStr">
         <is>
-          <t>Okres Piešťany</t>
+          <t>Okres Nitra</t>
         </is>
       </c>
       <c r="C5700">
-        <v>289</v>
+        <v>162</v>
       </c>
       <c r="D5700">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E5700">
-        <v>293</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5701">
@@ -108678,17 +108678,17 @@
       </c>
       <c r="B5701" t="inlineStr">
         <is>
-          <t>Okres Poprad</t>
+          <t>Okres Nové Mesto nad Váhom</t>
         </is>
       </c>
       <c r="C5701">
-        <v>661</v>
+        <v>14</v>
       </c>
       <c r="D5701">
+        <v>1</v>
+      </c>
+      <c r="E5701">
         <v>15</v>
-      </c>
-      <c r="E5701">
-        <v>676</v>
       </c>
     </row>
     <row r="5702">
@@ -108697,17 +108697,17 @@
       </c>
       <c r="B5702" t="inlineStr">
         <is>
-          <t>Okres Považská Bystrica</t>
+          <t>Okres Nové Zámky</t>
         </is>
       </c>
       <c r="C5702">
-        <v>575</v>
+        <v>3</v>
       </c>
       <c r="D5702">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E5702">
-        <v>591</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5703">
@@ -108716,17 +108716,17 @@
       </c>
       <c r="B5703" t="inlineStr">
         <is>
-          <t>Okres Prešov</t>
+          <t>Okres Partizánske</t>
         </is>
       </c>
       <c r="C5703">
-        <v>329</v>
+        <v>425</v>
       </c>
       <c r="D5703">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="E5703">
-        <v>348</v>
+        <v>503</v>
       </c>
     </row>
     <row r="5704">
@@ -108735,17 +108735,17 @@
       </c>
       <c r="B5704" t="inlineStr">
         <is>
-          <t>Okres Prievidza</t>
+          <t>Okres Pezinok</t>
         </is>
       </c>
       <c r="C5704">
-        <v>432</v>
+        <v>288</v>
       </c>
       <c r="D5704">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5704">
-        <v>441</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5705">
@@ -108754,17 +108754,17 @@
       </c>
       <c r="B5705" t="inlineStr">
         <is>
-          <t>Okres Púchov</t>
+          <t>Okres Piešťany</t>
         </is>
       </c>
       <c r="C5705">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="D5705">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E5705">
-        <v>0</v>
+        <v>714</v>
       </c>
     </row>
     <row r="5706">
@@ -108773,17 +108773,17 @@
       </c>
       <c r="B5706" t="inlineStr">
         <is>
-          <t>Okres Revúca</t>
+          <t>Okres Poprad</t>
         </is>
       </c>
       <c r="C5706">
-        <v>538</v>
+        <v>1070</v>
       </c>
       <c r="D5706">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="E5706">
-        <v>587</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="5707">
@@ -108792,17 +108792,17 @@
       </c>
       <c r="B5707" t="inlineStr">
         <is>
-          <t>Okres Rimavská Sobota</t>
+          <t>Okres Považská Bystrica</t>
         </is>
       </c>
       <c r="C5707">
-        <v>453</v>
+        <v>843</v>
       </c>
       <c r="D5707">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="E5707">
-        <v>464</v>
+        <v>878</v>
       </c>
     </row>
     <row r="5708">
@@ -108811,17 +108811,17 @@
       </c>
       <c r="B5708" t="inlineStr">
         <is>
-          <t>Okres Ružomberok</t>
+          <t>Okres Prešov</t>
         </is>
       </c>
       <c r="C5708">
-        <v>967</v>
+        <v>342</v>
       </c>
       <c r="D5708">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E5708">
-        <v>974</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5709">
@@ -108830,17 +108830,17 @@
       </c>
       <c r="B5709" t="inlineStr">
         <is>
-          <t>Okres Senica</t>
+          <t>Okres Prievidza</t>
         </is>
       </c>
       <c r="C5709">
-        <v>0</v>
+        <v>439</v>
       </c>
       <c r="D5709">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E5709">
-        <v>2</v>
+        <v>449</v>
       </c>
     </row>
     <row r="5710">
@@ -108849,17 +108849,17 @@
       </c>
       <c r="B5710" t="inlineStr">
         <is>
-          <t>Okres Skalica</t>
+          <t>Okres Púchov</t>
         </is>
       </c>
       <c r="C5710">
-        <v>459</v>
+        <v>0</v>
       </c>
       <c r="D5710">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E5710">
-        <v>467</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5711">
@@ -108868,17 +108868,17 @@
       </c>
       <c r="B5711" t="inlineStr">
         <is>
-          <t>Okres Sobrance</t>
+          <t>Okres Revúca</t>
         </is>
       </c>
       <c r="C5711">
-        <v>144</v>
+        <v>538</v>
       </c>
       <c r="D5711">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="E5711">
-        <v>150</v>
+        <v>587</v>
       </c>
     </row>
     <row r="5712">
@@ -108887,17 +108887,17 @@
       </c>
       <c r="B5712" t="inlineStr">
         <is>
-          <t>Okres Spišská Nová Ves</t>
+          <t>Okres Rimavská Sobota</t>
         </is>
       </c>
       <c r="C5712">
-        <v>135</v>
+        <v>468</v>
       </c>
       <c r="D5712">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E5712">
-        <v>142</v>
+        <v>489</v>
       </c>
     </row>
     <row r="5713">
@@ -108906,17 +108906,17 @@
       </c>
       <c r="B5713" t="inlineStr">
         <is>
-          <t>Okres Stará Ľubovňa</t>
+          <t>Okres Rožňava</t>
         </is>
       </c>
       <c r="C5713">
-        <v>239</v>
+        <v>555</v>
       </c>
       <c r="D5713">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E5713">
-        <v>246</v>
+        <v>572</v>
       </c>
     </row>
     <row r="5714">
@@ -108925,17 +108925,17 @@
       </c>
       <c r="B5714" t="inlineStr">
         <is>
-          <t>Okres Topoľčany</t>
+          <t>Okres Ružomberok</t>
         </is>
       </c>
       <c r="C5714">
-        <v>457</v>
+        <v>1089</v>
       </c>
       <c r="D5714">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E5714">
-        <v>487</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="5715">
@@ -108944,17 +108944,17 @@
       </c>
       <c r="B5715" t="inlineStr">
         <is>
-          <t>Okres Trebišov</t>
+          <t>Okres Senica</t>
         </is>
       </c>
       <c r="C5715">
-        <v>761</v>
+        <v>7</v>
       </c>
       <c r="D5715">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="E5715">
-        <v>782</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5716">
@@ -108963,17 +108963,17 @@
       </c>
       <c r="B5716" t="inlineStr">
         <is>
-          <t>Okres Trenčín</t>
+          <t>Okres Skalica</t>
         </is>
       </c>
       <c r="C5716">
-        <v>570</v>
+        <v>459</v>
       </c>
       <c r="D5716">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E5716">
-        <v>598</v>
+        <v>467</v>
       </c>
     </row>
     <row r="5717">
@@ -108982,17 +108982,17 @@
       </c>
       <c r="B5717" t="inlineStr">
         <is>
-          <t>Okres Trnava</t>
+          <t>Okres Sobrance</t>
         </is>
       </c>
       <c r="C5717">
-        <v>267</v>
+        <v>144</v>
       </c>
       <c r="D5717">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E5717">
-        <v>278</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5718">
@@ -109001,17 +109001,17 @@
       </c>
       <c r="B5718" t="inlineStr">
         <is>
-          <t>Okres Turčianske Teplice</t>
+          <t>Okres Spišská Nová Ves</t>
         </is>
       </c>
       <c r="C5718">
-        <v>210</v>
+        <v>145</v>
       </c>
       <c r="D5718">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E5718">
-        <v>212</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5719">
@@ -109020,17 +109020,17 @@
       </c>
       <c r="B5719" t="inlineStr">
         <is>
-          <t>Okres Veľký Krtíš</t>
+          <t>Okres Stará Ľubovňa</t>
         </is>
       </c>
       <c r="C5719">
-        <v>454</v>
+        <v>259</v>
       </c>
       <c r="D5719">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5719">
-        <v>463</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5720">
@@ -109039,17 +109039,17 @@
       </c>
       <c r="B5720" t="inlineStr">
         <is>
-          <t>Okres Vranov nad Topľou</t>
+          <t>Okres Stropkov</t>
         </is>
       </c>
       <c r="C5720">
-        <v>329</v>
+        <v>2</v>
       </c>
       <c r="D5720">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E5720">
-        <v>344</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5721">
@@ -109058,17 +109058,17 @@
       </c>
       <c r="B5721" t="inlineStr">
         <is>
-          <t>Okres Zvolen</t>
+          <t>Okres Šaľa</t>
         </is>
       </c>
       <c r="C5721">
-        <v>151</v>
+        <v>4</v>
       </c>
       <c r="D5721">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E5721">
-        <v>156</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5722">
@@ -109077,17 +109077,17 @@
       </c>
       <c r="B5722" t="inlineStr">
         <is>
-          <t>Okres Žiar nad Hronom</t>
+          <t>Okres Topoľčany</t>
         </is>
       </c>
       <c r="C5722">
-        <v>352</v>
+        <v>852</v>
       </c>
       <c r="D5722">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="E5722">
-        <v>368</v>
+        <v>916</v>
       </c>
     </row>
     <row r="5723">
@@ -109096,17 +109096,188 @@
       </c>
       <c r="B5723" t="inlineStr">
         <is>
+          <t>Okres Trebišov</t>
+        </is>
+      </c>
+      <c r="C5723">
+        <v>774</v>
+      </c>
+      <c r="D5723">
+        <v>21</v>
+      </c>
+      <c r="E5723">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="5724">
+      <c r="A5724" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B5724" t="inlineStr">
+        <is>
+          <t>Okres Trenčín</t>
+        </is>
+      </c>
+      <c r="C5724">
+        <v>571</v>
+      </c>
+      <c r="D5724">
+        <v>30</v>
+      </c>
+      <c r="E5724">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="5725">
+      <c r="A5725" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B5725" t="inlineStr">
+        <is>
+          <t>Okres Trnava</t>
+        </is>
+      </c>
+      <c r="C5725">
+        <v>272</v>
+      </c>
+      <c r="D5725">
+        <v>12</v>
+      </c>
+      <c r="E5725">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5726">
+      <c r="A5726" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B5726" t="inlineStr">
+        <is>
+          <t>Okres Turčianske Teplice</t>
+        </is>
+      </c>
+      <c r="C5726">
+        <v>210</v>
+      </c>
+      <c r="D5726">
+        <v>2</v>
+      </c>
+      <c r="E5726">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5727">
+      <c r="A5727" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B5727" t="inlineStr">
+        <is>
+          <t>Okres Tvrdošín</t>
+        </is>
+      </c>
+      <c r="C5727">
+        <v>236</v>
+      </c>
+      <c r="D5727">
+        <v>0</v>
+      </c>
+      <c r="E5727">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5728">
+      <c r="A5728" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B5728" t="inlineStr">
+        <is>
+          <t>Okres Veľký Krtíš</t>
+        </is>
+      </c>
+      <c r="C5728">
+        <v>454</v>
+      </c>
+      <c r="D5728">
+        <v>9</v>
+      </c>
+      <c r="E5728">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="5729">
+      <c r="A5729" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B5729" t="inlineStr">
+        <is>
+          <t>Okres Vranov nad Topľou</t>
+        </is>
+      </c>
+      <c r="C5729">
+        <v>335</v>
+      </c>
+      <c r="D5729">
+        <v>16</v>
+      </c>
+      <c r="E5729">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5730">
+      <c r="A5730" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B5730" t="inlineStr">
+        <is>
+          <t>Okres Zvolen</t>
+        </is>
+      </c>
+      <c r="C5730">
+        <v>151</v>
+      </c>
+      <c r="D5730">
+        <v>5</v>
+      </c>
+      <c r="E5730">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5731">
+      <c r="A5731" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B5731" t="inlineStr">
+        <is>
+          <t>Okres Žiar nad Hronom</t>
+        </is>
+      </c>
+      <c r="C5731">
+        <v>355</v>
+      </c>
+      <c r="D5731">
+        <v>16</v>
+      </c>
+      <c r="E5731">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5732">
+      <c r="A5732" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B5732" t="inlineStr">
+        <is>
           <t>Okres Žilina</t>
         </is>
       </c>
-      <c r="C5723">
-        <v>1060</v>
-      </c>
-      <c r="D5723">
-        <v>39</v>
-      </c>
-      <c r="E5723">
-        <v>1099</v>
+      <c r="C5732">
+        <v>1250</v>
+      </c>
+      <c r="D5732">
+        <v>41</v>
+      </c>
+      <c r="E5732">
+        <v>1291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>